<commit_message>
small changes to template desc, gdmt ontology updated
</commit_message>
<xml_diff>
--- a/template-description.xlsx
+++ b/template-description.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Secondary_Drive/work/repos/FAIR-data/generic-dataset-metadata-template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88232250-A652-6747-AD08-77D1F4E5D01A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0FA80AF-DE41-CB4C-8235-9850CAD6AC54}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="68800" windowHeight="28340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1056" uniqueCount="523">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1056" uniqueCount="524">
   <si>
     <t>Element 
 (CEDAR)</t>
@@ -1376,9 +1376,6 @@
     <t>An established standard to which the dataset distribution conforms to.</t>
   </si>
   <si>
-    <t>https://www.sitepoint.com/mime-types-complete-list/</t>
-  </si>
-  <si>
     <t>distributionMediaType</t>
   </si>
   <si>
@@ -1608,6 +1605,12 @@
   </si>
   <si>
     <t>BASE url</t>
+  </si>
+  <si>
+    <t>FDC</t>
+  </si>
+  <si>
+    <t>MIME Types list</t>
   </si>
 </sst>
 </file>
@@ -3158,472 +3161,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="41" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="41" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="41" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="41" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="41" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="41" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="28" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="28" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="41" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="41" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="28" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="35" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="35" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="35" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="35" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="38" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="38" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="35" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="35" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="35" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="38" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="38" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="26" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="26" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="30" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="24" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="34" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="34" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="34" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="34" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="31" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="26" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="26" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="35" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="35" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="35" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="35" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="37" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="37" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="37" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="37" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="26" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="31" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="31" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="31" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="31" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="38" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="38" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="11" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -3666,6 +3204,24 @@
     <xf numFmtId="0" fontId="11" fillId="19" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="37" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="37" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -3684,6 +3240,78 @@
     <xf numFmtId="0" fontId="7" fillId="25" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -3693,9 +3321,394 @@
     <xf numFmtId="0" fontId="11" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="28" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="30" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="30" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="35" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="35" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="35" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="35" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="37" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="37" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="35" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="35" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="34" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="34" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="34" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="34" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="30" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="24" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="35" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="35" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="38" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="38" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="35" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="35" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="35" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="38" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="38" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="38" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="38" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="41" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="41" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="41" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="41" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="41" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="41" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="41" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="41" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="15" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -3726,6 +3739,12 @@
     <xf numFmtId="0" fontId="11" fillId="15" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3733,30 +3752,14 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="30" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="30" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3990,10 +3993,10 @@
   <dimension ref="A1:P1034"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D85" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D151" sqref="D151"/>
+      <selection pane="bottomRight" activeCell="D28" sqref="D28:D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4015,11 +4018,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="640" t="s">
+      <c r="A1" s="612" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="640"/>
-      <c r="C1" s="640"/>
+      <c r="B1" s="612"/>
+      <c r="C1" s="612"/>
       <c r="D1" s="44" t="s">
         <v>1</v>
       </c>
@@ -4057,11 +4060,11 @@
       <c r="P1" s="1"/>
     </row>
     <row r="2" spans="1:16" ht="69" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="639" t="s">
+      <c r="A2" s="611" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="639"/>
-      <c r="C2" s="639"/>
+      <c r="B2" s="611"/>
+      <c r="C2" s="611"/>
       <c r="D2" s="126" t="s">
         <v>10</v>
       </c>
@@ -4093,18 +4096,18 @@
       <c r="P2" s="2"/>
     </row>
     <row r="3" spans="1:16" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="634" t="s">
+      <c r="A3" s="606" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="634"/>
-      <c r="C3" s="634"/>
-      <c r="D3" s="706" t="s">
+      <c r="B3" s="606"/>
+      <c r="C3" s="606"/>
+      <c r="D3" s="551" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="708">
+      <c r="E3" s="553">
         <v>1</v>
       </c>
-      <c r="F3" s="709" t="str">
+      <c r="F3" s="554" t="str">
         <f>Namespace &amp; $A3</f>
         <v>http://vocab.fairdatacollective.org/dataset/properties/ResourceType</v>
       </c>
@@ -4134,12 +4137,12 @@
       </c>
     </row>
     <row r="4" spans="1:16" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="635"/>
-      <c r="B4" s="635"/>
-      <c r="C4" s="635"/>
-      <c r="D4" s="707"/>
-      <c r="E4" s="702"/>
-      <c r="F4" s="710"/>
+      <c r="A4" s="607"/>
+      <c r="B4" s="607"/>
+      <c r="C4" s="607"/>
+      <c r="D4" s="552"/>
+      <c r="E4" s="547"/>
+      <c r="F4" s="555"/>
       <c r="G4" s="190" t="s">
         <v>22</v>
       </c>
@@ -4166,18 +4169,18 @@
       </c>
     </row>
     <row r="5" spans="1:16" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="636" t="s">
+      <c r="A5" s="608" t="s">
         <v>259</v>
       </c>
-      <c r="B5" s="636"/>
-      <c r="C5" s="636"/>
-      <c r="D5" s="670" t="s">
+      <c r="B5" s="608"/>
+      <c r="C5" s="608"/>
+      <c r="D5" s="634" t="s">
         <v>25</v>
       </c>
-      <c r="E5" s="664">
+      <c r="E5" s="628">
         <v>1</v>
       </c>
-      <c r="F5" s="667" t="str">
+      <c r="F5" s="631" t="str">
         <f>Namespace &amp; ($A5)</f>
         <v>http://vocab.fairdatacollective.org/dataset/properties/DatasetIdentifier</v>
       </c>
@@ -4207,12 +4210,12 @@
       </c>
     </row>
     <row r="6" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="637"/>
-      <c r="B6" s="637"/>
-      <c r="C6" s="637"/>
-      <c r="D6" s="671"/>
-      <c r="E6" s="665"/>
-      <c r="F6" s="668"/>
+      <c r="A6" s="609"/>
+      <c r="B6" s="609"/>
+      <c r="C6" s="609"/>
+      <c r="D6" s="635"/>
+      <c r="E6" s="629"/>
+      <c r="F6" s="632"/>
       <c r="G6" s="53" t="s">
         <v>29</v>
       </c>
@@ -4239,12 +4242,12 @@
       </c>
     </row>
     <row r="7" spans="1:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="638"/>
-      <c r="B7" s="638"/>
-      <c r="C7" s="638"/>
-      <c r="D7" s="672"/>
-      <c r="E7" s="666"/>
-      <c r="F7" s="669"/>
+      <c r="A7" s="610"/>
+      <c r="B7" s="610"/>
+      <c r="C7" s="610"/>
+      <c r="D7" s="636"/>
+      <c r="E7" s="630"/>
+      <c r="F7" s="633"/>
       <c r="G7" s="203" t="s">
         <v>32</v>
       </c>
@@ -4272,18 +4275,18 @@
       </c>
     </row>
     <row r="8" spans="1:16" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="590" t="s">
+      <c r="A8" s="676" t="s">
         <v>33</v>
       </c>
-      <c r="B8" s="590"/>
-      <c r="C8" s="590"/>
-      <c r="D8" s="697" t="s">
+      <c r="B8" s="676"/>
+      <c r="C8" s="676"/>
+      <c r="D8" s="542" t="s">
         <v>276</v>
       </c>
-      <c r="E8" s="700" t="s">
+      <c r="E8" s="545" t="s">
         <v>34</v>
       </c>
-      <c r="F8" s="703" t="str">
+      <c r="F8" s="548" t="str">
         <f>Namespace &amp; ($A8)</f>
         <v>http://vocab.fairdatacollective.org/dataset/properties/RelatedResources</v>
       </c>
@@ -4313,12 +4316,12 @@
       </c>
     </row>
     <row r="9" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="591"/>
-      <c r="B9" s="591"/>
-      <c r="C9" s="591"/>
-      <c r="D9" s="698"/>
-      <c r="E9" s="701"/>
-      <c r="F9" s="704"/>
+      <c r="A9" s="677"/>
+      <c r="B9" s="677"/>
+      <c r="C9" s="677"/>
+      <c r="D9" s="543"/>
+      <c r="E9" s="546"/>
+      <c r="F9" s="549"/>
       <c r="G9" s="59" t="s">
         <v>38</v>
       </c>
@@ -4345,12 +4348,12 @@
       </c>
     </row>
     <row r="10" spans="1:16" s="10" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="591"/>
-      <c r="B10" s="591"/>
-      <c r="C10" s="591"/>
-      <c r="D10" s="698"/>
-      <c r="E10" s="701"/>
-      <c r="F10" s="704"/>
+      <c r="A10" s="677"/>
+      <c r="B10" s="677"/>
+      <c r="C10" s="677"/>
+      <c r="D10" s="543"/>
+      <c r="E10" s="546"/>
+      <c r="F10" s="549"/>
       <c r="G10" s="59" t="s">
         <v>272</v>
       </c>
@@ -4378,12 +4381,12 @@
       </c>
     </row>
     <row r="11" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="591"/>
-      <c r="B11" s="591"/>
-      <c r="C11" s="591"/>
-      <c r="D11" s="698"/>
-      <c r="E11" s="701"/>
-      <c r="F11" s="704"/>
+      <c r="A11" s="677"/>
+      <c r="B11" s="677"/>
+      <c r="C11" s="677"/>
+      <c r="D11" s="543"/>
+      <c r="E11" s="546"/>
+      <c r="F11" s="549"/>
       <c r="G11" s="64" t="s">
         <v>41</v>
       </c>
@@ -4410,12 +4413,12 @@
       </c>
     </row>
     <row r="12" spans="1:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="592"/>
-      <c r="B12" s="592"/>
-      <c r="C12" s="592"/>
-      <c r="D12" s="699"/>
-      <c r="E12" s="702"/>
-      <c r="F12" s="705"/>
+      <c r="A12" s="678"/>
+      <c r="B12" s="678"/>
+      <c r="C12" s="678"/>
+      <c r="D12" s="544"/>
+      <c r="E12" s="547"/>
+      <c r="F12" s="550"/>
       <c r="G12" s="216" t="s">
         <v>42</v>
       </c>
@@ -4442,11 +4445,11 @@
       </c>
     </row>
     <row r="13" spans="1:16" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="597" t="s">
+      <c r="A13" s="680" t="s">
         <v>44</v>
       </c>
-      <c r="B13" s="597"/>
-      <c r="C13" s="597"/>
+      <c r="B13" s="680"/>
+      <c r="C13" s="680"/>
       <c r="D13" s="243" t="s">
         <v>45</v>
       </c>
@@ -4483,18 +4486,18 @@
       </c>
     </row>
     <row r="14" spans="1:16" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="598" t="s">
+      <c r="A14" s="681" t="s">
         <v>48</v>
       </c>
-      <c r="B14" s="598"/>
-      <c r="C14" s="598"/>
-      <c r="D14" s="675" t="s">
+      <c r="B14" s="681"/>
+      <c r="C14" s="681"/>
+      <c r="D14" s="639" t="s">
         <v>49</v>
       </c>
-      <c r="E14" s="677" t="s">
+      <c r="E14" s="570" t="s">
         <v>46</v>
       </c>
-      <c r="F14" s="673" t="str">
+      <c r="F14" s="637" t="str">
         <f>Namespace &amp; ($A14)</f>
         <v>http://vocab.fairdatacollective.org/dataset/properties/Language</v>
       </c>
@@ -4524,12 +4527,12 @@
       </c>
     </row>
     <row r="15" spans="1:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="599"/>
-      <c r="B15" s="599"/>
-      <c r="C15" s="599"/>
-      <c r="D15" s="676"/>
-      <c r="E15" s="678"/>
-      <c r="F15" s="674"/>
+      <c r="A15" s="682"/>
+      <c r="B15" s="682"/>
+      <c r="C15" s="682"/>
+      <c r="D15" s="640"/>
+      <c r="E15" s="571"/>
+      <c r="F15" s="638"/>
       <c r="G15" s="229" t="s">
         <v>51</v>
       </c>
@@ -4559,11 +4562,11 @@
       <c r="P15" s="11"/>
     </row>
     <row r="16" spans="1:16" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="600" t="s">
+      <c r="A16" s="683" t="s">
         <v>52</v>
       </c>
-      <c r="B16" s="600"/>
-      <c r="C16" s="600"/>
+      <c r="B16" s="683"/>
+      <c r="C16" s="683"/>
       <c r="D16" s="244" t="s">
         <v>53</v>
       </c>
@@ -4600,11 +4603,11 @@
       </c>
     </row>
     <row r="17" spans="1:16" s="11" customFormat="1" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="601" t="s">
+      <c r="A17" s="684" t="s">
         <v>57</v>
       </c>
-      <c r="B17" s="601"/>
-      <c r="C17" s="601"/>
+      <c r="B17" s="684"/>
+      <c r="C17" s="684"/>
       <c r="D17" s="78" t="s">
         <v>58</v>
       </c>
@@ -4643,11 +4646,11 @@
       <c r="P17"/>
     </row>
     <row r="18" spans="1:16" s="11" customFormat="1" ht="17" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="593" t="s">
+      <c r="A18" s="679" t="s">
         <v>62</v>
       </c>
-      <c r="B18" s="593"/>
-      <c r="C18" s="593"/>
+      <c r="B18" s="679"/>
+      <c r="C18" s="679"/>
       <c r="D18" s="245" t="s">
         <v>63</v>
       </c>
@@ -4671,17 +4674,17 @@
     </row>
     <row r="19" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="315"/>
-      <c r="B19" s="594" t="s">
-        <v>502</v>
-      </c>
-      <c r="C19" s="594"/>
-      <c r="D19" s="594" t="s">
-        <v>469</v>
-      </c>
-      <c r="E19" s="716" t="s">
+      <c r="B19" s="641" t="s">
+        <v>501</v>
+      </c>
+      <c r="C19" s="641"/>
+      <c r="D19" s="641" t="s">
+        <v>468</v>
+      </c>
+      <c r="E19" s="567" t="s">
         <v>34</v>
       </c>
-      <c r="F19" s="713" t="str">
+      <c r="F19" s="564" t="str">
         <f>Namespace&amp;($A19)</f>
         <v>http://vocab.fairdatacollective.org/dataset/properties/</v>
       </c>
@@ -4692,7 +4695,7 @@
         <v>307</v>
       </c>
       <c r="I19" s="128" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="J19" s="129" t="s">
         <v>34</v>
@@ -4704,7 +4707,7 @@
         <v>67</v>
       </c>
       <c r="M19" s="131" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="N19" s="131" t="s">
         <v>28</v>
@@ -4712,16 +4715,16 @@
     </row>
     <row r="20" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="315"/>
-      <c r="B20" s="595"/>
-      <c r="C20" s="595"/>
-      <c r="D20" s="595"/>
-      <c r="E20" s="717"/>
-      <c r="F20" s="714"/>
+      <c r="B20" s="642"/>
+      <c r="C20" s="642"/>
+      <c r="D20" s="642"/>
+      <c r="E20" s="568"/>
+      <c r="F20" s="565"/>
       <c r="G20" s="79" t="s">
+        <v>469</v>
+      </c>
+      <c r="H20" s="79" t="s">
         <v>470</v>
-      </c>
-      <c r="H20" s="79" t="s">
-        <v>471</v>
       </c>
       <c r="I20" s="80" t="s">
         <v>69</v>
@@ -4737,7 +4740,7 @@
         <v>http://vocab.fairdatacollective.org/dataset/properties/subjectIRI</v>
       </c>
       <c r="M20" s="83" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="N20" s="83" t="s">
         <v>28</v>
@@ -4745,11 +4748,11 @@
     </row>
     <row r="21" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="315"/>
-      <c r="B21" s="595"/>
-      <c r="C21" s="595"/>
-      <c r="D21" s="595"/>
-      <c r="E21" s="717"/>
-      <c r="F21" s="714"/>
+      <c r="B21" s="642"/>
+      <c r="C21" s="642"/>
+      <c r="D21" s="642"/>
+      <c r="E21" s="568"/>
+      <c r="F21" s="565"/>
       <c r="G21" s="83" t="s">
         <v>70</v>
       </c>
@@ -4770,7 +4773,7 @@
         <v>http://vocab.fairdatacollective.org/dataset/properties/subjectScheme</v>
       </c>
       <c r="M21" s="83" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="N21" s="83" t="s">
         <v>28</v>
@@ -4778,11 +4781,11 @@
     </row>
     <row r="22" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="315"/>
-      <c r="B22" s="596"/>
-      <c r="C22" s="596"/>
-      <c r="D22" s="596"/>
-      <c r="E22" s="718"/>
-      <c r="F22" s="715"/>
+      <c r="B22" s="643"/>
+      <c r="C22" s="643"/>
+      <c r="D22" s="643"/>
+      <c r="E22" s="569"/>
+      <c r="F22" s="566"/>
       <c r="G22" s="132" t="s">
         <v>71</v>
       </c>
@@ -4803,7 +4806,7 @@
         <v>http://vocab.fairdatacollective.org/dataset/properties/subjectSchemeIRI</v>
       </c>
       <c r="M22" s="136" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="N22" s="136" t="s">
         <v>28</v>
@@ -4817,7 +4820,7 @@
       <c r="E23" s="157"/>
       <c r="F23" s="158"/>
       <c r="G23" s="159" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="H23" s="159" t="s">
         <v>64</v>
@@ -4841,11 +4844,11 @@
       </c>
     </row>
     <row r="24" spans="1:16" s="14" customFormat="1" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="627" t="s">
+      <c r="A24" s="653" t="s">
         <v>72</v>
       </c>
-      <c r="B24" s="627"/>
-      <c r="C24" s="627"/>
+      <c r="B24" s="653"/>
+      <c r="C24" s="653"/>
       <c r="D24" s="246" t="s">
         <v>73</v>
       </c>
@@ -4867,17 +4870,17 @@
     </row>
     <row r="25" spans="1:16" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="17"/>
-      <c r="B25" s="628" t="s">
-        <v>453</v>
-      </c>
-      <c r="C25" s="628"/>
-      <c r="D25" s="628" t="s">
-        <v>479</v>
-      </c>
-      <c r="E25" s="650" t="s">
+      <c r="B25" s="622" t="s">
+        <v>452</v>
+      </c>
+      <c r="C25" s="622"/>
+      <c r="D25" s="622" t="s">
+        <v>478</v>
+      </c>
+      <c r="E25" s="558" t="s">
         <v>54</v>
       </c>
-      <c r="F25" s="653" t="str">
+      <c r="F25" s="625" t="str">
         <f>Namespace &amp; ($B25)</f>
         <v>http://vocab.fairdatacollective.org/dataset/properties/CreatorName</v>
       </c>
@@ -4908,11 +4911,11 @@
     </row>
     <row r="26" spans="1:16" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="17"/>
-      <c r="B26" s="629"/>
-      <c r="C26" s="629"/>
-      <c r="D26" s="629"/>
-      <c r="E26" s="651"/>
-      <c r="F26" s="654"/>
+      <c r="B26" s="623"/>
+      <c r="C26" s="623"/>
+      <c r="D26" s="623"/>
+      <c r="E26" s="559"/>
+      <c r="F26" s="626"/>
       <c r="G26" s="87" t="s">
         <v>79</v>
       </c>
@@ -4940,11 +4943,11 @@
     </row>
     <row r="27" spans="1:16" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="17"/>
-      <c r="B27" s="630"/>
-      <c r="C27" s="630"/>
-      <c r="D27" s="630"/>
-      <c r="E27" s="652"/>
-      <c r="F27" s="655"/>
+      <c r="B27" s="624"/>
+      <c r="C27" s="624"/>
+      <c r="D27" s="624"/>
+      <c r="E27" s="560"/>
+      <c r="F27" s="627"/>
       <c r="G27" s="141" t="s">
         <v>82</v>
       </c>
@@ -4972,17 +4975,17 @@
     </row>
     <row r="28" spans="1:16" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="17"/>
-      <c r="B28" s="628" t="s">
-        <v>454</v>
-      </c>
-      <c r="C28" s="628"/>
-      <c r="D28" s="628" t="s">
-        <v>478</v>
-      </c>
-      <c r="E28" s="650" t="s">
+      <c r="B28" s="622" t="s">
+        <v>453</v>
+      </c>
+      <c r="C28" s="622"/>
+      <c r="D28" s="622" t="s">
+        <v>477</v>
+      </c>
+      <c r="E28" s="558" t="s">
         <v>54</v>
       </c>
-      <c r="F28" s="653" t="str">
+      <c r="F28" s="625" t="str">
         <f>Namespace &amp; ($B28)</f>
         <v>http://vocab.fairdatacollective.org/dataset/properties/CreatorIdentifier</v>
       </c>
@@ -5014,11 +5017,11 @@
     </row>
     <row r="29" spans="1:16" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="17"/>
-      <c r="B29" s="629"/>
-      <c r="C29" s="629"/>
-      <c r="D29" s="629"/>
-      <c r="E29" s="651"/>
-      <c r="F29" s="654"/>
+      <c r="B29" s="623"/>
+      <c r="C29" s="623"/>
+      <c r="D29" s="623"/>
+      <c r="E29" s="559"/>
+      <c r="F29" s="626"/>
       <c r="G29" s="87" t="s">
         <v>93</v>
       </c>
@@ -5039,7 +5042,7 @@
         <v>http://vocab.fairdatacollective.org/dataset/properties/creatorIdentifierScheme</v>
       </c>
       <c r="M29" s="89" t="s">
-        <v>24</v>
+        <v>522</v>
       </c>
       <c r="N29" s="84" t="s">
         <v>94</v>
@@ -5047,11 +5050,11 @@
     </row>
     <row r="30" spans="1:16" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="17"/>
-      <c r="B30" s="630"/>
-      <c r="C30" s="630"/>
-      <c r="D30" s="630"/>
-      <c r="E30" s="652"/>
-      <c r="F30" s="655"/>
+      <c r="B30" s="624"/>
+      <c r="C30" s="624"/>
+      <c r="D30" s="624"/>
+      <c r="E30" s="560"/>
+      <c r="F30" s="627"/>
       <c r="G30" s="141" t="s">
         <v>95</v>
       </c>
@@ -5072,7 +5075,7 @@
         <v>http://vocab.fairdatacollective.org/dataset/properties/creatorIdentifierSchemeIRI</v>
       </c>
       <c r="M30" s="148" t="s">
-        <v>24</v>
+        <v>522</v>
       </c>
       <c r="N30" s="145" t="s">
         <v>96</v>
@@ -5080,17 +5083,17 @@
     </row>
     <row r="31" spans="1:16" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="17"/>
-      <c r="B31" s="628" t="s">
-        <v>455</v>
-      </c>
-      <c r="C31" s="628"/>
-      <c r="D31" s="628" t="s">
-        <v>477</v>
-      </c>
-      <c r="E31" s="650" t="s">
+      <c r="B31" s="622" t="s">
+        <v>454</v>
+      </c>
+      <c r="C31" s="622"/>
+      <c r="D31" s="622" t="s">
+        <v>476</v>
+      </c>
+      <c r="E31" s="558" t="s">
         <v>54</v>
       </c>
-      <c r="F31" s="711" t="str">
+      <c r="F31" s="556" t="str">
         <f>Namespace &amp; ($B31)</f>
         <v>http://vocab.fairdatacollective.org/dataset/properties/CreatorAffiliation</v>
       </c>
@@ -5122,11 +5125,11 @@
     </row>
     <row r="32" spans="1:16" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="17"/>
-      <c r="B32" s="629"/>
-      <c r="C32" s="629"/>
-      <c r="D32" s="629"/>
-      <c r="E32" s="651"/>
-      <c r="F32" s="711"/>
+      <c r="B32" s="623"/>
+      <c r="C32" s="623"/>
+      <c r="D32" s="623"/>
+      <c r="E32" s="559"/>
+      <c r="F32" s="556"/>
       <c r="G32" s="87" t="s">
         <v>100</v>
       </c>
@@ -5155,11 +5158,11 @@
     </row>
     <row r="33" spans="1:16" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="17"/>
-      <c r="B33" s="629"/>
-      <c r="C33" s="629"/>
-      <c r="D33" s="629"/>
-      <c r="E33" s="651"/>
-      <c r="F33" s="711"/>
+      <c r="B33" s="623"/>
+      <c r="C33" s="623"/>
+      <c r="D33" s="623"/>
+      <c r="E33" s="559"/>
+      <c r="F33" s="556"/>
       <c r="G33" s="87" t="s">
         <v>103</v>
       </c>
@@ -5180,7 +5183,7 @@
         <v>http://vocab.fairdatacollective.org/dataset/properties/creatorAffiliationIdentifierScheme</v>
       </c>
       <c r="M33" s="89" t="s">
-        <v>24</v>
+        <v>522</v>
       </c>
       <c r="N33" s="84" t="s">
         <v>104</v>
@@ -5188,11 +5191,11 @@
     </row>
     <row r="34" spans="1:16" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="17"/>
-      <c r="B34" s="630"/>
-      <c r="C34" s="630"/>
-      <c r="D34" s="630"/>
-      <c r="E34" s="652"/>
-      <c r="F34" s="712"/>
+      <c r="B34" s="624"/>
+      <c r="C34" s="624"/>
+      <c r="D34" s="624"/>
+      <c r="E34" s="560"/>
+      <c r="F34" s="557"/>
       <c r="G34" s="141" t="s">
         <v>105</v>
       </c>
@@ -5213,7 +5216,7 @@
         <v>http://vocab.fairdatacollective.org/dataset/properties/creatorAffiliationIdentifierSchemeIRI</v>
       </c>
       <c r="M34" s="148" t="s">
-        <v>24</v>
+        <v>522</v>
       </c>
       <c r="N34" s="145" t="s">
         <v>106</v>
@@ -5318,13 +5321,13 @@
       </c>
     </row>
     <row r="38" spans="1:16" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="631" t="s">
+      <c r="A38" s="654" t="s">
         <v>107</v>
       </c>
-      <c r="B38" s="631"/>
-      <c r="C38" s="631"/>
+      <c r="B38" s="654"/>
+      <c r="C38" s="654"/>
       <c r="D38" s="382" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="E38" s="383" t="s">
         <v>34</v>
@@ -5344,17 +5347,17 @@
     </row>
     <row r="39" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="424"/>
-      <c r="B39" s="632" t="s">
-        <v>464</v>
-      </c>
-      <c r="C39" s="632"/>
-      <c r="D39" s="641" t="s">
-        <v>480</v>
-      </c>
-      <c r="E39" s="568" t="s">
+      <c r="B39" s="655" t="s">
+        <v>463</v>
+      </c>
+      <c r="C39" s="655"/>
+      <c r="D39" s="613" t="s">
+        <v>479</v>
+      </c>
+      <c r="E39" s="616" t="s">
         <v>34</v>
       </c>
-      <c r="F39" s="647" t="str">
+      <c r="F39" s="561" t="str">
         <f>Namespace &amp; ($B39)</f>
         <v>http://vocab.fairdatacollective.org/dataset/properties/ContributorName</v>
       </c>
@@ -5385,16 +5388,16 @@
     </row>
     <row r="40" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="424"/>
-      <c r="B40" s="632"/>
-      <c r="C40" s="632"/>
-      <c r="D40" s="642"/>
-      <c r="E40" s="569"/>
-      <c r="F40" s="648"/>
+      <c r="B40" s="655"/>
+      <c r="C40" s="655"/>
+      <c r="D40" s="614"/>
+      <c r="E40" s="617"/>
+      <c r="F40" s="562"/>
       <c r="G40" s="394" t="s">
         <v>111</v>
       </c>
       <c r="H40" s="394" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="I40" s="395" t="s">
         <v>112</v>
@@ -5417,16 +5420,16 @@
     </row>
     <row r="41" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="424"/>
-      <c r="B41" s="632"/>
-      <c r="C41" s="632"/>
-      <c r="D41" s="643"/>
-      <c r="E41" s="570"/>
-      <c r="F41" s="649"/>
+      <c r="B41" s="655"/>
+      <c r="C41" s="655"/>
+      <c r="D41" s="615"/>
+      <c r="E41" s="618"/>
+      <c r="F41" s="563"/>
       <c r="G41" s="399" t="s">
         <v>113</v>
       </c>
       <c r="H41" s="399" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="I41" s="400" t="s">
         <v>114</v>
@@ -5449,17 +5452,17 @@
     </row>
     <row r="42" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" s="424"/>
-      <c r="B42" s="632" t="s">
-        <v>467</v>
-      </c>
-      <c r="C42" s="632"/>
-      <c r="D42" s="641" t="s">
-        <v>481</v>
-      </c>
-      <c r="E42" s="568" t="s">
+      <c r="B42" s="655" t="s">
+        <v>466</v>
+      </c>
+      <c r="C42" s="655"/>
+      <c r="D42" s="613" t="s">
+        <v>480</v>
+      </c>
+      <c r="E42" s="616" t="s">
         <v>34</v>
       </c>
-      <c r="F42" s="647" t="str">
+      <c r="F42" s="561" t="str">
         <f>Namespace &amp; ($B42)</f>
         <v>http://vocab.fairdatacollective.org/dataset/properties/ContributorIdentifier</v>
       </c>
@@ -5470,7 +5473,7 @@
         <v>327</v>
       </c>
       <c r="I42" s="405" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="J42" s="392">
         <v>1</v>
@@ -5491,11 +5494,11 @@
     </row>
     <row r="43" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="424"/>
-      <c r="B43" s="632"/>
-      <c r="C43" s="632"/>
-      <c r="D43" s="642"/>
-      <c r="E43" s="569"/>
-      <c r="F43" s="648"/>
+      <c r="B43" s="655"/>
+      <c r="C43" s="655"/>
+      <c r="D43" s="614"/>
+      <c r="E43" s="617"/>
+      <c r="F43" s="562"/>
       <c r="G43" s="394" t="s">
         <v>121</v>
       </c>
@@ -5516,7 +5519,7 @@
         <v>http://vocab.fairdatacollective.org/dataset/properties/contributorIdentifierScheme</v>
       </c>
       <c r="M43" s="406" t="s">
-        <v>24</v>
+        <v>522</v>
       </c>
       <c r="N43" s="398" t="s">
         <v>94</v>
@@ -5524,11 +5527,11 @@
     </row>
     <row r="44" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="424"/>
-      <c r="B44" s="632"/>
-      <c r="C44" s="632"/>
-      <c r="D44" s="643"/>
-      <c r="E44" s="570"/>
-      <c r="F44" s="649"/>
+      <c r="B44" s="655"/>
+      <c r="C44" s="655"/>
+      <c r="D44" s="615"/>
+      <c r="E44" s="618"/>
+      <c r="F44" s="563"/>
       <c r="G44" s="399" t="s">
         <v>122</v>
       </c>
@@ -5549,7 +5552,7 @@
         <v>http://vocab.fairdatacollective.org/dataset/properties/contributorIdentifierSchemeIRI</v>
       </c>
       <c r="M44" s="407" t="s">
-        <v>24</v>
+        <v>522</v>
       </c>
       <c r="N44" s="403" t="s">
         <v>96</v>
@@ -5557,17 +5560,17 @@
     </row>
     <row r="45" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="424"/>
-      <c r="B45" s="632" t="s">
-        <v>468</v>
-      </c>
-      <c r="C45" s="632"/>
-      <c r="D45" s="641" t="s">
-        <v>482</v>
-      </c>
-      <c r="E45" s="568" t="s">
+      <c r="B45" s="655" t="s">
+        <v>467</v>
+      </c>
+      <c r="C45" s="655"/>
+      <c r="D45" s="613" t="s">
+        <v>481</v>
+      </c>
+      <c r="E45" s="616" t="s">
         <v>34</v>
       </c>
-      <c r="F45" s="644" t="str">
+      <c r="F45" s="619" t="str">
         <f>Namespace &amp; ($B45)</f>
         <v>http://vocab.fairdatacollective.org/dataset/properties/ContributorAffiliation</v>
       </c>
@@ -5578,7 +5581,7 @@
         <v>330</v>
       </c>
       <c r="I45" s="405" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="J45" s="392" t="s">
         <v>46</v>
@@ -5599,11 +5602,11 @@
     </row>
     <row r="46" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="424"/>
-      <c r="B46" s="632"/>
-      <c r="C46" s="632"/>
-      <c r="D46" s="642"/>
-      <c r="E46" s="569"/>
-      <c r="F46" s="645"/>
+      <c r="B46" s="655"/>
+      <c r="C46" s="655"/>
+      <c r="D46" s="614"/>
+      <c r="E46" s="617"/>
+      <c r="F46" s="620"/>
       <c r="G46" s="394" t="s">
         <v>123</v>
       </c>
@@ -5632,13 +5635,13 @@
     </row>
     <row r="47" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="424"/>
-      <c r="B47" s="632"/>
-      <c r="C47" s="632"/>
-      <c r="D47" s="642"/>
-      <c r="E47" s="569"/>
-      <c r="F47" s="645"/>
+      <c r="B47" s="655"/>
+      <c r="C47" s="655"/>
+      <c r="D47" s="614"/>
+      <c r="E47" s="617"/>
+      <c r="F47" s="620"/>
       <c r="G47" s="394" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="H47" s="394" t="s">
         <v>333</v>
@@ -5657,7 +5660,7 @@
         <v>http://vocab.fairdatacollective.org/dataset/properties/contributorAffiliationIdentifierScheme</v>
       </c>
       <c r="M47" s="406" t="s">
-        <v>24</v>
+        <v>522</v>
       </c>
       <c r="N47" s="398" t="s">
         <v>104</v>
@@ -5665,11 +5668,11 @@
     </row>
     <row r="48" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="424"/>
-      <c r="B48" s="632"/>
-      <c r="C48" s="632"/>
-      <c r="D48" s="643"/>
-      <c r="E48" s="570"/>
-      <c r="F48" s="646"/>
+      <c r="B48" s="655"/>
+      <c r="C48" s="655"/>
+      <c r="D48" s="615"/>
+      <c r="E48" s="618"/>
+      <c r="F48" s="621"/>
       <c r="G48" s="399" t="s">
         <v>125</v>
       </c>
@@ -5690,7 +5693,7 @@
         <v>http://vocab.fairdatacollective.org/dataset/properties/contributorAffiliationIdentifierSchemeIRI</v>
       </c>
       <c r="M48" s="407" t="s">
-        <v>24</v>
+        <v>522</v>
       </c>
       <c r="N48" s="403" t="s">
         <v>106</v>
@@ -5746,7 +5749,7 @@
         <v>323</v>
       </c>
       <c r="I50" s="395" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="J50" s="396" t="s">
         <v>34</v>
@@ -5799,11 +5802,11 @@
       </c>
     </row>
     <row r="52" spans="1:16" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="633" t="s">
+      <c r="A52" s="656" t="s">
         <v>126</v>
       </c>
-      <c r="B52" s="633"/>
-      <c r="C52" s="633"/>
+      <c r="B52" s="656"/>
+      <c r="C52" s="656"/>
       <c r="D52" s="248" t="s">
         <v>437</v>
       </c>
@@ -5825,17 +5828,17 @@
     </row>
     <row r="53" spans="1:16" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="426"/>
-      <c r="B53" s="583" t="s">
+      <c r="B53" s="650" t="s">
+        <v>474</v>
+      </c>
+      <c r="C53" s="650"/>
+      <c r="D53" s="650" t="s">
         <v>475</v>
       </c>
-      <c r="C53" s="583"/>
-      <c r="D53" s="583" t="s">
-        <v>476</v>
-      </c>
-      <c r="E53" s="624" t="s">
+      <c r="E53" s="647" t="s">
         <v>54</v>
       </c>
-      <c r="F53" s="621" t="str">
+      <c r="F53" s="644" t="str">
         <f>Namespace &amp; ($B53)</f>
         <v>http://vocab.fairdatacollective.org/dataset/properties/PublisherIdentifier</v>
       </c>
@@ -5867,11 +5870,11 @@
     </row>
     <row r="54" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="426"/>
-      <c r="B54" s="584"/>
-      <c r="C54" s="584"/>
-      <c r="D54" s="584"/>
-      <c r="E54" s="625"/>
-      <c r="F54" s="622"/>
+      <c r="B54" s="651"/>
+      <c r="C54" s="651"/>
+      <c r="D54" s="651"/>
+      <c r="E54" s="648"/>
+      <c r="F54" s="645"/>
       <c r="G54" s="93" t="s">
         <v>136</v>
       </c>
@@ -5900,11 +5903,11 @@
     </row>
     <row r="55" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="426"/>
-      <c r="B55" s="585"/>
-      <c r="C55" s="585"/>
-      <c r="D55" s="585"/>
-      <c r="E55" s="626"/>
-      <c r="F55" s="623"/>
+      <c r="B55" s="652"/>
+      <c r="C55" s="652"/>
+      <c r="D55" s="652"/>
+      <c r="E55" s="649"/>
+      <c r="F55" s="646"/>
       <c r="G55" s="257" t="s">
         <v>137</v>
       </c>
@@ -6031,11 +6034,11 @@
       <c r="P58" s="10"/>
     </row>
     <row r="59" spans="1:16" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="586" t="s">
+      <c r="A59" s="673" t="s">
         <v>138</v>
       </c>
-      <c r="B59" s="586"/>
-      <c r="C59" s="586"/>
+      <c r="B59" s="673"/>
+      <c r="C59" s="673"/>
       <c r="D59" s="296" t="s">
         <v>139</v>
       </c>
@@ -6069,7 +6072,7 @@
         <v>345</v>
       </c>
       <c r="I60" s="104" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="J60" s="100">
         <v>1</v>
@@ -6090,17 +6093,17 @@
     </row>
     <row r="61" spans="1:16" s="10" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A61" s="428"/>
-      <c r="B61" s="550" t="s">
+      <c r="B61" s="600" t="s">
+        <v>484</v>
+      </c>
+      <c r="C61" s="600"/>
+      <c r="D61" s="600" t="s">
         <v>485</v>
       </c>
-      <c r="C61" s="550"/>
-      <c r="D61" s="550" t="s">
-        <v>486</v>
-      </c>
-      <c r="E61" s="553" t="s">
+      <c r="E61" s="597" t="s">
         <v>46</v>
       </c>
-      <c r="F61" s="719" t="str">
+      <c r="F61" s="594" t="str">
         <f>Namespace &amp; ($B61)</f>
         <v>http://vocab.fairdatacollective.org/dataset/properties/LicenseIdentifier</v>
       </c>
@@ -6134,11 +6137,11 @@
     </row>
     <row r="62" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="428"/>
-      <c r="B62" s="551"/>
-      <c r="C62" s="551"/>
-      <c r="D62" s="551"/>
-      <c r="E62" s="554"/>
-      <c r="F62" s="720"/>
+      <c r="B62" s="601"/>
+      <c r="C62" s="601"/>
+      <c r="D62" s="601"/>
+      <c r="E62" s="598"/>
+      <c r="F62" s="595"/>
       <c r="G62" s="98" t="s">
         <v>148</v>
       </c>
@@ -6167,11 +6170,11 @@
     </row>
     <row r="63" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="428"/>
-      <c r="B63" s="587"/>
-      <c r="C63" s="587"/>
-      <c r="D63" s="587"/>
-      <c r="E63" s="722"/>
-      <c r="F63" s="721"/>
+      <c r="B63" s="602"/>
+      <c r="C63" s="602"/>
+      <c r="D63" s="602"/>
+      <c r="E63" s="599"/>
+      <c r="F63" s="596"/>
       <c r="G63" s="290" t="s">
         <v>149</v>
       </c>
@@ -6212,7 +6215,7 @@
         <v>344</v>
       </c>
       <c r="I64" s="273" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="J64" s="274" t="s">
         <v>46</v>
@@ -6229,18 +6232,18 @@
       <c r="N64" s="277"/>
     </row>
     <row r="65" spans="1:14" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="588" t="s">
+      <c r="A65" s="674" t="s">
         <v>151</v>
       </c>
-      <c r="B65" s="588"/>
-      <c r="C65" s="588"/>
-      <c r="D65" s="617" t="s">
-        <v>520</v>
-      </c>
-      <c r="E65" s="619" t="s">
+      <c r="B65" s="674"/>
+      <c r="C65" s="674"/>
+      <c r="D65" s="666" t="s">
+        <v>519</v>
+      </c>
+      <c r="E65" s="668" t="s">
         <v>54</v>
       </c>
-      <c r="F65" s="617" t="str">
+      <c r="F65" s="666" t="str">
         <f>Namespace &amp; ($A65)</f>
         <v>http://vocab.fairdatacollective.org/dataset/properties/Date</v>
       </c>
@@ -6265,20 +6268,20 @@
       <c r="N65" s="308"/>
     </row>
     <row r="66" spans="1:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="588"/>
-      <c r="B66" s="588"/>
-      <c r="C66" s="588"/>
-      <c r="D66" s="618"/>
-      <c r="E66" s="620"/>
-      <c r="F66" s="618"/>
+      <c r="A66" s="674"/>
+      <c r="B66" s="674"/>
+      <c r="C66" s="674"/>
+      <c r="D66" s="667"/>
+      <c r="E66" s="669"/>
+      <c r="F66" s="667"/>
       <c r="G66" s="105" t="s">
+        <v>486</v>
+      </c>
+      <c r="H66" s="105" t="s">
         <v>487</v>
       </c>
-      <c r="H66" s="105" t="s">
+      <c r="I66" s="106" t="s">
         <v>488</v>
-      </c>
-      <c r="I66" s="106" t="s">
-        <v>489</v>
       </c>
       <c r="J66" s="107">
         <v>1</v>
@@ -6292,16 +6295,16 @@
         <v>24</v>
       </c>
       <c r="N66" s="109" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="67" spans="1:14" s="14" customFormat="1" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="589" t="s">
+      <c r="A67" s="675" t="s">
         <v>154</v>
       </c>
-      <c r="B67" s="589"/>
-      <c r="C67" s="589"/>
-      <c r="D67" s="740" t="s">
+      <c r="B67" s="675"/>
+      <c r="C67" s="675"/>
+      <c r="D67" s="603" t="s">
         <v>159</v>
       </c>
       <c r="E67" s="365" t="s">
@@ -6322,9 +6325,9 @@
     </row>
     <row r="68" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="372"/>
-      <c r="B68" s="615"/>
-      <c r="C68" s="615"/>
-      <c r="D68" s="741"/>
+      <c r="B68" s="664"/>
+      <c r="C68" s="664"/>
+      <c r="D68" s="604"/>
       <c r="E68" s="316"/>
       <c r="F68" s="317"/>
       <c r="G68" s="318" t="s">
@@ -6357,7 +6360,7 @@
       <c r="A69" s="372"/>
       <c r="B69" s="373"/>
       <c r="C69" s="322"/>
-      <c r="D69" s="741"/>
+      <c r="D69" s="604"/>
       <c r="E69" s="324"/>
       <c r="F69" s="317"/>
       <c r="G69" s="318" t="s">
@@ -6383,14 +6386,14 @@
         <v>24</v>
       </c>
       <c r="N69" s="318" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="70" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="372"/>
       <c r="B70" s="373"/>
       <c r="C70" s="322"/>
-      <c r="D70" s="741"/>
+      <c r="D70" s="604"/>
       <c r="E70" s="325"/>
       <c r="F70" s="317"/>
       <c r="G70" s="310" t="s">
@@ -6412,27 +6415,27 @@
         <v>443</v>
       </c>
       <c r="M70" s="314" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="N70" s="314" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="71" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="372"/>
       <c r="B71" s="373"/>
       <c r="C71" s="322"/>
-      <c r="D71" s="741"/>
+      <c r="D71" s="604"/>
       <c r="E71" s="325"/>
       <c r="F71" s="317"/>
       <c r="G71" s="310" t="s">
+        <v>445</v>
+      </c>
+      <c r="H71" s="310" t="s">
         <v>446</v>
       </c>
-      <c r="H71" s="310" t="s">
+      <c r="I71" s="311" t="s">
         <v>447</v>
-      </c>
-      <c r="I71" s="311" t="s">
-        <v>448</v>
       </c>
       <c r="J71" s="312">
         <v>1</v>
@@ -6445,7 +6448,7 @@
         <v>http://vocab.fairdatacollective.org/dataset/properties/distributionMediaType</v>
       </c>
       <c r="M71" s="314" t="s">
-        <v>445</v>
+        <v>523</v>
       </c>
       <c r="N71" s="314" t="s">
         <v>28</v>
@@ -6455,7 +6458,7 @@
       <c r="A72" s="372"/>
       <c r="B72" s="373"/>
       <c r="C72" s="322"/>
-      <c r="D72" s="742"/>
+      <c r="D72" s="605"/>
       <c r="E72" s="324"/>
       <c r="F72" s="317"/>
       <c r="G72" s="310" t="s">
@@ -6486,17 +6489,17 @@
     </row>
     <row r="73" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="372"/>
-      <c r="B73" s="603" t="s">
+      <c r="B73" s="658" t="s">
+        <v>490</v>
+      </c>
+      <c r="C73" s="658"/>
+      <c r="D73" s="578" t="s">
         <v>491</v>
       </c>
-      <c r="C73" s="603"/>
-      <c r="D73" s="682" t="s">
-        <v>492</v>
-      </c>
-      <c r="E73" s="606">
+      <c r="E73" s="575">
         <v>1</v>
       </c>
-      <c r="F73" s="679"/>
+      <c r="F73" s="572"/>
       <c r="G73" s="326" t="s">
         <v>163</v>
       </c>
@@ -6504,7 +6507,7 @@
         <v>350</v>
       </c>
       <c r="I73" s="327" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="J73" s="328">
         <v>1</v>
@@ -6525,11 +6528,11 @@
     </row>
     <row r="74" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="372"/>
-      <c r="B74" s="604"/>
-      <c r="C74" s="604"/>
-      <c r="D74" s="683"/>
-      <c r="E74" s="607"/>
-      <c r="F74" s="680"/>
+      <c r="B74" s="659"/>
+      <c r="C74" s="659"/>
+      <c r="D74" s="579"/>
+      <c r="E74" s="576"/>
+      <c r="F74" s="573"/>
       <c r="G74" s="310" t="s">
         <v>164</v>
       </c>
@@ -6537,7 +6540,7 @@
         <v>352</v>
       </c>
       <c r="I74" s="311" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="J74" s="312" t="s">
         <v>54</v>
@@ -6558,16 +6561,16 @@
     </row>
     <row r="75" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="372"/>
-      <c r="B75" s="605"/>
-      <c r="C75" s="605"/>
-      <c r="D75" s="684"/>
-      <c r="E75" s="608"/>
-      <c r="F75" s="681"/>
+      <c r="B75" s="660"/>
+      <c r="C75" s="660"/>
+      <c r="D75" s="580"/>
+      <c r="E75" s="577"/>
+      <c r="F75" s="574"/>
       <c r="G75" s="331" t="s">
+        <v>449</v>
+      </c>
+      <c r="H75" s="331" t="s">
         <v>450</v>
-      </c>
-      <c r="H75" s="331" t="s">
-        <v>451</v>
       </c>
       <c r="I75" s="332" t="s">
         <v>411</v>
@@ -6620,12 +6623,12 @@
     </row>
     <row r="77" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="372"/>
-      <c r="B77" s="616" t="s">
+      <c r="B77" s="665" t="s">
+        <v>492</v>
+      </c>
+      <c r="C77" s="665"/>
+      <c r="D77" s="358" t="s">
         <v>493</v>
-      </c>
-      <c r="C77" s="616"/>
-      <c r="D77" s="358" t="s">
-        <v>494</v>
       </c>
       <c r="E77" s="359" t="s">
         <v>54</v>
@@ -6645,17 +6648,17 @@
     </row>
     <row r="78" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="372"/>
-      <c r="B78" s="602"/>
-      <c r="C78" s="603" t="s">
+      <c r="B78" s="657"/>
+      <c r="C78" s="658" t="s">
+        <v>494</v>
+      </c>
+      <c r="D78" s="658" t="s">
         <v>495</v>
       </c>
-      <c r="D78" s="603" t="s">
-        <v>496</v>
-      </c>
-      <c r="E78" s="606">
+      <c r="E78" s="575">
         <v>1</v>
       </c>
-      <c r="F78" s="612" t="str">
+      <c r="F78" s="661" t="str">
         <f>Namespace &amp; ($C78)</f>
         <v>http://vocab.fairdatacollective.org/dataset/properties/DistributorName</v>
       </c>
@@ -6686,11 +6689,11 @@
     </row>
     <row r="79" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="372"/>
-      <c r="B79" s="602"/>
-      <c r="C79" s="604"/>
-      <c r="D79" s="604"/>
-      <c r="E79" s="607"/>
-      <c r="F79" s="613"/>
+      <c r="B79" s="657"/>
+      <c r="C79" s="659"/>
+      <c r="D79" s="659"/>
+      <c r="E79" s="576"/>
+      <c r="F79" s="662"/>
       <c r="G79" s="354" t="s">
         <v>170</v>
       </c>
@@ -6718,16 +6721,16 @@
     </row>
     <row r="80" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="372"/>
-      <c r="B80" s="602"/>
-      <c r="C80" s="605"/>
-      <c r="D80" s="605"/>
-      <c r="E80" s="608"/>
-      <c r="F80" s="614"/>
+      <c r="B80" s="657"/>
+      <c r="C80" s="660"/>
+      <c r="D80" s="660"/>
+      <c r="E80" s="577"/>
+      <c r="F80" s="663"/>
       <c r="G80" s="340" t="s">
         <v>172</v>
       </c>
       <c r="H80" s="340" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="I80" s="341" t="s">
         <v>173</v>
@@ -6750,17 +6753,17 @@
     </row>
     <row r="81" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="372"/>
-      <c r="B81" s="602"/>
-      <c r="C81" s="603" t="s">
+      <c r="B81" s="657"/>
+      <c r="C81" s="658" t="s">
+        <v>497</v>
+      </c>
+      <c r="D81" s="658" t="s">
         <v>498</v>
       </c>
-      <c r="D81" s="603" t="s">
-        <v>499</v>
-      </c>
-      <c r="E81" s="606">
+      <c r="E81" s="575">
         <v>1</v>
       </c>
-      <c r="F81" s="612" t="str">
+      <c r="F81" s="661" t="str">
         <f>Namespace &amp; ($C81)</f>
         <v>http://vocab.fairdatacollective.org/dataset/properties/DistributorIdentifier</v>
       </c>
@@ -6792,11 +6795,11 @@
     </row>
     <row r="82" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="372"/>
-      <c r="B82" s="602"/>
-      <c r="C82" s="604"/>
-      <c r="D82" s="604"/>
-      <c r="E82" s="607"/>
-      <c r="F82" s="613"/>
+      <c r="B82" s="657"/>
+      <c r="C82" s="659"/>
+      <c r="D82" s="659"/>
+      <c r="E82" s="576"/>
+      <c r="F82" s="662"/>
       <c r="G82" s="354" t="s">
         <v>181</v>
       </c>
@@ -6817,7 +6820,7 @@
         <v>http://vocab.fairdatacollective.org/dataset/properties/distributorIdentifierScheme</v>
       </c>
       <c r="M82" s="374" t="s">
-        <v>24</v>
+        <v>522</v>
       </c>
       <c r="N82" s="354" t="s">
         <v>94</v>
@@ -6825,11 +6828,11 @@
     </row>
     <row r="83" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="372"/>
-      <c r="B83" s="602"/>
-      <c r="C83" s="605"/>
-      <c r="D83" s="605"/>
-      <c r="E83" s="608"/>
-      <c r="F83" s="614"/>
+      <c r="B83" s="657"/>
+      <c r="C83" s="660"/>
+      <c r="D83" s="660"/>
+      <c r="E83" s="577"/>
+      <c r="F83" s="663"/>
       <c r="G83" s="340" t="s">
         <v>182</v>
       </c>
@@ -6850,7 +6853,7 @@
         <v>http://vocab.fairdatacollective.org/dataset/properties/distributorIdentifierSchemeIRI</v>
       </c>
       <c r="M83" s="344" t="s">
-        <v>24</v>
+        <v>522</v>
       </c>
       <c r="N83" s="340" t="s">
         <v>96</v>
@@ -6858,17 +6861,17 @@
     </row>
     <row r="84" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="372"/>
-      <c r="B84" s="602"/>
-      <c r="C84" s="603" t="s">
+      <c r="B84" s="657"/>
+      <c r="C84" s="658" t="s">
+        <v>499</v>
+      </c>
+      <c r="D84" s="658" t="s">
         <v>500</v>
       </c>
-      <c r="D84" s="603" t="s">
-        <v>501</v>
-      </c>
-      <c r="E84" s="606" t="s">
+      <c r="E84" s="575" t="s">
         <v>54</v>
       </c>
-      <c r="F84" s="609" t="str">
+      <c r="F84" s="670" t="str">
         <f>Namespace &amp; ($C84)</f>
         <v>http://vocab.fairdatacollective.org/dataset/properties/DistributorAffiliation</v>
       </c>
@@ -6900,11 +6903,11 @@
     </row>
     <row r="85" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="372"/>
-      <c r="B85" s="602"/>
-      <c r="C85" s="604"/>
-      <c r="D85" s="604"/>
-      <c r="E85" s="607"/>
-      <c r="F85" s="610"/>
+      <c r="B85" s="657"/>
+      <c r="C85" s="659"/>
+      <c r="D85" s="659"/>
+      <c r="E85" s="576"/>
+      <c r="F85" s="671"/>
       <c r="G85" s="354" t="s">
         <v>185</v>
       </c>
@@ -6933,11 +6936,11 @@
     </row>
     <row r="86" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="372"/>
-      <c r="B86" s="602"/>
-      <c r="C86" s="604"/>
-      <c r="D86" s="604"/>
-      <c r="E86" s="607"/>
-      <c r="F86" s="610"/>
+      <c r="B86" s="657"/>
+      <c r="C86" s="659"/>
+      <c r="D86" s="659"/>
+      <c r="E86" s="576"/>
+      <c r="F86" s="671"/>
       <c r="G86" s="354" t="s">
         <v>187</v>
       </c>
@@ -6958,7 +6961,7 @@
         <v>http://vocab.fairdatacollective.org/dataset/properties/distributorAffiliationIdentifierScheme</v>
       </c>
       <c r="M86" s="374" t="s">
-        <v>24</v>
+        <v>522</v>
       </c>
       <c r="N86" s="354" t="s">
         <v>104</v>
@@ -6966,11 +6969,11 @@
     </row>
     <row r="87" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="372"/>
-      <c r="B87" s="602"/>
-      <c r="C87" s="605"/>
-      <c r="D87" s="605"/>
-      <c r="E87" s="608"/>
-      <c r="F87" s="611"/>
+      <c r="B87" s="657"/>
+      <c r="C87" s="660"/>
+      <c r="D87" s="660"/>
+      <c r="E87" s="577"/>
+      <c r="F87" s="672"/>
       <c r="G87" s="340" t="s">
         <v>188</v>
       </c>
@@ -6991,7 +6994,7 @@
         <v>http://vocab.fairdatacollective.org/dataset/properties/distributorAffiliationIdentifierSchemeIRI</v>
       </c>
       <c r="M87" s="344" t="s">
-        <v>24</v>
+        <v>522</v>
       </c>
       <c r="N87" s="340" t="s">
         <v>106</v>
@@ -7056,7 +7059,7 @@
         <v>http://vocab.fairdatacollective.org/dataset/properties/distributorRole</v>
       </c>
       <c r="M89" s="374" t="s">
-        <v>24</v>
+        <v>522</v>
       </c>
       <c r="N89" s="354" t="s">
         <v>28</v>
@@ -7089,7 +7092,7 @@
         <v>http://vocab.fairdatacollective.org/dataset/properties/distributorType</v>
       </c>
       <c r="M90" s="353" t="s">
-        <v>24</v>
+        <v>522</v>
       </c>
       <c r="N90" s="349" t="s">
         <v>76</v>
@@ -7098,11 +7101,11 @@
       <c r="P90"/>
     </row>
     <row r="91" spans="1:16" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A91" s="576" t="s">
+      <c r="A91" s="693" t="s">
         <v>189</v>
       </c>
-      <c r="B91" s="576"/>
-      <c r="C91" s="576"/>
+      <c r="B91" s="693"/>
+      <c r="C91" s="693"/>
       <c r="D91" s="430" t="s">
         <v>410</v>
       </c>
@@ -7124,17 +7127,17 @@
     </row>
     <row r="92" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="426"/>
-      <c r="B92" s="577" t="s">
+      <c r="B92" s="581" t="s">
         <v>283</v>
       </c>
-      <c r="C92" s="577"/>
-      <c r="D92" s="577" t="s">
+      <c r="C92" s="581"/>
+      <c r="D92" s="581" t="s">
         <v>287</v>
       </c>
-      <c r="E92" s="685" t="s">
+      <c r="E92" s="584" t="s">
         <v>54</v>
       </c>
-      <c r="F92" s="692" t="str">
+      <c r="F92" s="589" t="str">
         <f>Namespace &amp; ($B92)</f>
         <v>http://vocab.fairdatacollective.org/dataset/properties/DataStream</v>
       </c>
@@ -7158,7 +7161,7 @@
         <v>http://vocab.fairdatacollective.org/dataset/properties/dataStream</v>
       </c>
       <c r="M92" s="447" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="N92" s="447" t="s">
         <v>28</v>
@@ -7166,11 +7169,11 @@
     </row>
     <row r="93" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="426"/>
-      <c r="B93" s="578"/>
-      <c r="C93" s="578"/>
-      <c r="D93" s="578"/>
-      <c r="E93" s="686"/>
-      <c r="F93" s="693"/>
+      <c r="B93" s="582"/>
+      <c r="C93" s="582"/>
+      <c r="D93" s="582"/>
+      <c r="E93" s="585"/>
+      <c r="F93" s="590"/>
       <c r="G93" s="110" t="s">
         <v>285</v>
       </c>
@@ -7191,7 +7194,7 @@
         <v>http://vocab.fairdatacollective.org/dataset/properties/dataStreamIRI</v>
       </c>
       <c r="M93" s="114" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="N93" s="114" t="s">
         <v>28</v>
@@ -7199,11 +7202,11 @@
     </row>
     <row r="94" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="426"/>
-      <c r="B94" s="578"/>
-      <c r="C94" s="578"/>
-      <c r="D94" s="578"/>
-      <c r="E94" s="686"/>
-      <c r="F94" s="693"/>
+      <c r="B94" s="582"/>
+      <c r="C94" s="582"/>
+      <c r="D94" s="582"/>
+      <c r="E94" s="585"/>
+      <c r="F94" s="590"/>
       <c r="G94" s="114" t="s">
         <v>191</v>
       </c>
@@ -7224,7 +7227,7 @@
         <v>http://vocab.fairdatacollective.org/dataset/properties/datastreamScheme</v>
       </c>
       <c r="M94" s="114" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="N94" s="114" t="s">
         <v>28</v>
@@ -7232,11 +7235,11 @@
     </row>
     <row r="95" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="426"/>
-      <c r="B95" s="579"/>
-      <c r="C95" s="579"/>
-      <c r="D95" s="579"/>
-      <c r="E95" s="687"/>
-      <c r="F95" s="694"/>
+      <c r="B95" s="583"/>
+      <c r="C95" s="583"/>
+      <c r="D95" s="583"/>
+      <c r="E95" s="586"/>
+      <c r="F95" s="591"/>
       <c r="G95" s="448" t="s">
         <v>286</v>
       </c>
@@ -7257,7 +7260,7 @@
         <v>http://vocab.fairdatacollective.org/dataset/properties/dataStreamSchemeIRI</v>
       </c>
       <c r="M95" s="451" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="N95" s="451" t="s">
         <v>28</v>
@@ -7265,17 +7268,17 @@
     </row>
     <row r="96" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" s="426"/>
-      <c r="B96" s="656"/>
-      <c r="C96" s="577" t="s">
+      <c r="B96" s="697"/>
+      <c r="C96" s="581" t="s">
         <v>281</v>
       </c>
-      <c r="D96" s="577" t="s">
+      <c r="D96" s="581" t="s">
         <v>368</v>
       </c>
-      <c r="E96" s="685">
+      <c r="E96" s="584">
         <v>1</v>
       </c>
-      <c r="F96" s="692" t="str">
+      <c r="F96" s="589" t="str">
         <f>Namespace &amp; ($C96)</f>
         <v>http://vocab.fairdatacollective.org/dataset/properties/DataSource</v>
       </c>
@@ -7299,7 +7302,7 @@
         <v>http://vocab.fairdatacollective.org/dataset/properties/dataSource</v>
       </c>
       <c r="M96" s="114" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="N96" s="447" t="s">
         <v>28</v>
@@ -7307,11 +7310,11 @@
     </row>
     <row r="97" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" s="426"/>
-      <c r="B97" s="656"/>
-      <c r="C97" s="578"/>
-      <c r="D97" s="578"/>
-      <c r="E97" s="686"/>
-      <c r="F97" s="693"/>
+      <c r="B97" s="697"/>
+      <c r="C97" s="582"/>
+      <c r="D97" s="582"/>
+      <c r="E97" s="585"/>
+      <c r="F97" s="590"/>
       <c r="G97" s="110" t="s">
         <v>195</v>
       </c>
@@ -7332,7 +7335,7 @@
         <v>http://vocab.fairdatacollective.org/dataset/properties/dataSourceIRI</v>
       </c>
       <c r="M97" s="114" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="N97" s="114" t="s">
         <v>28</v>
@@ -7340,11 +7343,11 @@
     </row>
     <row r="98" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="426"/>
-      <c r="B98" s="656"/>
-      <c r="C98" s="578"/>
-      <c r="D98" s="578"/>
-      <c r="E98" s="686"/>
-      <c r="F98" s="693"/>
+      <c r="B98" s="697"/>
+      <c r="C98" s="582"/>
+      <c r="D98" s="582"/>
+      <c r="E98" s="585"/>
+      <c r="F98" s="590"/>
       <c r="G98" s="110" t="s">
         <v>197</v>
       </c>
@@ -7365,7 +7368,7 @@
         <v>http://vocab.fairdatacollective.org/dataset/properties/dataSourceScheme</v>
       </c>
       <c r="M98" s="114" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="N98" s="114" t="s">
         <v>28</v>
@@ -7373,11 +7376,11 @@
     </row>
     <row r="99" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="426"/>
-      <c r="B99" s="656"/>
-      <c r="C99" s="579"/>
-      <c r="D99" s="579"/>
-      <c r="E99" s="687"/>
-      <c r="F99" s="694"/>
+      <c r="B99" s="697"/>
+      <c r="C99" s="583"/>
+      <c r="D99" s="583"/>
+      <c r="E99" s="586"/>
+      <c r="F99" s="591"/>
       <c r="G99" s="448" t="s">
         <v>198</v>
       </c>
@@ -7398,7 +7401,7 @@
         <v>http://vocab.fairdatacollective.org/dataset/properties/dataSourceSchemeIRI</v>
       </c>
       <c r="M99" s="451" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="N99" s="451" t="s">
         <v>28</v>
@@ -7406,17 +7409,17 @@
     </row>
     <row r="100" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="426"/>
-      <c r="B100" s="656"/>
-      <c r="C100" s="578" t="s">
+      <c r="B100" s="697"/>
+      <c r="C100" s="582" t="s">
         <v>282</v>
       </c>
-      <c r="D100" s="578" t="s">
+      <c r="D100" s="582" t="s">
         <v>288</v>
       </c>
-      <c r="E100" s="686" t="s">
+      <c r="E100" s="585" t="s">
         <v>54</v>
       </c>
-      <c r="F100" s="695" t="str">
+      <c r="F100" s="592" t="str">
         <f>Namespace &amp; ($C100)</f>
         <v>http://vocab.fairdatacollective.org/dataset/properties/Variable</v>
       </c>
@@ -7440,7 +7443,7 @@
         <v>http://vocab.fairdatacollective.org/dataset/properties/variable</v>
       </c>
       <c r="M100" s="114" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="N100" s="114" t="s">
         <v>28</v>
@@ -7448,11 +7451,11 @@
     </row>
     <row r="101" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" s="426"/>
-      <c r="B101" s="656"/>
-      <c r="C101" s="578"/>
-      <c r="D101" s="578"/>
-      <c r="E101" s="686"/>
-      <c r="F101" s="695"/>
+      <c r="B101" s="697"/>
+      <c r="C101" s="582"/>
+      <c r="D101" s="582"/>
+      <c r="E101" s="585"/>
+      <c r="F101" s="592"/>
       <c r="G101" s="110" t="s">
         <v>290</v>
       </c>
@@ -7473,7 +7476,7 @@
         <v>http://vocab.fairdatacollective.org/dataset/properties/variableIRI</v>
       </c>
       <c r="M101" s="114" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="N101" s="114" t="s">
         <v>28</v>
@@ -7481,11 +7484,11 @@
     </row>
     <row r="102" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A102" s="426"/>
-      <c r="B102" s="656"/>
-      <c r="C102" s="578"/>
-      <c r="D102" s="578"/>
-      <c r="E102" s="686"/>
-      <c r="F102" s="695"/>
+      <c r="B102" s="697"/>
+      <c r="C102" s="582"/>
+      <c r="D102" s="582"/>
+      <c r="E102" s="585"/>
+      <c r="F102" s="592"/>
       <c r="G102" s="110" t="s">
         <v>291</v>
       </c>
@@ -7506,7 +7509,7 @@
         <v>http://vocab.fairdatacollective.org/dataset/properties/variableScheme</v>
       </c>
       <c r="M102" s="114" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="N102" s="114" t="s">
         <v>28</v>
@@ -7514,11 +7517,11 @@
     </row>
     <row r="103" spans="1:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A103" s="427"/>
-      <c r="B103" s="657"/>
-      <c r="C103" s="688"/>
-      <c r="D103" s="688"/>
-      <c r="E103" s="689"/>
-      <c r="F103" s="696"/>
+      <c r="B103" s="698"/>
+      <c r="C103" s="587"/>
+      <c r="D103" s="587"/>
+      <c r="E103" s="588"/>
+      <c r="F103" s="593"/>
       <c r="G103" s="438" t="s">
         <v>292</v>
       </c>
@@ -7539,18 +7542,18 @@
         <v>http://vocab.fairdatacollective.org/dataset/properties/variableSchemeIRI</v>
       </c>
       <c r="M103" s="442" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="N103" s="442" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="104" spans="1:14" s="14" customFormat="1" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A104" s="580" t="s">
+      <c r="A104" s="694" t="s">
         <v>201</v>
       </c>
-      <c r="B104" s="580"/>
-      <c r="C104" s="580"/>
+      <c r="B104" s="694"/>
+      <c r="C104" s="694"/>
       <c r="D104" s="478" t="s">
         <v>202</v>
       </c>
@@ -7572,17 +7575,17 @@
     </row>
     <row r="105" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A105" s="424"/>
-      <c r="B105" s="565" t="s">
-        <v>505</v>
-      </c>
-      <c r="C105" s="565"/>
-      <c r="D105" s="581" t="s">
+      <c r="B105" s="685" t="s">
         <v>504</v>
       </c>
-      <c r="E105" s="690" t="s">
+      <c r="C105" s="685"/>
+      <c r="D105" s="695" t="s">
+        <v>503</v>
+      </c>
+      <c r="E105" s="699" t="s">
         <v>46</v>
       </c>
-      <c r="F105" s="571" t="str">
+      <c r="F105" s="688" t="str">
         <f>Namespace &amp; ($B105)</f>
         <v>http://vocab.fairdatacollective.org/dataset/properties/SpatialCoveragePoint</v>
       </c>
@@ -7614,11 +7617,11 @@
     </row>
     <row r="106" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A106" s="424"/>
-      <c r="B106" s="567"/>
-      <c r="C106" s="567"/>
-      <c r="D106" s="582"/>
-      <c r="E106" s="691"/>
-      <c r="F106" s="573"/>
+      <c r="B106" s="687"/>
+      <c r="C106" s="687"/>
+      <c r="D106" s="696"/>
+      <c r="E106" s="700"/>
+      <c r="F106" s="690"/>
       <c r="G106" s="458" t="s">
         <v>203</v>
       </c>
@@ -7647,17 +7650,17 @@
     </row>
     <row r="107" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A107" s="424"/>
-      <c r="B107" s="565" t="s">
+      <c r="B107" s="685" t="s">
+        <v>505</v>
+      </c>
+      <c r="C107" s="685"/>
+      <c r="D107" s="685" t="s">
         <v>506</v>
       </c>
-      <c r="C107" s="565"/>
-      <c r="D107" s="565" t="s">
-        <v>507</v>
-      </c>
-      <c r="E107" s="568" t="s">
+      <c r="E107" s="616" t="s">
         <v>46</v>
       </c>
-      <c r="F107" s="571" t="str">
+      <c r="F107" s="688" t="str">
         <f>Namespace &amp; ($B107)</f>
         <v>http://vocab.fairdatacollective.org/dataset/properties/SpatialCoverageBoundingBox</v>
       </c>
@@ -7689,11 +7692,11 @@
     </row>
     <row r="108" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A108" s="424"/>
-      <c r="B108" s="566"/>
-      <c r="C108" s="566"/>
-      <c r="D108" s="566"/>
-      <c r="E108" s="569"/>
-      <c r="F108" s="572"/>
+      <c r="B108" s="686"/>
+      <c r="C108" s="686"/>
+      <c r="D108" s="686"/>
+      <c r="E108" s="617"/>
+      <c r="F108" s="689"/>
       <c r="G108" s="468" t="s">
         <v>209</v>
       </c>
@@ -7722,11 +7725,11 @@
     </row>
     <row r="109" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A109" s="424"/>
-      <c r="B109" s="566"/>
-      <c r="C109" s="566"/>
-      <c r="D109" s="566"/>
-      <c r="E109" s="569"/>
-      <c r="F109" s="572"/>
+      <c r="B109" s="686"/>
+      <c r="C109" s="686"/>
+      <c r="D109" s="686"/>
+      <c r="E109" s="617"/>
+      <c r="F109" s="689"/>
       <c r="G109" s="468" t="s">
         <v>211</v>
       </c>
@@ -7755,11 +7758,11 @@
     </row>
     <row r="110" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A110" s="424"/>
-      <c r="B110" s="567"/>
-      <c r="C110" s="567"/>
-      <c r="D110" s="567"/>
-      <c r="E110" s="570"/>
-      <c r="F110" s="573"/>
+      <c r="B110" s="687"/>
+      <c r="C110" s="687"/>
+      <c r="D110" s="687"/>
+      <c r="E110" s="618"/>
+      <c r="F110" s="690"/>
       <c r="G110" s="473" t="s">
         <v>213</v>
       </c>
@@ -7788,17 +7791,17 @@
     </row>
     <row r="111" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A111" s="424"/>
-      <c r="B111" s="565" t="s">
+      <c r="B111" s="685" t="s">
+        <v>507</v>
+      </c>
+      <c r="C111" s="685"/>
+      <c r="D111" s="691" t="s">
         <v>508</v>
       </c>
-      <c r="C111" s="565"/>
-      <c r="D111" s="574" t="s">
-        <v>509</v>
-      </c>
-      <c r="E111" s="568" t="s">
+      <c r="E111" s="616" t="s">
         <v>46</v>
       </c>
-      <c r="F111" s="571" t="str">
+      <c r="F111" s="688" t="str">
         <f>Namespace &amp; ($B111)</f>
         <v>http://vocab.fairdatacollective.org/dataset/properties/SpatialCoveragePolygon</v>
       </c>
@@ -7830,11 +7833,11 @@
     </row>
     <row r="112" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A112" s="424"/>
-      <c r="B112" s="567"/>
-      <c r="C112" s="567"/>
-      <c r="D112" s="575"/>
-      <c r="E112" s="570"/>
-      <c r="F112" s="573"/>
+      <c r="B112" s="687"/>
+      <c r="C112" s="687"/>
+      <c r="D112" s="692"/>
+      <c r="E112" s="618"/>
+      <c r="F112" s="690"/>
       <c r="G112" s="458" t="s">
         <v>439</v>
       </c>
@@ -7895,18 +7898,18 @@
       </c>
     </row>
     <row r="114" spans="1:14" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A114" s="557" t="s">
+      <c r="A114" s="713" t="s">
         <v>217</v>
       </c>
-      <c r="B114" s="557"/>
-      <c r="C114" s="557"/>
-      <c r="D114" s="726" t="s">
+      <c r="B114" s="713"/>
+      <c r="C114" s="713"/>
+      <c r="D114" s="730" t="s">
         <v>218</v>
       </c>
-      <c r="E114" s="658" t="s">
+      <c r="E114" s="721" t="s">
         <v>46</v>
       </c>
-      <c r="F114" s="661" t="str">
+      <c r="F114" s="724" t="str">
         <f>Namespace &amp; ($A114)</f>
         <v>http://vocab.fairdatacollective.org/dataset/properties/VerticalCoverage</v>
       </c>
@@ -7937,12 +7940,12 @@
       </c>
     </row>
     <row r="115" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A115" s="558"/>
-      <c r="B115" s="558"/>
-      <c r="C115" s="558"/>
-      <c r="D115" s="727"/>
-      <c r="E115" s="659"/>
-      <c r="F115" s="662"/>
+      <c r="A115" s="714"/>
+      <c r="B115" s="714"/>
+      <c r="C115" s="714"/>
+      <c r="D115" s="731"/>
+      <c r="E115" s="722"/>
+      <c r="F115" s="725"/>
       <c r="G115" s="116" t="s">
         <v>221</v>
       </c>
@@ -7970,12 +7973,12 @@
       </c>
     </row>
     <row r="116" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A116" s="558"/>
-      <c r="B116" s="558"/>
-      <c r="C116" s="558"/>
-      <c r="D116" s="727"/>
-      <c r="E116" s="659"/>
-      <c r="F116" s="662"/>
+      <c r="A116" s="714"/>
+      <c r="B116" s="714"/>
+      <c r="C116" s="714"/>
+      <c r="D116" s="731"/>
+      <c r="E116" s="722"/>
+      <c r="F116" s="725"/>
       <c r="G116" s="116" t="s">
         <v>223</v>
       </c>
@@ -8003,12 +8006,12 @@
       </c>
     </row>
     <row r="117" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A117" s="558"/>
-      <c r="B117" s="558"/>
-      <c r="C117" s="558"/>
-      <c r="D117" s="727"/>
-      <c r="E117" s="659"/>
-      <c r="F117" s="662"/>
+      <c r="A117" s="714"/>
+      <c r="B117" s="714"/>
+      <c r="C117" s="714"/>
+      <c r="D117" s="731"/>
+      <c r="E117" s="722"/>
+      <c r="F117" s="725"/>
       <c r="G117" s="116" t="s">
         <v>224</v>
       </c>
@@ -8036,12 +8039,12 @@
       </c>
     </row>
     <row r="118" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A118" s="558"/>
-      <c r="B118" s="558"/>
-      <c r="C118" s="558"/>
-      <c r="D118" s="727"/>
-      <c r="E118" s="659"/>
-      <c r="F118" s="662"/>
+      <c r="A118" s="714"/>
+      <c r="B118" s="714"/>
+      <c r="C118" s="714"/>
+      <c r="D118" s="731"/>
+      <c r="E118" s="722"/>
+      <c r="F118" s="725"/>
       <c r="G118" s="116" t="s">
         <v>225</v>
       </c>
@@ -8069,12 +8072,12 @@
       </c>
     </row>
     <row r="119" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A119" s="558"/>
-      <c r="B119" s="558"/>
-      <c r="C119" s="558"/>
-      <c r="D119" s="727"/>
-      <c r="E119" s="659"/>
-      <c r="F119" s="662"/>
+      <c r="A119" s="714"/>
+      <c r="B119" s="714"/>
+      <c r="C119" s="714"/>
+      <c r="D119" s="731"/>
+      <c r="E119" s="722"/>
+      <c r="F119" s="725"/>
       <c r="G119" s="116" t="s">
         <v>226</v>
       </c>
@@ -8102,12 +8105,12 @@
       </c>
     </row>
     <row r="120" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A120" s="558"/>
-      <c r="B120" s="558"/>
-      <c r="C120" s="558"/>
-      <c r="D120" s="727"/>
-      <c r="E120" s="659"/>
-      <c r="F120" s="662"/>
+      <c r="A120" s="714"/>
+      <c r="B120" s="714"/>
+      <c r="C120" s="714"/>
+      <c r="D120" s="731"/>
+      <c r="E120" s="722"/>
+      <c r="F120" s="725"/>
       <c r="G120" s="116" t="s">
         <v>398</v>
       </c>
@@ -8135,16 +8138,16 @@
       </c>
     </row>
     <row r="121" spans="1:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A121" s="559"/>
-      <c r="B121" s="559"/>
-      <c r="C121" s="559"/>
-      <c r="D121" s="728"/>
-      <c r="E121" s="660"/>
-      <c r="F121" s="663"/>
-      <c r="G121" s="743" t="s">
+      <c r="A121" s="715"/>
+      <c r="B121" s="715"/>
+      <c r="C121" s="715"/>
+      <c r="D121" s="732"/>
+      <c r="E121" s="723"/>
+      <c r="F121" s="726"/>
+      <c r="G121" s="541" t="s">
         <v>408</v>
       </c>
-      <c r="H121" s="743" t="s">
+      <c r="H121" s="541" t="s">
         <v>423</v>
       </c>
       <c r="I121" s="498" t="s">
@@ -8168,18 +8171,18 @@
       </c>
     </row>
     <row r="122" spans="1:14" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A122" s="560" t="s">
+      <c r="A122" s="716" t="s">
         <v>227</v>
       </c>
-      <c r="B122" s="560"/>
-      <c r="C122" s="560"/>
-      <c r="D122" s="723" t="s">
+      <c r="B122" s="716"/>
+      <c r="C122" s="716"/>
+      <c r="D122" s="727" t="s">
         <v>228</v>
       </c>
-      <c r="E122" s="729" t="s">
+      <c r="E122" s="733" t="s">
         <v>46</v>
       </c>
-      <c r="F122" s="730" t="str">
+      <c r="F122" s="734" t="str">
         <f>Namespace &amp; ($A122)</f>
         <v>http://vocab.fairdatacollective.org/dataset/properties/TemporalCoverage</v>
       </c>
@@ -8210,12 +8213,12 @@
       </c>
     </row>
     <row r="123" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A123" s="561"/>
-      <c r="B123" s="561"/>
-      <c r="C123" s="561"/>
-      <c r="D123" s="724"/>
-      <c r="E123" s="701"/>
-      <c r="F123" s="731"/>
+      <c r="A123" s="717"/>
+      <c r="B123" s="717"/>
+      <c r="C123" s="717"/>
+      <c r="D123" s="728"/>
+      <c r="E123" s="546"/>
+      <c r="F123" s="735"/>
       <c r="G123" s="121" t="s">
         <v>231</v>
       </c>
@@ -8243,12 +8246,12 @@
       </c>
     </row>
     <row r="124" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A124" s="561"/>
-      <c r="B124" s="561"/>
-      <c r="C124" s="561"/>
-      <c r="D124" s="724"/>
-      <c r="E124" s="701"/>
-      <c r="F124" s="731"/>
+      <c r="A124" s="717"/>
+      <c r="B124" s="717"/>
+      <c r="C124" s="717"/>
+      <c r="D124" s="728"/>
+      <c r="E124" s="546"/>
+      <c r="F124" s="735"/>
       <c r="G124" s="121" t="s">
         <v>233</v>
       </c>
@@ -8276,12 +8279,12 @@
       </c>
     </row>
     <row r="125" spans="1:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A125" s="562"/>
-      <c r="B125" s="562"/>
-      <c r="C125" s="562"/>
-      <c r="D125" s="725"/>
-      <c r="E125" s="702"/>
-      <c r="F125" s="732"/>
+      <c r="A125" s="718"/>
+      <c r="B125" s="718"/>
+      <c r="C125" s="718"/>
+      <c r="D125" s="729"/>
+      <c r="E125" s="547"/>
+      <c r="F125" s="736"/>
       <c r="G125" s="507" t="s">
         <v>235</v>
       </c>
@@ -8309,13 +8312,13 @@
       </c>
     </row>
     <row r="126" spans="1:14" s="14" customFormat="1" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A126" s="563" t="s">
+      <c r="A126" s="719" t="s">
         <v>237</v>
       </c>
-      <c r="B126" s="563"/>
-      <c r="C126" s="563"/>
+      <c r="B126" s="719"/>
+      <c r="C126" s="719"/>
       <c r="D126" s="518" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="E126" s="519" t="s">
         <v>34</v>
@@ -8335,17 +8338,17 @@
     </row>
     <row r="127" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A127" s="428"/>
-      <c r="B127" s="547" t="s">
-        <v>511</v>
-      </c>
-      <c r="C127" s="547"/>
-      <c r="D127" s="541" t="s">
-        <v>514</v>
-      </c>
-      <c r="E127" s="544">
+      <c r="B127" s="707" t="s">
+        <v>510</v>
+      </c>
+      <c r="C127" s="707"/>
+      <c r="D127" s="701" t="s">
+        <v>513</v>
+      </c>
+      <c r="E127" s="704">
         <v>1</v>
       </c>
-      <c r="F127" s="541" t="str">
+      <c r="F127" s="701" t="str">
         <f>Namespace &amp; ($B127)</f>
         <v>http://vocab.fairdatacollective.org/dataset/properties/Award</v>
       </c>
@@ -8377,11 +8380,11 @@
     </row>
     <row r="128" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A128" s="428"/>
-      <c r="B128" s="548"/>
-      <c r="C128" s="548"/>
-      <c r="D128" s="542"/>
-      <c r="E128" s="545"/>
-      <c r="F128" s="542"/>
+      <c r="B128" s="708"/>
+      <c r="C128" s="708"/>
+      <c r="D128" s="702"/>
+      <c r="E128" s="705"/>
+      <c r="F128" s="702"/>
       <c r="G128" s="516" t="s">
         <v>240</v>
       </c>
@@ -8410,11 +8413,11 @@
     </row>
     <row r="129" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A129" s="428"/>
-      <c r="B129" s="564"/>
-      <c r="C129" s="564"/>
-      <c r="D129" s="543"/>
-      <c r="E129" s="546"/>
-      <c r="F129" s="543"/>
+      <c r="B129" s="720"/>
+      <c r="C129" s="720"/>
+      <c r="D129" s="703"/>
+      <c r="E129" s="706"/>
+      <c r="F129" s="703"/>
       <c r="G129" s="535" t="s">
         <v>242</v>
       </c>
@@ -8443,17 +8446,17 @@
     </row>
     <row r="130" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A130" s="428"/>
-      <c r="B130" s="547" t="s">
+      <c r="B130" s="707" t="s">
+        <v>511</v>
+      </c>
+      <c r="C130" s="707"/>
+      <c r="D130" s="600" t="s">
         <v>512</v>
       </c>
-      <c r="C130" s="547"/>
-      <c r="D130" s="550" t="s">
-        <v>513</v>
-      </c>
-      <c r="E130" s="553" t="s">
+      <c r="E130" s="597" t="s">
         <v>54</v>
       </c>
-      <c r="F130" s="541" t="str">
+      <c r="F130" s="701" t="str">
         <f>Namespace &amp; ($B130)</f>
         <v>http://vocab.fairdatacollective.org/dataset/properties/Funder</v>
       </c>
@@ -8485,11 +8488,11 @@
     </row>
     <row r="131" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A131" s="428"/>
-      <c r="B131" s="548"/>
-      <c r="C131" s="548"/>
-      <c r="D131" s="551"/>
-      <c r="E131" s="554"/>
-      <c r="F131" s="542"/>
+      <c r="B131" s="708"/>
+      <c r="C131" s="708"/>
+      <c r="D131" s="601"/>
+      <c r="E131" s="598"/>
+      <c r="F131" s="702"/>
       <c r="G131" s="512" t="s">
         <v>246</v>
       </c>
@@ -8518,11 +8521,11 @@
     </row>
     <row r="132" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A132" s="428"/>
-      <c r="B132" s="548"/>
-      <c r="C132" s="548"/>
-      <c r="D132" s="551"/>
-      <c r="E132" s="554"/>
-      <c r="F132" s="542"/>
+      <c r="B132" s="708"/>
+      <c r="C132" s="708"/>
+      <c r="D132" s="601"/>
+      <c r="E132" s="598"/>
+      <c r="F132" s="702"/>
       <c r="G132" s="516" t="s">
         <v>248</v>
       </c>
@@ -8543,7 +8546,7 @@
         <v>http://vocab.fairdatacollective.org/dataset/properties/funderIdentifierScheme</v>
       </c>
       <c r="M132" s="517" t="s">
-        <v>24</v>
+        <v>522</v>
       </c>
       <c r="N132" s="512" t="s">
         <v>28</v>
@@ -8551,11 +8554,11 @@
     </row>
     <row r="133" spans="1:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A133" s="429"/>
-      <c r="B133" s="549"/>
-      <c r="C133" s="549"/>
-      <c r="D133" s="552"/>
-      <c r="E133" s="555"/>
-      <c r="F133" s="556"/>
+      <c r="B133" s="709"/>
+      <c r="C133" s="709"/>
+      <c r="D133" s="710"/>
+      <c r="E133" s="711"/>
+      <c r="F133" s="712"/>
       <c r="G133" s="525" t="s">
         <v>250</v>
       </c>
@@ -8576,7 +8579,7 @@
         <v>http://vocab.fairdatacollective.org/dataset/properties/funderIdentifierSchemeIRI</v>
       </c>
       <c r="M133" s="529" t="s">
-        <v>24</v>
+        <v>522</v>
       </c>
       <c r="N133" s="530" t="s">
         <v>28</v>
@@ -8596,7 +8599,7 @@
     </row>
     <row r="137" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D137" s="540" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="H137" s="3"/>
       <c r="J137" s="9"/>
@@ -8635,20 +8638,20 @@
     </row>
     <row r="143" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D143" s="3" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="H143" s="3"/>
       <c r="J143" s="9"/>
     </row>
     <row r="144" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D144" s="3" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="J144" s="6"/>
     </row>
     <row r="145" spans="4:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D145" s="5" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="J145" s="6"/>
     </row>
@@ -8660,7 +8663,7 @@
     </row>
     <row r="147" spans="4:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D147" s="5" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="G147" s="7"/>
       <c r="H147" s="7"/>
@@ -8680,13 +8683,13 @@
     </row>
     <row r="150" spans="4:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D150" s="5" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="J150" s="6"/>
     </row>
     <row r="151" spans="4:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D151" s="16" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="J151" s="6"/>
     </row>
@@ -12225,30 +12228,87 @@
   </sheetData>
   <autoFilter ref="H1:N143" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <mergeCells count="134">
-    <mergeCell ref="D8:D12"/>
-    <mergeCell ref="E8:E12"/>
-    <mergeCell ref="F8:F12"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="F3:F4"/>
-    <mergeCell ref="F31:F34"/>
-    <mergeCell ref="E31:E34"/>
-    <mergeCell ref="F39:F41"/>
-    <mergeCell ref="F19:F22"/>
-    <mergeCell ref="E19:E22"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="F73:F75"/>
-    <mergeCell ref="E73:E75"/>
-    <mergeCell ref="D73:D75"/>
-    <mergeCell ref="D92:D95"/>
-    <mergeCell ref="E92:E95"/>
-    <mergeCell ref="D96:D99"/>
-    <mergeCell ref="E96:E99"/>
-    <mergeCell ref="D100:D103"/>
-    <mergeCell ref="E100:E103"/>
-    <mergeCell ref="F92:F95"/>
-    <mergeCell ref="F96:F99"/>
-    <mergeCell ref="F100:F103"/>
+    <mergeCell ref="D127:D129"/>
+    <mergeCell ref="E127:E129"/>
+    <mergeCell ref="F127:F129"/>
+    <mergeCell ref="B130:C133"/>
+    <mergeCell ref="D130:D133"/>
+    <mergeCell ref="E130:E133"/>
+    <mergeCell ref="F130:F133"/>
+    <mergeCell ref="A114:C121"/>
+    <mergeCell ref="A122:C125"/>
+    <mergeCell ref="A126:C126"/>
+    <mergeCell ref="B127:C129"/>
+    <mergeCell ref="E114:E121"/>
+    <mergeCell ref="F114:F121"/>
+    <mergeCell ref="D122:D125"/>
+    <mergeCell ref="D114:D121"/>
+    <mergeCell ref="E122:E125"/>
+    <mergeCell ref="F122:F125"/>
+    <mergeCell ref="B107:C110"/>
+    <mergeCell ref="D107:D110"/>
+    <mergeCell ref="E107:E110"/>
+    <mergeCell ref="F107:F110"/>
+    <mergeCell ref="B111:C112"/>
+    <mergeCell ref="D111:D112"/>
+    <mergeCell ref="E111:E112"/>
+    <mergeCell ref="F111:F112"/>
+    <mergeCell ref="A91:C91"/>
+    <mergeCell ref="B92:C95"/>
+    <mergeCell ref="A104:C104"/>
+    <mergeCell ref="B105:C106"/>
+    <mergeCell ref="D105:D106"/>
+    <mergeCell ref="B96:B99"/>
+    <mergeCell ref="B100:B103"/>
+    <mergeCell ref="E105:E106"/>
+    <mergeCell ref="F105:F106"/>
+    <mergeCell ref="C96:C99"/>
+    <mergeCell ref="C100:C103"/>
+    <mergeCell ref="A59:C59"/>
+    <mergeCell ref="B61:C63"/>
+    <mergeCell ref="A65:C66"/>
+    <mergeCell ref="A67:C67"/>
+    <mergeCell ref="A8:C12"/>
+    <mergeCell ref="A18:C18"/>
+    <mergeCell ref="B19:C22"/>
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="A14:C15"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="A17:C17"/>
+    <mergeCell ref="B84:B87"/>
+    <mergeCell ref="C84:C87"/>
+    <mergeCell ref="D84:D87"/>
+    <mergeCell ref="E84:E87"/>
+    <mergeCell ref="F84:F87"/>
+    <mergeCell ref="B81:B83"/>
+    <mergeCell ref="C81:C83"/>
+    <mergeCell ref="D81:D83"/>
+    <mergeCell ref="E81:E83"/>
+    <mergeCell ref="F81:F83"/>
+    <mergeCell ref="B78:B80"/>
+    <mergeCell ref="C78:C80"/>
+    <mergeCell ref="D78:D80"/>
+    <mergeCell ref="E78:E80"/>
+    <mergeCell ref="F78:F80"/>
+    <mergeCell ref="B68:C68"/>
+    <mergeCell ref="B77:C77"/>
+    <mergeCell ref="B73:C75"/>
+    <mergeCell ref="D65:D66"/>
+    <mergeCell ref="E65:E66"/>
+    <mergeCell ref="F65:F66"/>
+    <mergeCell ref="F53:F55"/>
+    <mergeCell ref="E53:E55"/>
+    <mergeCell ref="D53:D55"/>
+    <mergeCell ref="A24:C24"/>
+    <mergeCell ref="B25:C27"/>
+    <mergeCell ref="B28:C30"/>
+    <mergeCell ref="B31:C34"/>
+    <mergeCell ref="A38:C38"/>
+    <mergeCell ref="B39:C41"/>
+    <mergeCell ref="B42:C44"/>
+    <mergeCell ref="B45:C48"/>
+    <mergeCell ref="A52:C52"/>
+    <mergeCell ref="B53:C55"/>
     <mergeCell ref="F61:F63"/>
     <mergeCell ref="E61:E63"/>
     <mergeCell ref="D61:D63"/>
@@ -12273,92 +12333,35 @@
     <mergeCell ref="E25:E27"/>
     <mergeCell ref="F25:F27"/>
     <mergeCell ref="E5:E7"/>
+    <mergeCell ref="F73:F75"/>
+    <mergeCell ref="E73:E75"/>
+    <mergeCell ref="D73:D75"/>
+    <mergeCell ref="D92:D95"/>
+    <mergeCell ref="E92:E95"/>
+    <mergeCell ref="D96:D99"/>
+    <mergeCell ref="E96:E99"/>
+    <mergeCell ref="D100:D103"/>
+    <mergeCell ref="E100:E103"/>
+    <mergeCell ref="F92:F95"/>
+    <mergeCell ref="F96:F99"/>
+    <mergeCell ref="F100:F103"/>
+    <mergeCell ref="D8:D12"/>
+    <mergeCell ref="E8:E12"/>
+    <mergeCell ref="F8:F12"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="F31:F34"/>
+    <mergeCell ref="E31:E34"/>
+    <mergeCell ref="F39:F41"/>
+    <mergeCell ref="F19:F22"/>
+    <mergeCell ref="E19:E22"/>
+    <mergeCell ref="E14:E15"/>
     <mergeCell ref="F5:F7"/>
     <mergeCell ref="D5:D7"/>
     <mergeCell ref="F14:F15"/>
     <mergeCell ref="D14:D15"/>
     <mergeCell ref="D19:D22"/>
-    <mergeCell ref="F53:F55"/>
-    <mergeCell ref="E53:E55"/>
-    <mergeCell ref="D53:D55"/>
-    <mergeCell ref="A24:C24"/>
-    <mergeCell ref="B25:C27"/>
-    <mergeCell ref="B28:C30"/>
-    <mergeCell ref="B31:C34"/>
-    <mergeCell ref="A38:C38"/>
-    <mergeCell ref="B39:C41"/>
-    <mergeCell ref="B42:C44"/>
-    <mergeCell ref="B45:C48"/>
-    <mergeCell ref="A52:C52"/>
-    <mergeCell ref="B78:B80"/>
-    <mergeCell ref="C78:C80"/>
-    <mergeCell ref="D78:D80"/>
-    <mergeCell ref="E78:E80"/>
-    <mergeCell ref="F78:F80"/>
-    <mergeCell ref="B68:C68"/>
-    <mergeCell ref="B77:C77"/>
-    <mergeCell ref="B73:C75"/>
-    <mergeCell ref="D65:D66"/>
-    <mergeCell ref="E65:E66"/>
-    <mergeCell ref="F65:F66"/>
-    <mergeCell ref="B84:B87"/>
-    <mergeCell ref="C84:C87"/>
-    <mergeCell ref="D84:D87"/>
-    <mergeCell ref="E84:E87"/>
-    <mergeCell ref="F84:F87"/>
-    <mergeCell ref="B81:B83"/>
-    <mergeCell ref="C81:C83"/>
-    <mergeCell ref="D81:D83"/>
-    <mergeCell ref="E81:E83"/>
-    <mergeCell ref="F81:F83"/>
-    <mergeCell ref="B53:C55"/>
-    <mergeCell ref="A59:C59"/>
-    <mergeCell ref="B61:C63"/>
-    <mergeCell ref="A65:C66"/>
-    <mergeCell ref="A67:C67"/>
-    <mergeCell ref="A8:C12"/>
-    <mergeCell ref="A18:C18"/>
-    <mergeCell ref="B19:C22"/>
-    <mergeCell ref="A13:C13"/>
-    <mergeCell ref="A14:C15"/>
-    <mergeCell ref="A16:C16"/>
-    <mergeCell ref="A17:C17"/>
-    <mergeCell ref="B107:C110"/>
-    <mergeCell ref="D107:D110"/>
-    <mergeCell ref="E107:E110"/>
-    <mergeCell ref="F107:F110"/>
-    <mergeCell ref="B111:C112"/>
-    <mergeCell ref="D111:D112"/>
-    <mergeCell ref="E111:E112"/>
-    <mergeCell ref="F111:F112"/>
-    <mergeCell ref="A91:C91"/>
-    <mergeCell ref="B92:C95"/>
-    <mergeCell ref="A104:C104"/>
-    <mergeCell ref="B105:C106"/>
-    <mergeCell ref="D105:D106"/>
-    <mergeCell ref="B96:B99"/>
-    <mergeCell ref="B100:B103"/>
-    <mergeCell ref="E105:E106"/>
-    <mergeCell ref="F105:F106"/>
-    <mergeCell ref="C96:C99"/>
-    <mergeCell ref="C100:C103"/>
-    <mergeCell ref="D127:D129"/>
-    <mergeCell ref="E127:E129"/>
-    <mergeCell ref="F127:F129"/>
-    <mergeCell ref="B130:C133"/>
-    <mergeCell ref="D130:D133"/>
-    <mergeCell ref="E130:E133"/>
-    <mergeCell ref="F130:F133"/>
-    <mergeCell ref="A114:C121"/>
-    <mergeCell ref="A122:C125"/>
-    <mergeCell ref="A126:C126"/>
-    <mergeCell ref="B127:C129"/>
-    <mergeCell ref="E114:E121"/>
-    <mergeCell ref="F114:F121"/>
-    <mergeCell ref="D122:D125"/>
-    <mergeCell ref="D114:D121"/>
-    <mergeCell ref="E122:E125"/>
-    <mergeCell ref="F122:F125"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="M3" r:id="rId1" display="e.g., DataCiteSchema" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
@@ -12368,16 +12371,16 @@
     <hyperlink ref="M12" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
     <hyperlink ref="M36" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
     <hyperlink ref="M37" r:id="rId7" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="M29" r:id="rId8" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="M30" r:id="rId9" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="M33" r:id="rId10" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="M34" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="M29" r:id="rId8" display="DataCiteSchema" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="M30" r:id="rId9" display="DataCiteSchema" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="M33" r:id="rId10" display="DataCiteSchema" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="M34" r:id="rId11" display="DataCiteSchema" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
     <hyperlink ref="M60" r:id="rId12" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
     <hyperlink ref="M61" r:id="rId13" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
     <hyperlink ref="M62" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
     <hyperlink ref="M63" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
-    <hyperlink ref="M132" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
-    <hyperlink ref="M133" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="M132" r:id="rId16" display="DataCiteSchema" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="M133" r:id="rId17" display="DataCiteSchema" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
     <hyperlink ref="L4" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
     <hyperlink ref="L3" r:id="rId19" xr:uid="{79274165-A08F-504F-ABEF-86158BAB6E38}"/>
     <hyperlink ref="L5" r:id="rId20" xr:uid="{EB38BFB8-104C-9549-9590-CD747EA2AB6E}"/>
@@ -12389,17 +12392,17 @@
     <hyperlink ref="L13" r:id="rId26" xr:uid="{E40CF022-E2D9-024B-BA4B-36300D6EABED}"/>
     <hyperlink ref="M50" r:id="rId27" xr:uid="{F21891FB-61A7-3242-9AAA-F78E177BD42B}"/>
     <hyperlink ref="M51" r:id="rId28" xr:uid="{528FA186-ED8E-6B4E-8209-54BF5C699854}"/>
-    <hyperlink ref="M43" r:id="rId29" xr:uid="{512E7D48-D0BB-474E-81C8-84AF8AADE6CD}"/>
-    <hyperlink ref="M44" r:id="rId30" xr:uid="{9F3289B1-82D8-D94D-802C-C6C552D25A29}"/>
-    <hyperlink ref="M47" r:id="rId31" xr:uid="{6F22468B-C0E2-8E44-88CB-546D020C68F0}"/>
-    <hyperlink ref="M48" r:id="rId32" xr:uid="{A7D1F61F-E528-0C44-AC76-2EF1F8BEB3E9}"/>
+    <hyperlink ref="M43" r:id="rId29" display="DataCiteSchema" xr:uid="{512E7D48-D0BB-474E-81C8-84AF8AADE6CD}"/>
+    <hyperlink ref="M44" r:id="rId30" display="DataCiteSchema" xr:uid="{9F3289B1-82D8-D94D-802C-C6C552D25A29}"/>
+    <hyperlink ref="M47" r:id="rId31" display="DataCiteSchema" xr:uid="{6F22468B-C0E2-8E44-88CB-546D020C68F0}"/>
+    <hyperlink ref="M48" r:id="rId32" display="DataCiteSchema" xr:uid="{A7D1F61F-E528-0C44-AC76-2EF1F8BEB3E9}"/>
     <hyperlink ref="M64" r:id="rId33" xr:uid="{0CC4972C-ECFA-B440-9A75-02F82DDED55D}"/>
-    <hyperlink ref="M89" r:id="rId34" xr:uid="{9D6D4BCF-FB27-6D40-A7BD-017D1A5A4757}"/>
-    <hyperlink ref="M90" r:id="rId35" xr:uid="{A858633D-A581-7741-AFEF-6719BC41416C}"/>
-    <hyperlink ref="M82" r:id="rId36" xr:uid="{31DE2953-BF4E-694F-871C-448507278D9A}"/>
-    <hyperlink ref="M83" r:id="rId37" xr:uid="{8630DA0C-B932-C246-9078-95C72FB5BF91}"/>
-    <hyperlink ref="M86" r:id="rId38" xr:uid="{1B438F6A-F696-1841-A0B8-8C5CDE068A67}"/>
-    <hyperlink ref="M87" r:id="rId39" xr:uid="{DDF97B6B-BEE3-3C44-8345-9022D2F48A26}"/>
+    <hyperlink ref="M89" r:id="rId34" display="DataCiteSchema" xr:uid="{9D6D4BCF-FB27-6D40-A7BD-017D1A5A4757}"/>
+    <hyperlink ref="M90" r:id="rId35" display="DataCiteSchema" xr:uid="{A858633D-A581-7741-AFEF-6719BC41416C}"/>
+    <hyperlink ref="M82" r:id="rId36" display="DataCiteSchema" xr:uid="{31DE2953-BF4E-694F-871C-448507278D9A}"/>
+    <hyperlink ref="M83" r:id="rId37" display="DataCiteSchema" xr:uid="{8630DA0C-B932-C246-9078-95C72FB5BF91}"/>
+    <hyperlink ref="M86" r:id="rId38" display="DataCiteSchema" xr:uid="{1B438F6A-F696-1841-A0B8-8C5CDE068A67}"/>
+    <hyperlink ref="M87" r:id="rId39" display="DataCiteSchema" xr:uid="{DDF97B6B-BEE3-3C44-8345-9022D2F48A26}"/>
     <hyperlink ref="D151" r:id="rId40" display="https://fairdatacollective.org/" xr:uid="{F7D6490E-4341-0240-BE7B-5E8915480BD0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
@@ -12426,7 +12429,7 @@
       </c>
       <c r="B1" s="738"/>
       <c r="C1" s="20" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="D1" s="21" t="s">
         <v>54</v>
@@ -12445,17 +12448,17 @@
       <c r="M1" s="28"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A2" s="733"/>
-      <c r="B2" s="734" t="s">
-        <v>464</v>
-      </c>
-      <c r="C2" s="739" t="s">
-        <v>456</v>
-      </c>
-      <c r="D2" s="735" t="s">
+      <c r="A2" s="739"/>
+      <c r="B2" s="740" t="s">
+        <v>463</v>
+      </c>
+      <c r="C2" s="741" t="s">
+        <v>455</v>
+      </c>
+      <c r="D2" s="742" t="s">
         <v>54</v>
       </c>
-      <c r="E2" s="736" t="str">
+      <c r="E2" s="737" t="str">
         <f>Namespace &amp; LOWER($B2)</f>
         <v>http://vocab.fairdatacollective.org/dataset/properties/contributorname</v>
       </c>
@@ -12485,16 +12488,16 @@
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A3" s="733"/>
-      <c r="B3" s="734"/>
-      <c r="C3" s="739"/>
-      <c r="D3" s="735"/>
-      <c r="E3" s="736"/>
+      <c r="A3" s="739"/>
+      <c r="B3" s="740"/>
+      <c r="C3" s="741"/>
+      <c r="D3" s="742"/>
+      <c r="E3" s="737"/>
       <c r="F3" s="34" t="s">
         <v>111</v>
       </c>
       <c r="G3" s="35" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="H3" s="36" t="s">
         <v>112</v>
@@ -12516,16 +12519,16 @@
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A4" s="733"/>
-      <c r="B4" s="734"/>
-      <c r="C4" s="739"/>
-      <c r="D4" s="735"/>
-      <c r="E4" s="736"/>
+      <c r="A4" s="739"/>
+      <c r="B4" s="740"/>
+      <c r="C4" s="741"/>
+      <c r="D4" s="742"/>
+      <c r="E4" s="737"/>
       <c r="F4" s="34" t="s">
         <v>113</v>
       </c>
       <c r="G4" s="35" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="H4" s="36" t="s">
         <v>114</v>
@@ -12547,17 +12550,17 @@
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5" s="733"/>
-      <c r="B5" s="734" t="s">
-        <v>467</v>
-      </c>
-      <c r="C5" s="734" t="s">
-        <v>457</v>
-      </c>
-      <c r="D5" s="735" t="s">
+      <c r="A5" s="739"/>
+      <c r="B5" s="740" t="s">
+        <v>466</v>
+      </c>
+      <c r="C5" s="740" t="s">
+        <v>456</v>
+      </c>
+      <c r="D5" s="742" t="s">
         <v>54</v>
       </c>
-      <c r="E5" s="736" t="str">
+      <c r="E5" s="737" t="str">
         <f>Namespace &amp; LOWER($B5)</f>
         <v>http://vocab.fairdatacollective.org/dataset/properties/contributoridentifier</v>
       </c>
@@ -12568,7 +12571,7 @@
         <v>327</v>
       </c>
       <c r="H5" s="36" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="I5" s="32" t="s">
         <v>54</v>
@@ -12588,11 +12591,11 @@
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A6" s="733"/>
-      <c r="B6" s="734"/>
-      <c r="C6" s="734"/>
-      <c r="D6" s="735"/>
-      <c r="E6" s="736"/>
+      <c r="A6" s="739"/>
+      <c r="B6" s="740"/>
+      <c r="C6" s="740"/>
+      <c r="D6" s="742"/>
+      <c r="E6" s="737"/>
       <c r="F6" s="34" t="s">
         <v>121</v>
       </c>
@@ -12620,11 +12623,11 @@
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A7" s="733"/>
-      <c r="B7" s="734"/>
-      <c r="C7" s="734"/>
-      <c r="D7" s="735"/>
-      <c r="E7" s="736"/>
+      <c r="A7" s="739"/>
+      <c r="B7" s="740"/>
+      <c r="C7" s="740"/>
+      <c r="D7" s="742"/>
+      <c r="E7" s="737"/>
       <c r="F7" s="34" t="s">
         <v>122</v>
       </c>
@@ -12652,17 +12655,17 @@
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A8" s="733"/>
-      <c r="B8" s="734" t="s">
-        <v>468</v>
-      </c>
-      <c r="C8" s="734" t="s">
-        <v>459</v>
-      </c>
-      <c r="D8" s="735" t="s">
+      <c r="A8" s="739"/>
+      <c r="B8" s="740" t="s">
+        <v>467</v>
+      </c>
+      <c r="C8" s="740" t="s">
+        <v>458</v>
+      </c>
+      <c r="D8" s="742" t="s">
         <v>54</v>
       </c>
-      <c r="E8" s="737" t="str">
+      <c r="E8" s="743" t="str">
         <f>Namespace &amp; LOWER($B8)</f>
         <v>http://vocab.fairdatacollective.org/dataset/properties/contributoraffiliation</v>
       </c>
@@ -12673,7 +12676,7 @@
         <v>330</v>
       </c>
       <c r="H8" s="36" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="I8" s="32" t="s">
         <v>34</v>
@@ -12693,11 +12696,11 @@
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A9" s="733"/>
-      <c r="B9" s="734"/>
-      <c r="C9" s="734"/>
-      <c r="D9" s="735"/>
-      <c r="E9" s="737"/>
+      <c r="A9" s="739"/>
+      <c r="B9" s="740"/>
+      <c r="C9" s="740"/>
+      <c r="D9" s="742"/>
+      <c r="E9" s="743"/>
       <c r="F9" s="34" t="s">
         <v>123</v>
       </c>
@@ -12725,13 +12728,13 @@
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A10" s="733"/>
-      <c r="B10" s="734"/>
-      <c r="C10" s="734"/>
-      <c r="D10" s="735"/>
-      <c r="E10" s="737"/>
+      <c r="A10" s="739"/>
+      <c r="B10" s="740"/>
+      <c r="C10" s="740"/>
+      <c r="D10" s="742"/>
+      <c r="E10" s="743"/>
       <c r="F10" s="34" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="G10" s="35" t="s">
         <v>333</v>
@@ -12757,11 +12760,11 @@
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A11" s="733"/>
-      <c r="B11" s="734"/>
-      <c r="C11" s="734"/>
-      <c r="D11" s="735"/>
-      <c r="E11" s="737"/>
+      <c r="A11" s="739"/>
+      <c r="B11" s="740"/>
+      <c r="C11" s="740"/>
+      <c r="D11" s="742"/>
+      <c r="E11" s="743"/>
       <c r="F11" s="34" t="s">
         <v>125</v>
       </c>
@@ -12832,7 +12835,7 @@
         <v>323</v>
       </c>
       <c r="H13" s="36" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="I13" s="32" t="s">
         <v>34</v>
@@ -12885,22 +12888,22 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="C5:C7"/>
+    <mergeCell ref="D5:D7"/>
+    <mergeCell ref="E5:E7"/>
+    <mergeCell ref="A8:A11"/>
+    <mergeCell ref="B8:B11"/>
+    <mergeCell ref="C8:C11"/>
+    <mergeCell ref="D8:D11"/>
+    <mergeCell ref="E8:E11"/>
     <mergeCell ref="E2:E4"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="B2:B4"/>
     <mergeCell ref="C2:C4"/>
     <mergeCell ref="D2:D4"/>
-    <mergeCell ref="A8:A11"/>
-    <mergeCell ref="B8:B11"/>
-    <mergeCell ref="C8:C11"/>
-    <mergeCell ref="D8:D11"/>
-    <mergeCell ref="E8:E11"/>
-    <mergeCell ref="A5:A7"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="C5:C7"/>
-    <mergeCell ref="D5:D7"/>
-    <mergeCell ref="E5:E7"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="L13" r:id="rId1" xr:uid="{9ABA6EE5-7A54-DF40-9E10-C757BCBA07FF}"/>

</xml_diff>

<commit_message>
made all controlled terms and properties
</commit_message>
<xml_diff>
--- a/template-description.xlsx
+++ b/template-description.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Secondary_Drive/work/repos/FAIR-data/generic-dataset-metadata-template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0FA80AF-DE41-CB4C-8235-9850CAD6AC54}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67EE3CA1-D949-DC46-A530-D89FDEAE5BA7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="68800" windowHeight="28340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,6 +21,7 @@
     <definedName name="Namespace">'Dataset template'!$D$151</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -1764,7 +1765,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="43">
+  <fills count="42">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2011,12 +2012,6 @@
         <bgColor rgb="FFD8D8D8"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC8C8C8"/>
-        <bgColor rgb="FFD9D9D9"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="7">
     <border>
@@ -2089,7 +2084,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="744">
+  <cellXfs count="742">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -3113,7 +3108,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="41" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="42" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="41" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -3139,7 +3133,6 @@
     <xf numFmtId="0" fontId="11" fillId="41" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="42" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="41" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="41" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="41" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -3162,6 +3155,489 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="41" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="41" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="41" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="41" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="41" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="41" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="41" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="41" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="35" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="35" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="35" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="35" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="38" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="38" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="35" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="35" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="35" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="38" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="38" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="38" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="38" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="30" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="24" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="34" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="34" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="34" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="34" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="35" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="35" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="30" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="30" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="35" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="35" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="37" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="37" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="37" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="37" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -3174,8 +3650,6 @@
     <xf numFmtId="0" fontId="11" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -3204,24 +3678,6 @@
     <xf numFmtId="0" fontId="11" fillId="19" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="37" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="37" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -3246,183 +3702,6 @@
     <xf numFmtId="0" fontId="11" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="31" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="31" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="31" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="31" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="30" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="30" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="35" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="35" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="35" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="35" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="37" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="37" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -3453,312 +3732,26 @@
     <xf numFmtId="0" fontId="11" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="26" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="26" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="26" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="26" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="35" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="35" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="34" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="34" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="31" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="34" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="34" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="30" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="24" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="35" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="35" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="38" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="38" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="35" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="35" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="35" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="38" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="38" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="26" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="38" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="38" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="41" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="41" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="41" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="41" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="41" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="41" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="28" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="28" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="41" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="41" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="28" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3993,10 +3986,10 @@
   <dimension ref="A1:P1034"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D28" sqref="D28:D30"/>
+      <selection pane="bottomRight" activeCell="L24" sqref="L24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4018,11 +4011,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="612" t="s">
+      <c r="A1" s="669" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="612"/>
-      <c r="C1" s="612"/>
+      <c r="B1" s="669"/>
+      <c r="C1" s="669"/>
       <c r="D1" s="44" t="s">
         <v>1</v>
       </c>
@@ -4060,11 +4053,11 @@
       <c r="P1" s="1"/>
     </row>
     <row r="2" spans="1:16" ht="69" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="611" t="s">
+      <c r="A2" s="668" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="611"/>
-      <c r="C2" s="611"/>
+      <c r="B2" s="668"/>
+      <c r="C2" s="668"/>
       <c r="D2" s="126" t="s">
         <v>10</v>
       </c>
@@ -4096,18 +4089,18 @@
       <c r="P2" s="2"/>
     </row>
     <row r="3" spans="1:16" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="606" t="s">
+      <c r="A3" s="663" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="606"/>
-      <c r="C3" s="606"/>
-      <c r="D3" s="551" t="s">
+      <c r="B3" s="663"/>
+      <c r="C3" s="663"/>
+      <c r="D3" s="710" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="553">
+      <c r="E3" s="712">
         <v>1</v>
       </c>
-      <c r="F3" s="554" t="str">
+      <c r="F3" s="713" t="str">
         <f>Namespace &amp; $A3</f>
         <v>http://vocab.fairdatacollective.org/dataset/properties/ResourceType</v>
       </c>
@@ -4137,12 +4130,12 @@
       </c>
     </row>
     <row r="4" spans="1:16" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="607"/>
-      <c r="B4" s="607"/>
-      <c r="C4" s="607"/>
-      <c r="D4" s="552"/>
-      <c r="E4" s="547"/>
-      <c r="F4" s="555"/>
+      <c r="A4" s="664"/>
+      <c r="B4" s="664"/>
+      <c r="C4" s="664"/>
+      <c r="D4" s="711"/>
+      <c r="E4" s="578"/>
+      <c r="F4" s="714"/>
       <c r="G4" s="190" t="s">
         <v>22</v>
       </c>
@@ -4169,18 +4162,18 @@
       </c>
     </row>
     <row r="5" spans="1:16" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="608" t="s">
+      <c r="A5" s="665" t="s">
         <v>259</v>
       </c>
-      <c r="B5" s="608"/>
-      <c r="C5" s="608"/>
-      <c r="D5" s="634" t="s">
+      <c r="B5" s="665"/>
+      <c r="C5" s="665"/>
+      <c r="D5" s="728" t="s">
         <v>25</v>
       </c>
-      <c r="E5" s="628">
+      <c r="E5" s="685">
         <v>1</v>
       </c>
-      <c r="F5" s="631" t="str">
+      <c r="F5" s="725" t="str">
         <f>Namespace &amp; ($A5)</f>
         <v>http://vocab.fairdatacollective.org/dataset/properties/DatasetIdentifier</v>
       </c>
@@ -4210,12 +4203,12 @@
       </c>
     </row>
     <row r="6" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="609"/>
-      <c r="B6" s="609"/>
-      <c r="C6" s="609"/>
-      <c r="D6" s="635"/>
-      <c r="E6" s="629"/>
-      <c r="F6" s="632"/>
+      <c r="A6" s="666"/>
+      <c r="B6" s="666"/>
+      <c r="C6" s="666"/>
+      <c r="D6" s="729"/>
+      <c r="E6" s="686"/>
+      <c r="F6" s="726"/>
       <c r="G6" s="53" t="s">
         <v>29</v>
       </c>
@@ -4242,12 +4235,12 @@
       </c>
     </row>
     <row r="7" spans="1:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="610"/>
-      <c r="B7" s="610"/>
-      <c r="C7" s="610"/>
-      <c r="D7" s="636"/>
-      <c r="E7" s="630"/>
-      <c r="F7" s="633"/>
+      <c r="A7" s="667"/>
+      <c r="B7" s="667"/>
+      <c r="C7" s="667"/>
+      <c r="D7" s="730"/>
+      <c r="E7" s="687"/>
+      <c r="F7" s="727"/>
       <c r="G7" s="203" t="s">
         <v>32</v>
       </c>
@@ -4275,18 +4268,18 @@
       </c>
     </row>
     <row r="8" spans="1:16" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="676" t="s">
+      <c r="A8" s="609" t="s">
         <v>33</v>
       </c>
-      <c r="B8" s="676"/>
-      <c r="C8" s="676"/>
-      <c r="D8" s="542" t="s">
+      <c r="B8" s="609"/>
+      <c r="C8" s="609"/>
+      <c r="D8" s="703" t="s">
         <v>276</v>
       </c>
-      <c r="E8" s="545" t="s">
+      <c r="E8" s="706" t="s">
         <v>34</v>
       </c>
-      <c r="F8" s="548" t="str">
+      <c r="F8" s="707" t="str">
         <f>Namespace &amp; ($A8)</f>
         <v>http://vocab.fairdatacollective.org/dataset/properties/RelatedResources</v>
       </c>
@@ -4316,12 +4309,12 @@
       </c>
     </row>
     <row r="9" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="677"/>
-      <c r="B9" s="677"/>
-      <c r="C9" s="677"/>
-      <c r="D9" s="543"/>
-      <c r="E9" s="546"/>
-      <c r="F9" s="549"/>
+      <c r="A9" s="610"/>
+      <c r="B9" s="610"/>
+      <c r="C9" s="610"/>
+      <c r="D9" s="704"/>
+      <c r="E9" s="577"/>
+      <c r="F9" s="708"/>
       <c r="G9" s="59" t="s">
         <v>38</v>
       </c>
@@ -4348,12 +4341,12 @@
       </c>
     </row>
     <row r="10" spans="1:16" s="10" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="677"/>
-      <c r="B10" s="677"/>
-      <c r="C10" s="677"/>
-      <c r="D10" s="543"/>
-      <c r="E10" s="546"/>
-      <c r="F10" s="549"/>
+      <c r="A10" s="610"/>
+      <c r="B10" s="610"/>
+      <c r="C10" s="610"/>
+      <c r="D10" s="704"/>
+      <c r="E10" s="577"/>
+      <c r="F10" s="708"/>
       <c r="G10" s="59" t="s">
         <v>272</v>
       </c>
@@ -4381,12 +4374,12 @@
       </c>
     </row>
     <row r="11" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="677"/>
-      <c r="B11" s="677"/>
-      <c r="C11" s="677"/>
-      <c r="D11" s="543"/>
-      <c r="E11" s="546"/>
-      <c r="F11" s="549"/>
+      <c r="A11" s="610"/>
+      <c r="B11" s="610"/>
+      <c r="C11" s="610"/>
+      <c r="D11" s="704"/>
+      <c r="E11" s="577"/>
+      <c r="F11" s="708"/>
       <c r="G11" s="64" t="s">
         <v>41</v>
       </c>
@@ -4413,12 +4406,12 @@
       </c>
     </row>
     <row r="12" spans="1:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="678"/>
-      <c r="B12" s="678"/>
-      <c r="C12" s="678"/>
-      <c r="D12" s="544"/>
-      <c r="E12" s="547"/>
-      <c r="F12" s="550"/>
+      <c r="A12" s="611"/>
+      <c r="B12" s="611"/>
+      <c r="C12" s="611"/>
+      <c r="D12" s="705"/>
+      <c r="E12" s="578"/>
+      <c r="F12" s="709"/>
       <c r="G12" s="216" t="s">
         <v>42</v>
       </c>
@@ -4445,11 +4438,11 @@
       </c>
     </row>
     <row r="13" spans="1:16" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="680" t="s">
+      <c r="A13" s="616" t="s">
         <v>44</v>
       </c>
-      <c r="B13" s="680"/>
-      <c r="C13" s="680"/>
+      <c r="B13" s="616"/>
+      <c r="C13" s="616"/>
       <c r="D13" s="243" t="s">
         <v>45</v>
       </c>
@@ -4486,18 +4479,18 @@
       </c>
     </row>
     <row r="14" spans="1:16" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="681" t="s">
+      <c r="A14" s="617" t="s">
         <v>48</v>
       </c>
-      <c r="B14" s="681"/>
-      <c r="C14" s="681"/>
-      <c r="D14" s="639" t="s">
+      <c r="B14" s="617"/>
+      <c r="C14" s="617"/>
+      <c r="D14" s="733" t="s">
         <v>49</v>
       </c>
-      <c r="E14" s="570" t="s">
+      <c r="E14" s="723" t="s">
         <v>46</v>
       </c>
-      <c r="F14" s="637" t="str">
+      <c r="F14" s="731" t="str">
         <f>Namespace &amp; ($A14)</f>
         <v>http://vocab.fairdatacollective.org/dataset/properties/Language</v>
       </c>
@@ -4527,12 +4520,12 @@
       </c>
     </row>
     <row r="15" spans="1:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="682"/>
-      <c r="B15" s="682"/>
-      <c r="C15" s="682"/>
-      <c r="D15" s="640"/>
-      <c r="E15" s="571"/>
-      <c r="F15" s="638"/>
+      <c r="A15" s="618"/>
+      <c r="B15" s="618"/>
+      <c r="C15" s="618"/>
+      <c r="D15" s="734"/>
+      <c r="E15" s="724"/>
+      <c r="F15" s="732"/>
       <c r="G15" s="229" t="s">
         <v>51</v>
       </c>
@@ -4562,11 +4555,11 @@
       <c r="P15" s="11"/>
     </row>
     <row r="16" spans="1:16" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="683" t="s">
+      <c r="A16" s="619" t="s">
         <v>52</v>
       </c>
-      <c r="B16" s="683"/>
-      <c r="C16" s="683"/>
+      <c r="B16" s="619"/>
+      <c r="C16" s="619"/>
       <c r="D16" s="244" t="s">
         <v>53</v>
       </c>
@@ -4603,11 +4596,11 @@
       </c>
     </row>
     <row r="17" spans="1:16" s="11" customFormat="1" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="684" t="s">
+      <c r="A17" s="620" t="s">
         <v>57</v>
       </c>
-      <c r="B17" s="684"/>
-      <c r="C17" s="684"/>
+      <c r="B17" s="620"/>
+      <c r="C17" s="620"/>
       <c r="D17" s="78" t="s">
         <v>58</v>
       </c>
@@ -4646,11 +4639,11 @@
       <c r="P17"/>
     </row>
     <row r="18" spans="1:16" s="11" customFormat="1" ht="17" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="679" t="s">
+      <c r="A18" s="612" t="s">
         <v>62</v>
       </c>
-      <c r="B18" s="679"/>
-      <c r="C18" s="679"/>
+      <c r="B18" s="612"/>
+      <c r="C18" s="612"/>
       <c r="D18" s="245" t="s">
         <v>63</v>
       </c>
@@ -4674,17 +4667,17 @@
     </row>
     <row r="19" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="315"/>
-      <c r="B19" s="641" t="s">
+      <c r="B19" s="613" t="s">
         <v>501</v>
       </c>
-      <c r="C19" s="641"/>
-      <c r="D19" s="641" t="s">
+      <c r="C19" s="613"/>
+      <c r="D19" s="613" t="s">
         <v>468</v>
       </c>
-      <c r="E19" s="567" t="s">
+      <c r="E19" s="720" t="s">
         <v>34</v>
       </c>
-      <c r="F19" s="564" t="str">
+      <c r="F19" s="717" t="str">
         <f>Namespace&amp;($A19)</f>
         <v>http://vocab.fairdatacollective.org/dataset/properties/</v>
       </c>
@@ -4715,11 +4708,11 @@
     </row>
     <row r="20" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="315"/>
-      <c r="B20" s="642"/>
-      <c r="C20" s="642"/>
-      <c r="D20" s="642"/>
-      <c r="E20" s="568"/>
-      <c r="F20" s="565"/>
+      <c r="B20" s="614"/>
+      <c r="C20" s="614"/>
+      <c r="D20" s="614"/>
+      <c r="E20" s="721"/>
+      <c r="F20" s="718"/>
       <c r="G20" s="79" t="s">
         <v>469</v>
       </c>
@@ -4748,11 +4741,11 @@
     </row>
     <row r="21" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="315"/>
-      <c r="B21" s="642"/>
-      <c r="C21" s="642"/>
-      <c r="D21" s="642"/>
-      <c r="E21" s="568"/>
-      <c r="F21" s="565"/>
+      <c r="B21" s="614"/>
+      <c r="C21" s="614"/>
+      <c r="D21" s="614"/>
+      <c r="E21" s="721"/>
+      <c r="F21" s="718"/>
       <c r="G21" s="83" t="s">
         <v>70</v>
       </c>
@@ -4781,11 +4774,11 @@
     </row>
     <row r="22" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="315"/>
-      <c r="B22" s="643"/>
-      <c r="C22" s="643"/>
-      <c r="D22" s="643"/>
-      <c r="E22" s="569"/>
-      <c r="F22" s="566"/>
+      <c r="B22" s="615"/>
+      <c r="C22" s="615"/>
+      <c r="D22" s="615"/>
+      <c r="E22" s="722"/>
+      <c r="F22" s="719"/>
       <c r="G22" s="132" t="s">
         <v>71</v>
       </c>
@@ -4844,11 +4837,11 @@
       </c>
     </row>
     <row r="24" spans="1:16" s="14" customFormat="1" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="653" t="s">
+      <c r="A24" s="649" t="s">
         <v>72</v>
       </c>
-      <c r="B24" s="653"/>
-      <c r="C24" s="653"/>
+      <c r="B24" s="649"/>
+      <c r="C24" s="649"/>
       <c r="D24" s="246" t="s">
         <v>73</v>
       </c>
@@ -4870,17 +4863,17 @@
     </row>
     <row r="25" spans="1:16" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="17"/>
-      <c r="B25" s="622" t="s">
+      <c r="B25" s="650" t="s">
         <v>452</v>
       </c>
-      <c r="C25" s="622"/>
-      <c r="D25" s="622" t="s">
+      <c r="C25" s="650"/>
+      <c r="D25" s="650" t="s">
         <v>478</v>
       </c>
-      <c r="E25" s="558" t="s">
+      <c r="E25" s="679" t="s">
         <v>54</v>
       </c>
-      <c r="F25" s="625" t="str">
+      <c r="F25" s="682" t="str">
         <f>Namespace &amp; ($B25)</f>
         <v>http://vocab.fairdatacollective.org/dataset/properties/CreatorName</v>
       </c>
@@ -4911,11 +4904,11 @@
     </row>
     <row r="26" spans="1:16" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="17"/>
-      <c r="B26" s="623"/>
-      <c r="C26" s="623"/>
-      <c r="D26" s="623"/>
-      <c r="E26" s="559"/>
-      <c r="F26" s="626"/>
+      <c r="B26" s="651"/>
+      <c r="C26" s="651"/>
+      <c r="D26" s="651"/>
+      <c r="E26" s="680"/>
+      <c r="F26" s="683"/>
       <c r="G26" s="87" t="s">
         <v>79</v>
       </c>
@@ -4943,11 +4936,11 @@
     </row>
     <row r="27" spans="1:16" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="17"/>
-      <c r="B27" s="624"/>
-      <c r="C27" s="624"/>
-      <c r="D27" s="624"/>
-      <c r="E27" s="560"/>
-      <c r="F27" s="627"/>
+      <c r="B27" s="652"/>
+      <c r="C27" s="652"/>
+      <c r="D27" s="652"/>
+      <c r="E27" s="681"/>
+      <c r="F27" s="684"/>
       <c r="G27" s="141" t="s">
         <v>82</v>
       </c>
@@ -4975,17 +4968,17 @@
     </row>
     <row r="28" spans="1:16" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="17"/>
-      <c r="B28" s="622" t="s">
+      <c r="B28" s="650" t="s">
         <v>453</v>
       </c>
-      <c r="C28" s="622"/>
-      <c r="D28" s="622" t="s">
+      <c r="C28" s="650"/>
+      <c r="D28" s="650" t="s">
         <v>477</v>
       </c>
-      <c r="E28" s="558" t="s">
+      <c r="E28" s="679" t="s">
         <v>54</v>
       </c>
-      <c r="F28" s="625" t="str">
+      <c r="F28" s="682" t="str">
         <f>Namespace &amp; ($B28)</f>
         <v>http://vocab.fairdatacollective.org/dataset/properties/CreatorIdentifier</v>
       </c>
@@ -5017,11 +5010,11 @@
     </row>
     <row r="29" spans="1:16" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="17"/>
-      <c r="B29" s="623"/>
-      <c r="C29" s="623"/>
-      <c r="D29" s="623"/>
-      <c r="E29" s="559"/>
-      <c r="F29" s="626"/>
+      <c r="B29" s="651"/>
+      <c r="C29" s="651"/>
+      <c r="D29" s="651"/>
+      <c r="E29" s="680"/>
+      <c r="F29" s="683"/>
       <c r="G29" s="87" t="s">
         <v>93</v>
       </c>
@@ -5050,11 +5043,11 @@
     </row>
     <row r="30" spans="1:16" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="17"/>
-      <c r="B30" s="624"/>
-      <c r="C30" s="624"/>
-      <c r="D30" s="624"/>
-      <c r="E30" s="560"/>
-      <c r="F30" s="627"/>
+      <c r="B30" s="652"/>
+      <c r="C30" s="652"/>
+      <c r="D30" s="652"/>
+      <c r="E30" s="681"/>
+      <c r="F30" s="684"/>
       <c r="G30" s="141" t="s">
         <v>95</v>
       </c>
@@ -5083,17 +5076,17 @@
     </row>
     <row r="31" spans="1:16" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="17"/>
-      <c r="B31" s="622" t="s">
+      <c r="B31" s="650" t="s">
         <v>454</v>
       </c>
-      <c r="C31" s="622"/>
-      <c r="D31" s="622" t="s">
+      <c r="C31" s="650"/>
+      <c r="D31" s="650" t="s">
         <v>476</v>
       </c>
-      <c r="E31" s="558" t="s">
+      <c r="E31" s="679" t="s">
         <v>54</v>
       </c>
-      <c r="F31" s="556" t="str">
+      <c r="F31" s="715" t="str">
         <f>Namespace &amp; ($B31)</f>
         <v>http://vocab.fairdatacollective.org/dataset/properties/CreatorAffiliation</v>
       </c>
@@ -5125,11 +5118,11 @@
     </row>
     <row r="32" spans="1:16" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="17"/>
-      <c r="B32" s="623"/>
-      <c r="C32" s="623"/>
-      <c r="D32" s="623"/>
-      <c r="E32" s="559"/>
-      <c r="F32" s="556"/>
+      <c r="B32" s="651"/>
+      <c r="C32" s="651"/>
+      <c r="D32" s="651"/>
+      <c r="E32" s="680"/>
+      <c r="F32" s="715"/>
       <c r="G32" s="87" t="s">
         <v>100</v>
       </c>
@@ -5158,11 +5151,11 @@
     </row>
     <row r="33" spans="1:16" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="17"/>
-      <c r="B33" s="623"/>
-      <c r="C33" s="623"/>
-      <c r="D33" s="623"/>
-      <c r="E33" s="559"/>
-      <c r="F33" s="556"/>
+      <c r="B33" s="651"/>
+      <c r="C33" s="651"/>
+      <c r="D33" s="651"/>
+      <c r="E33" s="680"/>
+      <c r="F33" s="715"/>
       <c r="G33" s="87" t="s">
         <v>103</v>
       </c>
@@ -5191,11 +5184,11 @@
     </row>
     <row r="34" spans="1:16" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="17"/>
-      <c r="B34" s="624"/>
-      <c r="C34" s="624"/>
-      <c r="D34" s="624"/>
-      <c r="E34" s="560"/>
-      <c r="F34" s="557"/>
+      <c r="B34" s="652"/>
+      <c r="C34" s="652"/>
+      <c r="D34" s="652"/>
+      <c r="E34" s="681"/>
+      <c r="F34" s="716"/>
       <c r="G34" s="141" t="s">
         <v>105</v>
       </c>
@@ -5321,11 +5314,11 @@
       </c>
     </row>
     <row r="38" spans="1:16" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="654" t="s">
+      <c r="A38" s="653" t="s">
         <v>107</v>
       </c>
-      <c r="B38" s="654"/>
-      <c r="C38" s="654"/>
+      <c r="B38" s="653"/>
+      <c r="C38" s="653"/>
       <c r="D38" s="382" t="s">
         <v>462</v>
       </c>
@@ -5347,17 +5340,17 @@
     </row>
     <row r="39" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="424"/>
-      <c r="B39" s="655" t="s">
+      <c r="B39" s="654" t="s">
         <v>463</v>
       </c>
-      <c r="C39" s="655"/>
-      <c r="D39" s="613" t="s">
+      <c r="C39" s="654"/>
+      <c r="D39" s="670" t="s">
         <v>479</v>
       </c>
-      <c r="E39" s="616" t="s">
+      <c r="E39" s="585" t="s">
         <v>34</v>
       </c>
-      <c r="F39" s="561" t="str">
+      <c r="F39" s="676" t="str">
         <f>Namespace &amp; ($B39)</f>
         <v>http://vocab.fairdatacollective.org/dataset/properties/ContributorName</v>
       </c>
@@ -5388,11 +5381,11 @@
     </row>
     <row r="40" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="424"/>
-      <c r="B40" s="655"/>
-      <c r="C40" s="655"/>
-      <c r="D40" s="614"/>
-      <c r="E40" s="617"/>
-      <c r="F40" s="562"/>
+      <c r="B40" s="654"/>
+      <c r="C40" s="654"/>
+      <c r="D40" s="671"/>
+      <c r="E40" s="586"/>
+      <c r="F40" s="677"/>
       <c r="G40" s="394" t="s">
         <v>111</v>
       </c>
@@ -5420,11 +5413,11 @@
     </row>
     <row r="41" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="424"/>
-      <c r="B41" s="655"/>
-      <c r="C41" s="655"/>
-      <c r="D41" s="615"/>
-      <c r="E41" s="618"/>
-      <c r="F41" s="563"/>
+      <c r="B41" s="654"/>
+      <c r="C41" s="654"/>
+      <c r="D41" s="672"/>
+      <c r="E41" s="587"/>
+      <c r="F41" s="678"/>
       <c r="G41" s="399" t="s">
         <v>113</v>
       </c>
@@ -5452,17 +5445,17 @@
     </row>
     <row r="42" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" s="424"/>
-      <c r="B42" s="655" t="s">
+      <c r="B42" s="654" t="s">
         <v>466</v>
       </c>
-      <c r="C42" s="655"/>
-      <c r="D42" s="613" t="s">
+      <c r="C42" s="654"/>
+      <c r="D42" s="670" t="s">
         <v>480</v>
       </c>
-      <c r="E42" s="616" t="s">
+      <c r="E42" s="585" t="s">
         <v>34</v>
       </c>
-      <c r="F42" s="561" t="str">
+      <c r="F42" s="676" t="str">
         <f>Namespace &amp; ($B42)</f>
         <v>http://vocab.fairdatacollective.org/dataset/properties/ContributorIdentifier</v>
       </c>
@@ -5494,11 +5487,11 @@
     </row>
     <row r="43" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="424"/>
-      <c r="B43" s="655"/>
-      <c r="C43" s="655"/>
-      <c r="D43" s="614"/>
-      <c r="E43" s="617"/>
-      <c r="F43" s="562"/>
+      <c r="B43" s="654"/>
+      <c r="C43" s="654"/>
+      <c r="D43" s="671"/>
+      <c r="E43" s="586"/>
+      <c r="F43" s="677"/>
       <c r="G43" s="394" t="s">
         <v>121</v>
       </c>
@@ -5527,11 +5520,11 @@
     </row>
     <row r="44" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="424"/>
-      <c r="B44" s="655"/>
-      <c r="C44" s="655"/>
-      <c r="D44" s="615"/>
-      <c r="E44" s="618"/>
-      <c r="F44" s="563"/>
+      <c r="B44" s="654"/>
+      <c r="C44" s="654"/>
+      <c r="D44" s="672"/>
+      <c r="E44" s="587"/>
+      <c r="F44" s="678"/>
       <c r="G44" s="399" t="s">
         <v>122</v>
       </c>
@@ -5560,17 +5553,17 @@
     </row>
     <row r="45" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="424"/>
-      <c r="B45" s="655" t="s">
+      <c r="B45" s="654" t="s">
         <v>467</v>
       </c>
-      <c r="C45" s="655"/>
-      <c r="D45" s="613" t="s">
+      <c r="C45" s="654"/>
+      <c r="D45" s="670" t="s">
         <v>481</v>
       </c>
-      <c r="E45" s="616" t="s">
+      <c r="E45" s="585" t="s">
         <v>34</v>
       </c>
-      <c r="F45" s="619" t="str">
+      <c r="F45" s="673" t="str">
         <f>Namespace &amp; ($B45)</f>
         <v>http://vocab.fairdatacollective.org/dataset/properties/ContributorAffiliation</v>
       </c>
@@ -5602,11 +5595,11 @@
     </row>
     <row r="46" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="424"/>
-      <c r="B46" s="655"/>
-      <c r="C46" s="655"/>
-      <c r="D46" s="614"/>
-      <c r="E46" s="617"/>
-      <c r="F46" s="620"/>
+      <c r="B46" s="654"/>
+      <c r="C46" s="654"/>
+      <c r="D46" s="671"/>
+      <c r="E46" s="586"/>
+      <c r="F46" s="674"/>
       <c r="G46" s="394" t="s">
         <v>123</v>
       </c>
@@ -5635,11 +5628,11 @@
     </row>
     <row r="47" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="424"/>
-      <c r="B47" s="655"/>
-      <c r="C47" s="655"/>
-      <c r="D47" s="614"/>
-      <c r="E47" s="617"/>
-      <c r="F47" s="620"/>
+      <c r="B47" s="654"/>
+      <c r="C47" s="654"/>
+      <c r="D47" s="671"/>
+      <c r="E47" s="586"/>
+      <c r="F47" s="674"/>
       <c r="G47" s="394" t="s">
         <v>460</v>
       </c>
@@ -5668,11 +5661,11 @@
     </row>
     <row r="48" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="424"/>
-      <c r="B48" s="655"/>
-      <c r="C48" s="655"/>
-      <c r="D48" s="615"/>
-      <c r="E48" s="618"/>
-      <c r="F48" s="621"/>
+      <c r="B48" s="654"/>
+      <c r="C48" s="654"/>
+      <c r="D48" s="672"/>
+      <c r="E48" s="587"/>
+      <c r="F48" s="675"/>
       <c r="G48" s="399" t="s">
         <v>125</v>
       </c>
@@ -5802,11 +5795,11 @@
       </c>
     </row>
     <row r="52" spans="1:16" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="656" t="s">
+      <c r="A52" s="655" t="s">
         <v>126</v>
       </c>
-      <c r="B52" s="656"/>
-      <c r="C52" s="656"/>
+      <c r="B52" s="655"/>
+      <c r="C52" s="655"/>
       <c r="D52" s="248" t="s">
         <v>437</v>
       </c>
@@ -5828,17 +5821,17 @@
     </row>
     <row r="53" spans="1:16" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="426"/>
-      <c r="B53" s="650" t="s">
+      <c r="B53" s="646" t="s">
         <v>474</v>
       </c>
-      <c r="C53" s="650"/>
-      <c r="D53" s="650" t="s">
+      <c r="C53" s="646"/>
+      <c r="D53" s="646" t="s">
         <v>475</v>
       </c>
-      <c r="E53" s="647" t="s">
+      <c r="E53" s="643" t="s">
         <v>54</v>
       </c>
-      <c r="F53" s="644" t="str">
+      <c r="F53" s="640" t="str">
         <f>Namespace &amp; ($B53)</f>
         <v>http://vocab.fairdatacollective.org/dataset/properties/PublisherIdentifier</v>
       </c>
@@ -5870,11 +5863,11 @@
     </row>
     <row r="54" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="426"/>
-      <c r="B54" s="651"/>
-      <c r="C54" s="651"/>
-      <c r="D54" s="651"/>
-      <c r="E54" s="648"/>
-      <c r="F54" s="645"/>
+      <c r="B54" s="647"/>
+      <c r="C54" s="647"/>
+      <c r="D54" s="647"/>
+      <c r="E54" s="644"/>
+      <c r="F54" s="641"/>
       <c r="G54" s="93" t="s">
         <v>136</v>
       </c>
@@ -5903,11 +5896,11 @@
     </row>
     <row r="55" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="426"/>
-      <c r="B55" s="652"/>
-      <c r="C55" s="652"/>
-      <c r="D55" s="652"/>
-      <c r="E55" s="649"/>
-      <c r="F55" s="646"/>
+      <c r="B55" s="648"/>
+      <c r="C55" s="648"/>
+      <c r="D55" s="648"/>
+      <c r="E55" s="645"/>
+      <c r="F55" s="642"/>
       <c r="G55" s="257" t="s">
         <v>137</v>
       </c>
@@ -6034,11 +6027,11 @@
       <c r="P58" s="10"/>
     </row>
     <row r="59" spans="1:16" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="673" t="s">
+      <c r="A59" s="605" t="s">
         <v>138</v>
       </c>
-      <c r="B59" s="673"/>
-      <c r="C59" s="673"/>
+      <c r="B59" s="605"/>
+      <c r="C59" s="605"/>
       <c r="D59" s="296" t="s">
         <v>139</v>
       </c>
@@ -6093,17 +6086,17 @@
     </row>
     <row r="61" spans="1:16" s="10" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A61" s="428"/>
-      <c r="B61" s="600" t="s">
+      <c r="B61" s="549" t="s">
         <v>484</v>
       </c>
-      <c r="C61" s="600"/>
-      <c r="D61" s="600" t="s">
+      <c r="C61" s="549"/>
+      <c r="D61" s="549" t="s">
         <v>485</v>
       </c>
-      <c r="E61" s="597" t="s">
+      <c r="E61" s="552" t="s">
         <v>46</v>
       </c>
-      <c r="F61" s="594" t="str">
+      <c r="F61" s="656" t="str">
         <f>Namespace &amp; ($B61)</f>
         <v>http://vocab.fairdatacollective.org/dataset/properties/LicenseIdentifier</v>
       </c>
@@ -6137,11 +6130,11 @@
     </row>
     <row r="62" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="428"/>
-      <c r="B62" s="601"/>
-      <c r="C62" s="601"/>
-      <c r="D62" s="601"/>
-      <c r="E62" s="598"/>
-      <c r="F62" s="595"/>
+      <c r="B62" s="550"/>
+      <c r="C62" s="550"/>
+      <c r="D62" s="550"/>
+      <c r="E62" s="553"/>
+      <c r="F62" s="657"/>
       <c r="G62" s="98" t="s">
         <v>148</v>
       </c>
@@ -6170,11 +6163,11 @@
     </row>
     <row r="63" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="428"/>
-      <c r="B63" s="602"/>
-      <c r="C63" s="602"/>
-      <c r="D63" s="602"/>
-      <c r="E63" s="599"/>
-      <c r="F63" s="596"/>
+      <c r="B63" s="606"/>
+      <c r="C63" s="606"/>
+      <c r="D63" s="606"/>
+      <c r="E63" s="659"/>
+      <c r="F63" s="658"/>
       <c r="G63" s="290" t="s">
         <v>149</v>
       </c>
@@ -6232,18 +6225,18 @@
       <c r="N64" s="277"/>
     </row>
     <row r="65" spans="1:14" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="674" t="s">
+      <c r="A65" s="607" t="s">
         <v>151</v>
       </c>
-      <c r="B65" s="674"/>
-      <c r="C65" s="674"/>
-      <c r="D65" s="666" t="s">
+      <c r="B65" s="607"/>
+      <c r="C65" s="607"/>
+      <c r="D65" s="636" t="s">
         <v>519</v>
       </c>
-      <c r="E65" s="668" t="s">
+      <c r="E65" s="638" t="s">
         <v>54</v>
       </c>
-      <c r="F65" s="666" t="str">
+      <c r="F65" s="636" t="str">
         <f>Namespace &amp; ($A65)</f>
         <v>http://vocab.fairdatacollective.org/dataset/properties/Date</v>
       </c>
@@ -6268,12 +6261,12 @@
       <c r="N65" s="308"/>
     </row>
     <row r="66" spans="1:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="674"/>
-      <c r="B66" s="674"/>
-      <c r="C66" s="674"/>
-      <c r="D66" s="667"/>
-      <c r="E66" s="669"/>
-      <c r="F66" s="667"/>
+      <c r="A66" s="607"/>
+      <c r="B66" s="607"/>
+      <c r="C66" s="607"/>
+      <c r="D66" s="637"/>
+      <c r="E66" s="639"/>
+      <c r="F66" s="637"/>
       <c r="G66" s="105" t="s">
         <v>486</v>
       </c>
@@ -6299,12 +6292,12 @@
       </c>
     </row>
     <row r="67" spans="1:14" s="14" customFormat="1" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="675" t="s">
+      <c r="A67" s="608" t="s">
         <v>154</v>
       </c>
-      <c r="B67" s="675"/>
-      <c r="C67" s="675"/>
-      <c r="D67" s="603" t="s">
+      <c r="B67" s="608"/>
+      <c r="C67" s="608"/>
+      <c r="D67" s="660" t="s">
         <v>159</v>
       </c>
       <c r="E67" s="365" t="s">
@@ -6325,9 +6318,9 @@
     </row>
     <row r="68" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="372"/>
-      <c r="B68" s="664"/>
-      <c r="C68" s="664"/>
-      <c r="D68" s="604"/>
+      <c r="B68" s="634"/>
+      <c r="C68" s="634"/>
+      <c r="D68" s="661"/>
       <c r="E68" s="316"/>
       <c r="F68" s="317"/>
       <c r="G68" s="318" t="s">
@@ -6360,7 +6353,7 @@
       <c r="A69" s="372"/>
       <c r="B69" s="373"/>
       <c r="C69" s="322"/>
-      <c r="D69" s="604"/>
+      <c r="D69" s="661"/>
       <c r="E69" s="324"/>
       <c r="F69" s="317"/>
       <c r="G69" s="318" t="s">
@@ -6393,7 +6386,7 @@
       <c r="A70" s="372"/>
       <c r="B70" s="373"/>
       <c r="C70" s="322"/>
-      <c r="D70" s="604"/>
+      <c r="D70" s="661"/>
       <c r="E70" s="325"/>
       <c r="F70" s="317"/>
       <c r="G70" s="310" t="s">
@@ -6425,7 +6418,7 @@
       <c r="A71" s="372"/>
       <c r="B71" s="373"/>
       <c r="C71" s="322"/>
-      <c r="D71" s="604"/>
+      <c r="D71" s="661"/>
       <c r="E71" s="325"/>
       <c r="F71" s="317"/>
       <c r="G71" s="310" t="s">
@@ -6458,7 +6451,7 @@
       <c r="A72" s="372"/>
       <c r="B72" s="373"/>
       <c r="C72" s="322"/>
-      <c r="D72" s="605"/>
+      <c r="D72" s="662"/>
       <c r="E72" s="324"/>
       <c r="F72" s="317"/>
       <c r="G72" s="310" t="s">
@@ -6489,17 +6482,17 @@
     </row>
     <row r="73" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="372"/>
-      <c r="B73" s="658" t="s">
+      <c r="B73" s="622" t="s">
         <v>490</v>
       </c>
-      <c r="C73" s="658"/>
-      <c r="D73" s="578" t="s">
+      <c r="C73" s="622"/>
+      <c r="D73" s="691" t="s">
         <v>491</v>
       </c>
-      <c r="E73" s="575">
+      <c r="E73" s="625">
         <v>1</v>
       </c>
-      <c r="F73" s="572"/>
+      <c r="F73" s="688"/>
       <c r="G73" s="326" t="s">
         <v>163</v>
       </c>
@@ -6528,11 +6521,11 @@
     </row>
     <row r="74" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="372"/>
-      <c r="B74" s="659"/>
-      <c r="C74" s="659"/>
-      <c r="D74" s="579"/>
-      <c r="E74" s="576"/>
-      <c r="F74" s="573"/>
+      <c r="B74" s="623"/>
+      <c r="C74" s="623"/>
+      <c r="D74" s="692"/>
+      <c r="E74" s="626"/>
+      <c r="F74" s="689"/>
       <c r="G74" s="310" t="s">
         <v>164</v>
       </c>
@@ -6561,11 +6554,11 @@
     </row>
     <row r="75" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="372"/>
-      <c r="B75" s="660"/>
-      <c r="C75" s="660"/>
-      <c r="D75" s="580"/>
-      <c r="E75" s="577"/>
-      <c r="F75" s="574"/>
+      <c r="B75" s="624"/>
+      <c r="C75" s="624"/>
+      <c r="D75" s="693"/>
+      <c r="E75" s="627"/>
+      <c r="F75" s="690"/>
       <c r="G75" s="331" t="s">
         <v>449</v>
       </c>
@@ -6623,10 +6616,10 @@
     </row>
     <row r="77" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="372"/>
-      <c r="B77" s="665" t="s">
+      <c r="B77" s="635" t="s">
         <v>492</v>
       </c>
-      <c r="C77" s="665"/>
+      <c r="C77" s="635"/>
       <c r="D77" s="358" t="s">
         <v>493</v>
       </c>
@@ -6648,17 +6641,17 @@
     </row>
     <row r="78" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="372"/>
-      <c r="B78" s="657"/>
-      <c r="C78" s="658" t="s">
+      <c r="B78" s="621"/>
+      <c r="C78" s="622" t="s">
         <v>494</v>
       </c>
-      <c r="D78" s="658" t="s">
+      <c r="D78" s="622" t="s">
         <v>495</v>
       </c>
-      <c r="E78" s="575">
+      <c r="E78" s="625">
         <v>1</v>
       </c>
-      <c r="F78" s="661" t="str">
+      <c r="F78" s="631" t="str">
         <f>Namespace &amp; ($C78)</f>
         <v>http://vocab.fairdatacollective.org/dataset/properties/DistributorName</v>
       </c>
@@ -6689,11 +6682,11 @@
     </row>
     <row r="79" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="372"/>
-      <c r="B79" s="657"/>
-      <c r="C79" s="659"/>
-      <c r="D79" s="659"/>
-      <c r="E79" s="576"/>
-      <c r="F79" s="662"/>
+      <c r="B79" s="621"/>
+      <c r="C79" s="623"/>
+      <c r="D79" s="623"/>
+      <c r="E79" s="626"/>
+      <c r="F79" s="632"/>
       <c r="G79" s="354" t="s">
         <v>170</v>
       </c>
@@ -6721,11 +6714,11 @@
     </row>
     <row r="80" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="372"/>
-      <c r="B80" s="657"/>
-      <c r="C80" s="660"/>
-      <c r="D80" s="660"/>
-      <c r="E80" s="577"/>
-      <c r="F80" s="663"/>
+      <c r="B80" s="621"/>
+      <c r="C80" s="624"/>
+      <c r="D80" s="624"/>
+      <c r="E80" s="627"/>
+      <c r="F80" s="633"/>
       <c r="G80" s="340" t="s">
         <v>172</v>
       </c>
@@ -6753,17 +6746,17 @@
     </row>
     <row r="81" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="372"/>
-      <c r="B81" s="657"/>
-      <c r="C81" s="658" t="s">
+      <c r="B81" s="621"/>
+      <c r="C81" s="622" t="s">
         <v>497</v>
       </c>
-      <c r="D81" s="658" t="s">
+      <c r="D81" s="622" t="s">
         <v>498</v>
       </c>
-      <c r="E81" s="575">
+      <c r="E81" s="625">
         <v>1</v>
       </c>
-      <c r="F81" s="661" t="str">
+      <c r="F81" s="631" t="str">
         <f>Namespace &amp; ($C81)</f>
         <v>http://vocab.fairdatacollective.org/dataset/properties/DistributorIdentifier</v>
       </c>
@@ -6795,11 +6788,11 @@
     </row>
     <row r="82" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="372"/>
-      <c r="B82" s="657"/>
-      <c r="C82" s="659"/>
-      <c r="D82" s="659"/>
-      <c r="E82" s="576"/>
-      <c r="F82" s="662"/>
+      <c r="B82" s="621"/>
+      <c r="C82" s="623"/>
+      <c r="D82" s="623"/>
+      <c r="E82" s="626"/>
+      <c r="F82" s="632"/>
       <c r="G82" s="354" t="s">
         <v>181</v>
       </c>
@@ -6828,11 +6821,11 @@
     </row>
     <row r="83" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="372"/>
-      <c r="B83" s="657"/>
-      <c r="C83" s="660"/>
-      <c r="D83" s="660"/>
-      <c r="E83" s="577"/>
-      <c r="F83" s="663"/>
+      <c r="B83" s="621"/>
+      <c r="C83" s="624"/>
+      <c r="D83" s="624"/>
+      <c r="E83" s="627"/>
+      <c r="F83" s="633"/>
       <c r="G83" s="340" t="s">
         <v>182</v>
       </c>
@@ -6861,17 +6854,17 @@
     </row>
     <row r="84" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="372"/>
-      <c r="B84" s="657"/>
-      <c r="C84" s="658" t="s">
+      <c r="B84" s="621"/>
+      <c r="C84" s="622" t="s">
         <v>499</v>
       </c>
-      <c r="D84" s="658" t="s">
+      <c r="D84" s="622" t="s">
         <v>500</v>
       </c>
-      <c r="E84" s="575" t="s">
+      <c r="E84" s="625" t="s">
         <v>54</v>
       </c>
-      <c r="F84" s="670" t="str">
+      <c r="F84" s="628" t="str">
         <f>Namespace &amp; ($C84)</f>
         <v>http://vocab.fairdatacollective.org/dataset/properties/DistributorAffiliation</v>
       </c>
@@ -6903,11 +6896,11 @@
     </row>
     <row r="85" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="372"/>
-      <c r="B85" s="657"/>
-      <c r="C85" s="659"/>
-      <c r="D85" s="659"/>
-      <c r="E85" s="576"/>
-      <c r="F85" s="671"/>
+      <c r="B85" s="621"/>
+      <c r="C85" s="623"/>
+      <c r="D85" s="623"/>
+      <c r="E85" s="626"/>
+      <c r="F85" s="629"/>
       <c r="G85" s="354" t="s">
         <v>185</v>
       </c>
@@ -6936,11 +6929,11 @@
     </row>
     <row r="86" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="372"/>
-      <c r="B86" s="657"/>
-      <c r="C86" s="659"/>
-      <c r="D86" s="659"/>
-      <c r="E86" s="576"/>
-      <c r="F86" s="671"/>
+      <c r="B86" s="621"/>
+      <c r="C86" s="623"/>
+      <c r="D86" s="623"/>
+      <c r="E86" s="626"/>
+      <c r="F86" s="629"/>
       <c r="G86" s="354" t="s">
         <v>187</v>
       </c>
@@ -6969,11 +6962,11 @@
     </row>
     <row r="87" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="372"/>
-      <c r="B87" s="657"/>
-      <c r="C87" s="660"/>
-      <c r="D87" s="660"/>
-      <c r="E87" s="577"/>
-      <c r="F87" s="672"/>
+      <c r="B87" s="621"/>
+      <c r="C87" s="624"/>
+      <c r="D87" s="624"/>
+      <c r="E87" s="627"/>
+      <c r="F87" s="630"/>
       <c r="G87" s="340" t="s">
         <v>188</v>
       </c>
@@ -7101,11 +7094,11 @@
       <c r="P90"/>
     </row>
     <row r="91" spans="1:16" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A91" s="693" t="s">
+      <c r="A91" s="593" t="s">
         <v>189</v>
       </c>
-      <c r="B91" s="693"/>
-      <c r="C91" s="693"/>
+      <c r="B91" s="593"/>
+      <c r="C91" s="593"/>
       <c r="D91" s="430" t="s">
         <v>410</v>
       </c>
@@ -7127,17 +7120,17 @@
     </row>
     <row r="92" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="426"/>
-      <c r="B92" s="581" t="s">
+      <c r="B92" s="594" t="s">
         <v>283</v>
       </c>
-      <c r="C92" s="581"/>
-      <c r="D92" s="581" t="s">
+      <c r="C92" s="594"/>
+      <c r="D92" s="594" t="s">
         <v>287</v>
       </c>
-      <c r="E92" s="584" t="s">
+      <c r="E92" s="694" t="s">
         <v>54</v>
       </c>
-      <c r="F92" s="589" t="str">
+      <c r="F92" s="698" t="str">
         <f>Namespace &amp; ($B92)</f>
         <v>http://vocab.fairdatacollective.org/dataset/properties/DataStream</v>
       </c>
@@ -7169,11 +7162,11 @@
     </row>
     <row r="93" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="426"/>
-      <c r="B93" s="582"/>
-      <c r="C93" s="582"/>
-      <c r="D93" s="582"/>
-      <c r="E93" s="585"/>
-      <c r="F93" s="590"/>
+      <c r="B93" s="595"/>
+      <c r="C93" s="595"/>
+      <c r="D93" s="595"/>
+      <c r="E93" s="695"/>
+      <c r="F93" s="699"/>
       <c r="G93" s="110" t="s">
         <v>285</v>
       </c>
@@ -7202,11 +7195,11 @@
     </row>
     <row r="94" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="426"/>
-      <c r="B94" s="582"/>
-      <c r="C94" s="582"/>
-      <c r="D94" s="582"/>
-      <c r="E94" s="585"/>
-      <c r="F94" s="590"/>
+      <c r="B94" s="595"/>
+      <c r="C94" s="595"/>
+      <c r="D94" s="595"/>
+      <c r="E94" s="695"/>
+      <c r="F94" s="699"/>
       <c r="G94" s="114" t="s">
         <v>191</v>
       </c>
@@ -7235,11 +7228,11 @@
     </row>
     <row r="95" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="426"/>
-      <c r="B95" s="583"/>
-      <c r="C95" s="583"/>
-      <c r="D95" s="583"/>
-      <c r="E95" s="586"/>
-      <c r="F95" s="591"/>
+      <c r="B95" s="596"/>
+      <c r="C95" s="596"/>
+      <c r="D95" s="596"/>
+      <c r="E95" s="696"/>
+      <c r="F95" s="700"/>
       <c r="G95" s="448" t="s">
         <v>286</v>
       </c>
@@ -7268,17 +7261,17 @@
     </row>
     <row r="96" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" s="426"/>
-      <c r="B96" s="697"/>
-      <c r="C96" s="581" t="s">
+      <c r="B96" s="600"/>
+      <c r="C96" s="594" t="s">
         <v>281</v>
       </c>
-      <c r="D96" s="581" t="s">
+      <c r="D96" s="594" t="s">
         <v>368</v>
       </c>
-      <c r="E96" s="584">
+      <c r="E96" s="694">
         <v>1</v>
       </c>
-      <c r="F96" s="589" t="str">
+      <c r="F96" s="698" t="str">
         <f>Namespace &amp; ($C96)</f>
         <v>http://vocab.fairdatacollective.org/dataset/properties/DataSource</v>
       </c>
@@ -7310,11 +7303,11 @@
     </row>
     <row r="97" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" s="426"/>
-      <c r="B97" s="697"/>
-      <c r="C97" s="582"/>
-      <c r="D97" s="582"/>
-      <c r="E97" s="585"/>
-      <c r="F97" s="590"/>
+      <c r="B97" s="600"/>
+      <c r="C97" s="595"/>
+      <c r="D97" s="595"/>
+      <c r="E97" s="695"/>
+      <c r="F97" s="699"/>
       <c r="G97" s="110" t="s">
         <v>195</v>
       </c>
@@ -7343,11 +7336,11 @@
     </row>
     <row r="98" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="426"/>
-      <c r="B98" s="697"/>
-      <c r="C98" s="582"/>
-      <c r="D98" s="582"/>
-      <c r="E98" s="585"/>
-      <c r="F98" s="590"/>
+      <c r="B98" s="600"/>
+      <c r="C98" s="595"/>
+      <c r="D98" s="595"/>
+      <c r="E98" s="695"/>
+      <c r="F98" s="699"/>
       <c r="G98" s="110" t="s">
         <v>197</v>
       </c>
@@ -7376,11 +7369,11 @@
     </row>
     <row r="99" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="426"/>
-      <c r="B99" s="697"/>
-      <c r="C99" s="583"/>
-      <c r="D99" s="583"/>
-      <c r="E99" s="586"/>
-      <c r="F99" s="591"/>
+      <c r="B99" s="600"/>
+      <c r="C99" s="596"/>
+      <c r="D99" s="596"/>
+      <c r="E99" s="696"/>
+      <c r="F99" s="700"/>
       <c r="G99" s="448" t="s">
         <v>198</v>
       </c>
@@ -7409,17 +7402,17 @@
     </row>
     <row r="100" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="426"/>
-      <c r="B100" s="697"/>
-      <c r="C100" s="582" t="s">
+      <c r="B100" s="600"/>
+      <c r="C100" s="595" t="s">
         <v>282</v>
       </c>
-      <c r="D100" s="582" t="s">
+      <c r="D100" s="595" t="s">
         <v>288</v>
       </c>
-      <c r="E100" s="585" t="s">
+      <c r="E100" s="695" t="s">
         <v>54</v>
       </c>
-      <c r="F100" s="592" t="str">
+      <c r="F100" s="701" t="str">
         <f>Namespace &amp; ($C100)</f>
         <v>http://vocab.fairdatacollective.org/dataset/properties/Variable</v>
       </c>
@@ -7451,11 +7444,11 @@
     </row>
     <row r="101" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" s="426"/>
-      <c r="B101" s="697"/>
-      <c r="C101" s="582"/>
-      <c r="D101" s="582"/>
-      <c r="E101" s="585"/>
-      <c r="F101" s="592"/>
+      <c r="B101" s="600"/>
+      <c r="C101" s="595"/>
+      <c r="D101" s="595"/>
+      <c r="E101" s="695"/>
+      <c r="F101" s="701"/>
       <c r="G101" s="110" t="s">
         <v>290</v>
       </c>
@@ -7484,11 +7477,11 @@
     </row>
     <row r="102" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A102" s="426"/>
-      <c r="B102" s="697"/>
-      <c r="C102" s="582"/>
-      <c r="D102" s="582"/>
-      <c r="E102" s="585"/>
-      <c r="F102" s="592"/>
+      <c r="B102" s="600"/>
+      <c r="C102" s="595"/>
+      <c r="D102" s="595"/>
+      <c r="E102" s="695"/>
+      <c r="F102" s="701"/>
       <c r="G102" s="110" t="s">
         <v>291</v>
       </c>
@@ -7517,11 +7510,11 @@
     </row>
     <row r="103" spans="1:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A103" s="427"/>
-      <c r="B103" s="698"/>
-      <c r="C103" s="587"/>
-      <c r="D103" s="587"/>
-      <c r="E103" s="588"/>
-      <c r="F103" s="593"/>
+      <c r="B103" s="601"/>
+      <c r="C103" s="604"/>
+      <c r="D103" s="604"/>
+      <c r="E103" s="697"/>
+      <c r="F103" s="702"/>
       <c r="G103" s="438" t="s">
         <v>292</v>
       </c>
@@ -7549,11 +7542,11 @@
       </c>
     </row>
     <row r="104" spans="1:14" s="14" customFormat="1" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A104" s="694" t="s">
+      <c r="A104" s="597" t="s">
         <v>201</v>
       </c>
-      <c r="B104" s="694"/>
-      <c r="C104" s="694"/>
+      <c r="B104" s="597"/>
+      <c r="C104" s="597"/>
       <c r="D104" s="478" t="s">
         <v>202</v>
       </c>
@@ -7575,17 +7568,17 @@
     </row>
     <row r="105" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A105" s="424"/>
-      <c r="B105" s="685" t="s">
+      <c r="B105" s="582" t="s">
         <v>504</v>
       </c>
-      <c r="C105" s="685"/>
-      <c r="D105" s="695" t="s">
+      <c r="C105" s="582"/>
+      <c r="D105" s="598" t="s">
         <v>503</v>
       </c>
-      <c r="E105" s="699" t="s">
+      <c r="E105" s="602" t="s">
         <v>46</v>
       </c>
-      <c r="F105" s="688" t="str">
+      <c r="F105" s="588" t="str">
         <f>Namespace &amp; ($B105)</f>
         <v>http://vocab.fairdatacollective.org/dataset/properties/SpatialCoveragePoint</v>
       </c>
@@ -7617,11 +7610,11 @@
     </row>
     <row r="106" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A106" s="424"/>
-      <c r="B106" s="687"/>
-      <c r="C106" s="687"/>
-      <c r="D106" s="696"/>
-      <c r="E106" s="700"/>
-      <c r="F106" s="690"/>
+      <c r="B106" s="584"/>
+      <c r="C106" s="584"/>
+      <c r="D106" s="599"/>
+      <c r="E106" s="603"/>
+      <c r="F106" s="590"/>
       <c r="G106" s="458" t="s">
         <v>203</v>
       </c>
@@ -7650,17 +7643,17 @@
     </row>
     <row r="107" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A107" s="424"/>
-      <c r="B107" s="685" t="s">
+      <c r="B107" s="582" t="s">
         <v>505</v>
       </c>
-      <c r="C107" s="685"/>
-      <c r="D107" s="685" t="s">
+      <c r="C107" s="582"/>
+      <c r="D107" s="582" t="s">
         <v>506</v>
       </c>
-      <c r="E107" s="616" t="s">
+      <c r="E107" s="585" t="s">
         <v>46</v>
       </c>
-      <c r="F107" s="688" t="str">
+      <c r="F107" s="588" t="str">
         <f>Namespace &amp; ($B107)</f>
         <v>http://vocab.fairdatacollective.org/dataset/properties/SpatialCoverageBoundingBox</v>
       </c>
@@ -7692,11 +7685,11 @@
     </row>
     <row r="108" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A108" s="424"/>
-      <c r="B108" s="686"/>
-      <c r="C108" s="686"/>
-      <c r="D108" s="686"/>
-      <c r="E108" s="617"/>
-      <c r="F108" s="689"/>
+      <c r="B108" s="583"/>
+      <c r="C108" s="583"/>
+      <c r="D108" s="583"/>
+      <c r="E108" s="586"/>
+      <c r="F108" s="589"/>
       <c r="G108" s="468" t="s">
         <v>209</v>
       </c>
@@ -7725,11 +7718,11 @@
     </row>
     <row r="109" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A109" s="424"/>
-      <c r="B109" s="686"/>
-      <c r="C109" s="686"/>
-      <c r="D109" s="686"/>
-      <c r="E109" s="617"/>
-      <c r="F109" s="689"/>
+      <c r="B109" s="583"/>
+      <c r="C109" s="583"/>
+      <c r="D109" s="583"/>
+      <c r="E109" s="586"/>
+      <c r="F109" s="589"/>
       <c r="G109" s="468" t="s">
         <v>211</v>
       </c>
@@ -7758,11 +7751,11 @@
     </row>
     <row r="110" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A110" s="424"/>
-      <c r="B110" s="687"/>
-      <c r="C110" s="687"/>
-      <c r="D110" s="687"/>
-      <c r="E110" s="618"/>
-      <c r="F110" s="690"/>
+      <c r="B110" s="584"/>
+      <c r="C110" s="584"/>
+      <c r="D110" s="584"/>
+      <c r="E110" s="587"/>
+      <c r="F110" s="590"/>
       <c r="G110" s="473" t="s">
         <v>213</v>
       </c>
@@ -7791,17 +7784,17 @@
     </row>
     <row r="111" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A111" s="424"/>
-      <c r="B111" s="685" t="s">
+      <c r="B111" s="582" t="s">
         <v>507</v>
       </c>
-      <c r="C111" s="685"/>
-      <c r="D111" s="691" t="s">
+      <c r="C111" s="582"/>
+      <c r="D111" s="591" t="s">
         <v>508</v>
       </c>
-      <c r="E111" s="616" t="s">
+      <c r="E111" s="585" t="s">
         <v>46</v>
       </c>
-      <c r="F111" s="688" t="str">
+      <c r="F111" s="588" t="str">
         <f>Namespace &amp; ($B111)</f>
         <v>http://vocab.fairdatacollective.org/dataset/properties/SpatialCoveragePolygon</v>
       </c>
@@ -7833,11 +7826,11 @@
     </row>
     <row r="112" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A112" s="424"/>
-      <c r="B112" s="687"/>
-      <c r="C112" s="687"/>
-      <c r="D112" s="692"/>
-      <c r="E112" s="618"/>
-      <c r="F112" s="690"/>
+      <c r="B112" s="584"/>
+      <c r="C112" s="584"/>
+      <c r="D112" s="592"/>
+      <c r="E112" s="587"/>
+      <c r="F112" s="590"/>
       <c r="G112" s="458" t="s">
         <v>439</v>
       </c>
@@ -7898,18 +7891,18 @@
       </c>
     </row>
     <row r="114" spans="1:14" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A114" s="713" t="s">
+      <c r="A114" s="556" t="s">
         <v>217</v>
       </c>
-      <c r="B114" s="713"/>
-      <c r="C114" s="713"/>
-      <c r="D114" s="730" t="s">
+      <c r="B114" s="556"/>
+      <c r="C114" s="556"/>
+      <c r="D114" s="573" t="s">
         <v>218</v>
       </c>
-      <c r="E114" s="721" t="s">
+      <c r="E114" s="564" t="s">
         <v>46</v>
       </c>
-      <c r="F114" s="724" t="str">
+      <c r="F114" s="567" t="str">
         <f>Namespace &amp; ($A114)</f>
         <v>http://vocab.fairdatacollective.org/dataset/properties/VerticalCoverage</v>
       </c>
@@ -7940,12 +7933,12 @@
       </c>
     </row>
     <row r="115" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A115" s="714"/>
-      <c r="B115" s="714"/>
-      <c r="C115" s="714"/>
-      <c r="D115" s="731"/>
-      <c r="E115" s="722"/>
-      <c r="F115" s="725"/>
+      <c r="A115" s="557"/>
+      <c r="B115" s="557"/>
+      <c r="C115" s="557"/>
+      <c r="D115" s="574"/>
+      <c r="E115" s="565"/>
+      <c r="F115" s="568"/>
       <c r="G115" s="116" t="s">
         <v>221</v>
       </c>
@@ -7973,12 +7966,12 @@
       </c>
     </row>
     <row r="116" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A116" s="714"/>
-      <c r="B116" s="714"/>
-      <c r="C116" s="714"/>
-      <c r="D116" s="731"/>
-      <c r="E116" s="722"/>
-      <c r="F116" s="725"/>
+      <c r="A116" s="557"/>
+      <c r="B116" s="557"/>
+      <c r="C116" s="557"/>
+      <c r="D116" s="574"/>
+      <c r="E116" s="565"/>
+      <c r="F116" s="568"/>
       <c r="G116" s="116" t="s">
         <v>223</v>
       </c>
@@ -8006,12 +7999,12 @@
       </c>
     </row>
     <row r="117" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A117" s="714"/>
-      <c r="B117" s="714"/>
-      <c r="C117" s="714"/>
-      <c r="D117" s="731"/>
-      <c r="E117" s="722"/>
-      <c r="F117" s="725"/>
+      <c r="A117" s="557"/>
+      <c r="B117" s="557"/>
+      <c r="C117" s="557"/>
+      <c r="D117" s="574"/>
+      <c r="E117" s="565"/>
+      <c r="F117" s="568"/>
       <c r="G117" s="116" t="s">
         <v>224</v>
       </c>
@@ -8039,12 +8032,12 @@
       </c>
     </row>
     <row r="118" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A118" s="714"/>
-      <c r="B118" s="714"/>
-      <c r="C118" s="714"/>
-      <c r="D118" s="731"/>
-      <c r="E118" s="722"/>
-      <c r="F118" s="725"/>
+      <c r="A118" s="557"/>
+      <c r="B118" s="557"/>
+      <c r="C118" s="557"/>
+      <c r="D118" s="574"/>
+      <c r="E118" s="565"/>
+      <c r="F118" s="568"/>
       <c r="G118" s="116" t="s">
         <v>225</v>
       </c>
@@ -8072,12 +8065,12 @@
       </c>
     </row>
     <row r="119" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A119" s="714"/>
-      <c r="B119" s="714"/>
-      <c r="C119" s="714"/>
-      <c r="D119" s="731"/>
-      <c r="E119" s="722"/>
-      <c r="F119" s="725"/>
+      <c r="A119" s="557"/>
+      <c r="B119" s="557"/>
+      <c r="C119" s="557"/>
+      <c r="D119" s="574"/>
+      <c r="E119" s="565"/>
+      <c r="F119" s="568"/>
       <c r="G119" s="116" t="s">
         <v>226</v>
       </c>
@@ -8105,12 +8098,12 @@
       </c>
     </row>
     <row r="120" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A120" s="714"/>
-      <c r="B120" s="714"/>
-      <c r="C120" s="714"/>
-      <c r="D120" s="731"/>
-      <c r="E120" s="722"/>
-      <c r="F120" s="725"/>
+      <c r="A120" s="557"/>
+      <c r="B120" s="557"/>
+      <c r="C120" s="557"/>
+      <c r="D120" s="574"/>
+      <c r="E120" s="565"/>
+      <c r="F120" s="568"/>
       <c r="G120" s="116" t="s">
         <v>398</v>
       </c>
@@ -8138,16 +8131,16 @@
       </c>
     </row>
     <row r="121" spans="1:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A121" s="715"/>
-      <c r="B121" s="715"/>
-      <c r="C121" s="715"/>
-      <c r="D121" s="732"/>
-      <c r="E121" s="723"/>
-      <c r="F121" s="726"/>
-      <c r="G121" s="541" t="s">
+      <c r="A121" s="558"/>
+      <c r="B121" s="558"/>
+      <c r="C121" s="558"/>
+      <c r="D121" s="575"/>
+      <c r="E121" s="566"/>
+      <c r="F121" s="569"/>
+      <c r="G121" s="539" t="s">
         <v>408</v>
       </c>
-      <c r="H121" s="541" t="s">
+      <c r="H121" s="539" t="s">
         <v>423</v>
       </c>
       <c r="I121" s="498" t="s">
@@ -8171,18 +8164,18 @@
       </c>
     </row>
     <row r="122" spans="1:14" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A122" s="716" t="s">
+      <c r="A122" s="559" t="s">
         <v>227</v>
       </c>
-      <c r="B122" s="716"/>
-      <c r="C122" s="716"/>
-      <c r="D122" s="727" t="s">
+      <c r="B122" s="559"/>
+      <c r="C122" s="559"/>
+      <c r="D122" s="570" t="s">
         <v>228</v>
       </c>
-      <c r="E122" s="733" t="s">
+      <c r="E122" s="576" t="s">
         <v>46</v>
       </c>
-      <c r="F122" s="734" t="str">
+      <c r="F122" s="579" t="str">
         <f>Namespace &amp; ($A122)</f>
         <v>http://vocab.fairdatacollective.org/dataset/properties/TemporalCoverage</v>
       </c>
@@ -8213,12 +8206,12 @@
       </c>
     </row>
     <row r="123" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A123" s="717"/>
-      <c r="B123" s="717"/>
-      <c r="C123" s="717"/>
-      <c r="D123" s="728"/>
-      <c r="E123" s="546"/>
-      <c r="F123" s="735"/>
+      <c r="A123" s="560"/>
+      <c r="B123" s="560"/>
+      <c r="C123" s="560"/>
+      <c r="D123" s="571"/>
+      <c r="E123" s="577"/>
+      <c r="F123" s="580"/>
       <c r="G123" s="121" t="s">
         <v>231</v>
       </c>
@@ -8246,12 +8239,12 @@
       </c>
     </row>
     <row r="124" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A124" s="717"/>
-      <c r="B124" s="717"/>
-      <c r="C124" s="717"/>
-      <c r="D124" s="728"/>
-      <c r="E124" s="546"/>
-      <c r="F124" s="735"/>
+      <c r="A124" s="560"/>
+      <c r="B124" s="560"/>
+      <c r="C124" s="560"/>
+      <c r="D124" s="571"/>
+      <c r="E124" s="577"/>
+      <c r="F124" s="580"/>
       <c r="G124" s="121" t="s">
         <v>233</v>
       </c>
@@ -8279,12 +8272,12 @@
       </c>
     </row>
     <row r="125" spans="1:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A125" s="718"/>
-      <c r="B125" s="718"/>
-      <c r="C125" s="718"/>
-      <c r="D125" s="729"/>
-      <c r="E125" s="547"/>
-      <c r="F125" s="736"/>
+      <c r="A125" s="561"/>
+      <c r="B125" s="561"/>
+      <c r="C125" s="561"/>
+      <c r="D125" s="572"/>
+      <c r="E125" s="578"/>
+      <c r="F125" s="581"/>
       <c r="G125" s="507" t="s">
         <v>235</v>
       </c>
@@ -8312,79 +8305,79 @@
       </c>
     </row>
     <row r="126" spans="1:14" s="14" customFormat="1" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A126" s="719" t="s">
+      <c r="A126" s="562" t="s">
         <v>237</v>
       </c>
-      <c r="B126" s="719"/>
-      <c r="C126" s="719"/>
-      <c r="D126" s="518" t="s">
+      <c r="B126" s="562"/>
+      <c r="C126" s="562"/>
+      <c r="D126" s="517" t="s">
         <v>509</v>
       </c>
-      <c r="E126" s="519" t="s">
+      <c r="E126" s="518" t="s">
         <v>34</v>
       </c>
-      <c r="F126" s="520" t="str">
+      <c r="F126" s="519" t="str">
         <f>Namespace &amp; ($A126)</f>
         <v>http://vocab.fairdatacollective.org/dataset/properties/Funding</v>
       </c>
-      <c r="G126" s="521"/>
-      <c r="H126" s="521"/>
-      <c r="I126" s="522"/>
-      <c r="J126" s="523"/>
-      <c r="K126" s="524"/>
-      <c r="L126" s="524"/>
-      <c r="M126" s="521"/>
-      <c r="N126" s="521"/>
+      <c r="G126" s="520"/>
+      <c r="H126" s="520"/>
+      <c r="I126" s="521"/>
+      <c r="J126" s="522"/>
+      <c r="K126" s="523"/>
+      <c r="L126" s="523"/>
+      <c r="M126" s="520"/>
+      <c r="N126" s="520"/>
     </row>
     <row r="127" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A127" s="428"/>
-      <c r="B127" s="707" t="s">
+      <c r="B127" s="546" t="s">
         <v>510</v>
       </c>
-      <c r="C127" s="707"/>
-      <c r="D127" s="701" t="s">
+      <c r="C127" s="546"/>
+      <c r="D127" s="540" t="s">
         <v>513</v>
       </c>
-      <c r="E127" s="704">
+      <c r="E127" s="543">
         <v>1</v>
       </c>
-      <c r="F127" s="701" t="str">
+      <c r="F127" s="540" t="str">
         <f>Namespace &amp; ($B127)</f>
         <v>http://vocab.fairdatacollective.org/dataset/properties/Award</v>
       </c>
-      <c r="G127" s="531" t="s">
+      <c r="G127" s="529" t="s">
         <v>238</v>
       </c>
-      <c r="H127" s="531" t="s">
+      <c r="H127" s="529" t="s">
         <v>428</v>
       </c>
-      <c r="I127" s="532" t="s">
+      <c r="I127" s="530" t="s">
         <v>239</v>
       </c>
-      <c r="J127" s="533">
+      <c r="J127" s="531">
         <v>1</v>
       </c>
-      <c r="K127" s="534" t="s">
+      <c r="K127" s="532" t="s">
         <v>36</v>
       </c>
-      <c r="L127" s="534" t="str">
+      <c r="L127" s="532" t="str">
         <f t="shared" si="5"/>
         <v>http://vocab.fairdatacollective.org/dataset/properties/awardTitle</v>
       </c>
-      <c r="M127" s="531" t="s">
-        <v>28</v>
-      </c>
-      <c r="N127" s="531" t="s">
+      <c r="M127" s="529" t="s">
+        <v>28</v>
+      </c>
+      <c r="N127" s="529" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="128" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A128" s="428"/>
-      <c r="B128" s="708"/>
-      <c r="C128" s="708"/>
-      <c r="D128" s="702"/>
-      <c r="E128" s="705"/>
-      <c r="F128" s="702"/>
+      <c r="B128" s="547"/>
+      <c r="C128" s="547"/>
+      <c r="D128" s="541"/>
+      <c r="E128" s="544"/>
+      <c r="F128" s="541"/>
       <c r="G128" s="516" t="s">
         <v>240</v>
       </c>
@@ -8413,50 +8406,50 @@
     </row>
     <row r="129" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A129" s="428"/>
-      <c r="B129" s="720"/>
-      <c r="C129" s="720"/>
-      <c r="D129" s="703"/>
-      <c r="E129" s="706"/>
-      <c r="F129" s="703"/>
-      <c r="G129" s="535" t="s">
+      <c r="B129" s="563"/>
+      <c r="C129" s="563"/>
+      <c r="D129" s="542"/>
+      <c r="E129" s="545"/>
+      <c r="F129" s="542"/>
+      <c r="G129" s="533" t="s">
         <v>242</v>
       </c>
-      <c r="H129" s="535" t="s">
+      <c r="H129" s="533" t="s">
         <v>430</v>
       </c>
-      <c r="I129" s="536" t="s">
+      <c r="I129" s="534" t="s">
         <v>243</v>
       </c>
-      <c r="J129" s="537">
+      <c r="J129" s="535">
         <v>1</v>
       </c>
-      <c r="K129" s="538" t="s">
+      <c r="K129" s="536" t="s">
         <v>36</v>
       </c>
-      <c r="L129" s="538" t="str">
+      <c r="L129" s="536" t="str">
         <f t="shared" si="5"/>
         <v>http://vocab.fairdatacollective.org/dataset/properties/awardLocalIdentifier</v>
       </c>
-      <c r="M129" s="539" t="s">
-        <v>28</v>
-      </c>
-      <c r="N129" s="539" t="s">
+      <c r="M129" s="537" t="s">
+        <v>28</v>
+      </c>
+      <c r="N129" s="537" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="130" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A130" s="428"/>
-      <c r="B130" s="707" t="s">
+      <c r="B130" s="546" t="s">
         <v>511</v>
       </c>
-      <c r="C130" s="707"/>
-      <c r="D130" s="600" t="s">
+      <c r="C130" s="546"/>
+      <c r="D130" s="549" t="s">
         <v>512</v>
       </c>
-      <c r="E130" s="597" t="s">
+      <c r="E130" s="552" t="s">
         <v>54</v>
       </c>
-      <c r="F130" s="701" t="str">
+      <c r="F130" s="540" t="str">
         <f>Namespace &amp; ($B130)</f>
         <v>http://vocab.fairdatacollective.org/dataset/properties/Funder</v>
       </c>
@@ -8488,11 +8481,11 @@
     </row>
     <row r="131" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A131" s="428"/>
-      <c r="B131" s="708"/>
-      <c r="C131" s="708"/>
-      <c r="D131" s="601"/>
-      <c r="E131" s="598"/>
-      <c r="F131" s="702"/>
+      <c r="B131" s="547"/>
+      <c r="C131" s="547"/>
+      <c r="D131" s="550"/>
+      <c r="E131" s="553"/>
+      <c r="F131" s="541"/>
       <c r="G131" s="512" t="s">
         <v>246</v>
       </c>
@@ -8521,11 +8514,11 @@
     </row>
     <row r="132" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A132" s="428"/>
-      <c r="B132" s="708"/>
-      <c r="C132" s="708"/>
-      <c r="D132" s="601"/>
-      <c r="E132" s="598"/>
-      <c r="F132" s="702"/>
+      <c r="B132" s="547"/>
+      <c r="C132" s="547"/>
+      <c r="D132" s="550"/>
+      <c r="E132" s="553"/>
+      <c r="F132" s="541"/>
       <c r="G132" s="516" t="s">
         <v>248</v>
       </c>
@@ -8545,8 +8538,8 @@
         <f t="shared" si="5"/>
         <v>http://vocab.fairdatacollective.org/dataset/properties/funderIdentifierScheme</v>
       </c>
-      <c r="M132" s="517" t="s">
-        <v>522</v>
+      <c r="M132" s="512" t="s">
+        <v>28</v>
       </c>
       <c r="N132" s="512" t="s">
         <v>28</v>
@@ -8554,34 +8547,34 @@
     </row>
     <row r="133" spans="1:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A133" s="429"/>
-      <c r="B133" s="709"/>
-      <c r="C133" s="709"/>
-      <c r="D133" s="710"/>
-      <c r="E133" s="711"/>
-      <c r="F133" s="712"/>
-      <c r="G133" s="525" t="s">
+      <c r="B133" s="548"/>
+      <c r="C133" s="548"/>
+      <c r="D133" s="551"/>
+      <c r="E133" s="554"/>
+      <c r="F133" s="555"/>
+      <c r="G133" s="524" t="s">
         <v>250</v>
       </c>
-      <c r="H133" s="525" t="s">
+      <c r="H133" s="524" t="s">
         <v>434</v>
       </c>
-      <c r="I133" s="526" t="s">
+      <c r="I133" s="525" t="s">
         <v>251</v>
       </c>
-      <c r="J133" s="527" t="s">
+      <c r="J133" s="526" t="s">
         <v>46</v>
       </c>
-      <c r="K133" s="528" t="s">
+      <c r="K133" s="527" t="s">
         <v>68</v>
       </c>
-      <c r="L133" s="528" t="str">
+      <c r="L133" s="527" t="str">
         <f t="shared" si="5"/>
         <v>http://vocab.fairdatacollective.org/dataset/properties/funderIdentifierSchemeIRI</v>
       </c>
-      <c r="M133" s="529" t="s">
-        <v>522</v>
-      </c>
-      <c r="N133" s="530" t="s">
+      <c r="M133" s="512" t="s">
+        <v>28</v>
+      </c>
+      <c r="N133" s="528" t="s">
         <v>28</v>
       </c>
     </row>
@@ -8598,7 +8591,7 @@
       <c r="J136" s="6"/>
     </row>
     <row r="137" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D137" s="540" t="s">
+      <c r="D137" s="538" t="s">
         <v>517</v>
       </c>
       <c r="H137" s="3"/>
@@ -12228,87 +12221,27 @@
   </sheetData>
   <autoFilter ref="H1:N143" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <mergeCells count="134">
-    <mergeCell ref="D127:D129"/>
-    <mergeCell ref="E127:E129"/>
-    <mergeCell ref="F127:F129"/>
-    <mergeCell ref="B130:C133"/>
-    <mergeCell ref="D130:D133"/>
-    <mergeCell ref="E130:E133"/>
-    <mergeCell ref="F130:F133"/>
-    <mergeCell ref="A114:C121"/>
-    <mergeCell ref="A122:C125"/>
-    <mergeCell ref="A126:C126"/>
-    <mergeCell ref="B127:C129"/>
-    <mergeCell ref="E114:E121"/>
-    <mergeCell ref="F114:F121"/>
-    <mergeCell ref="D122:D125"/>
-    <mergeCell ref="D114:D121"/>
-    <mergeCell ref="E122:E125"/>
-    <mergeCell ref="F122:F125"/>
-    <mergeCell ref="B107:C110"/>
-    <mergeCell ref="D107:D110"/>
-    <mergeCell ref="E107:E110"/>
-    <mergeCell ref="F107:F110"/>
-    <mergeCell ref="B111:C112"/>
-    <mergeCell ref="D111:D112"/>
-    <mergeCell ref="E111:E112"/>
-    <mergeCell ref="F111:F112"/>
-    <mergeCell ref="A91:C91"/>
-    <mergeCell ref="B92:C95"/>
-    <mergeCell ref="A104:C104"/>
-    <mergeCell ref="B105:C106"/>
-    <mergeCell ref="D105:D106"/>
-    <mergeCell ref="B96:B99"/>
-    <mergeCell ref="B100:B103"/>
-    <mergeCell ref="E105:E106"/>
-    <mergeCell ref="F105:F106"/>
-    <mergeCell ref="C96:C99"/>
-    <mergeCell ref="C100:C103"/>
-    <mergeCell ref="A59:C59"/>
-    <mergeCell ref="B61:C63"/>
-    <mergeCell ref="A65:C66"/>
-    <mergeCell ref="A67:C67"/>
-    <mergeCell ref="A8:C12"/>
-    <mergeCell ref="A18:C18"/>
-    <mergeCell ref="B19:C22"/>
-    <mergeCell ref="A13:C13"/>
-    <mergeCell ref="A14:C15"/>
-    <mergeCell ref="A16:C16"/>
-    <mergeCell ref="A17:C17"/>
-    <mergeCell ref="B84:B87"/>
-    <mergeCell ref="C84:C87"/>
-    <mergeCell ref="D84:D87"/>
-    <mergeCell ref="E84:E87"/>
-    <mergeCell ref="F84:F87"/>
-    <mergeCell ref="B81:B83"/>
-    <mergeCell ref="C81:C83"/>
-    <mergeCell ref="D81:D83"/>
-    <mergeCell ref="E81:E83"/>
-    <mergeCell ref="F81:F83"/>
-    <mergeCell ref="B78:B80"/>
-    <mergeCell ref="C78:C80"/>
-    <mergeCell ref="D78:D80"/>
-    <mergeCell ref="E78:E80"/>
-    <mergeCell ref="F78:F80"/>
-    <mergeCell ref="B68:C68"/>
-    <mergeCell ref="B77:C77"/>
-    <mergeCell ref="B73:C75"/>
-    <mergeCell ref="D65:D66"/>
-    <mergeCell ref="E65:E66"/>
-    <mergeCell ref="F65:F66"/>
-    <mergeCell ref="F53:F55"/>
-    <mergeCell ref="E53:E55"/>
-    <mergeCell ref="D53:D55"/>
-    <mergeCell ref="A24:C24"/>
-    <mergeCell ref="B25:C27"/>
-    <mergeCell ref="B28:C30"/>
-    <mergeCell ref="B31:C34"/>
-    <mergeCell ref="A38:C38"/>
-    <mergeCell ref="B39:C41"/>
-    <mergeCell ref="B42:C44"/>
-    <mergeCell ref="B45:C48"/>
-    <mergeCell ref="A52:C52"/>
-    <mergeCell ref="B53:C55"/>
+    <mergeCell ref="E100:E103"/>
+    <mergeCell ref="F92:F95"/>
+    <mergeCell ref="F96:F99"/>
+    <mergeCell ref="F100:F103"/>
+    <mergeCell ref="D8:D12"/>
+    <mergeCell ref="E8:E12"/>
+    <mergeCell ref="F8:F12"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="F31:F34"/>
+    <mergeCell ref="E31:E34"/>
+    <mergeCell ref="F39:F41"/>
+    <mergeCell ref="F19:F22"/>
+    <mergeCell ref="E19:E22"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="F5:F7"/>
+    <mergeCell ref="D5:D7"/>
+    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="D19:D22"/>
     <mergeCell ref="F61:F63"/>
     <mergeCell ref="E61:E63"/>
     <mergeCell ref="D61:D63"/>
@@ -12333,35 +12266,95 @@
     <mergeCell ref="E25:E27"/>
     <mergeCell ref="F25:F27"/>
     <mergeCell ref="E5:E7"/>
+    <mergeCell ref="F53:F55"/>
+    <mergeCell ref="E53:E55"/>
+    <mergeCell ref="D53:D55"/>
+    <mergeCell ref="A24:C24"/>
+    <mergeCell ref="B25:C27"/>
+    <mergeCell ref="B28:C30"/>
+    <mergeCell ref="B31:C34"/>
+    <mergeCell ref="A38:C38"/>
+    <mergeCell ref="B39:C41"/>
+    <mergeCell ref="B42:C44"/>
+    <mergeCell ref="B45:C48"/>
+    <mergeCell ref="A52:C52"/>
+    <mergeCell ref="B53:C55"/>
+    <mergeCell ref="B78:B80"/>
+    <mergeCell ref="C78:C80"/>
+    <mergeCell ref="D78:D80"/>
+    <mergeCell ref="E78:E80"/>
+    <mergeCell ref="F78:F80"/>
+    <mergeCell ref="B68:C68"/>
+    <mergeCell ref="B77:C77"/>
+    <mergeCell ref="B73:C75"/>
+    <mergeCell ref="D65:D66"/>
+    <mergeCell ref="E65:E66"/>
+    <mergeCell ref="F65:F66"/>
     <mergeCell ref="F73:F75"/>
     <mergeCell ref="E73:E75"/>
     <mergeCell ref="D73:D75"/>
+    <mergeCell ref="B84:B87"/>
+    <mergeCell ref="C84:C87"/>
+    <mergeCell ref="D84:D87"/>
+    <mergeCell ref="E84:E87"/>
+    <mergeCell ref="F84:F87"/>
+    <mergeCell ref="B81:B83"/>
+    <mergeCell ref="C81:C83"/>
+    <mergeCell ref="D81:D83"/>
+    <mergeCell ref="E81:E83"/>
+    <mergeCell ref="F81:F83"/>
+    <mergeCell ref="A59:C59"/>
+    <mergeCell ref="B61:C63"/>
+    <mergeCell ref="A65:C66"/>
+    <mergeCell ref="A67:C67"/>
+    <mergeCell ref="A8:C12"/>
+    <mergeCell ref="A18:C18"/>
+    <mergeCell ref="B19:C22"/>
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="A14:C15"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="A17:C17"/>
+    <mergeCell ref="B107:C110"/>
+    <mergeCell ref="D107:D110"/>
+    <mergeCell ref="E107:E110"/>
+    <mergeCell ref="F107:F110"/>
+    <mergeCell ref="B111:C112"/>
+    <mergeCell ref="D111:D112"/>
+    <mergeCell ref="E111:E112"/>
+    <mergeCell ref="F111:F112"/>
+    <mergeCell ref="A91:C91"/>
+    <mergeCell ref="B92:C95"/>
+    <mergeCell ref="A104:C104"/>
+    <mergeCell ref="B105:C106"/>
+    <mergeCell ref="D105:D106"/>
+    <mergeCell ref="B96:B99"/>
+    <mergeCell ref="B100:B103"/>
+    <mergeCell ref="E105:E106"/>
+    <mergeCell ref="F105:F106"/>
+    <mergeCell ref="C96:C99"/>
+    <mergeCell ref="C100:C103"/>
     <mergeCell ref="D92:D95"/>
     <mergeCell ref="E92:E95"/>
     <mergeCell ref="D96:D99"/>
     <mergeCell ref="E96:E99"/>
     <mergeCell ref="D100:D103"/>
-    <mergeCell ref="E100:E103"/>
-    <mergeCell ref="F92:F95"/>
-    <mergeCell ref="F96:F99"/>
-    <mergeCell ref="F100:F103"/>
-    <mergeCell ref="D8:D12"/>
-    <mergeCell ref="E8:E12"/>
-    <mergeCell ref="F8:F12"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="F3:F4"/>
-    <mergeCell ref="F31:F34"/>
-    <mergeCell ref="E31:E34"/>
-    <mergeCell ref="F39:F41"/>
-    <mergeCell ref="F19:F22"/>
-    <mergeCell ref="E19:E22"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="F5:F7"/>
-    <mergeCell ref="D5:D7"/>
-    <mergeCell ref="F14:F15"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="D19:D22"/>
+    <mergeCell ref="D127:D129"/>
+    <mergeCell ref="E127:E129"/>
+    <mergeCell ref="F127:F129"/>
+    <mergeCell ref="B130:C133"/>
+    <mergeCell ref="D130:D133"/>
+    <mergeCell ref="E130:E133"/>
+    <mergeCell ref="F130:F133"/>
+    <mergeCell ref="A114:C121"/>
+    <mergeCell ref="A122:C125"/>
+    <mergeCell ref="A126:C126"/>
+    <mergeCell ref="B127:C129"/>
+    <mergeCell ref="E114:E121"/>
+    <mergeCell ref="F114:F121"/>
+    <mergeCell ref="D122:D125"/>
+    <mergeCell ref="D114:D121"/>
+    <mergeCell ref="E122:E125"/>
+    <mergeCell ref="F122:F125"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="M3" r:id="rId1" display="e.g., DataCiteSchema" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
@@ -12379,31 +12372,29 @@
     <hyperlink ref="M61" r:id="rId13" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
     <hyperlink ref="M62" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
     <hyperlink ref="M63" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
-    <hyperlink ref="M132" r:id="rId16" display="DataCiteSchema" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
-    <hyperlink ref="M133" r:id="rId17" display="DataCiteSchema" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
-    <hyperlink ref="L4" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="L3" r:id="rId19" xr:uid="{79274165-A08F-504F-ABEF-86158BAB6E38}"/>
-    <hyperlink ref="L5" r:id="rId20" xr:uid="{EB38BFB8-104C-9549-9590-CD747EA2AB6E}"/>
-    <hyperlink ref="L6" r:id="rId21" xr:uid="{F30A9924-D727-3841-A75B-86457F100CDE}"/>
-    <hyperlink ref="L9" r:id="rId22" xr:uid="{ACAFE479-E18E-2047-B209-085A9026CC0F}"/>
-    <hyperlink ref="L8" r:id="rId23" xr:uid="{AA8245AE-3C94-7147-8E40-35DCB3896ED9}"/>
-    <hyperlink ref="L11" r:id="rId24" xr:uid="{686CAE22-83EC-A34E-B091-F87EA6510ADC}"/>
-    <hyperlink ref="M10" r:id="rId25" xr:uid="{DE9DC848-A7C3-104D-B0CC-7DED37DA0AD1}"/>
-    <hyperlink ref="L13" r:id="rId26" xr:uid="{E40CF022-E2D9-024B-BA4B-36300D6EABED}"/>
-    <hyperlink ref="M50" r:id="rId27" xr:uid="{F21891FB-61A7-3242-9AAA-F78E177BD42B}"/>
-    <hyperlink ref="M51" r:id="rId28" xr:uid="{528FA186-ED8E-6B4E-8209-54BF5C699854}"/>
-    <hyperlink ref="M43" r:id="rId29" display="DataCiteSchema" xr:uid="{512E7D48-D0BB-474E-81C8-84AF8AADE6CD}"/>
-    <hyperlink ref="M44" r:id="rId30" display="DataCiteSchema" xr:uid="{9F3289B1-82D8-D94D-802C-C6C552D25A29}"/>
-    <hyperlink ref="M47" r:id="rId31" display="DataCiteSchema" xr:uid="{6F22468B-C0E2-8E44-88CB-546D020C68F0}"/>
-    <hyperlink ref="M48" r:id="rId32" display="DataCiteSchema" xr:uid="{A7D1F61F-E528-0C44-AC76-2EF1F8BEB3E9}"/>
-    <hyperlink ref="M64" r:id="rId33" xr:uid="{0CC4972C-ECFA-B440-9A75-02F82DDED55D}"/>
-    <hyperlink ref="M89" r:id="rId34" display="DataCiteSchema" xr:uid="{9D6D4BCF-FB27-6D40-A7BD-017D1A5A4757}"/>
-    <hyperlink ref="M90" r:id="rId35" display="DataCiteSchema" xr:uid="{A858633D-A581-7741-AFEF-6719BC41416C}"/>
-    <hyperlink ref="M82" r:id="rId36" display="DataCiteSchema" xr:uid="{31DE2953-BF4E-694F-871C-448507278D9A}"/>
-    <hyperlink ref="M83" r:id="rId37" display="DataCiteSchema" xr:uid="{8630DA0C-B932-C246-9078-95C72FB5BF91}"/>
-    <hyperlink ref="M86" r:id="rId38" display="DataCiteSchema" xr:uid="{1B438F6A-F696-1841-A0B8-8C5CDE068A67}"/>
-    <hyperlink ref="M87" r:id="rId39" display="DataCiteSchema" xr:uid="{DDF97B6B-BEE3-3C44-8345-9022D2F48A26}"/>
-    <hyperlink ref="D151" r:id="rId40" display="https://fairdatacollective.org/" xr:uid="{F7D6490E-4341-0240-BE7B-5E8915480BD0}"/>
+    <hyperlink ref="L4" r:id="rId16" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="L3" r:id="rId17" xr:uid="{79274165-A08F-504F-ABEF-86158BAB6E38}"/>
+    <hyperlink ref="L5" r:id="rId18" xr:uid="{EB38BFB8-104C-9549-9590-CD747EA2AB6E}"/>
+    <hyperlink ref="L6" r:id="rId19" xr:uid="{F30A9924-D727-3841-A75B-86457F100CDE}"/>
+    <hyperlink ref="L9" r:id="rId20" xr:uid="{ACAFE479-E18E-2047-B209-085A9026CC0F}"/>
+    <hyperlink ref="L8" r:id="rId21" xr:uid="{AA8245AE-3C94-7147-8E40-35DCB3896ED9}"/>
+    <hyperlink ref="L11" r:id="rId22" xr:uid="{686CAE22-83EC-A34E-B091-F87EA6510ADC}"/>
+    <hyperlink ref="M10" r:id="rId23" xr:uid="{DE9DC848-A7C3-104D-B0CC-7DED37DA0AD1}"/>
+    <hyperlink ref="L13" r:id="rId24" xr:uid="{E40CF022-E2D9-024B-BA4B-36300D6EABED}"/>
+    <hyperlink ref="M50" r:id="rId25" xr:uid="{F21891FB-61A7-3242-9AAA-F78E177BD42B}"/>
+    <hyperlink ref="M51" r:id="rId26" xr:uid="{528FA186-ED8E-6B4E-8209-54BF5C699854}"/>
+    <hyperlink ref="M43" r:id="rId27" display="DataCiteSchema" xr:uid="{512E7D48-D0BB-474E-81C8-84AF8AADE6CD}"/>
+    <hyperlink ref="M44" r:id="rId28" display="DataCiteSchema" xr:uid="{9F3289B1-82D8-D94D-802C-C6C552D25A29}"/>
+    <hyperlink ref="M47" r:id="rId29" display="DataCiteSchema" xr:uid="{6F22468B-C0E2-8E44-88CB-546D020C68F0}"/>
+    <hyperlink ref="M48" r:id="rId30" display="DataCiteSchema" xr:uid="{A7D1F61F-E528-0C44-AC76-2EF1F8BEB3E9}"/>
+    <hyperlink ref="M64" r:id="rId31" xr:uid="{0CC4972C-ECFA-B440-9A75-02F82DDED55D}"/>
+    <hyperlink ref="M89" r:id="rId32" display="DataCiteSchema" xr:uid="{9D6D4BCF-FB27-6D40-A7BD-017D1A5A4757}"/>
+    <hyperlink ref="M90" r:id="rId33" display="DataCiteSchema" xr:uid="{A858633D-A581-7741-AFEF-6719BC41416C}"/>
+    <hyperlink ref="M82" r:id="rId34" display="DataCiteSchema" xr:uid="{31DE2953-BF4E-694F-871C-448507278D9A}"/>
+    <hyperlink ref="M83" r:id="rId35" display="DataCiteSchema" xr:uid="{8630DA0C-B932-C246-9078-95C72FB5BF91}"/>
+    <hyperlink ref="M86" r:id="rId36" display="DataCiteSchema" xr:uid="{1B438F6A-F696-1841-A0B8-8C5CDE068A67}"/>
+    <hyperlink ref="M87" r:id="rId37" display="DataCiteSchema" xr:uid="{DDF97B6B-BEE3-3C44-8345-9022D2F48A26}"/>
+    <hyperlink ref="D151" r:id="rId38" display="https://fairdatacollective.org/" xr:uid="{F7D6490E-4341-0240-BE7B-5E8915480BD0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
@@ -12424,10 +12415,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A1" s="738" t="s">
+      <c r="A1" s="740" t="s">
         <v>107</v>
       </c>
-      <c r="B1" s="738"/>
+      <c r="B1" s="740"/>
       <c r="C1" s="20" t="s">
         <v>462</v>
       </c>
@@ -12448,17 +12439,17 @@
       <c r="M1" s="28"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A2" s="739"/>
-      <c r="B2" s="740" t="s">
+      <c r="A2" s="735"/>
+      <c r="B2" s="736" t="s">
         <v>463</v>
       </c>
       <c r="C2" s="741" t="s">
         <v>455</v>
       </c>
-      <c r="D2" s="742" t="s">
+      <c r="D2" s="737" t="s">
         <v>54</v>
       </c>
-      <c r="E2" s="737" t="str">
+      <c r="E2" s="738" t="str">
         <f>Namespace &amp; LOWER($B2)</f>
         <v>http://vocab.fairdatacollective.org/dataset/properties/contributorname</v>
       </c>
@@ -12488,11 +12479,11 @@
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A3" s="739"/>
-      <c r="B3" s="740"/>
+      <c r="A3" s="735"/>
+      <c r="B3" s="736"/>
       <c r="C3" s="741"/>
-      <c r="D3" s="742"/>
-      <c r="E3" s="737"/>
+      <c r="D3" s="737"/>
+      <c r="E3" s="738"/>
       <c r="F3" s="34" t="s">
         <v>111</v>
       </c>
@@ -12519,11 +12510,11 @@
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A4" s="739"/>
-      <c r="B4" s="740"/>
+      <c r="A4" s="735"/>
+      <c r="B4" s="736"/>
       <c r="C4" s="741"/>
-      <c r="D4" s="742"/>
-      <c r="E4" s="737"/>
+      <c r="D4" s="737"/>
+      <c r="E4" s="738"/>
       <c r="F4" s="34" t="s">
         <v>113</v>
       </c>
@@ -12550,17 +12541,17 @@
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5" s="739"/>
-      <c r="B5" s="740" t="s">
+      <c r="A5" s="735"/>
+      <c r="B5" s="736" t="s">
         <v>466</v>
       </c>
-      <c r="C5" s="740" t="s">
+      <c r="C5" s="736" t="s">
         <v>456</v>
       </c>
-      <c r="D5" s="742" t="s">
+      <c r="D5" s="737" t="s">
         <v>54</v>
       </c>
-      <c r="E5" s="737" t="str">
+      <c r="E5" s="738" t="str">
         <f>Namespace &amp; LOWER($B5)</f>
         <v>http://vocab.fairdatacollective.org/dataset/properties/contributoridentifier</v>
       </c>
@@ -12591,11 +12582,11 @@
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A6" s="739"/>
-      <c r="B6" s="740"/>
-      <c r="C6" s="740"/>
-      <c r="D6" s="742"/>
-      <c r="E6" s="737"/>
+      <c r="A6" s="735"/>
+      <c r="B6" s="736"/>
+      <c r="C6" s="736"/>
+      <c r="D6" s="737"/>
+      <c r="E6" s="738"/>
       <c r="F6" s="34" t="s">
         <v>121</v>
       </c>
@@ -12623,11 +12614,11 @@
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A7" s="739"/>
-      <c r="B7" s="740"/>
-      <c r="C7" s="740"/>
-      <c r="D7" s="742"/>
-      <c r="E7" s="737"/>
+      <c r="A7" s="735"/>
+      <c r="B7" s="736"/>
+      <c r="C7" s="736"/>
+      <c r="D7" s="737"/>
+      <c r="E7" s="738"/>
       <c r="F7" s="34" t="s">
         <v>122</v>
       </c>
@@ -12655,17 +12646,17 @@
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A8" s="739"/>
-      <c r="B8" s="740" t="s">
+      <c r="A8" s="735"/>
+      <c r="B8" s="736" t="s">
         <v>467</v>
       </c>
-      <c r="C8" s="740" t="s">
+      <c r="C8" s="736" t="s">
         <v>458</v>
       </c>
-      <c r="D8" s="742" t="s">
+      <c r="D8" s="737" t="s">
         <v>54</v>
       </c>
-      <c r="E8" s="743" t="str">
+      <c r="E8" s="739" t="str">
         <f>Namespace &amp; LOWER($B8)</f>
         <v>http://vocab.fairdatacollective.org/dataset/properties/contributoraffiliation</v>
       </c>
@@ -12696,11 +12687,11 @@
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A9" s="739"/>
-      <c r="B9" s="740"/>
-      <c r="C9" s="740"/>
-      <c r="D9" s="742"/>
-      <c r="E9" s="743"/>
+      <c r="A9" s="735"/>
+      <c r="B9" s="736"/>
+      <c r="C9" s="736"/>
+      <c r="D9" s="737"/>
+      <c r="E9" s="739"/>
       <c r="F9" s="34" t="s">
         <v>123</v>
       </c>
@@ -12728,11 +12719,11 @@
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A10" s="739"/>
-      <c r="B10" s="740"/>
-      <c r="C10" s="740"/>
-      <c r="D10" s="742"/>
-      <c r="E10" s="743"/>
+      <c r="A10" s="735"/>
+      <c r="B10" s="736"/>
+      <c r="C10" s="736"/>
+      <c r="D10" s="737"/>
+      <c r="E10" s="739"/>
       <c r="F10" s="34" t="s">
         <v>460</v>
       </c>
@@ -12760,11 +12751,11 @@
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A11" s="739"/>
-      <c r="B11" s="740"/>
-      <c r="C11" s="740"/>
-      <c r="D11" s="742"/>
-      <c r="E11" s="743"/>
+      <c r="A11" s="735"/>
+      <c r="B11" s="736"/>
+      <c r="C11" s="736"/>
+      <c r="D11" s="737"/>
+      <c r="E11" s="739"/>
       <c r="F11" s="34" t="s">
         <v>125</v>
       </c>
@@ -12888,22 +12879,22 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="A5:A7"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="C5:C7"/>
-    <mergeCell ref="D5:D7"/>
-    <mergeCell ref="E5:E7"/>
-    <mergeCell ref="A8:A11"/>
-    <mergeCell ref="B8:B11"/>
-    <mergeCell ref="C8:C11"/>
-    <mergeCell ref="D8:D11"/>
-    <mergeCell ref="E8:E11"/>
     <mergeCell ref="E2:E4"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="B2:B4"/>
     <mergeCell ref="C2:C4"/>
     <mergeCell ref="D2:D4"/>
+    <mergeCell ref="A8:A11"/>
+    <mergeCell ref="B8:B11"/>
+    <mergeCell ref="C8:C11"/>
+    <mergeCell ref="D8:D11"/>
+    <mergeCell ref="E8:E11"/>
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="C5:C7"/>
+    <mergeCell ref="D5:D7"/>
+    <mergeCell ref="E5:E7"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="L13" r:id="rId1" xr:uid="{9ABA6EE5-7A54-DF40-9E10-C757BCBA07FF}"/>

</xml_diff>

<commit_message>
re-org files and updated template and vocab entries in xlsx files
</commit_message>
<xml_diff>
--- a/template-description.xlsx
+++ b/template-description.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Secondary_Drive/work/repos/FAIR-data/generic-dataset-metadata-template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67EE3CA1-D949-DC46-A530-D89FDEAE5BA7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{0DD6CDDF-9082-E143-9B60-3B7C03608A63}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="68800" windowHeight="28340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="16800" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dataset template" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,6 @@
     <definedName name="Namespace">'Dataset template'!$D$151</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1056" uniqueCount="524">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1052" uniqueCount="524">
   <si>
     <t>Element 
 (CEDAR)</t>
@@ -1602,9 +1601,6 @@
     <t>Relevant dates related to the resource being described. One instance of date must be of datsetDateType=Published.</t>
   </si>
   <si>
-    <t>http://vocab.fairdatacollective.org/dataset/properties/</t>
-  </si>
-  <si>
     <t>BASE url</t>
   </si>
   <si>
@@ -1612,6 +1608,9 @@
   </si>
   <si>
     <t>MIME Types list</t>
+  </si>
+  <si>
+    <t>https://vocab.fairdatacollective.org/gdmt/property/</t>
   </si>
 </sst>
 </file>
@@ -3277,32 +3276,29 @@
     <xf numFmtId="0" fontId="11" fillId="15" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="35" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="35" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="38" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="38" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="35" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="35" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="35" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="35" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="38" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="38" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="35" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -3344,6 +3340,138 @@
     <xf numFmtId="0" fontId="11" fillId="16" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="24" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="34" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="34" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="34" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="34" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -3356,97 +3484,109 @@
     <xf numFmtId="0" fontId="13" fillId="30" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="24" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="35" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="35" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="30" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="30" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="35" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="35" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="37" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="37" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="37" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="37" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="34" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="34" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="34" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="34" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="31" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3465,159 +3605,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="26" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="26" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="26" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="35" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="35" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="30" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="30" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="35" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="35" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="37" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="37" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="37" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="37" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="31" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="31" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="31" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="31" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="16" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3731,6 +3718,18 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3986,10 +3985,10 @@
   <dimension ref="A1:P1034"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D99" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L24" sqref="L24"/>
+      <selection pane="bottomRight" activeCell="B107" sqref="B107:C110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4001,7 +4000,7 @@
     <col min="6" max="6" width="60.140625" style="12" customWidth="1"/>
     <col min="7" max="7" width="32.7109375" style="10" customWidth="1"/>
     <col min="8" max="8" width="32.7109375" customWidth="1"/>
-    <col min="9" max="9" width="80.42578125" customWidth="1"/>
+    <col min="9" max="9" width="34.140625" customWidth="1"/>
     <col min="10" max="10" width="19.28515625" customWidth="1"/>
     <col min="11" max="11" width="12.42578125" style="13" customWidth="1"/>
     <col min="12" max="12" width="56.42578125" style="13" customWidth="1"/>
@@ -4011,11 +4010,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="669" t="s">
+      <c r="A1" s="668" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="669"/>
-      <c r="C1" s="669"/>
+      <c r="B1" s="668"/>
+      <c r="C1" s="668"/>
       <c r="D1" s="44" t="s">
         <v>1</v>
       </c>
@@ -4053,11 +4052,11 @@
       <c r="P1" s="1"/>
     </row>
     <row r="2" spans="1:16" ht="69" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="668" t="s">
+      <c r="A2" s="667" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="668"/>
-      <c r="C2" s="668"/>
+      <c r="B2" s="667"/>
+      <c r="C2" s="667"/>
       <c r="D2" s="126" t="s">
         <v>10</v>
       </c>
@@ -4089,20 +4088,20 @@
       <c r="P2" s="2"/>
     </row>
     <row r="3" spans="1:16" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="663" t="s">
+      <c r="A3" s="662" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="663"/>
-      <c r="C3" s="663"/>
-      <c r="D3" s="710" t="s">
+      <c r="B3" s="662"/>
+      <c r="C3" s="662"/>
+      <c r="D3" s="706" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="712">
+      <c r="E3" s="708">
         <v>1</v>
       </c>
-      <c r="F3" s="713" t="str">
-        <f>Namespace &amp; $A3</f>
-        <v>http://vocab.fairdatacollective.org/dataset/properties/ResourceType</v>
+      <c r="F3" s="709" t="str">
+        <f>Namespace &amp; $A3 &amp; "Info"</f>
+        <v>https://vocab.fairdatacollective.org/gdmt/property/ResourceTypeInfo</v>
       </c>
       <c r="G3" s="183" t="s">
         <v>18</v>
@@ -4130,12 +4129,12 @@
       </c>
     </row>
     <row r="4" spans="1:16" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="664"/>
-      <c r="B4" s="664"/>
-      <c r="C4" s="664"/>
-      <c r="D4" s="711"/>
+      <c r="A4" s="663"/>
+      <c r="B4" s="663"/>
+      <c r="C4" s="663"/>
+      <c r="D4" s="707"/>
       <c r="E4" s="578"/>
-      <c r="F4" s="714"/>
+      <c r="F4" s="710"/>
       <c r="G4" s="190" t="s">
         <v>22</v>
       </c>
@@ -4162,20 +4161,20 @@
       </c>
     </row>
     <row r="5" spans="1:16" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="665" t="s">
+      <c r="A5" s="664" t="s">
         <v>259</v>
       </c>
-      <c r="B5" s="665"/>
-      <c r="C5" s="665"/>
-      <c r="D5" s="728" t="s">
+      <c r="B5" s="664"/>
+      <c r="C5" s="664"/>
+      <c r="D5" s="724" t="s">
         <v>25</v>
       </c>
-      <c r="E5" s="685">
+      <c r="E5" s="684">
         <v>1</v>
       </c>
-      <c r="F5" s="725" t="str">
-        <f>Namespace &amp; ($A5)</f>
-        <v>http://vocab.fairdatacollective.org/dataset/properties/DatasetIdentifier</v>
+      <c r="F5" s="721" t="str">
+        <f>Namespace &amp; ($A5) &amp; "Info"</f>
+        <v>https://vocab.fairdatacollective.org/gdmt/property/DatasetIdentifierInfo</v>
       </c>
       <c r="G5" s="197" t="s">
         <v>26</v>
@@ -4203,12 +4202,12 @@
       </c>
     </row>
     <row r="6" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="666"/>
-      <c r="B6" s="666"/>
-      <c r="C6" s="666"/>
-      <c r="D6" s="729"/>
-      <c r="E6" s="686"/>
-      <c r="F6" s="726"/>
+      <c r="A6" s="665"/>
+      <c r="B6" s="665"/>
+      <c r="C6" s="665"/>
+      <c r="D6" s="725"/>
+      <c r="E6" s="685"/>
+      <c r="F6" s="722"/>
       <c r="G6" s="53" t="s">
         <v>29</v>
       </c>
@@ -4235,12 +4234,12 @@
       </c>
     </row>
     <row r="7" spans="1:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="667"/>
-      <c r="B7" s="667"/>
-      <c r="C7" s="667"/>
-      <c r="D7" s="730"/>
-      <c r="E7" s="687"/>
-      <c r="F7" s="727"/>
+      <c r="A7" s="666"/>
+      <c r="B7" s="666"/>
+      <c r="C7" s="666"/>
+      <c r="D7" s="726"/>
+      <c r="E7" s="686"/>
+      <c r="F7" s="723"/>
       <c r="G7" s="203" t="s">
         <v>32</v>
       </c>
@@ -4258,7 +4257,7 @@
       </c>
       <c r="L7" s="207" t="str">
         <f>Namespace &amp; "identifiersubtype"</f>
-        <v>http://vocab.fairdatacollective.org/dataset/properties/identifiersubtype</v>
+        <v>https://vocab.fairdatacollective.org/gdmt/property/identifiersubtype</v>
       </c>
       <c r="M7" s="208" t="s">
         <v>28</v>
@@ -4268,20 +4267,20 @@
       </c>
     </row>
     <row r="8" spans="1:16" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="609" t="s">
+      <c r="A8" s="607" t="s">
         <v>33</v>
       </c>
-      <c r="B8" s="609"/>
-      <c r="C8" s="609"/>
-      <c r="D8" s="703" t="s">
+      <c r="B8" s="607"/>
+      <c r="C8" s="607"/>
+      <c r="D8" s="699" t="s">
         <v>276</v>
       </c>
-      <c r="E8" s="706" t="s">
+      <c r="E8" s="702" t="s">
         <v>34</v>
       </c>
-      <c r="F8" s="707" t="str">
-        <f>Namespace &amp; ($A8)</f>
-        <v>http://vocab.fairdatacollective.org/dataset/properties/RelatedResources</v>
+      <c r="F8" s="703" t="str">
+        <f>Namespace &amp; ($A8) &amp; "Info"</f>
+        <v>https://vocab.fairdatacollective.org/gdmt/property/RelatedResourcesInfo</v>
       </c>
       <c r="G8" s="210" t="s">
         <v>35</v>
@@ -4309,12 +4308,12 @@
       </c>
     </row>
     <row r="9" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="610"/>
-      <c r="B9" s="610"/>
-      <c r="C9" s="610"/>
-      <c r="D9" s="704"/>
+      <c r="A9" s="608"/>
+      <c r="B9" s="608"/>
+      <c r="C9" s="608"/>
+      <c r="D9" s="700"/>
       <c r="E9" s="577"/>
-      <c r="F9" s="708"/>
+      <c r="F9" s="704"/>
       <c r="G9" s="59" t="s">
         <v>38</v>
       </c>
@@ -4341,12 +4340,12 @@
       </c>
     </row>
     <row r="10" spans="1:16" s="10" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="610"/>
-      <c r="B10" s="610"/>
-      <c r="C10" s="610"/>
-      <c r="D10" s="704"/>
+      <c r="A10" s="608"/>
+      <c r="B10" s="608"/>
+      <c r="C10" s="608"/>
+      <c r="D10" s="700"/>
       <c r="E10" s="577"/>
-      <c r="F10" s="708"/>
+      <c r="F10" s="704"/>
       <c r="G10" s="59" t="s">
         <v>272</v>
       </c>
@@ -4364,7 +4363,7 @@
       </c>
       <c r="L10" s="63" t="str">
         <f>Namespace &amp; $G10</f>
-        <v>http://vocab.fairdatacollective.org/dataset/properties/relatedResourceIdentifierSubType</v>
+        <v>https://vocab.fairdatacollective.org/gdmt/property/relatedResourceIdentifierSubType</v>
       </c>
       <c r="M10" s="65" t="s">
         <v>24</v>
@@ -4374,12 +4373,12 @@
       </c>
     </row>
     <row r="11" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="610"/>
-      <c r="B11" s="610"/>
-      <c r="C11" s="610"/>
-      <c r="D11" s="704"/>
+      <c r="A11" s="608"/>
+      <c r="B11" s="608"/>
+      <c r="C11" s="608"/>
+      <c r="D11" s="700"/>
       <c r="E11" s="577"/>
-      <c r="F11" s="708"/>
+      <c r="F11" s="704"/>
       <c r="G11" s="64" t="s">
         <v>41</v>
       </c>
@@ -4406,12 +4405,12 @@
       </c>
     </row>
     <row r="12" spans="1:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="611"/>
-      <c r="B12" s="611"/>
-      <c r="C12" s="611"/>
-      <c r="D12" s="705"/>
+      <c r="A12" s="609"/>
+      <c r="B12" s="609"/>
+      <c r="C12" s="609"/>
+      <c r="D12" s="701"/>
       <c r="E12" s="578"/>
-      <c r="F12" s="709"/>
+      <c r="F12" s="705"/>
       <c r="G12" s="216" t="s">
         <v>42</v>
       </c>
@@ -4438,11 +4437,11 @@
       </c>
     </row>
     <row r="13" spans="1:16" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="616" t="s">
+      <c r="A13" s="614" t="s">
         <v>44</v>
       </c>
-      <c r="B13" s="616"/>
-      <c r="C13" s="616"/>
+      <c r="B13" s="614"/>
+      <c r="C13" s="614"/>
       <c r="D13" s="243" t="s">
         <v>45</v>
       </c>
@@ -4450,8 +4449,8 @@
         <v>46</v>
       </c>
       <c r="F13" s="68" t="str">
-        <f>Namespace &amp; ($A13)</f>
-        <v>http://vocab.fairdatacollective.org/dataset/properties/Version</v>
+        <f>Namespace &amp; ($A13) &amp; "Info"</f>
+        <v>https://vocab.fairdatacollective.org/gdmt/property/VersionInfo</v>
       </c>
       <c r="G13" s="69" t="s">
         <v>47</v>
@@ -4479,20 +4478,20 @@
       </c>
     </row>
     <row r="14" spans="1:16" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="617" t="s">
+      <c r="A14" s="615" t="s">
         <v>48</v>
       </c>
-      <c r="B14" s="617"/>
-      <c r="C14" s="617"/>
-      <c r="D14" s="733" t="s">
+      <c r="B14" s="615"/>
+      <c r="C14" s="615"/>
+      <c r="D14" s="729" t="s">
         <v>49</v>
       </c>
-      <c r="E14" s="723" t="s">
+      <c r="E14" s="719" t="s">
         <v>46</v>
       </c>
-      <c r="F14" s="731" t="str">
-        <f>Namespace &amp; ($A14)</f>
-        <v>http://vocab.fairdatacollective.org/dataset/properties/Language</v>
+      <c r="F14" s="727" t="str">
+        <f>Namespace &amp; ($A14) &amp; "Info"</f>
+        <v>https://vocab.fairdatacollective.org/gdmt/property/LanguageInfo</v>
       </c>
       <c r="G14" s="223" t="s">
         <v>50</v>
@@ -4520,12 +4519,12 @@
       </c>
     </row>
     <row r="15" spans="1:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="618"/>
-      <c r="B15" s="618"/>
-      <c r="C15" s="618"/>
-      <c r="D15" s="734"/>
-      <c r="E15" s="724"/>
-      <c r="F15" s="732"/>
+      <c r="A15" s="616"/>
+      <c r="B15" s="616"/>
+      <c r="C15" s="616"/>
+      <c r="D15" s="730"/>
+      <c r="E15" s="720"/>
+      <c r="F15" s="728"/>
       <c r="G15" s="229" t="s">
         <v>51</v>
       </c>
@@ -4535,15 +4534,15 @@
       <c r="I15" s="230" t="s">
         <v>413</v>
       </c>
-      <c r="J15" s="231" t="s">
-        <v>46</v>
+      <c r="J15" s="231">
+        <v>1</v>
       </c>
       <c r="K15" s="232" t="s">
         <v>68</v>
       </c>
       <c r="L15" s="233" t="str">
         <f>Namespace &amp; "primarylanguage"</f>
-        <v>http://vocab.fairdatacollective.org/dataset/properties/primarylanguage</v>
+        <v>https://vocab.fairdatacollective.org/gdmt/property/primarylanguage</v>
       </c>
       <c r="M15" s="234" t="s">
         <v>435</v>
@@ -4555,20 +4554,20 @@
       <c r="P15" s="11"/>
     </row>
     <row r="16" spans="1:16" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="619" t="s">
+      <c r="A16" s="617" t="s">
         <v>52</v>
       </c>
-      <c r="B16" s="619"/>
-      <c r="C16" s="619"/>
+      <c r="B16" s="617"/>
+      <c r="C16" s="617"/>
       <c r="D16" s="244" t="s">
         <v>53</v>
       </c>
-      <c r="E16" s="235" t="s">
-        <v>54</v>
+      <c r="E16" s="235">
+        <v>1</v>
       </c>
       <c r="F16" s="236" t="str">
-        <f>Namespace &amp; ($A16)</f>
-        <v>http://vocab.fairdatacollective.org/dataset/properties/Title</v>
+        <f>Namespace &amp; ($A16) &amp; "Info"</f>
+        <v>https://vocab.fairdatacollective.org/gdmt/property/TitleInfo</v>
       </c>
       <c r="G16" s="237" t="s">
         <v>55</v>
@@ -4596,20 +4595,20 @@
       </c>
     </row>
     <row r="17" spans="1:16" s="11" customFormat="1" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="620" t="s">
+      <c r="A17" s="618" t="s">
         <v>57</v>
       </c>
-      <c r="B17" s="620"/>
-      <c r="C17" s="620"/>
+      <c r="B17" s="618"/>
+      <c r="C17" s="618"/>
       <c r="D17" s="78" t="s">
         <v>58</v>
       </c>
-      <c r="E17" s="75" t="s">
-        <v>54</v>
+      <c r="E17" s="75">
+        <v>1</v>
       </c>
       <c r="F17" s="76" t="str">
-        <f>Namespace &amp; ($A17)</f>
-        <v>http://vocab.fairdatacollective.org/dataset/properties/Description</v>
+        <f>Namespace &amp; ($A17) &amp; "Info"</f>
+        <v>https://vocab.fairdatacollective.org/gdmt/property/DescriptionInfo</v>
       </c>
       <c r="G17" s="76" t="s">
         <v>59</v>
@@ -4639,11 +4638,11 @@
       <c r="P17"/>
     </row>
     <row r="18" spans="1:16" s="11" customFormat="1" ht="17" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="612" t="s">
+      <c r="A18" s="610" t="s">
         <v>62</v>
       </c>
-      <c r="B18" s="612"/>
-      <c r="C18" s="612"/>
+      <c r="B18" s="610"/>
+      <c r="C18" s="610"/>
       <c r="D18" s="245" t="s">
         <v>63</v>
       </c>
@@ -4651,8 +4650,8 @@
         <v>46</v>
       </c>
       <c r="F18" s="149" t="str">
-        <f>Namespace&amp;($A18)</f>
-        <v>http://vocab.fairdatacollective.org/dataset/properties/Subject</v>
+        <f>Namespace&amp;($A18) &amp; "Info"</f>
+        <v>https://vocab.fairdatacollective.org/gdmt/property/SubjectInfo</v>
       </c>
       <c r="G18" s="151"/>
       <c r="H18" s="151"/>
@@ -4667,19 +4666,19 @@
     </row>
     <row r="19" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="315"/>
-      <c r="B19" s="613" t="s">
+      <c r="B19" s="611" t="s">
         <v>501</v>
       </c>
-      <c r="C19" s="613"/>
-      <c r="D19" s="613" t="s">
+      <c r="C19" s="611"/>
+      <c r="D19" s="611" t="s">
         <v>468</v>
       </c>
-      <c r="E19" s="720" t="s">
+      <c r="E19" s="716" t="s">
         <v>34</v>
       </c>
-      <c r="F19" s="717" t="str">
-        <f>Namespace&amp;($A19)</f>
-        <v>http://vocab.fairdatacollective.org/dataset/properties/</v>
+      <c r="F19" s="713" t="str">
+        <f>Namespace&amp;($B19) &amp; "Info"</f>
+        <v>https://vocab.fairdatacollective.org/gdmt/property/ControlledTermsInfo</v>
       </c>
       <c r="G19" s="127" t="s">
         <v>66</v>
@@ -4708,11 +4707,11 @@
     </row>
     <row r="20" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="315"/>
-      <c r="B20" s="614"/>
-      <c r="C20" s="614"/>
-      <c r="D20" s="614"/>
-      <c r="E20" s="721"/>
-      <c r="F20" s="718"/>
+      <c r="B20" s="612"/>
+      <c r="C20" s="612"/>
+      <c r="D20" s="612"/>
+      <c r="E20" s="717"/>
+      <c r="F20" s="714"/>
       <c r="G20" s="79" t="s">
         <v>469</v>
       </c>
@@ -4730,7 +4729,7 @@
       </c>
       <c r="L20" s="82" t="str">
         <f>Namespace &amp; $G20</f>
-        <v>http://vocab.fairdatacollective.org/dataset/properties/subjectIRI</v>
+        <v>https://vocab.fairdatacollective.org/gdmt/property/subjectIRI</v>
       </c>
       <c r="M20" s="83" t="s">
         <v>502</v>
@@ -4741,11 +4740,11 @@
     </row>
     <row r="21" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="315"/>
-      <c r="B21" s="614"/>
-      <c r="C21" s="614"/>
-      <c r="D21" s="614"/>
-      <c r="E21" s="721"/>
-      <c r="F21" s="718"/>
+      <c r="B21" s="612"/>
+      <c r="C21" s="612"/>
+      <c r="D21" s="612"/>
+      <c r="E21" s="717"/>
+      <c r="F21" s="714"/>
       <c r="G21" s="83" t="s">
         <v>70</v>
       </c>
@@ -4763,7 +4762,7 @@
       </c>
       <c r="L21" s="82" t="str">
         <f>Namespace &amp; $G21</f>
-        <v>http://vocab.fairdatacollective.org/dataset/properties/subjectScheme</v>
+        <v>https://vocab.fairdatacollective.org/gdmt/property/subjectScheme</v>
       </c>
       <c r="M21" s="83" t="s">
         <v>502</v>
@@ -4774,11 +4773,11 @@
     </row>
     <row r="22" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="315"/>
-      <c r="B22" s="615"/>
-      <c r="C22" s="615"/>
-      <c r="D22" s="615"/>
-      <c r="E22" s="722"/>
-      <c r="F22" s="719"/>
+      <c r="B22" s="613"/>
+      <c r="C22" s="613"/>
+      <c r="D22" s="613"/>
+      <c r="E22" s="718"/>
+      <c r="F22" s="715"/>
       <c r="G22" s="132" t="s">
         <v>71</v>
       </c>
@@ -4796,7 +4795,7 @@
       </c>
       <c r="L22" s="135" t="str">
         <f>Namespace &amp; $G22</f>
-        <v>http://vocab.fairdatacollective.org/dataset/properties/subjectSchemeIRI</v>
+        <v>https://vocab.fairdatacollective.org/gdmt/property/subjectSchemeIRI</v>
       </c>
       <c r="M22" s="136" t="s">
         <v>502</v>
@@ -4829,7 +4828,7 @@
       </c>
       <c r="L23" s="162" t="str">
         <f>Namespace &amp; $G23</f>
-        <v>http://vocab.fairdatacollective.org/dataset/properties/keyword</v>
+        <v>https://vocab.fairdatacollective.org/gdmt/property/keyword</v>
       </c>
       <c r="M23" s="163"/>
       <c r="N23" s="164" t="s">
@@ -4837,11 +4836,11 @@
       </c>
     </row>
     <row r="24" spans="1:16" s="14" customFormat="1" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="649" t="s">
+      <c r="A24" s="652" t="s">
         <v>72</v>
       </c>
-      <c r="B24" s="649"/>
-      <c r="C24" s="649"/>
+      <c r="B24" s="652"/>
+      <c r="C24" s="652"/>
       <c r="D24" s="246" t="s">
         <v>73</v>
       </c>
@@ -4849,8 +4848,8 @@
         <v>54</v>
       </c>
       <c r="F24" s="166" t="str">
-        <f>Namespace &amp; ($A24)</f>
-        <v>http://vocab.fairdatacollective.org/dataset/properties/Creator</v>
+        <f>Namespace &amp; ($A24) &amp; "Info"</f>
+        <v>https://vocab.fairdatacollective.org/gdmt/property/CreatorInfo</v>
       </c>
       <c r="G24" s="167"/>
       <c r="H24" s="167"/>
@@ -4863,19 +4862,19 @@
     </row>
     <row r="25" spans="1:16" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="17"/>
-      <c r="B25" s="650" t="s">
+      <c r="B25" s="653" t="s">
         <v>452</v>
       </c>
-      <c r="C25" s="650"/>
-      <c r="D25" s="650" t="s">
+      <c r="C25" s="653"/>
+      <c r="D25" s="653" t="s">
         <v>478</v>
       </c>
-      <c r="E25" s="679" t="s">
+      <c r="E25" s="678" t="s">
         <v>54</v>
       </c>
-      <c r="F25" s="682" t="str">
-        <f>Namespace &amp; ($B25)</f>
-        <v>http://vocab.fairdatacollective.org/dataset/properties/CreatorName</v>
+      <c r="F25" s="681" t="str">
+        <f>Namespace &amp; ($B25) &amp; "Info"</f>
+        <v>https://vocab.fairdatacollective.org/gdmt/property/CreatorNameInfo</v>
       </c>
       <c r="G25" s="137" t="s">
         <v>85</v>
@@ -4904,11 +4903,11 @@
     </row>
     <row r="26" spans="1:16" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="17"/>
-      <c r="B26" s="651"/>
-      <c r="C26" s="651"/>
-      <c r="D26" s="651"/>
-      <c r="E26" s="680"/>
-      <c r="F26" s="683"/>
+      <c r="B26" s="654"/>
+      <c r="C26" s="654"/>
+      <c r="D26" s="654"/>
+      <c r="E26" s="679"/>
+      <c r="F26" s="682"/>
       <c r="G26" s="87" t="s">
         <v>79</v>
       </c>
@@ -4936,11 +4935,11 @@
     </row>
     <row r="27" spans="1:16" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="17"/>
-      <c r="B27" s="652"/>
-      <c r="C27" s="652"/>
-      <c r="D27" s="652"/>
-      <c r="E27" s="681"/>
-      <c r="F27" s="684"/>
+      <c r="B27" s="655"/>
+      <c r="C27" s="655"/>
+      <c r="D27" s="655"/>
+      <c r="E27" s="680"/>
+      <c r="F27" s="683"/>
       <c r="G27" s="141" t="s">
         <v>82</v>
       </c>
@@ -4968,19 +4967,19 @@
     </row>
     <row r="28" spans="1:16" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="17"/>
-      <c r="B28" s="650" t="s">
+      <c r="B28" s="653" t="s">
         <v>453</v>
       </c>
-      <c r="C28" s="650"/>
-      <c r="D28" s="650" t="s">
+      <c r="C28" s="653"/>
+      <c r="D28" s="653" t="s">
         <v>477</v>
       </c>
-      <c r="E28" s="679" t="s">
+      <c r="E28" s="678" t="s">
         <v>54</v>
       </c>
-      <c r="F28" s="682" t="str">
-        <f>Namespace &amp; ($B28)</f>
-        <v>http://vocab.fairdatacollective.org/dataset/properties/CreatorIdentifier</v>
+      <c r="F28" s="681" t="str">
+        <f>Namespace &amp; ($B28) &amp; "Info"</f>
+        <v>https://vocab.fairdatacollective.org/gdmt/property/CreatorIdentifierInfo</v>
       </c>
       <c r="G28" s="146" t="s">
         <v>91</v>
@@ -4999,7 +4998,7 @@
       </c>
       <c r="L28" s="140" t="str">
         <f t="shared" ref="L28:L34" si="0">Namespace &amp; $G28</f>
-        <v>http://vocab.fairdatacollective.org/dataset/properties/creatorIdentifier</v>
+        <v>https://vocab.fairdatacollective.org/gdmt/property/creatorIdentifier</v>
       </c>
       <c r="M28" s="137" t="s">
         <v>28</v>
@@ -5010,11 +5009,11 @@
     </row>
     <row r="29" spans="1:16" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="17"/>
-      <c r="B29" s="651"/>
-      <c r="C29" s="651"/>
-      <c r="D29" s="651"/>
-      <c r="E29" s="680"/>
-      <c r="F29" s="683"/>
+      <c r="B29" s="654"/>
+      <c r="C29" s="654"/>
+      <c r="D29" s="654"/>
+      <c r="E29" s="679"/>
+      <c r="F29" s="682"/>
       <c r="G29" s="87" t="s">
         <v>93</v>
       </c>
@@ -5032,10 +5031,10 @@
       </c>
       <c r="L29" s="86" t="str">
         <f t="shared" si="0"/>
-        <v>http://vocab.fairdatacollective.org/dataset/properties/creatorIdentifierScheme</v>
+        <v>https://vocab.fairdatacollective.org/gdmt/property/creatorIdentifierScheme</v>
       </c>
       <c r="M29" s="89" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="N29" s="84" t="s">
         <v>94</v>
@@ -5043,11 +5042,11 @@
     </row>
     <row r="30" spans="1:16" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="17"/>
-      <c r="B30" s="652"/>
-      <c r="C30" s="652"/>
-      <c r="D30" s="652"/>
-      <c r="E30" s="681"/>
-      <c r="F30" s="684"/>
+      <c r="B30" s="655"/>
+      <c r="C30" s="655"/>
+      <c r="D30" s="655"/>
+      <c r="E30" s="680"/>
+      <c r="F30" s="683"/>
       <c r="G30" s="141" t="s">
         <v>95</v>
       </c>
@@ -5065,10 +5064,10 @@
       </c>
       <c r="L30" s="144" t="str">
         <f t="shared" si="0"/>
-        <v>http://vocab.fairdatacollective.org/dataset/properties/creatorIdentifierSchemeIRI</v>
+        <v>https://vocab.fairdatacollective.org/gdmt/property/creatorIdentifierSchemeIRI</v>
       </c>
       <c r="M30" s="148" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="N30" s="145" t="s">
         <v>96</v>
@@ -5076,19 +5075,19 @@
     </row>
     <row r="31" spans="1:16" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="17"/>
-      <c r="B31" s="650" t="s">
+      <c r="B31" s="653" t="s">
         <v>454</v>
       </c>
-      <c r="C31" s="650"/>
-      <c r="D31" s="650" t="s">
+      <c r="C31" s="653"/>
+      <c r="D31" s="653" t="s">
         <v>476</v>
       </c>
-      <c r="E31" s="679" t="s">
-        <v>54</v>
-      </c>
-      <c r="F31" s="715" t="str">
-        <f>Namespace &amp; ($B31)</f>
-        <v>http://vocab.fairdatacollective.org/dataset/properties/CreatorAffiliation</v>
+      <c r="E31" s="678" t="s">
+        <v>34</v>
+      </c>
+      <c r="F31" s="711" t="str">
+        <f>Namespace &amp; ($B31) &amp; "Info"</f>
+        <v>https://vocab.fairdatacollective.org/gdmt/property/CreatorAffiliationInfo</v>
       </c>
       <c r="G31" s="87" t="s">
         <v>97</v>
@@ -5107,7 +5106,7 @@
       </c>
       <c r="L31" s="86" t="str">
         <f t="shared" si="0"/>
-        <v>http://vocab.fairdatacollective.org/dataset/properties/creatorAffiliation</v>
+        <v>https://vocab.fairdatacollective.org/gdmt/property/creatorAffiliation</v>
       </c>
       <c r="M31" s="84" t="s">
         <v>28</v>
@@ -5118,11 +5117,11 @@
     </row>
     <row r="32" spans="1:16" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="17"/>
-      <c r="B32" s="651"/>
-      <c r="C32" s="651"/>
-      <c r="D32" s="651"/>
-      <c r="E32" s="680"/>
-      <c r="F32" s="715"/>
+      <c r="B32" s="654"/>
+      <c r="C32" s="654"/>
+      <c r="D32" s="654"/>
+      <c r="E32" s="679"/>
+      <c r="F32" s="711"/>
       <c r="G32" s="87" t="s">
         <v>100</v>
       </c>
@@ -5140,7 +5139,7 @@
       </c>
       <c r="L32" s="86" t="str">
         <f t="shared" si="0"/>
-        <v>http://vocab.fairdatacollective.org/dataset/properties/creatorAffiliationIdentifier</v>
+        <v>https://vocab.fairdatacollective.org/gdmt/property/creatorAffiliationIdentifier</v>
       </c>
       <c r="M32" s="84" t="s">
         <v>28</v>
@@ -5151,11 +5150,11 @@
     </row>
     <row r="33" spans="1:16" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="17"/>
-      <c r="B33" s="651"/>
-      <c r="C33" s="651"/>
-      <c r="D33" s="651"/>
-      <c r="E33" s="680"/>
-      <c r="F33" s="715"/>
+      <c r="B33" s="654"/>
+      <c r="C33" s="654"/>
+      <c r="D33" s="654"/>
+      <c r="E33" s="679"/>
+      <c r="F33" s="711"/>
       <c r="G33" s="87" t="s">
         <v>103</v>
       </c>
@@ -5173,10 +5172,10 @@
       </c>
       <c r="L33" s="86" t="str">
         <f t="shared" si="0"/>
-        <v>http://vocab.fairdatacollective.org/dataset/properties/creatorAffiliationIdentifierScheme</v>
+        <v>https://vocab.fairdatacollective.org/gdmt/property/creatorAffiliationIdentifierScheme</v>
       </c>
       <c r="M33" s="89" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="N33" s="84" t="s">
         <v>104</v>
@@ -5184,11 +5183,11 @@
     </row>
     <row r="34" spans="1:16" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="17"/>
-      <c r="B34" s="652"/>
-      <c r="C34" s="652"/>
-      <c r="D34" s="652"/>
-      <c r="E34" s="681"/>
-      <c r="F34" s="716"/>
+      <c r="B34" s="655"/>
+      <c r="C34" s="655"/>
+      <c r="D34" s="655"/>
+      <c r="E34" s="680"/>
+      <c r="F34" s="712"/>
       <c r="G34" s="141" t="s">
         <v>105</v>
       </c>
@@ -5206,10 +5205,10 @@
       </c>
       <c r="L34" s="144" t="str">
         <f t="shared" si="0"/>
-        <v>http://vocab.fairdatacollective.org/dataset/properties/creatorAffiliationIdentifierSchemeIRI</v>
+        <v>https://vocab.fairdatacollective.org/gdmt/property/creatorAffiliationIdentifierSchemeIRI</v>
       </c>
       <c r="M34" s="148" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="N34" s="145" t="s">
         <v>106</v>
@@ -5271,7 +5270,7 @@
       </c>
       <c r="L36" s="86" t="str">
         <f>Namespace &amp; $G36</f>
-        <v>http://vocab.fairdatacollective.org/dataset/properties/creatorRole</v>
+        <v>https://vocab.fairdatacollective.org/gdmt/property/creatorRole</v>
       </c>
       <c r="M36" s="89" t="s">
         <v>24</v>
@@ -5304,7 +5303,7 @@
       </c>
       <c r="L37" s="180" t="str">
         <f>Namespace &amp; $G37</f>
-        <v>http://vocab.fairdatacollective.org/dataset/properties/creatorType</v>
+        <v>https://vocab.fairdatacollective.org/gdmt/property/creatorType</v>
       </c>
       <c r="M37" s="181" t="s">
         <v>24</v>
@@ -5314,11 +5313,11 @@
       </c>
     </row>
     <row r="38" spans="1:16" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="653" t="s">
+      <c r="A38" s="656" t="s">
         <v>107</v>
       </c>
-      <c r="B38" s="653"/>
-      <c r="C38" s="653"/>
+      <c r="B38" s="656"/>
+      <c r="C38" s="656"/>
       <c r="D38" s="382" t="s">
         <v>462</v>
       </c>
@@ -5326,8 +5325,8 @@
         <v>34</v>
       </c>
       <c r="F38" s="384" t="str">
-        <f>Namespace &amp; ($A38)</f>
-        <v>http://vocab.fairdatacollective.org/dataset/properties/Contributor</v>
+        <f>Namespace &amp; ($A38) &amp; "Info"</f>
+        <v>https://vocab.fairdatacollective.org/gdmt/property/ContributorInfo</v>
       </c>
       <c r="G38" s="385"/>
       <c r="H38" s="385"/>
@@ -5340,19 +5339,19 @@
     </row>
     <row r="39" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="424"/>
-      <c r="B39" s="654" t="s">
+      <c r="B39" s="657" t="s">
         <v>463</v>
       </c>
-      <c r="C39" s="654"/>
-      <c r="D39" s="670" t="s">
+      <c r="C39" s="657"/>
+      <c r="D39" s="669" t="s">
         <v>479</v>
       </c>
-      <c r="E39" s="585" t="s">
+      <c r="E39" s="582" t="s">
         <v>34</v>
       </c>
-      <c r="F39" s="676" t="str">
-        <f>Namespace &amp; ($B39)</f>
-        <v>http://vocab.fairdatacollective.org/dataset/properties/ContributorName</v>
+      <c r="F39" s="675" t="str">
+        <f>Namespace &amp; ($B39) &amp; "Info"</f>
+        <v>https://vocab.fairdatacollective.org/gdmt/property/ContributorNameInfo</v>
       </c>
       <c r="G39" s="390" t="s">
         <v>115</v>
@@ -5381,11 +5380,11 @@
     </row>
     <row r="40" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="424"/>
-      <c r="B40" s="654"/>
-      <c r="C40" s="654"/>
-      <c r="D40" s="671"/>
-      <c r="E40" s="586"/>
-      <c r="F40" s="677"/>
+      <c r="B40" s="657"/>
+      <c r="C40" s="657"/>
+      <c r="D40" s="670"/>
+      <c r="E40" s="583"/>
+      <c r="F40" s="676"/>
       <c r="G40" s="394" t="s">
         <v>111</v>
       </c>
@@ -5413,11 +5412,11 @@
     </row>
     <row r="41" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="424"/>
-      <c r="B41" s="654"/>
-      <c r="C41" s="654"/>
-      <c r="D41" s="672"/>
-      <c r="E41" s="587"/>
-      <c r="F41" s="678"/>
+      <c r="B41" s="657"/>
+      <c r="C41" s="657"/>
+      <c r="D41" s="671"/>
+      <c r="E41" s="584"/>
+      <c r="F41" s="677"/>
       <c r="G41" s="399" t="s">
         <v>113</v>
       </c>
@@ -5445,19 +5444,19 @@
     </row>
     <row r="42" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" s="424"/>
-      <c r="B42" s="654" t="s">
+      <c r="B42" s="657" t="s">
         <v>466</v>
       </c>
-      <c r="C42" s="654"/>
-      <c r="D42" s="670" t="s">
+      <c r="C42" s="657"/>
+      <c r="D42" s="669" t="s">
         <v>480</v>
       </c>
-      <c r="E42" s="585" t="s">
+      <c r="E42" s="582" t="s">
         <v>34</v>
       </c>
-      <c r="F42" s="676" t="str">
-        <f>Namespace &amp; ($B42)</f>
-        <v>http://vocab.fairdatacollective.org/dataset/properties/ContributorIdentifier</v>
+      <c r="F42" s="675" t="str">
+        <f>Namespace &amp; ($B42) &amp; "Info"</f>
+        <v>https://vocab.fairdatacollective.org/gdmt/property/ContributorIdentifierInfo</v>
       </c>
       <c r="G42" s="404" t="s">
         <v>120</v>
@@ -5476,7 +5475,7 @@
       </c>
       <c r="L42" s="393" t="str">
         <f t="shared" ref="L42:L48" si="1">Namespace &amp; $G42</f>
-        <v>http://vocab.fairdatacollective.org/dataset/properties/contributorIdentifier</v>
+        <v>https://vocab.fairdatacollective.org/gdmt/property/contributorIdentifier</v>
       </c>
       <c r="M42" s="390" t="s">
         <v>28</v>
@@ -5487,11 +5486,11 @@
     </row>
     <row r="43" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="424"/>
-      <c r="B43" s="654"/>
-      <c r="C43" s="654"/>
-      <c r="D43" s="671"/>
-      <c r="E43" s="586"/>
-      <c r="F43" s="677"/>
+      <c r="B43" s="657"/>
+      <c r="C43" s="657"/>
+      <c r="D43" s="670"/>
+      <c r="E43" s="583"/>
+      <c r="F43" s="676"/>
       <c r="G43" s="394" t="s">
         <v>121</v>
       </c>
@@ -5509,10 +5508,10 @@
       </c>
       <c r="L43" s="397" t="str">
         <f t="shared" si="1"/>
-        <v>http://vocab.fairdatacollective.org/dataset/properties/contributorIdentifierScheme</v>
+        <v>https://vocab.fairdatacollective.org/gdmt/property/contributorIdentifierScheme</v>
       </c>
       <c r="M43" s="406" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="N43" s="398" t="s">
         <v>94</v>
@@ -5520,11 +5519,11 @@
     </row>
     <row r="44" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="424"/>
-      <c r="B44" s="654"/>
-      <c r="C44" s="654"/>
-      <c r="D44" s="672"/>
-      <c r="E44" s="587"/>
-      <c r="F44" s="678"/>
+      <c r="B44" s="657"/>
+      <c r="C44" s="657"/>
+      <c r="D44" s="671"/>
+      <c r="E44" s="584"/>
+      <c r="F44" s="677"/>
       <c r="G44" s="399" t="s">
         <v>122</v>
       </c>
@@ -5542,10 +5541,10 @@
       </c>
       <c r="L44" s="402" t="str">
         <f t="shared" si="1"/>
-        <v>http://vocab.fairdatacollective.org/dataset/properties/contributorIdentifierSchemeIRI</v>
+        <v>https://vocab.fairdatacollective.org/gdmt/property/contributorIdentifierSchemeIRI</v>
       </c>
       <c r="M44" s="407" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="N44" s="403" t="s">
         <v>96</v>
@@ -5553,19 +5552,19 @@
     </row>
     <row r="45" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="424"/>
-      <c r="B45" s="654" t="s">
+      <c r="B45" s="657" t="s">
         <v>467</v>
       </c>
-      <c r="C45" s="654"/>
-      <c r="D45" s="670" t="s">
+      <c r="C45" s="657"/>
+      <c r="D45" s="669" t="s">
         <v>481</v>
       </c>
-      <c r="E45" s="585" t="s">
+      <c r="E45" s="582" t="s">
         <v>34</v>
       </c>
-      <c r="F45" s="673" t="str">
-        <f>Namespace &amp; ($B45)</f>
-        <v>http://vocab.fairdatacollective.org/dataset/properties/ContributorAffiliation</v>
+      <c r="F45" s="672" t="str">
+        <f>Namespace &amp; ($B45) &amp; "Info"</f>
+        <v>https://vocab.fairdatacollective.org/gdmt/property/ContributorAffiliationInfo</v>
       </c>
       <c r="G45" s="404" t="s">
         <v>331</v>
@@ -5584,7 +5583,7 @@
       </c>
       <c r="L45" s="393" t="str">
         <f t="shared" si="1"/>
-        <v>http://vocab.fairdatacollective.org/dataset/properties/contributorAffiliation</v>
+        <v>https://vocab.fairdatacollective.org/gdmt/property/contributorAffiliation</v>
       </c>
       <c r="M45" s="390" t="s">
         <v>28</v>
@@ -5595,11 +5594,11 @@
     </row>
     <row r="46" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="424"/>
-      <c r="B46" s="654"/>
-      <c r="C46" s="654"/>
-      <c r="D46" s="671"/>
-      <c r="E46" s="586"/>
-      <c r="F46" s="674"/>
+      <c r="B46" s="657"/>
+      <c r="C46" s="657"/>
+      <c r="D46" s="670"/>
+      <c r="E46" s="583"/>
+      <c r="F46" s="673"/>
       <c r="G46" s="394" t="s">
         <v>123</v>
       </c>
@@ -5617,7 +5616,7 @@
       </c>
       <c r="L46" s="397" t="str">
         <f t="shared" si="1"/>
-        <v>http://vocab.fairdatacollective.org/dataset/properties/contributorAffiliationIdentifier</v>
+        <v>https://vocab.fairdatacollective.org/gdmt/property/contributorAffiliationIdentifier</v>
       </c>
       <c r="M46" s="398" t="s">
         <v>28</v>
@@ -5628,11 +5627,11 @@
     </row>
     <row r="47" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="424"/>
-      <c r="B47" s="654"/>
-      <c r="C47" s="654"/>
-      <c r="D47" s="671"/>
-      <c r="E47" s="586"/>
-      <c r="F47" s="674"/>
+      <c r="B47" s="657"/>
+      <c r="C47" s="657"/>
+      <c r="D47" s="670"/>
+      <c r="E47" s="583"/>
+      <c r="F47" s="673"/>
       <c r="G47" s="394" t="s">
         <v>460</v>
       </c>
@@ -5650,10 +5649,10 @@
       </c>
       <c r="L47" s="397" t="str">
         <f t="shared" si="1"/>
-        <v>http://vocab.fairdatacollective.org/dataset/properties/contributorAffiliationIdentifierScheme</v>
+        <v>https://vocab.fairdatacollective.org/gdmt/property/contributorAffiliationIdentifierScheme</v>
       </c>
       <c r="M47" s="406" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="N47" s="398" t="s">
         <v>104</v>
@@ -5661,11 +5660,11 @@
     </row>
     <row r="48" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="424"/>
-      <c r="B48" s="654"/>
-      <c r="C48" s="654"/>
-      <c r="D48" s="672"/>
-      <c r="E48" s="587"/>
-      <c r="F48" s="675"/>
+      <c r="B48" s="657"/>
+      <c r="C48" s="657"/>
+      <c r="D48" s="671"/>
+      <c r="E48" s="584"/>
+      <c r="F48" s="674"/>
       <c r="G48" s="399" t="s">
         <v>125</v>
       </c>
@@ -5683,10 +5682,10 @@
       </c>
       <c r="L48" s="402" t="str">
         <f t="shared" si="1"/>
-        <v>http://vocab.fairdatacollective.org/dataset/properties/contributorAffiliationIdentifierSchemeIRI</v>
+        <v>https://vocab.fairdatacollective.org/gdmt/property/contributorAffiliationIdentifierSchemeIRI</v>
       </c>
       <c r="M48" s="407" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="N48" s="403" t="s">
         <v>106</v>
@@ -5752,7 +5751,7 @@
       </c>
       <c r="L50" s="397" t="str">
         <f>Namespace &amp; $G50</f>
-        <v>http://vocab.fairdatacollective.org/dataset/properties/contributorRole</v>
+        <v>https://vocab.fairdatacollective.org/gdmt/property/contributorRole</v>
       </c>
       <c r="M50" s="406" t="s">
         <v>24</v>
@@ -5785,7 +5784,7 @@
       </c>
       <c r="L51" s="421" t="str">
         <f>Namespace &amp; $G51</f>
-        <v>http://vocab.fairdatacollective.org/dataset/properties/contributorType</v>
+        <v>https://vocab.fairdatacollective.org/gdmt/property/contributorType</v>
       </c>
       <c r="M51" s="422" t="s">
         <v>24</v>
@@ -5795,11 +5794,11 @@
       </c>
     </row>
     <row r="52" spans="1:16" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="655" t="s">
+      <c r="A52" s="658" t="s">
         <v>126</v>
       </c>
-      <c r="B52" s="655"/>
-      <c r="C52" s="655"/>
+      <c r="B52" s="658"/>
+      <c r="C52" s="658"/>
       <c r="D52" s="248" t="s">
         <v>437</v>
       </c>
@@ -5807,8 +5806,8 @@
         <v>1</v>
       </c>
       <c r="F52" s="248" t="str">
-        <f>Namespace &amp; ($A52)</f>
-        <v>http://vocab.fairdatacollective.org/dataset/properties/Publisher</v>
+        <f>Namespace &amp; ($A52) &amp; "Info"</f>
+        <v>https://vocab.fairdatacollective.org/gdmt/property/PublisherInfo</v>
       </c>
       <c r="G52" s="93"/>
       <c r="H52" s="93"/>
@@ -5821,19 +5820,19 @@
     </row>
     <row r="53" spans="1:16" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="426"/>
-      <c r="B53" s="646" t="s">
+      <c r="B53" s="633" t="s">
         <v>474</v>
       </c>
-      <c r="C53" s="646"/>
-      <c r="D53" s="646" t="s">
+      <c r="C53" s="633"/>
+      <c r="D53" s="633" t="s">
         <v>475</v>
       </c>
-      <c r="E53" s="643" t="s">
+      <c r="E53" s="690" t="s">
         <v>54</v>
       </c>
-      <c r="F53" s="640" t="str">
-        <f>Namespace &amp; ($B53)</f>
-        <v>http://vocab.fairdatacollective.org/dataset/properties/PublisherIdentifier</v>
+      <c r="F53" s="687" t="str">
+        <f>Namespace &amp; ($B53) &amp; "Info"</f>
+        <v>https://vocab.fairdatacollective.org/gdmt/property/PublisherIdentifierInfo</v>
       </c>
       <c r="G53" s="252" t="s">
         <v>134</v>
@@ -5852,7 +5851,7 @@
       </c>
       <c r="L53" s="255" t="str">
         <f>Namespace &amp; $G53</f>
-        <v>http://vocab.fairdatacollective.org/dataset/properties/publisherIdentifier</v>
+        <v>https://vocab.fairdatacollective.org/gdmt/property/publisherIdentifier</v>
       </c>
       <c r="M53" s="256" t="s">
         <v>28</v>
@@ -5863,11 +5862,11 @@
     </row>
     <row r="54" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="426"/>
-      <c r="B54" s="647"/>
-      <c r="C54" s="647"/>
-      <c r="D54" s="647"/>
-      <c r="E54" s="644"/>
-      <c r="F54" s="641"/>
+      <c r="B54" s="634"/>
+      <c r="C54" s="634"/>
+      <c r="D54" s="634"/>
+      <c r="E54" s="691"/>
+      <c r="F54" s="688"/>
       <c r="G54" s="93" t="s">
         <v>136</v>
       </c>
@@ -5885,7 +5884,7 @@
       </c>
       <c r="L54" s="96" t="str">
         <f>Namespace &amp; $G54</f>
-        <v>http://vocab.fairdatacollective.org/dataset/properties/publisherIdentifierScheme</v>
+        <v>https://vocab.fairdatacollective.org/gdmt/property/publisherIdentifierScheme</v>
       </c>
       <c r="M54" s="97" t="s">
         <v>24</v>
@@ -5896,11 +5895,11 @@
     </row>
     <row r="55" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="426"/>
-      <c r="B55" s="648"/>
-      <c r="C55" s="648"/>
-      <c r="D55" s="648"/>
-      <c r="E55" s="645"/>
-      <c r="F55" s="642"/>
+      <c r="B55" s="635"/>
+      <c r="C55" s="635"/>
+      <c r="D55" s="635"/>
+      <c r="E55" s="692"/>
+      <c r="F55" s="689"/>
       <c r="G55" s="257" t="s">
         <v>137</v>
       </c>
@@ -5918,7 +5917,7 @@
       </c>
       <c r="L55" s="260" t="str">
         <f>Namespace &amp; $G55</f>
-        <v>http://vocab.fairdatacollective.org/dataset/properties/publisherIdentifierSchemeIRI</v>
+        <v>https://vocab.fairdatacollective.org/gdmt/property/publisherIdentifierSchemeIRI</v>
       </c>
       <c r="M55" s="261" t="s">
         <v>24</v>
@@ -6015,7 +6014,7 @@
       </c>
       <c r="L58" s="267" t="str">
         <f>Namespace &amp; $G58</f>
-        <v>http://vocab.fairdatacollective.org/dataset/properties/publisherAddress</v>
+        <v>https://vocab.fairdatacollective.org/gdmt/property/publisherAddress</v>
       </c>
       <c r="M58" s="268" t="s">
         <v>28</v>
@@ -6027,11 +6026,11 @@
       <c r="P58" s="10"/>
     </row>
     <row r="59" spans="1:16" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="605" t="s">
+      <c r="A59" s="648" t="s">
         <v>138</v>
       </c>
-      <c r="B59" s="605"/>
-      <c r="C59" s="605"/>
+      <c r="B59" s="648"/>
+      <c r="C59" s="648"/>
       <c r="D59" s="296" t="s">
         <v>139</v>
       </c>
@@ -6039,8 +6038,8 @@
         <v>1</v>
       </c>
       <c r="F59" s="298" t="str">
-        <f>Namespace &amp; ($A59)</f>
-        <v>http://vocab.fairdatacollective.org/dataset/properties/Rights</v>
+        <f>Namespace &amp; ($A59) &amp; "Info"</f>
+        <v>https://vocab.fairdatacollective.org/gdmt/property/RightsInfo</v>
       </c>
       <c r="G59" s="278"/>
       <c r="H59" s="278"/>
@@ -6075,7 +6074,7 @@
       </c>
       <c r="L60" s="101" t="str">
         <f>Namespace &amp; $G60</f>
-        <v>http://vocab.fairdatacollective.org/dataset/properties/licenseName</v>
+        <v>https://vocab.fairdatacollective.org/gdmt/property/licenseName</v>
       </c>
       <c r="M60" s="102" t="s">
         <v>142</v>
@@ -6096,9 +6095,9 @@
       <c r="E61" s="552" t="s">
         <v>46</v>
       </c>
-      <c r="F61" s="656" t="str">
-        <f>Namespace &amp; ($B61)</f>
-        <v>http://vocab.fairdatacollective.org/dataset/properties/LicenseIdentifier</v>
+      <c r="F61" s="731" t="str">
+        <f>Namespace &amp; ($B61) &amp; "Info"</f>
+        <v>https://vocab.fairdatacollective.org/gdmt/property/LicenseIdentifierInfo</v>
       </c>
       <c r="G61" s="284" t="s">
         <v>145</v>
@@ -6117,7 +6116,7 @@
       </c>
       <c r="L61" s="287" t="str">
         <f>Namespace &amp; $G61</f>
-        <v>http://vocab.fairdatacollective.org/dataset/properties/licenseIdentifier</v>
+        <v>https://vocab.fairdatacollective.org/gdmt/property/licenseIdentifier</v>
       </c>
       <c r="M61" s="288" t="s">
         <v>142</v>
@@ -6134,7 +6133,7 @@
       <c r="C62" s="550"/>
       <c r="D62" s="550"/>
       <c r="E62" s="553"/>
-      <c r="F62" s="657"/>
+      <c r="F62" s="732"/>
       <c r="G62" s="98" t="s">
         <v>148</v>
       </c>
@@ -6152,7 +6151,7 @@
       </c>
       <c r="L62" s="101" t="str">
         <f>Namespace &amp; $G62</f>
-        <v>http://vocab.fairdatacollective.org/dataset/properties/licenseIdentifierScheme</v>
+        <v>https://vocab.fairdatacollective.org/gdmt/property/licenseIdentifierScheme</v>
       </c>
       <c r="M62" s="102" t="s">
         <v>142</v>
@@ -6163,11 +6162,11 @@
     </row>
     <row r="63" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="428"/>
-      <c r="B63" s="606"/>
-      <c r="C63" s="606"/>
-      <c r="D63" s="606"/>
-      <c r="E63" s="659"/>
-      <c r="F63" s="658"/>
+      <c r="B63" s="649"/>
+      <c r="C63" s="649"/>
+      <c r="D63" s="649"/>
+      <c r="E63" s="734"/>
+      <c r="F63" s="733"/>
       <c r="G63" s="290" t="s">
         <v>149</v>
       </c>
@@ -6185,7 +6184,7 @@
       </c>
       <c r="L63" s="293" t="str">
         <f>Namespace &amp; $G63</f>
-        <v>http://vocab.fairdatacollective.org/dataset/properties/licenseIdentifierSchemeIRI</v>
+        <v>https://vocab.fairdatacollective.org/gdmt/property/licenseIdentifierSchemeIRI</v>
       </c>
       <c r="M63" s="294" t="s">
         <v>142</v>
@@ -6225,20 +6224,20 @@
       <c r="N64" s="277"/>
     </row>
     <row r="65" spans="1:14" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="607" t="s">
+      <c r="A65" s="650" t="s">
         <v>151</v>
       </c>
-      <c r="B65" s="607"/>
-      <c r="C65" s="607"/>
-      <c r="D65" s="636" t="s">
+      <c r="B65" s="650"/>
+      <c r="C65" s="650"/>
+      <c r="D65" s="638" t="s">
         <v>519</v>
       </c>
-      <c r="E65" s="638" t="s">
+      <c r="E65" s="640" t="s">
         <v>54</v>
       </c>
-      <c r="F65" s="636" t="str">
-        <f>Namespace &amp; ($A65)</f>
-        <v>http://vocab.fairdatacollective.org/dataset/properties/Date</v>
+      <c r="F65" s="638" t="str">
+        <f>Namespace &amp; ($A65) &amp; "Info"</f>
+        <v>https://vocab.fairdatacollective.org/gdmt/property/DateInfo</v>
       </c>
       <c r="G65" s="304" t="s">
         <v>152</v>
@@ -6255,18 +6254,18 @@
       <c r="K65" s="307"/>
       <c r="L65" s="307" t="str">
         <f t="shared" ref="L65:L69" si="2">Namespace &amp; $G65</f>
-        <v>http://vocab.fairdatacollective.org/dataset/properties/datasetDate</v>
+        <v>https://vocab.fairdatacollective.org/gdmt/property/datasetDate</v>
       </c>
       <c r="M65" s="308"/>
       <c r="N65" s="308"/>
     </row>
     <row r="66" spans="1:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="607"/>
-      <c r="B66" s="607"/>
-      <c r="C66" s="607"/>
-      <c r="D66" s="637"/>
-      <c r="E66" s="639"/>
-      <c r="F66" s="637"/>
+      <c r="A66" s="650"/>
+      <c r="B66" s="650"/>
+      <c r="C66" s="650"/>
+      <c r="D66" s="639"/>
+      <c r="E66" s="641"/>
+      <c r="F66" s="639"/>
       <c r="G66" s="105" t="s">
         <v>486</v>
       </c>
@@ -6282,7 +6281,7 @@
       <c r="K66" s="108"/>
       <c r="L66" s="108" t="str">
         <f t="shared" si="2"/>
-        <v>http://vocab.fairdatacollective.org/dataset/properties/datasetDateType</v>
+        <v>https://vocab.fairdatacollective.org/gdmt/property/datasetDateType</v>
       </c>
       <c r="M66" s="109" t="s">
         <v>24</v>
@@ -6292,20 +6291,20 @@
       </c>
     </row>
     <row r="67" spans="1:14" s="14" customFormat="1" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="608" t="s">
+      <c r="A67" s="651" t="s">
         <v>154</v>
       </c>
-      <c r="B67" s="608"/>
-      <c r="C67" s="608"/>
-      <c r="D67" s="660" t="s">
+      <c r="B67" s="651"/>
+      <c r="C67" s="651"/>
+      <c r="D67" s="659" t="s">
         <v>159</v>
       </c>
       <c r="E67" s="365" t="s">
         <v>34</v>
       </c>
       <c r="F67" s="366" t="str">
-        <f>Namespace &amp; ($A67)</f>
-        <v>http://vocab.fairdatacollective.org/dataset/properties/Distribution</v>
+        <f>Namespace &amp; ($A67) &amp; "Info"</f>
+        <v>https://vocab.fairdatacollective.org/gdmt/property/DistributionInfo</v>
       </c>
       <c r="G67" s="367"/>
       <c r="H67" s="367"/>
@@ -6318,9 +6317,9 @@
     </row>
     <row r="68" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="372"/>
-      <c r="B68" s="634"/>
-      <c r="C68" s="634"/>
-      <c r="D68" s="661"/>
+      <c r="B68" s="636"/>
+      <c r="C68" s="636"/>
+      <c r="D68" s="660"/>
       <c r="E68" s="316"/>
       <c r="F68" s="317"/>
       <c r="G68" s="318" t="s">
@@ -6340,7 +6339,7 @@
       </c>
       <c r="L68" s="321" t="str">
         <f t="shared" si="2"/>
-        <v>http://vocab.fairdatacollective.org/dataset/properties/distributionIdentifier</v>
+        <v>https://vocab.fairdatacollective.org/gdmt/property/distributionIdentifier</v>
       </c>
       <c r="M68" s="318" t="s">
         <v>24</v>
@@ -6353,7 +6352,7 @@
       <c r="A69" s="372"/>
       <c r="B69" s="373"/>
       <c r="C69" s="322"/>
-      <c r="D69" s="661"/>
+      <c r="D69" s="660"/>
       <c r="E69" s="324"/>
       <c r="F69" s="317"/>
       <c r="G69" s="318" t="s">
@@ -6373,7 +6372,7 @@
       </c>
       <c r="L69" s="321" t="str">
         <f t="shared" si="2"/>
-        <v>http://vocab.fairdatacollective.org/dataset/properties/distributionIdentifierType</v>
+        <v>https://vocab.fairdatacollective.org/gdmt/property/distributionIdentifierType</v>
       </c>
       <c r="M69" s="318" t="s">
         <v>24</v>
@@ -6386,7 +6385,7 @@
       <c r="A70" s="372"/>
       <c r="B70" s="373"/>
       <c r="C70" s="322"/>
-      <c r="D70" s="661"/>
+      <c r="D70" s="660"/>
       <c r="E70" s="325"/>
       <c r="F70" s="317"/>
       <c r="G70" s="310" t="s">
@@ -6418,7 +6417,7 @@
       <c r="A71" s="372"/>
       <c r="B71" s="373"/>
       <c r="C71" s="322"/>
-      <c r="D71" s="661"/>
+      <c r="D71" s="660"/>
       <c r="E71" s="325"/>
       <c r="F71" s="317"/>
       <c r="G71" s="310" t="s">
@@ -6438,10 +6437,10 @@
       </c>
       <c r="L71" s="313" t="str">
         <f t="shared" ref="L71:L76" si="3">Namespace &amp; $G71</f>
-        <v>http://vocab.fairdatacollective.org/dataset/properties/distributionMediaType</v>
+        <v>https://vocab.fairdatacollective.org/gdmt/property/distributionMediaType</v>
       </c>
       <c r="M71" s="314" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="N71" s="314" t="s">
         <v>28</v>
@@ -6451,7 +6450,7 @@
       <c r="A72" s="372"/>
       <c r="B72" s="373"/>
       <c r="C72" s="322"/>
-      <c r="D72" s="662"/>
+      <c r="D72" s="661"/>
       <c r="E72" s="324"/>
       <c r="F72" s="317"/>
       <c r="G72" s="310" t="s">
@@ -6471,7 +6470,7 @@
       </c>
       <c r="L72" s="313" t="str">
         <f t="shared" si="3"/>
-        <v>http://vocab.fairdatacollective.org/dataset/properties/distributionSize</v>
+        <v>https://vocab.fairdatacollective.org/gdmt/property/distributionSize</v>
       </c>
       <c r="M72" s="314" t="s">
         <v>28</v>
@@ -6482,17 +6481,17 @@
     </row>
     <row r="73" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="372"/>
-      <c r="B73" s="622" t="s">
+      <c r="B73" s="621" t="s">
         <v>490</v>
       </c>
-      <c r="C73" s="622"/>
-      <c r="D73" s="691" t="s">
+      <c r="C73" s="621"/>
+      <c r="D73" s="645" t="s">
         <v>491</v>
       </c>
-      <c r="E73" s="625">
+      <c r="E73" s="624">
         <v>1</v>
       </c>
-      <c r="F73" s="688"/>
+      <c r="F73" s="642"/>
       <c r="G73" s="326" t="s">
         <v>163</v>
       </c>
@@ -6510,7 +6509,7 @@
       </c>
       <c r="L73" s="329" t="str">
         <f t="shared" si="3"/>
-        <v>http://vocab.fairdatacollective.org/dataset/properties/distributionAccessProtocol</v>
+        <v>https://vocab.fairdatacollective.org/gdmt/property/distributionAccessProtocol</v>
       </c>
       <c r="M73" s="330" t="s">
         <v>194</v>
@@ -6521,11 +6520,11 @@
     </row>
     <row r="74" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="372"/>
-      <c r="B74" s="623"/>
-      <c r="C74" s="623"/>
-      <c r="D74" s="692"/>
-      <c r="E74" s="626"/>
-      <c r="F74" s="689"/>
+      <c r="B74" s="622"/>
+      <c r="C74" s="622"/>
+      <c r="D74" s="646"/>
+      <c r="E74" s="625"/>
+      <c r="F74" s="643"/>
       <c r="G74" s="310" t="s">
         <v>164</v>
       </c>
@@ -6543,7 +6542,7 @@
       </c>
       <c r="L74" s="313" t="str">
         <f t="shared" si="3"/>
-        <v>http://vocab.fairdatacollective.org/dataset/properties/distributionAccessConfiguration</v>
+        <v>https://vocab.fairdatacollective.org/gdmt/property/distributionAccessConfiguration</v>
       </c>
       <c r="M74" s="314" t="s">
         <v>28</v>
@@ -6554,11 +6553,11 @@
     </row>
     <row r="75" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="372"/>
-      <c r="B75" s="624"/>
-      <c r="C75" s="624"/>
-      <c r="D75" s="693"/>
-      <c r="E75" s="627"/>
-      <c r="F75" s="690"/>
+      <c r="B75" s="623"/>
+      <c r="C75" s="623"/>
+      <c r="D75" s="647"/>
+      <c r="E75" s="626"/>
+      <c r="F75" s="644"/>
       <c r="G75" s="331" t="s">
         <v>449</v>
       </c>
@@ -6576,7 +6575,7 @@
       </c>
       <c r="L75" s="334" t="str">
         <f t="shared" si="3"/>
-        <v>http://vocab.fairdatacollective.org/dataset/properties/distributionQueryStatement</v>
+        <v>https://vocab.fairdatacollective.org/gdmt/property/distributionQueryStatement</v>
       </c>
       <c r="M75" s="335" t="s">
         <v>28</v>
@@ -6609,17 +6608,17 @@
       </c>
       <c r="L76" s="313" t="str">
         <f t="shared" si="3"/>
-        <v>http://vocab.fairdatacollective.org/dataset/properties/distributionDate</v>
+        <v>https://vocab.fairdatacollective.org/gdmt/property/distributionDate</v>
       </c>
       <c r="M76" s="314"/>
       <c r="N76" s="314"/>
     </row>
     <row r="77" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="372"/>
-      <c r="B77" s="635" t="s">
+      <c r="B77" s="637" t="s">
         <v>492</v>
       </c>
-      <c r="C77" s="635"/>
+      <c r="C77" s="637"/>
       <c r="D77" s="358" t="s">
         <v>493</v>
       </c>
@@ -6627,8 +6626,8 @@
         <v>54</v>
       </c>
       <c r="F77" s="360" t="str">
-        <f>Namespace &amp; ($B77)</f>
-        <v>http://vocab.fairdatacollective.org/dataset/properties/Distributor</v>
+        <f>Namespace &amp; ($B77) &amp; "Info"</f>
+        <v>https://vocab.fairdatacollective.org/gdmt/property/DistributorInfo</v>
       </c>
       <c r="G77" s="361"/>
       <c r="H77" s="361"/>
@@ -6641,19 +6640,19 @@
     </row>
     <row r="78" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="372"/>
-      <c r="B78" s="621"/>
-      <c r="C78" s="622" t="s">
+      <c r="B78" s="620"/>
+      <c r="C78" s="621" t="s">
         <v>494</v>
       </c>
-      <c r="D78" s="622" t="s">
+      <c r="D78" s="621" t="s">
         <v>495</v>
       </c>
-      <c r="E78" s="625">
+      <c r="E78" s="624">
         <v>1</v>
       </c>
-      <c r="F78" s="631" t="str">
-        <f>Namespace &amp; ($C78)</f>
-        <v>http://vocab.fairdatacollective.org/dataset/properties/DistributorName</v>
+      <c r="F78" s="630" t="str">
+        <f>Namespace &amp; ($C78) &amp; "Info"</f>
+        <v>https://vocab.fairdatacollective.org/gdmt/property/DistributorNameInfo</v>
       </c>
       <c r="G78" s="336" t="s">
         <v>174</v>
@@ -6682,11 +6681,11 @@
     </row>
     <row r="79" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="372"/>
-      <c r="B79" s="621"/>
-      <c r="C79" s="623"/>
-      <c r="D79" s="623"/>
-      <c r="E79" s="626"/>
-      <c r="F79" s="632"/>
+      <c r="B79" s="620"/>
+      <c r="C79" s="622"/>
+      <c r="D79" s="622"/>
+      <c r="E79" s="625"/>
+      <c r="F79" s="631"/>
       <c r="G79" s="354" t="s">
         <v>170</v>
       </c>
@@ -6714,11 +6713,11 @@
     </row>
     <row r="80" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="372"/>
-      <c r="B80" s="621"/>
-      <c r="C80" s="624"/>
-      <c r="D80" s="624"/>
-      <c r="E80" s="627"/>
-      <c r="F80" s="633"/>
+      <c r="B80" s="620"/>
+      <c r="C80" s="623"/>
+      <c r="D80" s="623"/>
+      <c r="E80" s="626"/>
+      <c r="F80" s="632"/>
       <c r="G80" s="340" t="s">
         <v>172</v>
       </c>
@@ -6746,19 +6745,19 @@
     </row>
     <row r="81" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="372"/>
-      <c r="B81" s="621"/>
-      <c r="C81" s="622" t="s">
+      <c r="B81" s="620"/>
+      <c r="C81" s="621" t="s">
         <v>497</v>
       </c>
-      <c r="D81" s="622" t="s">
+      <c r="D81" s="621" t="s">
         <v>498</v>
       </c>
-      <c r="E81" s="625">
+      <c r="E81" s="624">
         <v>1</v>
       </c>
-      <c r="F81" s="631" t="str">
-        <f>Namespace &amp; ($C81)</f>
-        <v>http://vocab.fairdatacollective.org/dataset/properties/DistributorIdentifier</v>
+      <c r="F81" s="630" t="str">
+        <f>Namespace &amp; ($C81) &amp; "Info"</f>
+        <v>https://vocab.fairdatacollective.org/gdmt/property/DistributorIdentifierInfo</v>
       </c>
       <c r="G81" s="336" t="s">
         <v>179</v>
@@ -6777,7 +6776,7 @@
       </c>
       <c r="L81" s="339" t="str">
         <f t="shared" ref="L81:L87" si="4">Namespace &amp; $G81</f>
-        <v>http://vocab.fairdatacollective.org/dataset/properties/distributorIdentifier</v>
+        <v>https://vocab.fairdatacollective.org/gdmt/property/distributorIdentifier</v>
       </c>
       <c r="M81" s="336" t="s">
         <v>28</v>
@@ -6788,11 +6787,11 @@
     </row>
     <row r="82" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="372"/>
-      <c r="B82" s="621"/>
-      <c r="C82" s="623"/>
-      <c r="D82" s="623"/>
-      <c r="E82" s="626"/>
-      <c r="F82" s="632"/>
+      <c r="B82" s="620"/>
+      <c r="C82" s="622"/>
+      <c r="D82" s="622"/>
+      <c r="E82" s="625"/>
+      <c r="F82" s="631"/>
       <c r="G82" s="354" t="s">
         <v>181</v>
       </c>
@@ -6810,10 +6809,10 @@
       </c>
       <c r="L82" s="357" t="str">
         <f t="shared" si="4"/>
-        <v>http://vocab.fairdatacollective.org/dataset/properties/distributorIdentifierScheme</v>
+        <v>https://vocab.fairdatacollective.org/gdmt/property/distributorIdentifierScheme</v>
       </c>
       <c r="M82" s="374" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="N82" s="354" t="s">
         <v>94</v>
@@ -6821,11 +6820,11 @@
     </row>
     <row r="83" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="372"/>
-      <c r="B83" s="621"/>
-      <c r="C83" s="624"/>
-      <c r="D83" s="624"/>
-      <c r="E83" s="627"/>
-      <c r="F83" s="633"/>
+      <c r="B83" s="620"/>
+      <c r="C83" s="623"/>
+      <c r="D83" s="623"/>
+      <c r="E83" s="626"/>
+      <c r="F83" s="632"/>
       <c r="G83" s="340" t="s">
         <v>182</v>
       </c>
@@ -6843,10 +6842,10 @@
       </c>
       <c r="L83" s="343" t="str">
         <f t="shared" si="4"/>
-        <v>http://vocab.fairdatacollective.org/dataset/properties/distributorIdentifierSchemeIRI</v>
+        <v>https://vocab.fairdatacollective.org/gdmt/property/distributorIdentifierSchemeIRI</v>
       </c>
       <c r="M83" s="344" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="N83" s="340" t="s">
         <v>96</v>
@@ -6854,19 +6853,19 @@
     </row>
     <row r="84" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="372"/>
-      <c r="B84" s="621"/>
-      <c r="C84" s="622" t="s">
+      <c r="B84" s="620"/>
+      <c r="C84" s="621" t="s">
         <v>499</v>
       </c>
-      <c r="D84" s="622" t="s">
+      <c r="D84" s="621" t="s">
         <v>500</v>
       </c>
-      <c r="E84" s="625" t="s">
+      <c r="E84" s="624" t="s">
         <v>54</v>
       </c>
-      <c r="F84" s="628" t="str">
-        <f>Namespace &amp; ($C84)</f>
-        <v>http://vocab.fairdatacollective.org/dataset/properties/DistributorAffiliation</v>
+      <c r="F84" s="627" t="str">
+        <f>Namespace &amp; ($C84) &amp; "Info"</f>
+        <v>https://vocab.fairdatacollective.org/gdmt/property/DistributorAffiliationInfo</v>
       </c>
       <c r="G84" s="336" t="s">
         <v>183</v>
@@ -6885,7 +6884,7 @@
       </c>
       <c r="L84" s="339" t="str">
         <f t="shared" si="4"/>
-        <v>http://vocab.fairdatacollective.org/dataset/properties/distributorAffiliation</v>
+        <v>https://vocab.fairdatacollective.org/gdmt/property/distributorAffiliation</v>
       </c>
       <c r="M84" s="336" t="s">
         <v>28</v>
@@ -6896,11 +6895,11 @@
     </row>
     <row r="85" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="372"/>
-      <c r="B85" s="621"/>
-      <c r="C85" s="623"/>
-      <c r="D85" s="623"/>
-      <c r="E85" s="626"/>
-      <c r="F85" s="629"/>
+      <c r="B85" s="620"/>
+      <c r="C85" s="622"/>
+      <c r="D85" s="622"/>
+      <c r="E85" s="625"/>
+      <c r="F85" s="628"/>
       <c r="G85" s="354" t="s">
         <v>185</v>
       </c>
@@ -6918,7 +6917,7 @@
       </c>
       <c r="L85" s="357" t="str">
         <f t="shared" si="4"/>
-        <v>http://vocab.fairdatacollective.org/dataset/properties/distributorAffiliationIdentifier</v>
+        <v>https://vocab.fairdatacollective.org/gdmt/property/distributorAffiliationIdentifier</v>
       </c>
       <c r="M85" s="354" t="s">
         <v>28</v>
@@ -6929,11 +6928,11 @@
     </row>
     <row r="86" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="372"/>
-      <c r="B86" s="621"/>
-      <c r="C86" s="623"/>
-      <c r="D86" s="623"/>
-      <c r="E86" s="626"/>
-      <c r="F86" s="629"/>
+      <c r="B86" s="620"/>
+      <c r="C86" s="622"/>
+      <c r="D86" s="622"/>
+      <c r="E86" s="625"/>
+      <c r="F86" s="628"/>
       <c r="G86" s="354" t="s">
         <v>187</v>
       </c>
@@ -6951,10 +6950,10 @@
       </c>
       <c r="L86" s="357" t="str">
         <f t="shared" si="4"/>
-        <v>http://vocab.fairdatacollective.org/dataset/properties/distributorAffiliationIdentifierScheme</v>
+        <v>https://vocab.fairdatacollective.org/gdmt/property/distributorAffiliationIdentifierScheme</v>
       </c>
       <c r="M86" s="374" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="N86" s="354" t="s">
         <v>104</v>
@@ -6962,11 +6961,11 @@
     </row>
     <row r="87" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="372"/>
-      <c r="B87" s="621"/>
-      <c r="C87" s="624"/>
-      <c r="D87" s="624"/>
-      <c r="E87" s="627"/>
-      <c r="F87" s="630"/>
+      <c r="B87" s="620"/>
+      <c r="C87" s="623"/>
+      <c r="D87" s="623"/>
+      <c r="E87" s="626"/>
+      <c r="F87" s="629"/>
       <c r="G87" s="340" t="s">
         <v>188</v>
       </c>
@@ -6984,10 +6983,10 @@
       </c>
       <c r="L87" s="343" t="str">
         <f t="shared" si="4"/>
-        <v>http://vocab.fairdatacollective.org/dataset/properties/distributorAffiliationIdentifierSchemeIRI</v>
+        <v>https://vocab.fairdatacollective.org/gdmt/property/distributorAffiliationIdentifierSchemeIRI</v>
       </c>
       <c r="M87" s="344" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="N87" s="340" t="s">
         <v>106</v>
@@ -7049,10 +7048,10 @@
       </c>
       <c r="L89" s="357" t="str">
         <f>Namespace &amp; $G89</f>
-        <v>http://vocab.fairdatacollective.org/dataset/properties/distributorRole</v>
+        <v>https://vocab.fairdatacollective.org/gdmt/property/distributorRole</v>
       </c>
       <c r="M89" s="374" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="N89" s="354" t="s">
         <v>28</v>
@@ -7082,10 +7081,10 @@
       </c>
       <c r="L90" s="352" t="str">
         <f>Namespace &amp; $G90</f>
-        <v>http://vocab.fairdatacollective.org/dataset/properties/distributorType</v>
+        <v>https://vocab.fairdatacollective.org/gdmt/property/distributorType</v>
       </c>
       <c r="M90" s="353" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="N90" s="349" t="s">
         <v>76</v>
@@ -7094,11 +7093,11 @@
       <c r="P90"/>
     </row>
     <row r="91" spans="1:16" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A91" s="593" t="s">
+      <c r="A91" s="592" t="s">
         <v>189</v>
       </c>
-      <c r="B91" s="593"/>
-      <c r="C91" s="593"/>
+      <c r="B91" s="592"/>
+      <c r="C91" s="592"/>
       <c r="D91" s="430" t="s">
         <v>410</v>
       </c>
@@ -7106,8 +7105,8 @@
         <v>46</v>
       </c>
       <c r="F91" s="432" t="str">
-        <f>Namespace &amp; ($A91)</f>
-        <v>http://vocab.fairdatacollective.org/dataset/properties/Content</v>
+        <f>Namespace &amp; ($A91) &amp; "Info"</f>
+        <v>https://vocab.fairdatacollective.org/gdmt/property/ContentInfo</v>
       </c>
       <c r="G91" s="433"/>
       <c r="H91" s="433"/>
@@ -7120,19 +7119,19 @@
     </row>
     <row r="92" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="426"/>
-      <c r="B92" s="594" t="s">
+      <c r="B92" s="593" t="s">
         <v>283</v>
       </c>
-      <c r="C92" s="594"/>
-      <c r="D92" s="594" t="s">
+      <c r="C92" s="593"/>
+      <c r="D92" s="593" t="s">
         <v>287</v>
       </c>
-      <c r="E92" s="694" t="s">
+      <c r="E92" s="604" t="s">
         <v>54</v>
       </c>
-      <c r="F92" s="698" t="str">
-        <f>Namespace &amp; ($B92)</f>
-        <v>http://vocab.fairdatacollective.org/dataset/properties/DataStream</v>
+      <c r="F92" s="694" t="str">
+        <f>Namespace &amp; ($B92) &amp; "Info"</f>
+        <v>https://vocab.fairdatacollective.org/gdmt/property/DataStreamInfo</v>
       </c>
       <c r="G92" s="443" t="s">
         <v>284</v>
@@ -7151,7 +7150,7 @@
       </c>
       <c r="L92" s="446" t="str">
         <f t="shared" ref="L92:L133" si="5">Namespace &amp; $G92</f>
-        <v>http://vocab.fairdatacollective.org/dataset/properties/dataStream</v>
+        <v>https://vocab.fairdatacollective.org/gdmt/property/dataStream</v>
       </c>
       <c r="M92" s="447" t="s">
         <v>502</v>
@@ -7162,11 +7161,11 @@
     </row>
     <row r="93" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="426"/>
-      <c r="B93" s="595"/>
-      <c r="C93" s="595"/>
-      <c r="D93" s="595"/>
-      <c r="E93" s="695"/>
-      <c r="F93" s="699"/>
+      <c r="B93" s="594"/>
+      <c r="C93" s="594"/>
+      <c r="D93" s="594"/>
+      <c r="E93" s="605"/>
+      <c r="F93" s="695"/>
       <c r="G93" s="110" t="s">
         <v>285</v>
       </c>
@@ -7184,7 +7183,7 @@
       </c>
       <c r="L93" s="113" t="str">
         <f t="shared" si="5"/>
-        <v>http://vocab.fairdatacollective.org/dataset/properties/dataStreamIRI</v>
+        <v>https://vocab.fairdatacollective.org/gdmt/property/dataStreamIRI</v>
       </c>
       <c r="M93" s="114" t="s">
         <v>502</v>
@@ -7195,11 +7194,11 @@
     </row>
     <row r="94" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="426"/>
-      <c r="B94" s="595"/>
-      <c r="C94" s="595"/>
-      <c r="D94" s="595"/>
-      <c r="E94" s="695"/>
-      <c r="F94" s="699"/>
+      <c r="B94" s="594"/>
+      <c r="C94" s="594"/>
+      <c r="D94" s="594"/>
+      <c r="E94" s="605"/>
+      <c r="F94" s="695"/>
       <c r="G94" s="114" t="s">
         <v>191</v>
       </c>
@@ -7217,7 +7216,7 @@
       </c>
       <c r="L94" s="113" t="str">
         <f t="shared" si="5"/>
-        <v>http://vocab.fairdatacollective.org/dataset/properties/datastreamScheme</v>
+        <v>https://vocab.fairdatacollective.org/gdmt/property/datastreamScheme</v>
       </c>
       <c r="M94" s="114" t="s">
         <v>502</v>
@@ -7228,11 +7227,11 @@
     </row>
     <row r="95" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="426"/>
-      <c r="B95" s="596"/>
-      <c r="C95" s="596"/>
-      <c r="D95" s="596"/>
-      <c r="E95" s="696"/>
-      <c r="F95" s="700"/>
+      <c r="B95" s="595"/>
+      <c r="C95" s="595"/>
+      <c r="D95" s="595"/>
+      <c r="E95" s="606"/>
+      <c r="F95" s="696"/>
       <c r="G95" s="448" t="s">
         <v>286</v>
       </c>
@@ -7250,7 +7249,7 @@
       </c>
       <c r="L95" s="450" t="str">
         <f t="shared" si="5"/>
-        <v>http://vocab.fairdatacollective.org/dataset/properties/dataStreamSchemeIRI</v>
+        <v>https://vocab.fairdatacollective.org/gdmt/property/dataStreamSchemeIRI</v>
       </c>
       <c r="M95" s="451" t="s">
         <v>502</v>
@@ -7261,19 +7260,19 @@
     </row>
     <row r="96" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" s="426"/>
-      <c r="B96" s="600"/>
-      <c r="C96" s="594" t="s">
+      <c r="B96" s="599"/>
+      <c r="C96" s="593" t="s">
         <v>281</v>
       </c>
-      <c r="D96" s="594" t="s">
+      <c r="D96" s="593" t="s">
         <v>368</v>
       </c>
-      <c r="E96" s="694">
+      <c r="E96" s="604">
         <v>1</v>
       </c>
-      <c r="F96" s="698" t="str">
-        <f>Namespace &amp; ($C96)</f>
-        <v>http://vocab.fairdatacollective.org/dataset/properties/DataSource</v>
+      <c r="F96" s="694" t="str">
+        <f>Namespace &amp; ($C96) &amp; "Info"</f>
+        <v>https://vocab.fairdatacollective.org/gdmt/property/DataSourceInfo</v>
       </c>
       <c r="G96" s="443" t="s">
         <v>192</v>
@@ -7292,7 +7291,7 @@
       </c>
       <c r="L96" s="446" t="str">
         <f t="shared" si="5"/>
-        <v>http://vocab.fairdatacollective.org/dataset/properties/dataSource</v>
+        <v>https://vocab.fairdatacollective.org/gdmt/property/dataSource</v>
       </c>
       <c r="M96" s="114" t="s">
         <v>502</v>
@@ -7303,11 +7302,11 @@
     </row>
     <row r="97" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" s="426"/>
-      <c r="B97" s="600"/>
-      <c r="C97" s="595"/>
-      <c r="D97" s="595"/>
-      <c r="E97" s="695"/>
-      <c r="F97" s="699"/>
+      <c r="B97" s="599"/>
+      <c r="C97" s="594"/>
+      <c r="D97" s="594"/>
+      <c r="E97" s="605"/>
+      <c r="F97" s="695"/>
       <c r="G97" s="110" t="s">
         <v>195</v>
       </c>
@@ -7325,7 +7324,7 @@
       </c>
       <c r="L97" s="113" t="str">
         <f t="shared" si="5"/>
-        <v>http://vocab.fairdatacollective.org/dataset/properties/dataSourceIRI</v>
+        <v>https://vocab.fairdatacollective.org/gdmt/property/dataSourceIRI</v>
       </c>
       <c r="M97" s="114" t="s">
         <v>502</v>
@@ -7336,11 +7335,11 @@
     </row>
     <row r="98" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="426"/>
-      <c r="B98" s="600"/>
-      <c r="C98" s="595"/>
-      <c r="D98" s="595"/>
-      <c r="E98" s="695"/>
-      <c r="F98" s="699"/>
+      <c r="B98" s="599"/>
+      <c r="C98" s="594"/>
+      <c r="D98" s="594"/>
+      <c r="E98" s="605"/>
+      <c r="F98" s="695"/>
       <c r="G98" s="110" t="s">
         <v>197</v>
       </c>
@@ -7358,7 +7357,7 @@
       </c>
       <c r="L98" s="113" t="str">
         <f t="shared" si="5"/>
-        <v>http://vocab.fairdatacollective.org/dataset/properties/dataSourceScheme</v>
+        <v>https://vocab.fairdatacollective.org/gdmt/property/dataSourceScheme</v>
       </c>
       <c r="M98" s="114" t="s">
         <v>502</v>
@@ -7369,11 +7368,11 @@
     </row>
     <row r="99" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="426"/>
-      <c r="B99" s="600"/>
-      <c r="C99" s="596"/>
-      <c r="D99" s="596"/>
-      <c r="E99" s="696"/>
-      <c r="F99" s="700"/>
+      <c r="B99" s="599"/>
+      <c r="C99" s="595"/>
+      <c r="D99" s="595"/>
+      <c r="E99" s="606"/>
+      <c r="F99" s="696"/>
       <c r="G99" s="448" t="s">
         <v>198</v>
       </c>
@@ -7391,7 +7390,7 @@
       </c>
       <c r="L99" s="450" t="str">
         <f t="shared" si="5"/>
-        <v>http://vocab.fairdatacollective.org/dataset/properties/dataSourceSchemeIRI</v>
+        <v>https://vocab.fairdatacollective.org/gdmt/property/dataSourceSchemeIRI</v>
       </c>
       <c r="M99" s="451" t="s">
         <v>502</v>
@@ -7402,19 +7401,19 @@
     </row>
     <row r="100" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="426"/>
-      <c r="B100" s="600"/>
-      <c r="C100" s="595" t="s">
+      <c r="B100" s="599"/>
+      <c r="C100" s="594" t="s">
         <v>282</v>
       </c>
-      <c r="D100" s="595" t="s">
+      <c r="D100" s="594" t="s">
         <v>288</v>
       </c>
-      <c r="E100" s="695" t="s">
+      <c r="E100" s="605" t="s">
         <v>54</v>
       </c>
-      <c r="F100" s="701" t="str">
-        <f>Namespace &amp; ($C100)</f>
-        <v>http://vocab.fairdatacollective.org/dataset/properties/Variable</v>
+      <c r="F100" s="697" t="str">
+        <f>Namespace &amp; ($C100) &amp; "Info"</f>
+        <v>https://vocab.fairdatacollective.org/gdmt/property/VariableInfo</v>
       </c>
       <c r="G100" s="110" t="s">
         <v>289</v>
@@ -7433,7 +7432,7 @@
       </c>
       <c r="L100" s="113" t="str">
         <f t="shared" si="5"/>
-        <v>http://vocab.fairdatacollective.org/dataset/properties/variable</v>
+        <v>https://vocab.fairdatacollective.org/gdmt/property/variable</v>
       </c>
       <c r="M100" s="114" t="s">
         <v>502</v>
@@ -7444,11 +7443,11 @@
     </row>
     <row r="101" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" s="426"/>
-      <c r="B101" s="600"/>
-      <c r="C101" s="595"/>
-      <c r="D101" s="595"/>
-      <c r="E101" s="695"/>
-      <c r="F101" s="701"/>
+      <c r="B101" s="599"/>
+      <c r="C101" s="594"/>
+      <c r="D101" s="594"/>
+      <c r="E101" s="605"/>
+      <c r="F101" s="697"/>
       <c r="G101" s="110" t="s">
         <v>290</v>
       </c>
@@ -7466,7 +7465,7 @@
       </c>
       <c r="L101" s="113" t="str">
         <f t="shared" si="5"/>
-        <v>http://vocab.fairdatacollective.org/dataset/properties/variableIRI</v>
+        <v>https://vocab.fairdatacollective.org/gdmt/property/variableIRI</v>
       </c>
       <c r="M101" s="114" t="s">
         <v>502</v>
@@ -7477,11 +7476,11 @@
     </row>
     <row r="102" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A102" s="426"/>
-      <c r="B102" s="600"/>
-      <c r="C102" s="595"/>
-      <c r="D102" s="595"/>
-      <c r="E102" s="695"/>
-      <c r="F102" s="701"/>
+      <c r="B102" s="599"/>
+      <c r="C102" s="594"/>
+      <c r="D102" s="594"/>
+      <c r="E102" s="605"/>
+      <c r="F102" s="697"/>
       <c r="G102" s="110" t="s">
         <v>291</v>
       </c>
@@ -7499,7 +7498,7 @@
       </c>
       <c r="L102" s="113" t="str">
         <f t="shared" si="5"/>
-        <v>http://vocab.fairdatacollective.org/dataset/properties/variableScheme</v>
+        <v>https://vocab.fairdatacollective.org/gdmt/property/variableScheme</v>
       </c>
       <c r="M102" s="114" t="s">
         <v>502</v>
@@ -7510,11 +7509,11 @@
     </row>
     <row r="103" spans="1:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A103" s="427"/>
-      <c r="B103" s="601"/>
-      <c r="C103" s="604"/>
-      <c r="D103" s="604"/>
-      <c r="E103" s="697"/>
-      <c r="F103" s="702"/>
+      <c r="B103" s="600"/>
+      <c r="C103" s="603"/>
+      <c r="D103" s="603"/>
+      <c r="E103" s="693"/>
+      <c r="F103" s="698"/>
       <c r="G103" s="438" t="s">
         <v>292</v>
       </c>
@@ -7532,7 +7531,7 @@
       </c>
       <c r="L103" s="441" t="str">
         <f t="shared" si="5"/>
-        <v>http://vocab.fairdatacollective.org/dataset/properties/variableSchemeIRI</v>
+        <v>https://vocab.fairdatacollective.org/gdmt/property/variableSchemeIRI</v>
       </c>
       <c r="M103" s="442" t="s">
         <v>502</v>
@@ -7542,11 +7541,11 @@
       </c>
     </row>
     <row r="104" spans="1:14" s="14" customFormat="1" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A104" s="597" t="s">
+      <c r="A104" s="596" t="s">
         <v>201</v>
       </c>
-      <c r="B104" s="597"/>
-      <c r="C104" s="597"/>
+      <c r="B104" s="596"/>
+      <c r="C104" s="596"/>
       <c r="D104" s="478" t="s">
         <v>202</v>
       </c>
@@ -7554,8 +7553,8 @@
         <v>46</v>
       </c>
       <c r="F104" s="480" t="str">
-        <f>Namespace &amp; ($A104)</f>
-        <v>http://vocab.fairdatacollective.org/dataset/properties/SpatialCoverage</v>
+        <f>Namespace &amp; ($A104) &amp; "Info"</f>
+        <v>https://vocab.fairdatacollective.org/gdmt/property/SpatialCoverageInfo</v>
       </c>
       <c r="G104" s="481"/>
       <c r="H104" s="481"/>
@@ -7568,19 +7567,19 @@
     </row>
     <row r="105" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A105" s="424"/>
-      <c r="B105" s="582" t="s">
+      <c r="B105" s="588" t="s">
         <v>504</v>
       </c>
-      <c r="C105" s="582"/>
-      <c r="D105" s="598" t="s">
+      <c r="C105" s="588"/>
+      <c r="D105" s="597" t="s">
         <v>503</v>
       </c>
-      <c r="E105" s="602" t="s">
+      <c r="E105" s="601" t="s">
         <v>46</v>
       </c>
-      <c r="F105" s="588" t="str">
-        <f>Namespace &amp; ($B105)</f>
-        <v>http://vocab.fairdatacollective.org/dataset/properties/SpatialCoveragePoint</v>
+      <c r="F105" s="585" t="str">
+        <f>Namespace &amp; ($B105) &amp; "Info"</f>
+        <v>https://vocab.fairdatacollective.org/gdmt/property/SpatialCoveragePointInfo</v>
       </c>
       <c r="G105" s="453" t="s">
         <v>205</v>
@@ -7599,7 +7598,7 @@
       </c>
       <c r="L105" s="456" t="str">
         <f t="shared" si="5"/>
-        <v>http://vocab.fairdatacollective.org/dataset/properties/pointLatitude</v>
+        <v>https://vocab.fairdatacollective.org/gdmt/property/pointLatitude</v>
       </c>
       <c r="M105" s="457" t="s">
         <v>28</v>
@@ -7610,11 +7609,11 @@
     </row>
     <row r="106" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A106" s="424"/>
-      <c r="B106" s="584"/>
-      <c r="C106" s="584"/>
-      <c r="D106" s="599"/>
-      <c r="E106" s="603"/>
-      <c r="F106" s="590"/>
+      <c r="B106" s="589"/>
+      <c r="C106" s="589"/>
+      <c r="D106" s="598"/>
+      <c r="E106" s="602"/>
+      <c r="F106" s="587"/>
       <c r="G106" s="458" t="s">
         <v>203</v>
       </c>
@@ -7632,7 +7631,7 @@
       </c>
       <c r="L106" s="461" t="str">
         <f t="shared" si="5"/>
-        <v>http://vocab.fairdatacollective.org/dataset/properties/pointLongitude</v>
+        <v>https://vocab.fairdatacollective.org/gdmt/property/pointLongitude</v>
       </c>
       <c r="M106" s="462" t="s">
         <v>28</v>
@@ -7643,19 +7642,19 @@
     </row>
     <row r="107" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A107" s="424"/>
-      <c r="B107" s="582" t="s">
+      <c r="B107" s="588" t="s">
         <v>505</v>
       </c>
-      <c r="C107" s="582"/>
-      <c r="D107" s="582" t="s">
+      <c r="C107" s="588"/>
+      <c r="D107" s="588" t="s">
         <v>506</v>
       </c>
-      <c r="E107" s="585" t="s">
+      <c r="E107" s="582" t="s">
         <v>46</v>
       </c>
-      <c r="F107" s="588" t="str">
-        <f>Namespace &amp; ($B107)</f>
-        <v>http://vocab.fairdatacollective.org/dataset/properties/SpatialCoverageBoundingBox</v>
+      <c r="F107" s="585" t="str">
+        <f>Namespace &amp; ($B107) &amp; "Info"</f>
+        <v>https://vocab.fairdatacollective.org/gdmt/property/SpatialCoverageBoundingBoxInfo</v>
       </c>
       <c r="G107" s="463" t="s">
         <v>207</v>
@@ -7674,7 +7673,7 @@
       </c>
       <c r="L107" s="466" t="str">
         <f t="shared" si="5"/>
-        <v>http://vocab.fairdatacollective.org/dataset/properties/westBoundLongitude</v>
+        <v>https://vocab.fairdatacollective.org/gdmt/property/westBoundLongitude</v>
       </c>
       <c r="M107" s="467" t="s">
         <v>28</v>
@@ -7685,11 +7684,11 @@
     </row>
     <row r="108" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A108" s="424"/>
-      <c r="B108" s="583"/>
-      <c r="C108" s="583"/>
-      <c r="D108" s="583"/>
-      <c r="E108" s="586"/>
-      <c r="F108" s="589"/>
+      <c r="B108" s="619"/>
+      <c r="C108" s="619"/>
+      <c r="D108" s="619"/>
+      <c r="E108" s="583"/>
+      <c r="F108" s="586"/>
       <c r="G108" s="468" t="s">
         <v>209</v>
       </c>
@@ -7707,7 +7706,7 @@
       </c>
       <c r="L108" s="471" t="str">
         <f t="shared" si="5"/>
-        <v>http://vocab.fairdatacollective.org/dataset/properties/eastBoundLongitude</v>
+        <v>https://vocab.fairdatacollective.org/gdmt/property/eastBoundLongitude</v>
       </c>
       <c r="M108" s="472" t="s">
         <v>28</v>
@@ -7718,11 +7717,11 @@
     </row>
     <row r="109" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A109" s="424"/>
-      <c r="B109" s="583"/>
-      <c r="C109" s="583"/>
-      <c r="D109" s="583"/>
-      <c r="E109" s="586"/>
-      <c r="F109" s="589"/>
+      <c r="B109" s="619"/>
+      <c r="C109" s="619"/>
+      <c r="D109" s="619"/>
+      <c r="E109" s="583"/>
+      <c r="F109" s="586"/>
       <c r="G109" s="468" t="s">
         <v>211</v>
       </c>
@@ -7740,7 +7739,7 @@
       </c>
       <c r="L109" s="471" t="str">
         <f t="shared" si="5"/>
-        <v>http://vocab.fairdatacollective.org/dataset/properties/southBoundLatitude</v>
+        <v>https://vocab.fairdatacollective.org/gdmt/property/southBoundLatitude</v>
       </c>
       <c r="M109" s="472" t="s">
         <v>28</v>
@@ -7751,11 +7750,11 @@
     </row>
     <row r="110" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A110" s="424"/>
-      <c r="B110" s="584"/>
-      <c r="C110" s="584"/>
-      <c r="D110" s="584"/>
-      <c r="E110" s="587"/>
-      <c r="F110" s="590"/>
+      <c r="B110" s="589"/>
+      <c r="C110" s="589"/>
+      <c r="D110" s="589"/>
+      <c r="E110" s="584"/>
+      <c r="F110" s="587"/>
       <c r="G110" s="473" t="s">
         <v>213</v>
       </c>
@@ -7773,7 +7772,7 @@
       </c>
       <c r="L110" s="476" t="str">
         <f t="shared" si="5"/>
-        <v>http://vocab.fairdatacollective.org/dataset/properties/northBoundLatitude</v>
+        <v>https://vocab.fairdatacollective.org/gdmt/property/northBoundLatitude</v>
       </c>
       <c r="M110" s="477" t="s">
         <v>28</v>
@@ -7784,19 +7783,19 @@
     </row>
     <row r="111" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A111" s="424"/>
-      <c r="B111" s="582" t="s">
+      <c r="B111" s="588" t="s">
         <v>507</v>
       </c>
-      <c r="C111" s="582"/>
-      <c r="D111" s="591" t="s">
+      <c r="C111" s="588"/>
+      <c r="D111" s="590" t="s">
         <v>508</v>
       </c>
-      <c r="E111" s="585" t="s">
+      <c r="E111" s="582" t="s">
         <v>46</v>
       </c>
-      <c r="F111" s="588" t="str">
-        <f>Namespace &amp; ($B111)</f>
-        <v>http://vocab.fairdatacollective.org/dataset/properties/SpatialCoveragePolygon</v>
+      <c r="F111" s="585" t="str">
+        <f>Namespace &amp; ($B111) &amp; "Info"</f>
+        <v>https://vocab.fairdatacollective.org/gdmt/property/SpatialCoveragePolygonInfo</v>
       </c>
       <c r="G111" s="453" t="s">
         <v>438</v>
@@ -7815,7 +7814,7 @@
       </c>
       <c r="L111" s="466" t="str">
         <f t="shared" si="5"/>
-        <v>http://vocab.fairdatacollective.org/dataset/properties/polygonPointLatitude</v>
+        <v>https://vocab.fairdatacollective.org/gdmt/property/polygonPointLatitude</v>
       </c>
       <c r="M111" s="467" t="s">
         <v>28</v>
@@ -7826,11 +7825,11 @@
     </row>
     <row r="112" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A112" s="424"/>
-      <c r="B112" s="584"/>
-      <c r="C112" s="584"/>
-      <c r="D112" s="592"/>
-      <c r="E112" s="587"/>
-      <c r="F112" s="590"/>
+      <c r="B112" s="589"/>
+      <c r="C112" s="589"/>
+      <c r="D112" s="591"/>
+      <c r="E112" s="584"/>
+      <c r="F112" s="587"/>
       <c r="G112" s="458" t="s">
         <v>439</v>
       </c>
@@ -7848,7 +7847,7 @@
       </c>
       <c r="L112" s="476" t="str">
         <f t="shared" si="5"/>
-        <v>http://vocab.fairdatacollective.org/dataset/properties/polygonPointLongitude</v>
+        <v>https://vocab.fairdatacollective.org/gdmt/property/polygonPointLongitude</v>
       </c>
       <c r="M112" s="477" t="s">
         <v>28</v>
@@ -7881,7 +7880,7 @@
       </c>
       <c r="L113" s="491" t="str">
         <f>Namespace &amp; $G113</f>
-        <v>http://vocab.fairdatacollective.org/dataset/properties/geoLocationDescription</v>
+        <v>https://vocab.fairdatacollective.org/gdmt/property/geoLocationDescription</v>
       </c>
       <c r="M113" s="492" t="s">
         <v>28</v>
@@ -7903,8 +7902,8 @@
         <v>46</v>
       </c>
       <c r="F114" s="567" t="str">
-        <f>Namespace &amp; ($A114)</f>
-        <v>http://vocab.fairdatacollective.org/dataset/properties/VerticalCoverage</v>
+        <f>Namespace &amp; ($A114) &amp; "Info"</f>
+        <v>https://vocab.fairdatacollective.org/gdmt/property/VerticalCoverageInfo</v>
       </c>
       <c r="G114" s="493" t="s">
         <v>219</v>
@@ -7923,7 +7922,7 @@
       </c>
       <c r="L114" s="496" t="str">
         <f t="shared" si="5"/>
-        <v>http://vocab.fairdatacollective.org/dataset/properties/verticalExtentMaximumValue</v>
+        <v>https://vocab.fairdatacollective.org/gdmt/property/verticalExtentMaximumValue</v>
       </c>
       <c r="M114" s="497" t="s">
         <v>28</v>
@@ -7956,7 +7955,7 @@
       </c>
       <c r="L115" s="119" t="str">
         <f t="shared" si="5"/>
-        <v>http://vocab.fairdatacollective.org/dataset/properties/verticalExtentMinimumValue</v>
+        <v>https://vocab.fairdatacollective.org/gdmt/property/verticalExtentMinimumValue</v>
       </c>
       <c r="M115" s="120" t="s">
         <v>28</v>
@@ -7989,7 +7988,7 @@
       </c>
       <c r="L116" s="119" t="str">
         <f t="shared" si="5"/>
-        <v>http://vocab.fairdatacollective.org/dataset/properties/verticalExtentUnit</v>
+        <v>https://vocab.fairdatacollective.org/gdmt/property/verticalExtentUnit</v>
       </c>
       <c r="M116" s="120" t="s">
         <v>194</v>
@@ -8022,7 +8021,7 @@
       </c>
       <c r="L117" s="119" t="str">
         <f t="shared" si="5"/>
-        <v>http://vocab.fairdatacollective.org/dataset/properties/verticalExtentUnitIRI</v>
+        <v>https://vocab.fairdatacollective.org/gdmt/property/verticalExtentUnitIRI</v>
       </c>
       <c r="M117" s="120" t="s">
         <v>194</v>
@@ -8055,7 +8054,7 @@
       </c>
       <c r="L118" s="119" t="str">
         <f t="shared" si="5"/>
-        <v>http://vocab.fairdatacollective.org/dataset/properties/verticalExtentUnitScheme</v>
+        <v>https://vocab.fairdatacollective.org/gdmt/property/verticalExtentUnitScheme</v>
       </c>
       <c r="M118" s="120" t="s">
         <v>194</v>
@@ -8088,7 +8087,7 @@
       </c>
       <c r="L119" s="119" t="str">
         <f t="shared" si="5"/>
-        <v>http://vocab.fairdatacollective.org/dataset/properties/verticalExtentUnitSchemeIRI</v>
+        <v>https://vocab.fairdatacollective.org/gdmt/property/verticalExtentUnitSchemeIRI</v>
       </c>
       <c r="M119" s="120" t="s">
         <v>194</v>
@@ -8113,15 +8112,15 @@
       <c r="I120" s="117" t="s">
         <v>407</v>
       </c>
-      <c r="J120" s="118" t="s">
-        <v>46</v>
+      <c r="J120" s="118">
+        <v>1</v>
       </c>
       <c r="K120" s="119" t="s">
         <v>68</v>
       </c>
       <c r="L120" s="119" t="str">
         <f t="shared" si="5"/>
-        <v>http://vocab.fairdatacollective.org/dataset/properties/verticalExtentDatum</v>
+        <v>https://vocab.fairdatacollective.org/gdmt/property/verticalExtentDatum</v>
       </c>
       <c r="M120" s="120" t="s">
         <v>194</v>
@@ -8154,7 +8153,7 @@
       </c>
       <c r="L121" s="500" t="str">
         <f t="shared" si="5"/>
-        <v>http://vocab.fairdatacollective.org/dataset/properties/verticalExtentDatumIRI</v>
+        <v>https://vocab.fairdatacollective.org/gdmt/property/verticalExtentDatumIRI</v>
       </c>
       <c r="M121" s="501" t="s">
         <v>194</v>
@@ -8176,8 +8175,8 @@
         <v>46</v>
       </c>
       <c r="F122" s="579" t="str">
-        <f>Namespace &amp; ($A122)</f>
-        <v>http://vocab.fairdatacollective.org/dataset/properties/TemporalCoverage</v>
+        <f>Namespace &amp; ($A122) &amp; "Info"</f>
+        <v>https://vocab.fairdatacollective.org/gdmt/property/TemporalCoverageInfo</v>
       </c>
       <c r="G122" s="502" t="s">
         <v>229</v>
@@ -8196,7 +8195,7 @@
       </c>
       <c r="L122" s="505" t="str">
         <f t="shared" si="5"/>
-        <v>http://vocab.fairdatacollective.org/dataset/properties/temporalExtentMinimumValue</v>
+        <v>https://vocab.fairdatacollective.org/gdmt/property/temporalExtentMinimumValue</v>
       </c>
       <c r="M122" s="506" t="s">
         <v>28</v>
@@ -8229,7 +8228,7 @@
       </c>
       <c r="L123" s="124" t="str">
         <f t="shared" si="5"/>
-        <v>http://vocab.fairdatacollective.org/dataset/properties/temporalExtentMaximumValue</v>
+        <v>https://vocab.fairdatacollective.org/gdmt/property/temporalExtentMaximumValue</v>
       </c>
       <c r="M123" s="125" t="s">
         <v>28</v>
@@ -8262,7 +8261,7 @@
       </c>
       <c r="L124" s="124" t="str">
         <f t="shared" si="5"/>
-        <v>http://vocab.fairdatacollective.org/dataset/properties/temporalResolution</v>
+        <v>https://vocab.fairdatacollective.org/gdmt/property/temporalResolution</v>
       </c>
       <c r="M124" s="125" t="s">
         <v>28</v>
@@ -8295,7 +8294,7 @@
       </c>
       <c r="L125" s="510" t="str">
         <f t="shared" si="5"/>
-        <v>http://vocab.fairdatacollective.org/dataset/properties/duration</v>
+        <v>https://vocab.fairdatacollective.org/gdmt/property/duration</v>
       </c>
       <c r="M125" s="511" t="s">
         <v>28</v>
@@ -8317,8 +8316,8 @@
         <v>34</v>
       </c>
       <c r="F126" s="519" t="str">
-        <f>Namespace &amp; ($A126)</f>
-        <v>http://vocab.fairdatacollective.org/dataset/properties/Funding</v>
+        <f>Namespace &amp; ($A126) &amp; "Info"</f>
+        <v>https://vocab.fairdatacollective.org/gdmt/property/FundingInfo</v>
       </c>
       <c r="G126" s="520"/>
       <c r="H126" s="520"/>
@@ -8342,8 +8341,8 @@
         <v>1</v>
       </c>
       <c r="F127" s="540" t="str">
-        <f>Namespace &amp; ($B127)</f>
-        <v>http://vocab.fairdatacollective.org/dataset/properties/Award</v>
+        <f>Namespace &amp; ($B127) &amp; "Info"</f>
+        <v>https://vocab.fairdatacollective.org/gdmt/property/AwardInfo</v>
       </c>
       <c r="G127" s="529" t="s">
         <v>238</v>
@@ -8362,7 +8361,7 @@
       </c>
       <c r="L127" s="532" t="str">
         <f t="shared" si="5"/>
-        <v>http://vocab.fairdatacollective.org/dataset/properties/awardTitle</v>
+        <v>https://vocab.fairdatacollective.org/gdmt/property/awardTitle</v>
       </c>
       <c r="M127" s="529" t="s">
         <v>28</v>
@@ -8395,7 +8394,7 @@
       </c>
       <c r="L128" s="515" t="str">
         <f t="shared" si="5"/>
-        <v>http://vocab.fairdatacollective.org/dataset/properties/awardPageIRI</v>
+        <v>https://vocab.fairdatacollective.org/gdmt/property/awardPageIRI</v>
       </c>
       <c r="M128" s="512" t="s">
         <v>28</v>
@@ -8428,7 +8427,7 @@
       </c>
       <c r="L129" s="536" t="str">
         <f t="shared" si="5"/>
-        <v>http://vocab.fairdatacollective.org/dataset/properties/awardLocalIdentifier</v>
+        <v>https://vocab.fairdatacollective.org/gdmt/property/awardLocalIdentifier</v>
       </c>
       <c r="M129" s="537" t="s">
         <v>28</v>
@@ -8450,8 +8449,8 @@
         <v>54</v>
       </c>
       <c r="F130" s="540" t="str">
-        <f>Namespace &amp; ($B130)</f>
-        <v>http://vocab.fairdatacollective.org/dataset/properties/Funder</v>
+        <f>Namespace &amp; ($B130)  &amp; "Info"</f>
+        <v>https://vocab.fairdatacollective.org/gdmt/property/FunderInfo</v>
       </c>
       <c r="G130" s="512" t="s">
         <v>244</v>
@@ -8470,7 +8469,7 @@
       </c>
       <c r="L130" s="515" t="str">
         <f t="shared" si="5"/>
-        <v>http://vocab.fairdatacollective.org/dataset/properties/funderName</v>
+        <v>https://vocab.fairdatacollective.org/gdmt/property/funderName</v>
       </c>
       <c r="M130" s="512" t="s">
         <v>28</v>
@@ -8503,7 +8502,7 @@
       </c>
       <c r="L131" s="515" t="str">
         <f t="shared" si="5"/>
-        <v>http://vocab.fairdatacollective.org/dataset/properties/funderIdentifier</v>
+        <v>https://vocab.fairdatacollective.org/gdmt/property/funderIdentifier</v>
       </c>
       <c r="M131" s="512" t="s">
         <v>28</v>
@@ -8536,7 +8535,7 @@
       </c>
       <c r="L132" s="515" t="str">
         <f t="shared" si="5"/>
-        <v>http://vocab.fairdatacollective.org/dataset/properties/funderIdentifierScheme</v>
+        <v>https://vocab.fairdatacollective.org/gdmt/property/funderIdentifierScheme</v>
       </c>
       <c r="M132" s="512" t="s">
         <v>28</v>
@@ -8569,7 +8568,7 @@
       </c>
       <c r="L133" s="527" t="str">
         <f t="shared" si="5"/>
-        <v>http://vocab.fairdatacollective.org/dataset/properties/funderIdentifierSchemeIRI</v>
+        <v>https://vocab.fairdatacollective.org/gdmt/property/funderIdentifierSchemeIRI</v>
       </c>
       <c r="M133" s="512" t="s">
         <v>28</v>
@@ -8676,13 +8675,13 @@
     </row>
     <row r="150" spans="4:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D150" s="5" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="J150" s="6"/>
     </row>
     <row r="151" spans="4:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D151" s="16" t="s">
-        <v>520</v>
+        <v>523</v>
       </c>
       <c r="J151" s="6"/>
     </row>
@@ -12221,6 +12220,16 @@
   </sheetData>
   <autoFilter ref="H1:N143" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <mergeCells count="134">
+    <mergeCell ref="D5:D7"/>
+    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="D19:D22"/>
+    <mergeCell ref="F61:F63"/>
+    <mergeCell ref="E61:E63"/>
+    <mergeCell ref="D61:D63"/>
+    <mergeCell ref="F53:F55"/>
+    <mergeCell ref="E53:E55"/>
+    <mergeCell ref="D53:D55"/>
     <mergeCell ref="E100:E103"/>
     <mergeCell ref="F92:F95"/>
     <mergeCell ref="F96:F99"/>
@@ -12228,24 +12237,12 @@
     <mergeCell ref="D8:D12"/>
     <mergeCell ref="E8:E12"/>
     <mergeCell ref="F8:F12"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="F3:F4"/>
     <mergeCell ref="F31:F34"/>
     <mergeCell ref="E31:E34"/>
     <mergeCell ref="F39:F41"/>
     <mergeCell ref="F19:F22"/>
     <mergeCell ref="E19:E22"/>
     <mergeCell ref="E14:E15"/>
-    <mergeCell ref="F5:F7"/>
-    <mergeCell ref="D5:D7"/>
-    <mergeCell ref="F14:F15"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="D19:D22"/>
-    <mergeCell ref="F61:F63"/>
-    <mergeCell ref="E61:E63"/>
-    <mergeCell ref="D61:D63"/>
-    <mergeCell ref="D67:D72"/>
     <mergeCell ref="A3:C4"/>
     <mergeCell ref="A5:C7"/>
     <mergeCell ref="A2:C2"/>
@@ -12266,18 +12263,17 @@
     <mergeCell ref="E25:E27"/>
     <mergeCell ref="F25:F27"/>
     <mergeCell ref="E5:E7"/>
-    <mergeCell ref="F53:F55"/>
-    <mergeCell ref="E53:E55"/>
-    <mergeCell ref="D53:D55"/>
-    <mergeCell ref="A24:C24"/>
-    <mergeCell ref="B25:C27"/>
-    <mergeCell ref="B28:C30"/>
-    <mergeCell ref="B31:C34"/>
-    <mergeCell ref="A38:C38"/>
-    <mergeCell ref="B39:C41"/>
-    <mergeCell ref="B42:C44"/>
-    <mergeCell ref="B45:C48"/>
-    <mergeCell ref="A52:C52"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="F5:F7"/>
+    <mergeCell ref="E84:E87"/>
+    <mergeCell ref="F84:F87"/>
+    <mergeCell ref="B81:B83"/>
+    <mergeCell ref="C81:C83"/>
+    <mergeCell ref="D81:D83"/>
+    <mergeCell ref="E81:E83"/>
+    <mergeCell ref="F81:F83"/>
     <mergeCell ref="B53:C55"/>
     <mergeCell ref="B78:B80"/>
     <mergeCell ref="C78:C80"/>
@@ -12293,20 +12289,8 @@
     <mergeCell ref="F73:F75"/>
     <mergeCell ref="E73:E75"/>
     <mergeCell ref="D73:D75"/>
-    <mergeCell ref="B84:B87"/>
-    <mergeCell ref="C84:C87"/>
-    <mergeCell ref="D84:D87"/>
-    <mergeCell ref="E84:E87"/>
-    <mergeCell ref="F84:F87"/>
-    <mergeCell ref="B81:B83"/>
-    <mergeCell ref="C81:C83"/>
-    <mergeCell ref="D81:D83"/>
-    <mergeCell ref="E81:E83"/>
-    <mergeCell ref="F81:F83"/>
     <mergeCell ref="A59:C59"/>
     <mergeCell ref="B61:C63"/>
-    <mergeCell ref="A65:C66"/>
-    <mergeCell ref="A67:C67"/>
     <mergeCell ref="A8:C12"/>
     <mergeCell ref="A18:C18"/>
     <mergeCell ref="B19:C22"/>
@@ -12316,6 +12300,21 @@
     <mergeCell ref="A17:C17"/>
     <mergeCell ref="B107:C110"/>
     <mergeCell ref="D107:D110"/>
+    <mergeCell ref="B84:B87"/>
+    <mergeCell ref="C84:C87"/>
+    <mergeCell ref="D84:D87"/>
+    <mergeCell ref="A65:C66"/>
+    <mergeCell ref="A67:C67"/>
+    <mergeCell ref="A24:C24"/>
+    <mergeCell ref="B25:C27"/>
+    <mergeCell ref="B28:C30"/>
+    <mergeCell ref="B31:C34"/>
+    <mergeCell ref="A38:C38"/>
+    <mergeCell ref="B39:C41"/>
+    <mergeCell ref="B42:C44"/>
+    <mergeCell ref="B45:C48"/>
+    <mergeCell ref="A52:C52"/>
+    <mergeCell ref="D67:D72"/>
     <mergeCell ref="E107:E110"/>
     <mergeCell ref="F107:F110"/>
     <mergeCell ref="B111:C112"/>
@@ -12427,7 +12426,7 @@
       </c>
       <c r="E1" s="22" t="str">
         <f>Namespace &amp; LOWER($A1)</f>
-        <v>http://vocab.fairdatacollective.org/dataset/properties/contributor</v>
+        <v>https://vocab.fairdatacollective.org/gdmt/property/contributor</v>
       </c>
       <c r="F1" s="23"/>
       <c r="G1" s="24"/>
@@ -12451,7 +12450,7 @@
       </c>
       <c r="E2" s="738" t="str">
         <f>Namespace &amp; LOWER($B2)</f>
-        <v>http://vocab.fairdatacollective.org/dataset/properties/contributorname</v>
+        <v>https://vocab.fairdatacollective.org/gdmt/property/contributorname</v>
       </c>
       <c r="F2" s="29" t="s">
         <v>115</v>
@@ -12553,7 +12552,7 @@
       </c>
       <c r="E5" s="738" t="str">
         <f>Namespace &amp; LOWER($B5)</f>
-        <v>http://vocab.fairdatacollective.org/dataset/properties/contributoridentifier</v>
+        <v>https://vocab.fairdatacollective.org/gdmt/property/contributoridentifier</v>
       </c>
       <c r="F5" s="34" t="s">
         <v>120</v>
@@ -12572,7 +12571,7 @@
       </c>
       <c r="K5" s="33" t="str">
         <f t="shared" ref="K5:K11" si="0">Namespace &amp; $F5</f>
-        <v>http://vocab.fairdatacollective.org/dataset/properties/contributorIdentifier</v>
+        <v>https://vocab.fairdatacollective.org/gdmt/property/contributorIdentifier</v>
       </c>
       <c r="L5" s="29" t="s">
         <v>28</v>
@@ -12604,7 +12603,7 @@
       </c>
       <c r="K6" s="33" t="str">
         <f t="shared" si="0"/>
-        <v>http://vocab.fairdatacollective.org/dataset/properties/contributorIdentifierScheme</v>
+        <v>https://vocab.fairdatacollective.org/gdmt/property/contributorIdentifierScheme</v>
       </c>
       <c r="L6" s="37" t="s">
         <v>24</v>
@@ -12636,7 +12635,7 @@
       </c>
       <c r="K7" s="33" t="str">
         <f t="shared" si="0"/>
-        <v>http://vocab.fairdatacollective.org/dataset/properties/contributorIdentifierSchemeIRI</v>
+        <v>https://vocab.fairdatacollective.org/gdmt/property/contributorIdentifierSchemeIRI</v>
       </c>
       <c r="L7" s="37" t="s">
         <v>24</v>
@@ -12658,7 +12657,7 @@
       </c>
       <c r="E8" s="739" t="str">
         <f>Namespace &amp; LOWER($B8)</f>
-        <v>http://vocab.fairdatacollective.org/dataset/properties/contributoraffiliation</v>
+        <v>https://vocab.fairdatacollective.org/gdmt/property/contributoraffiliation</v>
       </c>
       <c r="F8" s="34" t="s">
         <v>331</v>
@@ -12677,7 +12676,7 @@
       </c>
       <c r="K8" s="33" t="str">
         <f t="shared" si="0"/>
-        <v>http://vocab.fairdatacollective.org/dataset/properties/contributorAffiliation</v>
+        <v>https://vocab.fairdatacollective.org/gdmt/property/contributorAffiliation</v>
       </c>
       <c r="L8" s="29" t="s">
         <v>28</v>
@@ -12709,7 +12708,7 @@
       </c>
       <c r="K9" s="33" t="str">
         <f t="shared" si="0"/>
-        <v>http://vocab.fairdatacollective.org/dataset/properties/contributorAffiliationIdentifier</v>
+        <v>https://vocab.fairdatacollective.org/gdmt/property/contributorAffiliationIdentifier</v>
       </c>
       <c r="L9" s="29" t="s">
         <v>28</v>
@@ -12741,7 +12740,7 @@
       </c>
       <c r="K10" s="33" t="str">
         <f t="shared" si="0"/>
-        <v>http://vocab.fairdatacollective.org/dataset/properties/contributorAffiliationIdentifierScheme</v>
+        <v>https://vocab.fairdatacollective.org/gdmt/property/contributorAffiliationIdentifierScheme</v>
       </c>
       <c r="L10" s="37" t="s">
         <v>24</v>
@@ -12773,7 +12772,7 @@
       </c>
       <c r="K11" s="33" t="str">
         <f t="shared" si="0"/>
-        <v>http://vocab.fairdatacollective.org/dataset/properties/contributorAffiliationIdentifierSchemeIRI</v>
+        <v>https://vocab.fairdatacollective.org/gdmt/property/contributorAffiliationIdentifierSchemeIRI</v>
       </c>
       <c r="L11" s="37" t="s">
         <v>24</v>
@@ -12836,7 +12835,7 @@
       </c>
       <c r="K13" s="33" t="str">
         <f>Namespace &amp; $F13</f>
-        <v>http://vocab.fairdatacollective.org/dataset/properties/contributorRole</v>
+        <v>https://vocab.fairdatacollective.org/gdmt/property/contributorRole</v>
       </c>
       <c r="L13" s="37" t="s">
         <v>24</v>
@@ -12868,7 +12867,7 @@
       </c>
       <c r="K14" s="33" t="str">
         <f>Namespace &amp; $F14</f>
-        <v>http://vocab.fairdatacollective.org/dataset/properties/contributorType</v>
+        <v>https://vocab.fairdatacollective.org/gdmt/property/contributorType</v>
       </c>
       <c r="L14" s="37" t="s">
         <v>24</v>

</xml_diff>

<commit_message>
updated template description and vocabulary due to issues with bioportal not processing "owl:DataProperty"
</commit_message>
<xml_diff>
--- a/template-description.xlsx
+++ b/template-description.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Secondary_Drive/work/repos/FAIR-data/generic-dataset-metadata-template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF421368-6A8E-2D41-A86A-288517FF656B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B96259B1-314F-6140-9370-C69555C090DF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="34400" yWindow="460" windowWidth="34400" windowHeight="28340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1025" uniqueCount="523">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1028" uniqueCount="525">
   <si>
     <t>Element 
 (CEDAR)</t>
@@ -1514,9 +1514,6 @@
     <t>Distributor</t>
   </si>
   <si>
-    <t>Information about this distributor of the dataset. The Distributor includes primarily the system doing the distribution, but can include the person or persons responsible as well, for example the person who reformsts the dataset for this distribution.</t>
-  </si>
-  <si>
     <t>DistributorName</t>
   </si>
   <si>
@@ -1608,6 +1605,15 @@
   </si>
   <si>
     <t>License Identifier Scheme IRI</t>
+  </si>
+  <si>
+    <t>1..1</t>
+  </si>
+  <si>
+    <t>Information about the distributor of this dataset distribution. The Distributor includes primarily the system doing the distribution, but can include the person or persons responsible as well, for example the person who reformed the dataset for this distribution.</t>
+  </si>
+  <si>
+    <t>http://vocab.fairdatacollective.org/gdmt/hasDistributionAccess</t>
   </si>
 </sst>
 </file>
@@ -2080,7 +2086,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="747">
+  <cellXfs count="744">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -3142,607 +3148,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="26" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="26" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="26" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="26" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="37" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="37" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="35" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="35" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="35" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="35" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="37" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="37" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="34" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="34" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="34" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="34" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="31" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="31" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="31" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="31" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="31" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="24" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="35" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="35" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="30" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="35" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="35" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="30" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="38" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="38" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="35" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="35" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="35" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="38" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="38" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="26" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="38" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="38" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="41" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="41" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="41" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="41" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="41" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="41" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="28" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="28" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="41" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="41" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="28" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="19" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="11" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3758,11 +3163,603 @@
     <xf numFmtId="0" fontId="11" fillId="30" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="41" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="41" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="41" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="41" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="41" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="41" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="41" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="41" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="35" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="35" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="38" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="38" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="35" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="35" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="35" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="35" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="35" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="38" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="38" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="38" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="38" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="24" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="30" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="35" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="35" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="35" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="35" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="30" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="34" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="34" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="37" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="37" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="37" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="37" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="16" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="34" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="34" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3997,10 +3994,10 @@
   <dimension ref="A1:P1034"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="F44" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="K81" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L67" sqref="L67"/>
+      <selection pane="bottomRight" activeCell="G130" sqref="G130:L133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4022,11 +4019,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="601" t="s">
+      <c r="A1" s="668" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="601"/>
-      <c r="C1" s="601"/>
+      <c r="B1" s="668"/>
+      <c r="C1" s="668"/>
       <c r="D1" s="44" t="s">
         <v>1</v>
       </c>
@@ -4064,11 +4061,11 @@
       <c r="P1" s="1"/>
     </row>
     <row r="2" spans="1:16" ht="69" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="600" t="s">
+      <c r="A2" s="667" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="600"/>
-      <c r="C2" s="600"/>
+      <c r="B2" s="667"/>
+      <c r="C2" s="667"/>
       <c r="D2" s="121" t="s">
         <v>10</v>
       </c>
@@ -4100,18 +4097,18 @@
       <c r="P2" s="2"/>
     </row>
     <row r="3" spans="1:16" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="595" t="s">
+      <c r="A3" s="662" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="595"/>
-      <c r="C3" s="595"/>
-      <c r="D3" s="620" t="s">
+      <c r="B3" s="662"/>
+      <c r="C3" s="662"/>
+      <c r="D3" s="684" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="622">
+      <c r="E3" s="686">
         <v>1</v>
       </c>
-      <c r="F3" s="623" t="str">
+      <c r="F3" s="687" t="str">
         <f>Namespace &amp; "has" &amp; $A3 &amp; "Info"</f>
         <v>http://vocab.fairdatacollective.org/gdmt/hasResourceTypeInfo</v>
       </c>
@@ -4142,12 +4139,12 @@
       </c>
     </row>
     <row r="4" spans="1:16" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="596"/>
-      <c r="B4" s="596"/>
-      <c r="C4" s="596"/>
-      <c r="D4" s="621"/>
-      <c r="E4" s="575"/>
-      <c r="F4" s="624"/>
+      <c r="A4" s="663"/>
+      <c r="B4" s="663"/>
+      <c r="C4" s="663"/>
+      <c r="D4" s="685"/>
+      <c r="E4" s="581"/>
+      <c r="F4" s="688"/>
       <c r="G4" s="185" t="s">
         <v>22</v>
       </c>
@@ -4175,18 +4172,18 @@
       </c>
     </row>
     <row r="5" spans="1:16" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="597" t="s">
+      <c r="A5" s="664" t="s">
         <v>259</v>
       </c>
-      <c r="B5" s="597"/>
-      <c r="C5" s="597"/>
-      <c r="D5" s="535" t="s">
+      <c r="B5" s="664"/>
+      <c r="C5" s="664"/>
+      <c r="D5" s="720" t="s">
         <v>25</v>
       </c>
-      <c r="E5" s="617">
+      <c r="E5" s="681">
         <v>1</v>
       </c>
-      <c r="F5" s="625" t="str">
+      <c r="F5" s="689" t="str">
         <f>Namespace &amp; "has" &amp; ($A5) &amp; "Info"</f>
         <v>http://vocab.fairdatacollective.org/gdmt/hasDatasetIdentifierInfo</v>
       </c>
@@ -4216,12 +4213,12 @@
       </c>
     </row>
     <row r="6" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="598"/>
-      <c r="B6" s="598"/>
-      <c r="C6" s="598"/>
-      <c r="D6" s="536"/>
-      <c r="E6" s="618"/>
-      <c r="F6" s="626"/>
+      <c r="A6" s="665"/>
+      <c r="B6" s="665"/>
+      <c r="C6" s="665"/>
+      <c r="D6" s="721"/>
+      <c r="E6" s="682"/>
+      <c r="F6" s="690"/>
       <c r="G6" s="53" t="s">
         <v>29</v>
       </c>
@@ -4248,12 +4245,12 @@
       </c>
     </row>
     <row r="7" spans="1:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="599"/>
-      <c r="B7" s="599"/>
-      <c r="C7" s="599"/>
-      <c r="D7" s="537"/>
-      <c r="E7" s="619"/>
-      <c r="F7" s="627"/>
+      <c r="A7" s="666"/>
+      <c r="B7" s="666"/>
+      <c r="C7" s="666"/>
+      <c r="D7" s="722"/>
+      <c r="E7" s="683"/>
+      <c r="F7" s="691"/>
       <c r="G7" s="198" t="s">
         <v>32</v>
       </c>
@@ -4281,18 +4278,18 @@
       </c>
     </row>
     <row r="8" spans="1:16" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="652" t="s">
+      <c r="A8" s="610" t="s">
         <v>33</v>
       </c>
-      <c r="B8" s="652"/>
-      <c r="C8" s="652"/>
-      <c r="D8" s="570" t="s">
+      <c r="B8" s="610"/>
+      <c r="C8" s="610"/>
+      <c r="D8" s="699" t="s">
         <v>276</v>
       </c>
-      <c r="E8" s="573" t="s">
+      <c r="E8" s="702" t="s">
         <v>34</v>
       </c>
-      <c r="F8" s="576" t="str">
+      <c r="F8" s="703" t="str">
         <f>Namespace &amp; "has" &amp; ($A8) &amp; "Info"</f>
         <v>http://vocab.fairdatacollective.org/gdmt/hasRelatedResourcesInfo</v>
       </c>
@@ -4322,12 +4319,12 @@
       </c>
     </row>
     <row r="9" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="653"/>
-      <c r="B9" s="653"/>
-      <c r="C9" s="653"/>
-      <c r="D9" s="571"/>
-      <c r="E9" s="574"/>
-      <c r="F9" s="577"/>
+      <c r="A9" s="611"/>
+      <c r="B9" s="611"/>
+      <c r="C9" s="611"/>
+      <c r="D9" s="700"/>
+      <c r="E9" s="580"/>
+      <c r="F9" s="704"/>
       <c r="G9" s="59" t="s">
         <v>38</v>
       </c>
@@ -4355,12 +4352,12 @@
       </c>
     </row>
     <row r="10" spans="1:16" s="10" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="653"/>
-      <c r="B10" s="653"/>
-      <c r="C10" s="653"/>
-      <c r="D10" s="571"/>
-      <c r="E10" s="574"/>
-      <c r="F10" s="577"/>
+      <c r="A10" s="611"/>
+      <c r="B10" s="611"/>
+      <c r="C10" s="611"/>
+      <c r="D10" s="700"/>
+      <c r="E10" s="580"/>
+      <c r="F10" s="704"/>
       <c r="G10" s="59" t="s">
         <v>272</v>
       </c>
@@ -4389,12 +4386,12 @@
       </c>
     </row>
     <row r="11" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="653"/>
-      <c r="B11" s="653"/>
-      <c r="C11" s="653"/>
-      <c r="D11" s="571"/>
-      <c r="E11" s="574"/>
-      <c r="F11" s="577"/>
+      <c r="A11" s="611"/>
+      <c r="B11" s="611"/>
+      <c r="C11" s="611"/>
+      <c r="D11" s="700"/>
+      <c r="E11" s="580"/>
+      <c r="F11" s="704"/>
       <c r="G11" s="64" t="s">
         <v>41</v>
       </c>
@@ -4422,12 +4419,12 @@
       </c>
     </row>
     <row r="12" spans="1:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="654"/>
-      <c r="B12" s="654"/>
-      <c r="C12" s="654"/>
-      <c r="D12" s="572"/>
-      <c r="E12" s="575"/>
-      <c r="F12" s="578"/>
+      <c r="A12" s="612"/>
+      <c r="B12" s="612"/>
+      <c r="C12" s="612"/>
+      <c r="D12" s="701"/>
+      <c r="E12" s="581"/>
+      <c r="F12" s="705"/>
       <c r="G12" s="211" t="s">
         <v>42</v>
       </c>
@@ -4455,11 +4452,11 @@
       </c>
     </row>
     <row r="13" spans="1:16" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="656" t="s">
+      <c r="A13" s="617" t="s">
         <v>44</v>
       </c>
-      <c r="B13" s="656"/>
-      <c r="C13" s="656"/>
+      <c r="B13" s="617"/>
+      <c r="C13" s="617"/>
       <c r="D13" s="238" t="s">
         <v>45</v>
       </c>
@@ -4496,18 +4493,18 @@
       </c>
     </row>
     <row r="14" spans="1:16" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="657" t="s">
+      <c r="A14" s="618" t="s">
         <v>48</v>
       </c>
-      <c r="B14" s="657"/>
-      <c r="C14" s="657"/>
-      <c r="D14" s="540" t="s">
+      <c r="B14" s="618"/>
+      <c r="C14" s="618"/>
+      <c r="D14" s="725" t="s">
         <v>49</v>
       </c>
-      <c r="E14" s="593" t="s">
+      <c r="E14" s="715" t="s">
         <v>46</v>
       </c>
-      <c r="F14" s="538" t="str">
+      <c r="F14" s="723" t="str">
         <f>Namespace &amp; "has" &amp; ($A14) &amp; "Info"</f>
         <v>http://vocab.fairdatacollective.org/gdmt/hasLanguageInfo</v>
       </c>
@@ -4537,12 +4534,12 @@
       </c>
     </row>
     <row r="15" spans="1:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="658"/>
-      <c r="B15" s="658"/>
-      <c r="C15" s="658"/>
-      <c r="D15" s="541"/>
-      <c r="E15" s="594"/>
-      <c r="F15" s="539"/>
+      <c r="A15" s="619"/>
+      <c r="B15" s="619"/>
+      <c r="C15" s="619"/>
+      <c r="D15" s="726"/>
+      <c r="E15" s="716"/>
+      <c r="F15" s="724"/>
       <c r="G15" s="224" t="s">
         <v>51</v>
       </c>
@@ -4572,11 +4569,11 @@
       <c r="P15" s="11"/>
     </row>
     <row r="16" spans="1:16" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="659" t="s">
+      <c r="A16" s="620" t="s">
         <v>52</v>
       </c>
-      <c r="B16" s="659"/>
-      <c r="C16" s="659"/>
+      <c r="B16" s="620"/>
+      <c r="C16" s="620"/>
       <c r="D16" s="239" t="s">
         <v>53</v>
       </c>
@@ -4613,11 +4610,11 @@
       </c>
     </row>
     <row r="17" spans="1:16" s="11" customFormat="1" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="660" t="s">
+      <c r="A17" s="621" t="s">
         <v>57</v>
       </c>
-      <c r="B17" s="660"/>
-      <c r="C17" s="660"/>
+      <c r="B17" s="621"/>
+      <c r="C17" s="621"/>
       <c r="D17" s="78" t="s">
         <v>58</v>
       </c>
@@ -4656,11 +4653,11 @@
       <c r="P17"/>
     </row>
     <row r="18" spans="1:16" s="11" customFormat="1" ht="17" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="655" t="s">
+      <c r="A18" s="613" t="s">
         <v>62</v>
       </c>
-      <c r="B18" s="655"/>
-      <c r="C18" s="655"/>
+      <c r="B18" s="613"/>
+      <c r="C18" s="613"/>
       <c r="D18" s="240" t="s">
         <v>63</v>
       </c>
@@ -4684,17 +4681,17 @@
     </row>
     <row r="19" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="310"/>
-      <c r="B19" s="542" t="s">
-        <v>499</v>
-      </c>
-      <c r="C19" s="542"/>
-      <c r="D19" s="542" t="s">
+      <c r="B19" s="614" t="s">
+        <v>498</v>
+      </c>
+      <c r="C19" s="614"/>
+      <c r="D19" s="614" t="s">
         <v>466</v>
       </c>
-      <c r="E19" s="590" t="s">
+      <c r="E19" s="712" t="s">
         <v>34</v>
       </c>
-      <c r="F19" s="587" t="str">
+      <c r="F19" s="709" t="str">
         <f>Namespace&amp;($B19) &amp; "Info"</f>
         <v>http://vocab.fairdatacollective.org/gdmt/ControlledTermsInfo</v>
       </c>
@@ -4717,7 +4714,7 @@
         <v>67</v>
       </c>
       <c r="M19" s="126" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="N19" s="126" t="s">
         <v>28</v>
@@ -4725,11 +4722,11 @@
     </row>
     <row r="20" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="310"/>
-      <c r="B20" s="543"/>
-      <c r="C20" s="543"/>
-      <c r="D20" s="543"/>
-      <c r="E20" s="591"/>
-      <c r="F20" s="588"/>
+      <c r="B20" s="615"/>
+      <c r="C20" s="615"/>
+      <c r="D20" s="615"/>
+      <c r="E20" s="713"/>
+      <c r="F20" s="710"/>
       <c r="G20" s="79" t="s">
         <v>467</v>
       </c>
@@ -4750,7 +4747,7 @@
         <v>http://vocab.fairdatacollective.org/gdmt/hasSubjectIRI</v>
       </c>
       <c r="M20" s="83" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="N20" s="83" t="s">
         <v>28</v>
@@ -4758,11 +4755,11 @@
     </row>
     <row r="21" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="310"/>
-      <c r="B21" s="543"/>
-      <c r="C21" s="543"/>
-      <c r="D21" s="543"/>
-      <c r="E21" s="591"/>
-      <c r="F21" s="588"/>
+      <c r="B21" s="615"/>
+      <c r="C21" s="615"/>
+      <c r="D21" s="615"/>
+      <c r="E21" s="713"/>
+      <c r="F21" s="710"/>
       <c r="G21" s="83" t="s">
         <v>70</v>
       </c>
@@ -4783,7 +4780,7 @@
         <v>http://vocab.fairdatacollective.org/gdmt/hasSubjectScheme</v>
       </c>
       <c r="M21" s="83" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="N21" s="83" t="s">
         <v>28</v>
@@ -4791,11 +4788,11 @@
     </row>
     <row r="22" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="310"/>
-      <c r="B22" s="544"/>
-      <c r="C22" s="544"/>
-      <c r="D22" s="544"/>
-      <c r="E22" s="592"/>
-      <c r="F22" s="589"/>
+      <c r="B22" s="616"/>
+      <c r="C22" s="616"/>
+      <c r="D22" s="616"/>
+      <c r="E22" s="714"/>
+      <c r="F22" s="711"/>
       <c r="G22" s="127" t="s">
         <v>71</v>
       </c>
@@ -4816,7 +4813,7 @@
         <v>http://vocab.fairdatacollective.org/gdmt/hasSubjectSchemeIRI</v>
       </c>
       <c r="M22" s="131" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="N22" s="131" t="s">
         <v>28</v>
@@ -4854,11 +4851,11 @@
       </c>
     </row>
     <row r="24" spans="1:16" s="14" customFormat="1" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="665" t="s">
+      <c r="A24" s="630" t="s">
         <v>72</v>
       </c>
-      <c r="B24" s="665"/>
-      <c r="C24" s="665"/>
+      <c r="B24" s="630"/>
+      <c r="C24" s="630"/>
       <c r="D24" s="241" t="s">
         <v>73</v>
       </c>
@@ -4880,17 +4877,17 @@
     </row>
     <row r="25" spans="1:16" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="17"/>
-      <c r="B25" s="611" t="s">
+      <c r="B25" s="631" t="s">
         <v>450</v>
       </c>
-      <c r="C25" s="611"/>
-      <c r="D25" s="611" t="s">
+      <c r="C25" s="631"/>
+      <c r="D25" s="631" t="s">
         <v>476</v>
       </c>
-      <c r="E25" s="581" t="s">
-        <v>54</v>
-      </c>
-      <c r="F25" s="614" t="str">
+      <c r="E25" s="675" t="s">
+        <v>46</v>
+      </c>
+      <c r="F25" s="678" t="str">
         <f>Namespace &amp; "has" &amp; ($B25) &amp; "Info"</f>
         <v>http://vocab.fairdatacollective.org/gdmt/hasCreatorNameInfo</v>
       </c>
@@ -4921,11 +4918,11 @@
     </row>
     <row r="26" spans="1:16" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="17"/>
-      <c r="B26" s="612"/>
-      <c r="C26" s="612"/>
-      <c r="D26" s="612"/>
-      <c r="E26" s="582"/>
-      <c r="F26" s="615"/>
+      <c r="B26" s="632"/>
+      <c r="C26" s="632"/>
+      <c r="D26" s="632"/>
+      <c r="E26" s="676"/>
+      <c r="F26" s="679"/>
       <c r="G26" s="87" t="s">
         <v>79</v>
       </c>
@@ -4953,11 +4950,11 @@
     </row>
     <row r="27" spans="1:16" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="17"/>
-      <c r="B27" s="613"/>
-      <c r="C27" s="613"/>
-      <c r="D27" s="613"/>
-      <c r="E27" s="583"/>
-      <c r="F27" s="616"/>
+      <c r="B27" s="633"/>
+      <c r="C27" s="633"/>
+      <c r="D27" s="633"/>
+      <c r="E27" s="677"/>
+      <c r="F27" s="680"/>
       <c r="G27" s="136" t="s">
         <v>82</v>
       </c>
@@ -4985,17 +4982,17 @@
     </row>
     <row r="28" spans="1:16" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="17"/>
-      <c r="B28" s="611" t="s">
+      <c r="B28" s="631" t="s">
         <v>451</v>
       </c>
-      <c r="C28" s="611"/>
-      <c r="D28" s="611" t="s">
+      <c r="C28" s="631"/>
+      <c r="D28" s="631" t="s">
         <v>475</v>
       </c>
-      <c r="E28" s="581" t="s">
-        <v>54</v>
-      </c>
-      <c r="F28" s="614" t="str">
+      <c r="E28" s="675" t="s">
+        <v>522</v>
+      </c>
+      <c r="F28" s="678" t="str">
         <f>Namespace &amp; "has" &amp; ($B28) &amp; "Info"</f>
         <v>http://vocab.fairdatacollective.org/gdmt/hasCreatorIdentifierInfo</v>
       </c>
@@ -5015,7 +5012,7 @@
         <v>20</v>
       </c>
       <c r="L28" s="135" t="str">
-        <f>Namespace &amp; "has" &amp; SUBSTITUTE($H28, " ", "")</f>
+        <f t="shared" ref="L28:L34" si="0">Namespace &amp; "has" &amp; SUBSTITUTE($H28, " ", "")</f>
         <v>http://vocab.fairdatacollective.org/gdmt/hasCreatorIdentifier</v>
       </c>
       <c r="M28" s="132" t="s">
@@ -5027,11 +5024,11 @@
     </row>
     <row r="29" spans="1:16" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="17"/>
-      <c r="B29" s="612"/>
-      <c r="C29" s="612"/>
-      <c r="D29" s="612"/>
-      <c r="E29" s="582"/>
-      <c r="F29" s="615"/>
+      <c r="B29" s="632"/>
+      <c r="C29" s="632"/>
+      <c r="D29" s="632"/>
+      <c r="E29" s="676"/>
+      <c r="F29" s="679"/>
       <c r="G29" s="87" t="s">
         <v>93</v>
       </c>
@@ -5048,7 +5045,7 @@
         <v>20</v>
       </c>
       <c r="L29" s="86" t="str">
-        <f>Namespace &amp; "has" &amp; SUBSTITUTE($H29, " ", "")</f>
+        <f t="shared" si="0"/>
         <v>http://vocab.fairdatacollective.org/gdmt/hasCreatorIdentifierScheme</v>
       </c>
       <c r="M29" s="89" t="str">
@@ -5061,11 +5058,11 @@
     </row>
     <row r="30" spans="1:16" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="17"/>
-      <c r="B30" s="613"/>
-      <c r="C30" s="613"/>
-      <c r="D30" s="613"/>
-      <c r="E30" s="583"/>
-      <c r="F30" s="616"/>
+      <c r="B30" s="633"/>
+      <c r="C30" s="633"/>
+      <c r="D30" s="633"/>
+      <c r="E30" s="677"/>
+      <c r="F30" s="680"/>
       <c r="G30" s="136" t="s">
         <v>95</v>
       </c>
@@ -5082,7 +5079,7 @@
         <v>20</v>
       </c>
       <c r="L30" s="139" t="str">
-        <f>Namespace &amp; "has" &amp; SUBSTITUTE($H30, " ", "")</f>
+        <f t="shared" si="0"/>
         <v>http://vocab.fairdatacollective.org/gdmt/hasCreatorIdentifierSchemeIRI</v>
       </c>
       <c r="M30" s="143" t="str">
@@ -5095,17 +5092,17 @@
     </row>
     <row r="31" spans="1:16" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="17"/>
-      <c r="B31" s="611" t="s">
+      <c r="B31" s="631" t="s">
         <v>452</v>
       </c>
-      <c r="C31" s="611"/>
-      <c r="D31" s="611" t="s">
+      <c r="C31" s="631"/>
+      <c r="D31" s="631" t="s">
         <v>474</v>
       </c>
-      <c r="E31" s="581" t="s">
+      <c r="E31" s="675" t="s">
         <v>34</v>
       </c>
-      <c r="F31" s="733" t="str">
+      <c r="F31" s="706" t="str">
         <f>Namespace &amp; "has" &amp; ($B31) &amp; "Info"</f>
         <v>http://vocab.fairdatacollective.org/gdmt/hasCreatorAffiliationInfo</v>
       </c>
@@ -5125,7 +5122,7 @@
         <v>36</v>
       </c>
       <c r="L31" s="135" t="str">
-        <f>Namespace &amp; "has" &amp; SUBSTITUTE($H31, " ", "")</f>
+        <f t="shared" si="0"/>
         <v>http://vocab.fairdatacollective.org/gdmt/hasCreatorAffiliation</v>
       </c>
       <c r="M31" s="84" t="s">
@@ -5137,11 +5134,11 @@
     </row>
     <row r="32" spans="1:16" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="17"/>
-      <c r="B32" s="612"/>
-      <c r="C32" s="612"/>
-      <c r="D32" s="612"/>
-      <c r="E32" s="582"/>
-      <c r="F32" s="579"/>
+      <c r="B32" s="632"/>
+      <c r="C32" s="632"/>
+      <c r="D32" s="632"/>
+      <c r="E32" s="676"/>
+      <c r="F32" s="707"/>
       <c r="G32" s="87" t="s">
         <v>100</v>
       </c>
@@ -5158,7 +5155,7 @@
         <v>36</v>
       </c>
       <c r="L32" s="86" t="str">
-        <f>Namespace &amp; "has" &amp; SUBSTITUTE($H32, " ", "")</f>
+        <f t="shared" si="0"/>
         <v>http://vocab.fairdatacollective.org/gdmt/hasCreatorAffiliationIdentifier</v>
       </c>
       <c r="M32" s="84" t="s">
@@ -5170,11 +5167,11 @@
     </row>
     <row r="33" spans="1:16" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="17"/>
-      <c r="B33" s="612"/>
-      <c r="C33" s="612"/>
-      <c r="D33" s="612"/>
-      <c r="E33" s="582"/>
-      <c r="F33" s="579"/>
+      <c r="B33" s="632"/>
+      <c r="C33" s="632"/>
+      <c r="D33" s="632"/>
+      <c r="E33" s="676"/>
+      <c r="F33" s="707"/>
       <c r="G33" s="87" t="s">
         <v>103</v>
       </c>
@@ -5191,7 +5188,7 @@
         <v>36</v>
       </c>
       <c r="L33" s="86" t="str">
-        <f>Namespace &amp; "has" &amp; SUBSTITUTE($H33, " ", "")</f>
+        <f t="shared" si="0"/>
         <v>http://vocab.fairdatacollective.org/gdmt/hasCreatorAffiliationIdentifierScheme</v>
       </c>
       <c r="M33" s="89" t="str">
@@ -5204,11 +5201,11 @@
     </row>
     <row r="34" spans="1:16" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="17"/>
-      <c r="B34" s="613"/>
-      <c r="C34" s="613"/>
-      <c r="D34" s="613"/>
-      <c r="E34" s="583"/>
-      <c r="F34" s="580"/>
+      <c r="B34" s="633"/>
+      <c r="C34" s="633"/>
+      <c r="D34" s="633"/>
+      <c r="E34" s="677"/>
+      <c r="F34" s="708"/>
       <c r="G34" s="136" t="s">
         <v>105</v>
       </c>
@@ -5225,7 +5222,7 @@
         <v>36</v>
       </c>
       <c r="L34" s="139" t="str">
-        <f>Namespace &amp; "has" &amp; SUBSTITUTE($H34, " ", "")</f>
+        <f t="shared" si="0"/>
         <v>http://vocab.fairdatacollective.org/gdmt/hasCreatorAffiliationIdentifierSchemeIRI</v>
       </c>
       <c r="M34" s="143" t="str">
@@ -5337,11 +5334,11 @@
       </c>
     </row>
     <row r="38" spans="1:16" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="666" t="s">
+      <c r="A38" s="634" t="s">
         <v>107</v>
       </c>
-      <c r="B38" s="666"/>
-      <c r="C38" s="666"/>
+      <c r="B38" s="634"/>
+      <c r="C38" s="634"/>
       <c r="D38" s="377" t="s">
         <v>460</v>
       </c>
@@ -5363,17 +5360,17 @@
     </row>
     <row r="39" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="419"/>
-      <c r="B39" s="667" t="s">
+      <c r="B39" s="635" t="s">
         <v>461</v>
       </c>
-      <c r="C39" s="667"/>
-      <c r="D39" s="602" t="s">
+      <c r="C39" s="635"/>
+      <c r="D39" s="636" t="s">
         <v>477</v>
       </c>
-      <c r="E39" s="605" t="s">
+      <c r="E39" s="585" t="s">
         <v>34</v>
       </c>
-      <c r="F39" s="584" t="str">
+      <c r="F39" s="672" t="str">
         <f>Namespace &amp; "has" &amp; ($B39) &amp; "Info"</f>
         <v>http://vocab.fairdatacollective.org/gdmt/hasContributorNameInfo</v>
       </c>
@@ -5404,11 +5401,11 @@
     </row>
     <row r="40" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="419"/>
-      <c r="B40" s="667"/>
-      <c r="C40" s="667"/>
-      <c r="D40" s="603"/>
-      <c r="E40" s="606"/>
-      <c r="F40" s="585"/>
+      <c r="B40" s="635"/>
+      <c r="C40" s="635"/>
+      <c r="D40" s="637"/>
+      <c r="E40" s="586"/>
+      <c r="F40" s="673"/>
       <c r="G40" s="389" t="s">
         <v>111</v>
       </c>
@@ -5436,11 +5433,11 @@
     </row>
     <row r="41" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="419"/>
-      <c r="B41" s="667"/>
-      <c r="C41" s="667"/>
-      <c r="D41" s="604"/>
-      <c r="E41" s="607"/>
-      <c r="F41" s="586"/>
+      <c r="B41" s="635"/>
+      <c r="C41" s="635"/>
+      <c r="D41" s="638"/>
+      <c r="E41" s="587"/>
+      <c r="F41" s="674"/>
       <c r="G41" s="394" t="s">
         <v>113</v>
       </c>
@@ -5468,17 +5465,17 @@
     </row>
     <row r="42" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" s="419"/>
-      <c r="B42" s="602" t="s">
+      <c r="B42" s="636" t="s">
         <v>464</v>
       </c>
-      <c r="C42" s="602"/>
-      <c r="D42" s="602" t="s">
+      <c r="C42" s="636"/>
+      <c r="D42" s="636" t="s">
         <v>478</v>
       </c>
-      <c r="E42" s="605" t="s">
+      <c r="E42" s="585" t="s">
         <v>34</v>
       </c>
-      <c r="F42" s="584" t="str">
+      <c r="F42" s="672" t="str">
         <f>Namespace &amp; "has" &amp; ($B42) &amp; "Info"</f>
         <v>http://vocab.fairdatacollective.org/gdmt/hasContributorIdentifierInfo</v>
       </c>
@@ -5498,7 +5495,7 @@
         <v>36</v>
       </c>
       <c r="L42" s="388" t="str">
-        <f>Namespace &amp; "has" &amp; SUBSTITUTE($H42, " ", "")</f>
+        <f t="shared" ref="L42:L48" si="1">Namespace &amp; "has" &amp; SUBSTITUTE($H42, " ", "")</f>
         <v>http://vocab.fairdatacollective.org/gdmt/hasContributorIdentifier</v>
       </c>
       <c r="M42" s="385" t="s">
@@ -5510,11 +5507,11 @@
     </row>
     <row r="43" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="419"/>
-      <c r="B43" s="603"/>
-      <c r="C43" s="603"/>
-      <c r="D43" s="603"/>
-      <c r="E43" s="606"/>
-      <c r="F43" s="585"/>
+      <c r="B43" s="637"/>
+      <c r="C43" s="637"/>
+      <c r="D43" s="637"/>
+      <c r="E43" s="586"/>
+      <c r="F43" s="673"/>
       <c r="G43" s="389" t="s">
         <v>121</v>
       </c>
@@ -5531,7 +5528,7 @@
         <v>36</v>
       </c>
       <c r="L43" s="392" t="str">
-        <f>Namespace &amp; "has" &amp; SUBSTITUTE($H43, " ", "")</f>
+        <f t="shared" si="1"/>
         <v>http://vocab.fairdatacollective.org/gdmt/hasContributorIdentifierScheme</v>
       </c>
       <c r="M43" s="401" t="str">
@@ -5544,11 +5541,11 @@
     </row>
     <row r="44" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="419"/>
-      <c r="B44" s="604"/>
-      <c r="C44" s="604"/>
-      <c r="D44" s="604"/>
-      <c r="E44" s="607"/>
-      <c r="F44" s="586"/>
+      <c r="B44" s="638"/>
+      <c r="C44" s="638"/>
+      <c r="D44" s="638"/>
+      <c r="E44" s="587"/>
+      <c r="F44" s="674"/>
       <c r="G44" s="394" t="s">
         <v>122</v>
       </c>
@@ -5565,7 +5562,7 @@
         <v>36</v>
       </c>
       <c r="L44" s="397" t="str">
-        <f>Namespace &amp; "has" &amp; SUBSTITUTE($H44, " ", "")</f>
+        <f t="shared" si="1"/>
         <v>http://vocab.fairdatacollective.org/gdmt/hasContributorIdentifierSchemeIRI</v>
       </c>
       <c r="M44" s="402" t="str">
@@ -5578,17 +5575,17 @@
     </row>
     <row r="45" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="419"/>
-      <c r="B45" s="602" t="s">
+      <c r="B45" s="636" t="s">
         <v>465</v>
       </c>
-      <c r="C45" s="602"/>
-      <c r="D45" s="602" t="s">
+      <c r="C45" s="636"/>
+      <c r="D45" s="636" t="s">
         <v>479</v>
       </c>
-      <c r="E45" s="605" t="s">
+      <c r="E45" s="585" t="s">
         <v>34</v>
       </c>
-      <c r="F45" s="608" t="str">
+      <c r="F45" s="669" t="str">
         <f>Namespace &amp; "has" &amp; ($B45) &amp; "Info"</f>
         <v>http://vocab.fairdatacollective.org/gdmt/hasContributorAffiliationInfo</v>
       </c>
@@ -5608,7 +5605,7 @@
         <v>36</v>
       </c>
       <c r="L45" s="388" t="str">
-        <f>Namespace &amp; "has" &amp; SUBSTITUTE($H45, " ", "")</f>
+        <f t="shared" si="1"/>
         <v>http://vocab.fairdatacollective.org/gdmt/hasContributorAffiliation</v>
       </c>
       <c r="M45" s="385" t="s">
@@ -5620,11 +5617,11 @@
     </row>
     <row r="46" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="419"/>
-      <c r="B46" s="603"/>
-      <c r="C46" s="603"/>
-      <c r="D46" s="603"/>
-      <c r="E46" s="606"/>
-      <c r="F46" s="609"/>
+      <c r="B46" s="637"/>
+      <c r="C46" s="637"/>
+      <c r="D46" s="637"/>
+      <c r="E46" s="586"/>
+      <c r="F46" s="670"/>
       <c r="G46" s="389" t="s">
         <v>123</v>
       </c>
@@ -5641,7 +5638,7 @@
         <v>36</v>
       </c>
       <c r="L46" s="392" t="str">
-        <f>Namespace &amp; "has" &amp; SUBSTITUTE($H46, " ", "")</f>
+        <f t="shared" si="1"/>
         <v>http://vocab.fairdatacollective.org/gdmt/hasContributorAffiliationIdentifier</v>
       </c>
       <c r="M46" s="393" t="s">
@@ -5653,11 +5650,11 @@
     </row>
     <row r="47" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="419"/>
-      <c r="B47" s="603"/>
-      <c r="C47" s="603"/>
-      <c r="D47" s="603"/>
-      <c r="E47" s="606"/>
-      <c r="F47" s="609"/>
+      <c r="B47" s="637"/>
+      <c r="C47" s="637"/>
+      <c r="D47" s="637"/>
+      <c r="E47" s="586"/>
+      <c r="F47" s="670"/>
       <c r="G47" s="389" t="s">
         <v>458</v>
       </c>
@@ -5674,7 +5671,7 @@
         <v>36</v>
       </c>
       <c r="L47" s="392" t="str">
-        <f>Namespace &amp; "has" &amp; SUBSTITUTE($H47, " ", "")</f>
+        <f t="shared" si="1"/>
         <v>http://vocab.fairdatacollective.org/gdmt/hasContributorAffiliationIdentifierScheme</v>
       </c>
       <c r="M47" s="401" t="str">
@@ -5687,11 +5684,11 @@
     </row>
     <row r="48" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="419"/>
-      <c r="B48" s="604"/>
-      <c r="C48" s="604"/>
-      <c r="D48" s="604"/>
-      <c r="E48" s="607"/>
-      <c r="F48" s="610"/>
+      <c r="B48" s="638"/>
+      <c r="C48" s="638"/>
+      <c r="D48" s="638"/>
+      <c r="E48" s="587"/>
+      <c r="F48" s="671"/>
       <c r="G48" s="394" t="s">
         <v>125</v>
       </c>
@@ -5708,7 +5705,7 @@
         <v>36</v>
       </c>
       <c r="L48" s="397" t="str">
-        <f>Namespace &amp; "has" &amp; SUBSTITUTE($H48, " ", "")</f>
+        <f t="shared" si="1"/>
         <v>http://vocab.fairdatacollective.org/gdmt/hasContributorAffiliationIdentifierSchemeIRI</v>
       </c>
       <c r="M48" s="402" t="str">
@@ -5824,11 +5821,11 @@
       </c>
     </row>
     <row r="52" spans="1:16" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="668" t="s">
+      <c r="A52" s="639" t="s">
         <v>126</v>
       </c>
-      <c r="B52" s="668"/>
-      <c r="C52" s="668"/>
+      <c r="B52" s="639"/>
+      <c r="C52" s="639"/>
       <c r="D52" s="243" t="s">
         <v>435</v>
       </c>
@@ -5850,17 +5847,17 @@
     </row>
     <row r="53" spans="1:16" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="421"/>
-      <c r="B53" s="560" t="s">
+      <c r="B53" s="648" t="s">
         <v>472</v>
       </c>
-      <c r="C53" s="560"/>
-      <c r="D53" s="560" t="s">
+      <c r="C53" s="648"/>
+      <c r="D53" s="648" t="s">
         <v>473</v>
       </c>
-      <c r="E53" s="557" t="s">
+      <c r="E53" s="734" t="s">
         <v>54</v>
       </c>
-      <c r="F53" s="554" t="str">
+      <c r="F53" s="731" t="str">
         <f>Namespace &amp; "has" &amp; ($B53) &amp; "Info"</f>
         <v>http://vocab.fairdatacollective.org/gdmt/hasPublisherIdentifierInfo</v>
       </c>
@@ -5892,11 +5889,11 @@
     </row>
     <row r="54" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="421"/>
-      <c r="B54" s="561"/>
-      <c r="C54" s="561"/>
-      <c r="D54" s="561"/>
-      <c r="E54" s="558"/>
-      <c r="F54" s="555"/>
+      <c r="B54" s="649"/>
+      <c r="C54" s="649"/>
+      <c r="D54" s="649"/>
+      <c r="E54" s="735"/>
+      <c r="F54" s="732"/>
       <c r="G54" s="93" t="s">
         <v>136</v>
       </c>
@@ -5926,11 +5923,11 @@
     </row>
     <row r="55" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="421"/>
-      <c r="B55" s="562"/>
-      <c r="C55" s="562"/>
-      <c r="D55" s="562"/>
-      <c r="E55" s="559"/>
-      <c r="F55" s="556"/>
+      <c r="B55" s="650"/>
+      <c r="C55" s="650"/>
+      <c r="D55" s="650"/>
+      <c r="E55" s="736"/>
+      <c r="F55" s="733"/>
       <c r="G55" s="252" t="s">
         <v>137</v>
       </c>
@@ -6058,11 +6055,11 @@
       <c r="P58" s="10"/>
     </row>
     <row r="59" spans="1:16" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="651" t="s">
+      <c r="A59" s="660" t="s">
         <v>138</v>
       </c>
-      <c r="B59" s="651"/>
-      <c r="C59" s="651"/>
+      <c r="B59" s="660"/>
+      <c r="C59" s="660"/>
       <c r="D59" s="291" t="s">
         <v>139</v>
       </c>
@@ -6117,17 +6114,17 @@
     </row>
     <row r="61" spans="1:16" s="10" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A61" s="423"/>
-      <c r="B61" s="551" t="s">
+      <c r="B61" s="552" t="s">
         <v>482</v>
       </c>
-      <c r="C61" s="551"/>
-      <c r="D61" s="551" t="s">
+      <c r="C61" s="552"/>
+      <c r="D61" s="552" t="s">
         <v>483</v>
       </c>
-      <c r="E61" s="548" t="s">
+      <c r="E61" s="555" t="s">
         <v>46</v>
       </c>
-      <c r="F61" s="545" t="str">
+      <c r="F61" s="727" t="str">
         <f>Namespace &amp; "has" &amp; ($B61) &amp; "Info"</f>
         <v>http://vocab.fairdatacollective.org/gdmt/hasLicenseIdentifierInfo</v>
       </c>
@@ -6161,16 +6158,16 @@
     </row>
     <row r="62" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="423"/>
-      <c r="B62" s="552"/>
-      <c r="C62" s="552"/>
-      <c r="D62" s="552"/>
-      <c r="E62" s="549"/>
-      <c r="F62" s="546"/>
+      <c r="B62" s="553"/>
+      <c r="C62" s="553"/>
+      <c r="D62" s="553"/>
+      <c r="E62" s="556"/>
+      <c r="F62" s="728"/>
       <c r="G62" s="98" t="s">
         <v>148</v>
       </c>
       <c r="H62" s="98" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="I62" s="99" t="s">
         <v>380</v>
@@ -6194,16 +6191,16 @@
     </row>
     <row r="63" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="423"/>
-      <c r="B63" s="553"/>
-      <c r="C63" s="553"/>
-      <c r="D63" s="553"/>
-      <c r="E63" s="550"/>
-      <c r="F63" s="547"/>
+      <c r="B63" s="661"/>
+      <c r="C63" s="661"/>
+      <c r="D63" s="661"/>
+      <c r="E63" s="730"/>
+      <c r="F63" s="729"/>
       <c r="G63" s="285" t="s">
         <v>149</v>
       </c>
       <c r="H63" s="285" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="I63" s="286" t="s">
         <v>381</v>
@@ -6256,18 +6253,18 @@
       <c r="N64" s="272"/>
     </row>
     <row r="65" spans="1:14" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="734" t="s">
+      <c r="A65" s="627" t="s">
         <v>151</v>
       </c>
-      <c r="B65" s="734"/>
-      <c r="C65" s="734"/>
-      <c r="D65" s="643" t="s">
-        <v>517</v>
-      </c>
-      <c r="E65" s="644" t="s">
+      <c r="B65" s="627"/>
+      <c r="C65" s="627"/>
+      <c r="D65" s="653" t="s">
+        <v>516</v>
+      </c>
+      <c r="E65" s="655" t="s">
         <v>54</v>
       </c>
-      <c r="F65" s="643" t="str">
+      <c r="F65" s="653" t="str">
         <f>Namespace &amp; "has" &amp; ($A65) &amp; "Info"</f>
         <v>http://vocab.fairdatacollective.org/gdmt/hasDateInfo</v>
       </c>
@@ -6283,7 +6280,9 @@
       <c r="J65" s="301">
         <v>1</v>
       </c>
-      <c r="K65" s="302"/>
+      <c r="K65" s="302" t="s">
+        <v>20</v>
+      </c>
       <c r="L65" s="302" t="str">
         <f>Namespace &amp; "has" &amp; SUBSTITUTE($H65, " ", "")</f>
         <v>http://vocab.fairdatacollective.org/gdmt/hasDatasetDate</v>
@@ -6294,44 +6293,46 @@
       <c r="N65" s="303"/>
     </row>
     <row r="66" spans="1:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="735"/>
-      <c r="B66" s="735"/>
-      <c r="C66" s="735"/>
-      <c r="D66" s="736"/>
-      <c r="E66" s="737"/>
-      <c r="F66" s="736"/>
-      <c r="G66" s="738" t="s">
+      <c r="A66" s="628"/>
+      <c r="B66" s="628"/>
+      <c r="C66" s="628"/>
+      <c r="D66" s="654"/>
+      <c r="E66" s="656"/>
+      <c r="F66" s="654"/>
+      <c r="G66" s="535" t="s">
         <v>484</v>
       </c>
-      <c r="H66" s="738" t="s">
+      <c r="H66" s="535" t="s">
         <v>485</v>
       </c>
-      <c r="I66" s="739" t="s">
+      <c r="I66" s="536" t="s">
         <v>486</v>
       </c>
-      <c r="J66" s="740">
+      <c r="J66" s="537">
         <v>1</v>
       </c>
-      <c r="K66" s="741"/>
-      <c r="L66" s="741" t="str">
+      <c r="K66" s="538" t="s">
+        <v>20</v>
+      </c>
+      <c r="L66" s="538" t="str">
         <f>Namespace &amp; "has" &amp; SUBSTITUTE($H66, " ", "")</f>
         <v>http://vocab.fairdatacollective.org/gdmt/hasDatasetDateType</v>
       </c>
-      <c r="M66" s="742" t="str">
+      <c r="M66" s="539" t="str">
         <f>Namespace</f>
         <v>http://vocab.fairdatacollective.org/gdmt/</v>
       </c>
-      <c r="N66" s="742" t="s">
+      <c r="N66" s="539" t="s">
         <v>487</v>
       </c>
     </row>
     <row r="67" spans="1:14" s="14" customFormat="1" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="664" t="s">
+      <c r="A67" s="629" t="s">
         <v>154</v>
       </c>
-      <c r="B67" s="664"/>
-      <c r="C67" s="664"/>
-      <c r="D67" s="669" t="s">
+      <c r="B67" s="629"/>
+      <c r="C67" s="629"/>
+      <c r="D67" s="640" t="s">
         <v>159</v>
       </c>
       <c r="E67" s="360" t="s">
@@ -6352,9 +6353,9 @@
     </row>
     <row r="68" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="367"/>
-      <c r="B68" s="641"/>
-      <c r="C68" s="641"/>
-      <c r="D68" s="670"/>
+      <c r="B68" s="651"/>
+      <c r="C68" s="651"/>
+      <c r="D68" s="641"/>
       <c r="E68" s="311"/>
       <c r="F68" s="312"/>
       <c r="G68" s="313" t="s">
@@ -6388,7 +6389,7 @@
       <c r="A69" s="367"/>
       <c r="B69" s="368"/>
       <c r="C69" s="317"/>
-      <c r="D69" s="670"/>
+      <c r="D69" s="641"/>
       <c r="E69" s="319"/>
       <c r="F69" s="312"/>
       <c r="G69" s="313" t="s">
@@ -6422,7 +6423,7 @@
       <c r="A70" s="367"/>
       <c r="B70" s="368"/>
       <c r="C70" s="317"/>
-      <c r="D70" s="670"/>
+      <c r="D70" s="641"/>
       <c r="E70" s="320"/>
       <c r="F70" s="312"/>
       <c r="G70" s="305" t="s">
@@ -6444,17 +6445,17 @@
         <v>441</v>
       </c>
       <c r="M70" s="309" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="N70" s="309" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="71" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="367"/>
       <c r="B71" s="368"/>
       <c r="C71" s="317"/>
-      <c r="D71" s="670"/>
+      <c r="D71" s="641"/>
       <c r="E71" s="320"/>
       <c r="F71" s="312"/>
       <c r="G71" s="305" t="s">
@@ -6473,11 +6474,11 @@
         <v>20</v>
       </c>
       <c r="L71" s="316" t="str">
-        <f>Namespace &amp; "has" &amp; SUBSTITUTE($H71, " ", "")</f>
+        <f t="shared" ref="L71:L76" si="2">Namespace &amp; "has" &amp; SUBSTITUTE($H71, " ", "")</f>
         <v>http://vocab.fairdatacollective.org/gdmt/hasDistributionMediaType</v>
       </c>
       <c r="M71" s="309" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="N71" s="309" t="s">
         <v>28</v>
@@ -6487,7 +6488,7 @@
       <c r="A72" s="367"/>
       <c r="B72" s="368"/>
       <c r="C72" s="317"/>
-      <c r="D72" s="670"/>
+      <c r="D72" s="641"/>
       <c r="E72" s="319"/>
       <c r="F72" s="312"/>
       <c r="G72" s="305" t="s">
@@ -6506,7 +6507,7 @@
         <v>36</v>
       </c>
       <c r="L72" s="316" t="str">
-        <f>Namespace &amp; "has" &amp; SUBSTITUTE($H72, " ", "")</f>
+        <f t="shared" si="2"/>
         <v>http://vocab.fairdatacollective.org/gdmt/hasDistributionSize</v>
       </c>
       <c r="M72" s="309" t="s">
@@ -6518,17 +6519,19 @@
     </row>
     <row r="73" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="367"/>
-      <c r="B73" s="635" t="s">
+      <c r="B73" s="624" t="s">
         <v>488</v>
       </c>
-      <c r="C73" s="635"/>
-      <c r="D73" s="648" t="s">
+      <c r="C73" s="624"/>
+      <c r="D73" s="657" t="s">
         <v>489</v>
       </c>
-      <c r="E73" s="628">
+      <c r="E73" s="642">
         <v>1</v>
       </c>
-      <c r="F73" s="645"/>
+      <c r="F73" s="657" t="s">
+        <v>524</v>
+      </c>
       <c r="G73" s="321" t="s">
         <v>163</v>
       </c>
@@ -6544,8 +6547,8 @@
       <c r="K73" s="324" t="s">
         <v>36</v>
       </c>
-      <c r="L73" s="743" t="str">
-        <f>Namespace &amp; "has" &amp; SUBSTITUTE($H73, " ", "")</f>
+      <c r="L73" s="540" t="str">
+        <f t="shared" si="2"/>
         <v>http://vocab.fairdatacollective.org/gdmt/hasDistributionAccessProtocol</v>
       </c>
       <c r="M73" s="325" t="s">
@@ -6557,11 +6560,11 @@
     </row>
     <row r="74" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="367"/>
-      <c r="B74" s="636"/>
-      <c r="C74" s="636"/>
-      <c r="D74" s="649"/>
-      <c r="E74" s="629"/>
-      <c r="F74" s="646"/>
+      <c r="B74" s="625"/>
+      <c r="C74" s="625"/>
+      <c r="D74" s="658"/>
+      <c r="E74" s="643"/>
+      <c r="F74" s="658"/>
       <c r="G74" s="305" t="s">
         <v>164</v>
       </c>
@@ -6578,7 +6581,7 @@
         <v>36</v>
       </c>
       <c r="L74" s="316" t="str">
-        <f>Namespace &amp; "has" &amp; SUBSTITUTE($H74, " ", "")</f>
+        <f t="shared" si="2"/>
         <v>http://vocab.fairdatacollective.org/gdmt/hasDistributionAccessConfiguration</v>
       </c>
       <c r="M74" s="309" t="s">
@@ -6590,11 +6593,11 @@
     </row>
     <row r="75" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="367"/>
-      <c r="B75" s="637"/>
-      <c r="C75" s="637"/>
-      <c r="D75" s="650"/>
-      <c r="E75" s="630"/>
-      <c r="F75" s="647"/>
+      <c r="B75" s="626"/>
+      <c r="C75" s="626"/>
+      <c r="D75" s="659"/>
+      <c r="E75" s="644"/>
+      <c r="F75" s="659"/>
       <c r="G75" s="326" t="s">
         <v>447</v>
       </c>
@@ -6610,8 +6613,8 @@
       <c r="K75" s="329" t="s">
         <v>36</v>
       </c>
-      <c r="L75" s="744" t="str">
-        <f>Namespace &amp; "has" &amp; SUBSTITUTE($H75, " ", "")</f>
+      <c r="L75" s="541" t="str">
+        <f t="shared" si="2"/>
         <v>http://vocab.fairdatacollective.org/gdmt/hasDistributionQueryStatement</v>
       </c>
       <c r="M75" s="330" t="s">
@@ -6644,7 +6647,7 @@
         <v>20</v>
       </c>
       <c r="L76" s="316" t="str">
-        <f>Namespace &amp; "has" &amp; SUBSTITUTE($H76, " ", "")</f>
+        <f t="shared" si="2"/>
         <v>http://vocab.fairdatacollective.org/gdmt/hasDistributionDate</v>
       </c>
       <c r="M76" s="309" t="s">
@@ -6654,12 +6657,12 @@
     </row>
     <row r="77" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="367"/>
-      <c r="B77" s="642" t="s">
+      <c r="B77" s="652" t="s">
         <v>490</v>
       </c>
-      <c r="C77" s="642"/>
+      <c r="C77" s="652"/>
       <c r="D77" s="353" t="s">
-        <v>491</v>
+        <v>523</v>
       </c>
       <c r="E77" s="354" t="s">
         <v>54</v>
@@ -6679,17 +6682,17 @@
     </row>
     <row r="78" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="367"/>
-      <c r="B78" s="634"/>
-      <c r="C78" s="635" t="s">
+      <c r="B78" s="623"/>
+      <c r="C78" s="624" t="s">
+        <v>491</v>
+      </c>
+      <c r="D78" s="624" t="s">
         <v>492</v>
       </c>
-      <c r="D78" s="635" t="s">
-        <v>493</v>
-      </c>
-      <c r="E78" s="628">
+      <c r="E78" s="642">
         <v>1</v>
       </c>
-      <c r="F78" s="638" t="str">
+      <c r="F78" s="645" t="str">
         <f>Namespace &amp; "has" &amp; ($C78) &amp; "Info"</f>
         <v>http://vocab.fairdatacollective.org/gdmt/hasDistributorNameInfo</v>
       </c>
@@ -6720,11 +6723,11 @@
     </row>
     <row r="79" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="367"/>
-      <c r="B79" s="634"/>
-      <c r="C79" s="636"/>
-      <c r="D79" s="636"/>
-      <c r="E79" s="629"/>
-      <c r="F79" s="639"/>
+      <c r="B79" s="623"/>
+      <c r="C79" s="625"/>
+      <c r="D79" s="625"/>
+      <c r="E79" s="643"/>
+      <c r="F79" s="646"/>
       <c r="G79" s="349" t="s">
         <v>170</v>
       </c>
@@ -6752,16 +6755,16 @@
     </row>
     <row r="80" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="367"/>
-      <c r="B80" s="634"/>
-      <c r="C80" s="637"/>
-      <c r="D80" s="637"/>
-      <c r="E80" s="630"/>
-      <c r="F80" s="640"/>
+      <c r="B80" s="623"/>
+      <c r="C80" s="626"/>
+      <c r="D80" s="626"/>
+      <c r="E80" s="644"/>
+      <c r="F80" s="647"/>
       <c r="G80" s="335" t="s">
         <v>172</v>
       </c>
       <c r="H80" s="335" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="I80" s="336" t="s">
         <v>173</v>
@@ -6784,17 +6787,17 @@
     </row>
     <row r="81" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="367"/>
-      <c r="B81" s="634"/>
-      <c r="C81" s="635" t="s">
+      <c r="B81" s="623"/>
+      <c r="C81" s="624" t="s">
+        <v>494</v>
+      </c>
+      <c r="D81" s="624" t="s">
         <v>495</v>
       </c>
-      <c r="D81" s="635" t="s">
-        <v>496</v>
-      </c>
-      <c r="E81" s="628">
+      <c r="E81" s="642">
         <v>1</v>
       </c>
-      <c r="F81" s="638" t="str">
+      <c r="F81" s="645" t="str">
         <f>Namespace &amp; "has" &amp; ($C81) &amp; "Info"</f>
         <v>http://vocab.fairdatacollective.org/gdmt/hasDistributorIdentifierInfo</v>
       </c>
@@ -6813,8 +6816,8 @@
       <c r="K81" s="334" t="s">
         <v>20</v>
       </c>
-      <c r="L81" s="743" t="str">
-        <f>Namespace &amp; "has" &amp; SUBSTITUTE($H81, " ", "")</f>
+      <c r="L81" s="540" t="str">
+        <f t="shared" ref="L81:L87" si="3">Namespace &amp; "has" &amp; SUBSTITUTE($H81, " ", "")</f>
         <v>http://vocab.fairdatacollective.org/gdmt/hasDistributorIdentifier</v>
       </c>
       <c r="M81" s="331" t="s">
@@ -6826,11 +6829,11 @@
     </row>
     <row r="82" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="367"/>
-      <c r="B82" s="634"/>
-      <c r="C82" s="636"/>
-      <c r="D82" s="636"/>
-      <c r="E82" s="629"/>
-      <c r="F82" s="639"/>
+      <c r="B82" s="623"/>
+      <c r="C82" s="625"/>
+      <c r="D82" s="625"/>
+      <c r="E82" s="643"/>
+      <c r="F82" s="646"/>
       <c r="G82" s="349" t="s">
         <v>181</v>
       </c>
@@ -6847,7 +6850,7 @@
         <v>20</v>
       </c>
       <c r="L82" s="316" t="str">
-        <f>Namespace &amp; "has" &amp; SUBSTITUTE($H82, " ", "")</f>
+        <f t="shared" si="3"/>
         <v>http://vocab.fairdatacollective.org/gdmt/hasDistributorIdentifierScheme</v>
       </c>
       <c r="M82" s="369" t="str">
@@ -6860,11 +6863,11 @@
     </row>
     <row r="83" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="367"/>
-      <c r="B83" s="634"/>
-      <c r="C83" s="637"/>
-      <c r="D83" s="637"/>
-      <c r="E83" s="630"/>
-      <c r="F83" s="640"/>
+      <c r="B83" s="623"/>
+      <c r="C83" s="626"/>
+      <c r="D83" s="626"/>
+      <c r="E83" s="644"/>
+      <c r="F83" s="647"/>
       <c r="G83" s="335" t="s">
         <v>182</v>
       </c>
@@ -6880,8 +6883,8 @@
       <c r="K83" s="338" t="s">
         <v>20</v>
       </c>
-      <c r="L83" s="744" t="str">
-        <f>Namespace &amp; "has" &amp; SUBSTITUTE($H83, " ", "")</f>
+      <c r="L83" s="541" t="str">
+        <f t="shared" si="3"/>
         <v>http://vocab.fairdatacollective.org/gdmt/hasDistributorIdentifierSchemeIRI</v>
       </c>
       <c r="M83" s="339" t="str">
@@ -6894,17 +6897,17 @@
     </row>
     <row r="84" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="367"/>
-      <c r="B84" s="634"/>
-      <c r="C84" s="635" t="s">
+      <c r="B84" s="623"/>
+      <c r="C84" s="624" t="s">
+        <v>496</v>
+      </c>
+      <c r="D84" s="624" t="s">
         <v>497</v>
       </c>
-      <c r="D84" s="635" t="s">
-        <v>498</v>
-      </c>
-      <c r="E84" s="628" t="s">
+      <c r="E84" s="642" t="s">
         <v>54</v>
       </c>
-      <c r="F84" s="631" t="str">
+      <c r="F84" s="717" t="str">
         <f>Namespace &amp; "has" &amp; ($C84) &amp; "Info"</f>
         <v>http://vocab.fairdatacollective.org/gdmt/hasDistributorAffiliationInfo</v>
       </c>
@@ -6923,8 +6926,8 @@
       <c r="K84" s="334" t="s">
         <v>36</v>
       </c>
-      <c r="L84" s="743" t="str">
-        <f>Namespace &amp; "has" &amp; SUBSTITUTE($H84, " ", "")</f>
+      <c r="L84" s="540" t="str">
+        <f t="shared" si="3"/>
         <v>http://vocab.fairdatacollective.org/gdmt/hasDistributorAffiliation</v>
       </c>
       <c r="M84" s="331" t="s">
@@ -6936,11 +6939,11 @@
     </row>
     <row r="85" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="367"/>
-      <c r="B85" s="634"/>
-      <c r="C85" s="636"/>
-      <c r="D85" s="636"/>
-      <c r="E85" s="629"/>
-      <c r="F85" s="632"/>
+      <c r="B85" s="623"/>
+      <c r="C85" s="625"/>
+      <c r="D85" s="625"/>
+      <c r="E85" s="643"/>
+      <c r="F85" s="718"/>
       <c r="G85" s="349" t="s">
         <v>185</v>
       </c>
@@ -6957,7 +6960,7 @@
         <v>36</v>
       </c>
       <c r="L85" s="316" t="str">
-        <f>Namespace &amp; "has" &amp; SUBSTITUTE($H85, " ", "")</f>
+        <f t="shared" si="3"/>
         <v>http://vocab.fairdatacollective.org/gdmt/hasDistributorAffiliationIdentifier</v>
       </c>
       <c r="M85" s="349" t="s">
@@ -6969,11 +6972,11 @@
     </row>
     <row r="86" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="367"/>
-      <c r="B86" s="634"/>
-      <c r="C86" s="636"/>
-      <c r="D86" s="636"/>
-      <c r="E86" s="629"/>
-      <c r="F86" s="632"/>
+      <c r="B86" s="623"/>
+      <c r="C86" s="625"/>
+      <c r="D86" s="625"/>
+      <c r="E86" s="643"/>
+      <c r="F86" s="718"/>
       <c r="G86" s="349" t="s">
         <v>187</v>
       </c>
@@ -6990,7 +6993,7 @@
         <v>36</v>
       </c>
       <c r="L86" s="316" t="str">
-        <f>Namespace &amp; "has" &amp; SUBSTITUTE($H86, " ", "")</f>
+        <f t="shared" si="3"/>
         <v>http://vocab.fairdatacollective.org/gdmt/hasDistributorAffiliationIdentifierScheme</v>
       </c>
       <c r="M86" s="369" t="str">
@@ -7003,11 +7006,11 @@
     </row>
     <row r="87" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="367"/>
-      <c r="B87" s="634"/>
-      <c r="C87" s="637"/>
-      <c r="D87" s="637"/>
-      <c r="E87" s="630"/>
-      <c r="F87" s="633"/>
+      <c r="B87" s="623"/>
+      <c r="C87" s="626"/>
+      <c r="D87" s="626"/>
+      <c r="E87" s="644"/>
+      <c r="F87" s="719"/>
       <c r="G87" s="335" t="s">
         <v>188</v>
       </c>
@@ -7023,8 +7026,8 @@
       <c r="K87" s="338" t="s">
         <v>36</v>
       </c>
-      <c r="L87" s="744" t="str">
-        <f>Namespace &amp; "has" &amp; SUBSTITUTE($H87, " ", "")</f>
+      <c r="L87" s="541" t="str">
+        <f t="shared" si="3"/>
         <v>http://vocab.fairdatacollective.org/gdmt/hasDistributorAffiliationIdentifierSchemeIRI</v>
       </c>
       <c r="M87" s="339" t="str">
@@ -7138,11 +7141,11 @@
       <c r="P90"/>
     </row>
     <row r="91" spans="1:16" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A91" s="676" t="s">
+      <c r="A91" s="595" t="s">
         <v>189</v>
       </c>
-      <c r="B91" s="676"/>
-      <c r="C91" s="676"/>
+      <c r="B91" s="595"/>
+      <c r="C91" s="595"/>
       <c r="D91" s="425" t="s">
         <v>408</v>
       </c>
@@ -7164,17 +7167,17 @@
     </row>
     <row r="92" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="421"/>
-      <c r="B92" s="677" t="s">
+      <c r="B92" s="596" t="s">
         <v>283</v>
       </c>
-      <c r="C92" s="677"/>
-      <c r="D92" s="677" t="s">
+      <c r="C92" s="596"/>
+      <c r="D92" s="596" t="s">
         <v>287</v>
       </c>
-      <c r="E92" s="688" t="s">
+      <c r="E92" s="607" t="s">
         <v>54</v>
       </c>
-      <c r="F92" s="565" t="str">
+      <c r="F92" s="693" t="str">
         <f>Namespace &amp; "has" &amp; ($B92) &amp; "Info"</f>
         <v>http://vocab.fairdatacollective.org/gdmt/hasDataStreamInfo</v>
       </c>
@@ -7194,11 +7197,11 @@
         <v>20</v>
       </c>
       <c r="L92" s="441" t="str">
-        <f>Namespace &amp; "has" &amp; SUBSTITUTE($H92, " ", "")</f>
+        <f t="shared" ref="L92:L103" si="4">Namespace &amp; "has" &amp; SUBSTITUTE($H92, " ", "")</f>
         <v>http://vocab.fairdatacollective.org/gdmt/hasDataStream</v>
       </c>
       <c r="M92" s="442" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="N92" s="442" t="s">
         <v>28</v>
@@ -7206,11 +7209,11 @@
     </row>
     <row r="93" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="421"/>
-      <c r="B93" s="678"/>
-      <c r="C93" s="678"/>
-      <c r="D93" s="678"/>
-      <c r="E93" s="563"/>
-      <c r="F93" s="566"/>
+      <c r="B93" s="597"/>
+      <c r="C93" s="597"/>
+      <c r="D93" s="597"/>
+      <c r="E93" s="608"/>
+      <c r="F93" s="694"/>
       <c r="G93" s="105" t="s">
         <v>285</v>
       </c>
@@ -7227,11 +7230,11 @@
         <v>68</v>
       </c>
       <c r="L93" s="108" t="str">
-        <f>Namespace &amp; "has" &amp; SUBSTITUTE($H93, " ", "")</f>
+        <f t="shared" si="4"/>
         <v>http://vocab.fairdatacollective.org/gdmt/hasDataStreamIRI</v>
       </c>
       <c r="M93" s="109" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="N93" s="109" t="s">
         <v>28</v>
@@ -7239,11 +7242,11 @@
     </row>
     <row r="94" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="421"/>
-      <c r="B94" s="678"/>
-      <c r="C94" s="678"/>
-      <c r="D94" s="678"/>
-      <c r="E94" s="563"/>
-      <c r="F94" s="566"/>
+      <c r="B94" s="597"/>
+      <c r="C94" s="597"/>
+      <c r="D94" s="597"/>
+      <c r="E94" s="608"/>
+      <c r="F94" s="694"/>
       <c r="G94" s="109" t="s">
         <v>191</v>
       </c>
@@ -7260,11 +7263,11 @@
         <v>68</v>
       </c>
       <c r="L94" s="108" t="str">
-        <f>Namespace &amp; "has" &amp; SUBSTITUTE($H94, " ", "")</f>
+        <f t="shared" si="4"/>
         <v>http://vocab.fairdatacollective.org/gdmt/hasDataStreamScheme</v>
       </c>
       <c r="M94" s="109" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="N94" s="109" t="s">
         <v>28</v>
@@ -7272,11 +7275,11 @@
     </row>
     <row r="95" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="421"/>
-      <c r="B95" s="679"/>
-      <c r="C95" s="679"/>
-      <c r="D95" s="679"/>
-      <c r="E95" s="689"/>
-      <c r="F95" s="567"/>
+      <c r="B95" s="598"/>
+      <c r="C95" s="598"/>
+      <c r="D95" s="598"/>
+      <c r="E95" s="609"/>
+      <c r="F95" s="695"/>
       <c r="G95" s="443" t="s">
         <v>286</v>
       </c>
@@ -7293,11 +7296,11 @@
         <v>68</v>
       </c>
       <c r="L95" s="445" t="str">
-        <f>Namespace &amp; "has" &amp; SUBSTITUTE($H95, " ", "")</f>
+        <f t="shared" si="4"/>
         <v>http://vocab.fairdatacollective.org/gdmt/hasDataStreamSchemeIRI</v>
       </c>
       <c r="M95" s="446" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="N95" s="446" t="s">
         <v>28</v>
@@ -7305,17 +7308,17 @@
     </row>
     <row r="96" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" s="421"/>
-      <c r="B96" s="683"/>
-      <c r="C96" s="677" t="s">
+      <c r="B96" s="602"/>
+      <c r="C96" s="596" t="s">
         <v>281</v>
       </c>
-      <c r="D96" s="677" t="s">
+      <c r="D96" s="596" t="s">
         <v>366</v>
       </c>
-      <c r="E96" s="688">
+      <c r="E96" s="607">
         <v>1</v>
       </c>
-      <c r="F96" s="565" t="str">
+      <c r="F96" s="693" t="str">
         <f>Namespace &amp; "has" &amp; ($C96) &amp; "Info"</f>
         <v>http://vocab.fairdatacollective.org/gdmt/hasDataSourceInfo</v>
       </c>
@@ -7335,11 +7338,11 @@
         <v>20</v>
       </c>
       <c r="L96" s="441" t="str">
-        <f>Namespace &amp; "has" &amp; SUBSTITUTE($H96, " ", "")</f>
+        <f t="shared" si="4"/>
         <v>http://vocab.fairdatacollective.org/gdmt/hasDataSource</v>
       </c>
       <c r="M96" s="109" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="N96" s="442" t="s">
         <v>28</v>
@@ -7347,11 +7350,11 @@
     </row>
     <row r="97" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" s="421"/>
-      <c r="B97" s="683"/>
-      <c r="C97" s="678"/>
-      <c r="D97" s="678"/>
-      <c r="E97" s="563"/>
-      <c r="F97" s="566"/>
+      <c r="B97" s="602"/>
+      <c r="C97" s="597"/>
+      <c r="D97" s="597"/>
+      <c r="E97" s="608"/>
+      <c r="F97" s="694"/>
       <c r="G97" s="105" t="s">
         <v>195</v>
       </c>
@@ -7368,11 +7371,11 @@
         <v>36</v>
       </c>
       <c r="L97" s="108" t="str">
-        <f>Namespace &amp; "has" &amp; SUBSTITUTE($H97, " ", "")</f>
+        <f t="shared" si="4"/>
         <v>http://vocab.fairdatacollective.org/gdmt/hasDataSourceIRI</v>
       </c>
       <c r="M97" s="109" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="N97" s="109" t="s">
         <v>28</v>
@@ -7380,11 +7383,11 @@
     </row>
     <row r="98" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="421"/>
-      <c r="B98" s="683"/>
-      <c r="C98" s="678"/>
-      <c r="D98" s="678"/>
-      <c r="E98" s="563"/>
-      <c r="F98" s="566"/>
+      <c r="B98" s="602"/>
+      <c r="C98" s="597"/>
+      <c r="D98" s="597"/>
+      <c r="E98" s="608"/>
+      <c r="F98" s="694"/>
       <c r="G98" s="105" t="s">
         <v>197</v>
       </c>
@@ -7401,11 +7404,11 @@
         <v>68</v>
       </c>
       <c r="L98" s="108" t="str">
-        <f>Namespace &amp; "has" &amp; SUBSTITUTE($H98, " ", "")</f>
+        <f t="shared" si="4"/>
         <v>http://vocab.fairdatacollective.org/gdmt/hasDataSourceScheme</v>
       </c>
       <c r="M98" s="109" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="N98" s="109" t="s">
         <v>28</v>
@@ -7413,11 +7416,11 @@
     </row>
     <row r="99" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="421"/>
-      <c r="B99" s="683"/>
-      <c r="C99" s="679"/>
-      <c r="D99" s="679"/>
-      <c r="E99" s="689"/>
-      <c r="F99" s="567"/>
+      <c r="B99" s="602"/>
+      <c r="C99" s="598"/>
+      <c r="D99" s="598"/>
+      <c r="E99" s="609"/>
+      <c r="F99" s="695"/>
       <c r="G99" s="443" t="s">
         <v>198</v>
       </c>
@@ -7434,11 +7437,11 @@
         <v>68</v>
       </c>
       <c r="L99" s="445" t="str">
-        <f>Namespace &amp; "has" &amp; SUBSTITUTE($H99, " ", "")</f>
+        <f t="shared" si="4"/>
         <v>http://vocab.fairdatacollective.org/gdmt/hasDataSourceSchemaIRI</v>
       </c>
       <c r="M99" s="446" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="N99" s="446" t="s">
         <v>28</v>
@@ -7446,17 +7449,17 @@
     </row>
     <row r="100" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="421"/>
-      <c r="B100" s="683"/>
-      <c r="C100" s="677" t="s">
+      <c r="B100" s="602"/>
+      <c r="C100" s="596" t="s">
         <v>282</v>
       </c>
-      <c r="D100" s="677" t="s">
+      <c r="D100" s="596" t="s">
         <v>288</v>
       </c>
-      <c r="E100" s="688" t="s">
+      <c r="E100" s="607" t="s">
         <v>54</v>
       </c>
-      <c r="F100" s="745" t="str">
+      <c r="F100" s="696" t="str">
         <f>Namespace &amp; "has" &amp; ($C100) &amp; "Info"</f>
         <v>http://vocab.fairdatacollective.org/gdmt/hasVariableInfo</v>
       </c>
@@ -7476,11 +7479,11 @@
         <v>36</v>
       </c>
       <c r="L100" s="441" t="str">
-        <f>Namespace &amp; "has" &amp; SUBSTITUTE($H100, " ", "")</f>
+        <f t="shared" si="4"/>
         <v>http://vocab.fairdatacollective.org/gdmt/hasVariable</v>
       </c>
       <c r="M100" s="109" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="N100" s="109" t="s">
         <v>28</v>
@@ -7488,11 +7491,11 @@
     </row>
     <row r="101" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" s="421"/>
-      <c r="B101" s="683"/>
-      <c r="C101" s="678"/>
-      <c r="D101" s="678"/>
-      <c r="E101" s="563"/>
-      <c r="F101" s="568"/>
+      <c r="B101" s="602"/>
+      <c r="C101" s="597"/>
+      <c r="D101" s="597"/>
+      <c r="E101" s="608"/>
+      <c r="F101" s="697"/>
       <c r="G101" s="105" t="s">
         <v>290</v>
       </c>
@@ -7509,11 +7512,11 @@
         <v>68</v>
       </c>
       <c r="L101" s="108" t="str">
-        <f>Namespace &amp; "has" &amp; SUBSTITUTE($H101, " ", "")</f>
+        <f t="shared" si="4"/>
         <v>http://vocab.fairdatacollective.org/gdmt/hasVariableIRI</v>
       </c>
       <c r="M101" s="109" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="N101" s="109" t="s">
         <v>28</v>
@@ -7521,11 +7524,11 @@
     </row>
     <row r="102" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A102" s="421"/>
-      <c r="B102" s="683"/>
-      <c r="C102" s="678"/>
-      <c r="D102" s="678"/>
-      <c r="E102" s="563"/>
-      <c r="F102" s="568"/>
+      <c r="B102" s="602"/>
+      <c r="C102" s="597"/>
+      <c r="D102" s="597"/>
+      <c r="E102" s="608"/>
+      <c r="F102" s="697"/>
       <c r="G102" s="105" t="s">
         <v>291</v>
       </c>
@@ -7542,11 +7545,11 @@
         <v>68</v>
       </c>
       <c r="L102" s="108" t="str">
-        <f>Namespace &amp; "has" &amp; SUBSTITUTE($H102, " ", "")</f>
+        <f t="shared" si="4"/>
         <v>http://vocab.fairdatacollective.org/gdmt/hasVariableScheme</v>
       </c>
       <c r="M102" s="109" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="N102" s="109" t="s">
         <v>28</v>
@@ -7554,11 +7557,11 @@
     </row>
     <row r="103" spans="1:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A103" s="422"/>
-      <c r="B103" s="684"/>
-      <c r="C103" s="687"/>
-      <c r="D103" s="687"/>
-      <c r="E103" s="564"/>
-      <c r="F103" s="569"/>
+      <c r="B103" s="603"/>
+      <c r="C103" s="606"/>
+      <c r="D103" s="606"/>
+      <c r="E103" s="692"/>
+      <c r="F103" s="698"/>
       <c r="G103" s="433" t="s">
         <v>292</v>
       </c>
@@ -7575,22 +7578,22 @@
         <v>68</v>
       </c>
       <c r="L103" s="436" t="str">
-        <f>Namespace &amp; "has" &amp; SUBSTITUTE($H103, " ", "")</f>
+        <f t="shared" si="4"/>
         <v>http://vocab.fairdatacollective.org/gdmt/hasVariableSchemeIRI</v>
       </c>
       <c r="M103" s="437" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="N103" s="437" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="104" spans="1:14" s="14" customFormat="1" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A104" s="680" t="s">
+      <c r="A104" s="599" t="s">
         <v>201</v>
       </c>
-      <c r="B104" s="680"/>
-      <c r="C104" s="680"/>
+      <c r="B104" s="599"/>
+      <c r="C104" s="599"/>
       <c r="D104" s="473" t="s">
         <v>202</v>
       </c>
@@ -7612,17 +7615,17 @@
     </row>
     <row r="105" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A105" s="419"/>
-      <c r="B105" s="661" t="s">
-        <v>502</v>
-      </c>
-      <c r="C105" s="661"/>
-      <c r="D105" s="681" t="s">
+      <c r="B105" s="591" t="s">
         <v>501</v>
       </c>
-      <c r="E105" s="685" t="s">
+      <c r="C105" s="591"/>
+      <c r="D105" s="600" t="s">
+        <v>500</v>
+      </c>
+      <c r="E105" s="604" t="s">
         <v>46</v>
       </c>
-      <c r="F105" s="671" t="str">
+      <c r="F105" s="588" t="str">
         <f>Namespace &amp; "has" &amp; ($B105) &amp; "Info"</f>
         <v>http://vocab.fairdatacollective.org/gdmt/hasSpatialCoveragePointInfo</v>
       </c>
@@ -7642,7 +7645,7 @@
         <v>68</v>
       </c>
       <c r="L105" s="451" t="str">
-        <f>Namespace &amp; "has" &amp; SUBSTITUTE($H105, " ", "")</f>
+        <f t="shared" ref="L105:L125" si="5">Namespace &amp; "has" &amp; SUBSTITUTE($H105, " ", "")</f>
         <v>http://vocab.fairdatacollective.org/gdmt/hasPointLatitude</v>
       </c>
       <c r="M105" s="452" t="s">
@@ -7654,11 +7657,11 @@
     </row>
     <row r="106" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A106" s="419"/>
-      <c r="B106" s="663"/>
-      <c r="C106" s="663"/>
-      <c r="D106" s="682"/>
-      <c r="E106" s="686"/>
-      <c r="F106" s="673"/>
+      <c r="B106" s="592"/>
+      <c r="C106" s="592"/>
+      <c r="D106" s="601"/>
+      <c r="E106" s="605"/>
+      <c r="F106" s="590"/>
       <c r="G106" s="453" t="s">
         <v>203</v>
       </c>
@@ -7675,7 +7678,7 @@
         <v>68</v>
       </c>
       <c r="L106" s="456" t="str">
-        <f>Namespace &amp; "has" &amp; SUBSTITUTE($H106, " ", "")</f>
+        <f t="shared" si="5"/>
         <v>http://vocab.fairdatacollective.org/gdmt/hasPointLongitude</v>
       </c>
       <c r="M106" s="457" t="s">
@@ -7687,17 +7690,17 @@
     </row>
     <row r="107" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A107" s="419"/>
-      <c r="B107" s="661" t="s">
+      <c r="B107" s="591" t="s">
+        <v>502</v>
+      </c>
+      <c r="C107" s="591"/>
+      <c r="D107" s="591" t="s">
         <v>503</v>
       </c>
-      <c r="C107" s="661"/>
-      <c r="D107" s="661" t="s">
-        <v>504</v>
-      </c>
-      <c r="E107" s="605" t="s">
+      <c r="E107" s="585" t="s">
         <v>46</v>
       </c>
-      <c r="F107" s="671" t="str">
+      <c r="F107" s="588" t="str">
         <f>Namespace &amp; "has" &amp; ($B107) &amp; "Info"</f>
         <v>http://vocab.fairdatacollective.org/gdmt/hasSpatialCoverageBoundingBoxInfo</v>
       </c>
@@ -7717,7 +7720,7 @@
         <v>68</v>
       </c>
       <c r="L107" s="451" t="str">
-        <f>Namespace &amp; "has" &amp; SUBSTITUTE($H107, " ", "")</f>
+        <f t="shared" si="5"/>
         <v>http://vocab.fairdatacollective.org/gdmt/hasWestLongitudinalBoundary</v>
       </c>
       <c r="M107" s="462" t="s">
@@ -7729,11 +7732,11 @@
     </row>
     <row r="108" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A108" s="419"/>
-      <c r="B108" s="662"/>
-      <c r="C108" s="662"/>
-      <c r="D108" s="662"/>
-      <c r="E108" s="606"/>
-      <c r="F108" s="672"/>
+      <c r="B108" s="622"/>
+      <c r="C108" s="622"/>
+      <c r="D108" s="622"/>
+      <c r="E108" s="586"/>
+      <c r="F108" s="589"/>
       <c r="G108" s="463" t="s">
         <v>209</v>
       </c>
@@ -7749,8 +7752,8 @@
       <c r="K108" s="466" t="s">
         <v>68</v>
       </c>
-      <c r="L108" s="746" t="str">
-        <f>Namespace &amp; "has" &amp; SUBSTITUTE($H108, " ", "")</f>
+      <c r="L108" s="542" t="str">
+        <f t="shared" si="5"/>
         <v>http://vocab.fairdatacollective.org/gdmt/hasEastLongitudinalBoundary</v>
       </c>
       <c r="M108" s="467" t="s">
@@ -7762,11 +7765,11 @@
     </row>
     <row r="109" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A109" s="419"/>
-      <c r="B109" s="662"/>
-      <c r="C109" s="662"/>
-      <c r="D109" s="662"/>
-      <c r="E109" s="606"/>
-      <c r="F109" s="672"/>
+      <c r="B109" s="622"/>
+      <c r="C109" s="622"/>
+      <c r="D109" s="622"/>
+      <c r="E109" s="586"/>
+      <c r="F109" s="589"/>
       <c r="G109" s="463" t="s">
         <v>211</v>
       </c>
@@ -7782,8 +7785,8 @@
       <c r="K109" s="466" t="s">
         <v>68</v>
       </c>
-      <c r="L109" s="746" t="str">
-        <f>Namespace &amp; "has" &amp; SUBSTITUTE($H109, " ", "")</f>
+      <c r="L109" s="542" t="str">
+        <f t="shared" si="5"/>
         <v>http://vocab.fairdatacollective.org/gdmt/hasSouthLongitudinalBoundary</v>
       </c>
       <c r="M109" s="467" t="s">
@@ -7795,11 +7798,11 @@
     </row>
     <row r="110" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A110" s="419"/>
-      <c r="B110" s="663"/>
-      <c r="C110" s="663"/>
-      <c r="D110" s="663"/>
-      <c r="E110" s="607"/>
-      <c r="F110" s="673"/>
+      <c r="B110" s="592"/>
+      <c r="C110" s="592"/>
+      <c r="D110" s="592"/>
+      <c r="E110" s="587"/>
+      <c r="F110" s="590"/>
       <c r="G110" s="468" t="s">
         <v>213</v>
       </c>
@@ -7816,7 +7819,7 @@
         <v>68</v>
       </c>
       <c r="L110" s="456" t="str">
-        <f>Namespace &amp; "has" &amp; SUBSTITUTE($H110, " ", "")</f>
+        <f t="shared" si="5"/>
         <v>http://vocab.fairdatacollective.org/gdmt/hasNorthLongitudinalBoundary</v>
       </c>
       <c r="M110" s="472" t="s">
@@ -7828,17 +7831,17 @@
     </row>
     <row r="111" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A111" s="419"/>
-      <c r="B111" s="661" t="s">
+      <c r="B111" s="591" t="s">
+        <v>504</v>
+      </c>
+      <c r="C111" s="591"/>
+      <c r="D111" s="593" t="s">
         <v>505</v>
       </c>
-      <c r="C111" s="661"/>
-      <c r="D111" s="674" t="s">
-        <v>506</v>
-      </c>
-      <c r="E111" s="605" t="s">
+      <c r="E111" s="585" t="s">
         <v>46</v>
       </c>
-      <c r="F111" s="671" t="str">
+      <c r="F111" s="588" t="str">
         <f>Namespace &amp; "has" &amp; ($B111) &amp; "Info"</f>
         <v>http://vocab.fairdatacollective.org/gdmt/hasSpatialCoveragePolygonInfo</v>
       </c>
@@ -7858,7 +7861,7 @@
         <v>68</v>
       </c>
       <c r="L111" s="451" t="str">
-        <f>Namespace &amp; "has" &amp; SUBSTITUTE($H111, " ", "")</f>
+        <f t="shared" si="5"/>
         <v>http://vocab.fairdatacollective.org/gdmt/hasPolygonPointLatitude</v>
       </c>
       <c r="M111" s="462" t="s">
@@ -7870,11 +7873,11 @@
     </row>
     <row r="112" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A112" s="419"/>
-      <c r="B112" s="663"/>
-      <c r="C112" s="663"/>
-      <c r="D112" s="675"/>
-      <c r="E112" s="607"/>
-      <c r="F112" s="673"/>
+      <c r="B112" s="592"/>
+      <c r="C112" s="592"/>
+      <c r="D112" s="594"/>
+      <c r="E112" s="587"/>
+      <c r="F112" s="590"/>
       <c r="G112" s="453" t="s">
         <v>437</v>
       </c>
@@ -7891,7 +7894,7 @@
         <v>68</v>
       </c>
       <c r="L112" s="456" t="str">
-        <f>Namespace &amp; "has" &amp; SUBSTITUTE($H112, " ", "")</f>
+        <f t="shared" si="5"/>
         <v>http://vocab.fairdatacollective.org/gdmt/hasPolygonPointLongitude</v>
       </c>
       <c r="M112" s="472" t="s">
@@ -7924,7 +7927,7 @@
         <v>68</v>
       </c>
       <c r="L113" s="451" t="str">
-        <f>Namespace &amp; "has" &amp; SUBSTITUTE($H113, " ", "")</f>
+        <f t="shared" si="5"/>
         <v>http://vocab.fairdatacollective.org/gdmt/hasGeospatialLocationDescription</v>
       </c>
       <c r="M113" s="487" t="s">
@@ -7935,18 +7938,18 @@
       </c>
     </row>
     <row r="114" spans="1:14" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A114" s="702" t="s">
+      <c r="A114" s="559" t="s">
         <v>217</v>
       </c>
-      <c r="B114" s="702"/>
-      <c r="C114" s="702"/>
-      <c r="D114" s="719" t="s">
+      <c r="B114" s="559"/>
+      <c r="C114" s="559"/>
+      <c r="D114" s="576" t="s">
         <v>218</v>
       </c>
-      <c r="E114" s="710" t="s">
+      <c r="E114" s="567" t="s">
         <v>46</v>
       </c>
-      <c r="F114" s="713" t="str">
+      <c r="F114" s="570" t="str">
         <f>Namespace &amp; "has" &amp; ($A114) &amp; "Info"</f>
         <v>http://vocab.fairdatacollective.org/gdmt/hasVerticalCoverageInfo</v>
       </c>
@@ -7966,7 +7969,7 @@
         <v>68</v>
       </c>
       <c r="L114" s="491" t="str">
-        <f>Namespace &amp; "has" &amp; SUBSTITUTE($H114, " ", "")</f>
+        <f t="shared" si="5"/>
         <v>http://vocab.fairdatacollective.org/gdmt/hasVerticalExtentMaximumValue</v>
       </c>
       <c r="M114" s="492" t="s">
@@ -7977,12 +7980,12 @@
       </c>
     </row>
     <row r="115" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A115" s="703"/>
-      <c r="B115" s="703"/>
-      <c r="C115" s="703"/>
-      <c r="D115" s="720"/>
-      <c r="E115" s="711"/>
-      <c r="F115" s="714"/>
+      <c r="A115" s="560"/>
+      <c r="B115" s="560"/>
+      <c r="C115" s="560"/>
+      <c r="D115" s="577"/>
+      <c r="E115" s="568"/>
+      <c r="F115" s="571"/>
       <c r="G115" s="111" t="s">
         <v>221</v>
       </c>
@@ -7999,7 +8002,7 @@
         <v>68</v>
       </c>
       <c r="L115" s="114" t="str">
-        <f>Namespace &amp; "has" &amp; SUBSTITUTE($H115, " ", "")</f>
+        <f t="shared" si="5"/>
         <v>http://vocab.fairdatacollective.org/gdmt/hasVerticalExtentMinimumValue</v>
       </c>
       <c r="M115" s="115" t="s">
@@ -8010,12 +8013,12 @@
       </c>
     </row>
     <row r="116" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A116" s="703"/>
-      <c r="B116" s="703"/>
-      <c r="C116" s="703"/>
-      <c r="D116" s="720"/>
-      <c r="E116" s="711"/>
-      <c r="F116" s="714"/>
+      <c r="A116" s="560"/>
+      <c r="B116" s="560"/>
+      <c r="C116" s="560"/>
+      <c r="D116" s="577"/>
+      <c r="E116" s="568"/>
+      <c r="F116" s="571"/>
       <c r="G116" s="111" t="s">
         <v>223</v>
       </c>
@@ -8032,7 +8035,7 @@
         <v>68</v>
       </c>
       <c r="L116" s="114" t="str">
-        <f>Namespace &amp; "has" &amp; SUBSTITUTE($H116, " ", "")</f>
+        <f t="shared" si="5"/>
         <v>http://vocab.fairdatacollective.org/gdmt/hasVerticalExtentUnit</v>
       </c>
       <c r="M116" s="115" t="s">
@@ -8043,12 +8046,12 @@
       </c>
     </row>
     <row r="117" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A117" s="703"/>
-      <c r="B117" s="703"/>
-      <c r="C117" s="703"/>
-      <c r="D117" s="720"/>
-      <c r="E117" s="711"/>
-      <c r="F117" s="714"/>
+      <c r="A117" s="560"/>
+      <c r="B117" s="560"/>
+      <c r="C117" s="560"/>
+      <c r="D117" s="577"/>
+      <c r="E117" s="568"/>
+      <c r="F117" s="571"/>
       <c r="G117" s="111" t="s">
         <v>224</v>
       </c>
@@ -8065,7 +8068,7 @@
         <v>68</v>
       </c>
       <c r="L117" s="114" t="str">
-        <f>Namespace &amp; "has" &amp; SUBSTITUTE($H117, " ", "")</f>
+        <f t="shared" si="5"/>
         <v>http://vocab.fairdatacollective.org/gdmt/hasVerticalExtentUnitIRI</v>
       </c>
       <c r="M117" s="115" t="s">
@@ -8076,12 +8079,12 @@
       </c>
     </row>
     <row r="118" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A118" s="703"/>
-      <c r="B118" s="703"/>
-      <c r="C118" s="703"/>
-      <c r="D118" s="720"/>
-      <c r="E118" s="711"/>
-      <c r="F118" s="714"/>
+      <c r="A118" s="560"/>
+      <c r="B118" s="560"/>
+      <c r="C118" s="560"/>
+      <c r="D118" s="577"/>
+      <c r="E118" s="568"/>
+      <c r="F118" s="571"/>
       <c r="G118" s="111" t="s">
         <v>225</v>
       </c>
@@ -8098,7 +8101,7 @@
         <v>68</v>
       </c>
       <c r="L118" s="114" t="str">
-        <f>Namespace &amp; "has" &amp; SUBSTITUTE($H118, " ", "")</f>
+        <f t="shared" si="5"/>
         <v>http://vocab.fairdatacollective.org/gdmt/hasVerticalExtentUnitScheme</v>
       </c>
       <c r="M118" s="115" t="s">
@@ -8109,12 +8112,12 @@
       </c>
     </row>
     <row r="119" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A119" s="703"/>
-      <c r="B119" s="703"/>
-      <c r="C119" s="703"/>
-      <c r="D119" s="720"/>
-      <c r="E119" s="711"/>
-      <c r="F119" s="714"/>
+      <c r="A119" s="560"/>
+      <c r="B119" s="560"/>
+      <c r="C119" s="560"/>
+      <c r="D119" s="577"/>
+      <c r="E119" s="568"/>
+      <c r="F119" s="571"/>
       <c r="G119" s="111" t="s">
         <v>226</v>
       </c>
@@ -8131,7 +8134,7 @@
         <v>68</v>
       </c>
       <c r="L119" s="114" t="str">
-        <f>Namespace &amp; "has" &amp; SUBSTITUTE($H119, " ", "")</f>
+        <f t="shared" si="5"/>
         <v>http://vocab.fairdatacollective.org/gdmt/hasVerticalExtentUnitSchemeURI</v>
       </c>
       <c r="M119" s="115" t="s">
@@ -8142,12 +8145,12 @@
       </c>
     </row>
     <row r="120" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A120" s="703"/>
-      <c r="B120" s="703"/>
-      <c r="C120" s="703"/>
-      <c r="D120" s="720"/>
-      <c r="E120" s="711"/>
-      <c r="F120" s="714"/>
+      <c r="A120" s="560"/>
+      <c r="B120" s="560"/>
+      <c r="C120" s="560"/>
+      <c r="D120" s="577"/>
+      <c r="E120" s="568"/>
+      <c r="F120" s="571"/>
       <c r="G120" s="111" t="s">
         <v>396</v>
       </c>
@@ -8164,7 +8167,7 @@
         <v>68</v>
       </c>
       <c r="L120" s="114" t="str">
-        <f>Namespace &amp; "has" &amp; SUBSTITUTE($H120, " ", "")</f>
+        <f t="shared" si="5"/>
         <v>http://vocab.fairdatacollective.org/gdmt/hasVerticalExtentDatum</v>
       </c>
       <c r="M120" s="115" t="s">
@@ -8175,12 +8178,12 @@
       </c>
     </row>
     <row r="121" spans="1:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A121" s="704"/>
-      <c r="B121" s="704"/>
-      <c r="C121" s="704"/>
-      <c r="D121" s="721"/>
-      <c r="E121" s="712"/>
-      <c r="F121" s="715"/>
+      <c r="A121" s="561"/>
+      <c r="B121" s="561"/>
+      <c r="C121" s="561"/>
+      <c r="D121" s="578"/>
+      <c r="E121" s="569"/>
+      <c r="F121" s="572"/>
       <c r="G121" s="534" t="s">
         <v>406</v>
       </c>
@@ -8197,7 +8200,7 @@
         <v>68</v>
       </c>
       <c r="L121" s="495" t="str">
-        <f>Namespace &amp; "has" &amp; SUBSTITUTE($H121, " ", "")</f>
+        <f t="shared" si="5"/>
         <v>http://vocab.fairdatacollective.org/gdmt/hasVerticalExtentDatumIRI</v>
       </c>
       <c r="M121" s="496" t="s">
@@ -8208,18 +8211,18 @@
       </c>
     </row>
     <row r="122" spans="1:14" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A122" s="705" t="s">
+      <c r="A122" s="562" t="s">
         <v>227</v>
       </c>
-      <c r="B122" s="705"/>
-      <c r="C122" s="705"/>
-      <c r="D122" s="716" t="s">
+      <c r="B122" s="562"/>
+      <c r="C122" s="562"/>
+      <c r="D122" s="573" t="s">
         <v>228</v>
       </c>
-      <c r="E122" s="722" t="s">
+      <c r="E122" s="579" t="s">
         <v>46</v>
       </c>
-      <c r="F122" s="723" t="str">
+      <c r="F122" s="582" t="str">
         <f>Namespace &amp; "has" &amp; ($A122) &amp; "Info"</f>
         <v>http://vocab.fairdatacollective.org/gdmt/hasTemporalCoverageInfo</v>
       </c>
@@ -8239,7 +8242,7 @@
         <v>36</v>
       </c>
       <c r="L122" s="500" t="str">
-        <f>Namespace &amp; "has" &amp; SUBSTITUTE($H122, " ", "")</f>
+        <f t="shared" si="5"/>
         <v>http://vocab.fairdatacollective.org/gdmt/hasTemporalExtentMinimumValue</v>
       </c>
       <c r="M122" s="501" t="s">
@@ -8250,12 +8253,12 @@
       </c>
     </row>
     <row r="123" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A123" s="706"/>
-      <c r="B123" s="706"/>
-      <c r="C123" s="706"/>
-      <c r="D123" s="717"/>
-      <c r="E123" s="574"/>
-      <c r="F123" s="724"/>
+      <c r="A123" s="563"/>
+      <c r="B123" s="563"/>
+      <c r="C123" s="563"/>
+      <c r="D123" s="574"/>
+      <c r="E123" s="580"/>
+      <c r="F123" s="583"/>
       <c r="G123" s="116" t="s">
         <v>231</v>
       </c>
@@ -8272,7 +8275,7 @@
         <v>36</v>
       </c>
       <c r="L123" s="119" t="str">
-        <f>Namespace &amp; "has" &amp; SUBSTITUTE($H123, " ", "")</f>
+        <f t="shared" si="5"/>
         <v>http://vocab.fairdatacollective.org/gdmt/hasTemporalExtentMaximumValue</v>
       </c>
       <c r="M123" s="120" t="s">
@@ -8283,12 +8286,12 @@
       </c>
     </row>
     <row r="124" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A124" s="706"/>
-      <c r="B124" s="706"/>
-      <c r="C124" s="706"/>
-      <c r="D124" s="717"/>
-      <c r="E124" s="574"/>
-      <c r="F124" s="724"/>
+      <c r="A124" s="563"/>
+      <c r="B124" s="563"/>
+      <c r="C124" s="563"/>
+      <c r="D124" s="574"/>
+      <c r="E124" s="580"/>
+      <c r="F124" s="583"/>
       <c r="G124" s="116" t="s">
         <v>233</v>
       </c>
@@ -8305,7 +8308,7 @@
         <v>36</v>
       </c>
       <c r="L124" s="119" t="str">
-        <f>Namespace &amp; "has" &amp; SUBSTITUTE($H124, " ", "")</f>
+        <f t="shared" si="5"/>
         <v>http://vocab.fairdatacollective.org/gdmt/hasTemporalResolution</v>
       </c>
       <c r="M124" s="120" t="s">
@@ -8316,12 +8319,12 @@
       </c>
     </row>
     <row r="125" spans="1:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A125" s="707"/>
-      <c r="B125" s="707"/>
-      <c r="C125" s="707"/>
-      <c r="D125" s="718"/>
-      <c r="E125" s="575"/>
-      <c r="F125" s="725"/>
+      <c r="A125" s="564"/>
+      <c r="B125" s="564"/>
+      <c r="C125" s="564"/>
+      <c r="D125" s="575"/>
+      <c r="E125" s="581"/>
+      <c r="F125" s="584"/>
       <c r="G125" s="502" t="s">
         <v>235</v>
       </c>
@@ -8338,7 +8341,7 @@
         <v>36</v>
       </c>
       <c r="L125" s="505" t="str">
-        <f>Namespace &amp; "has" &amp; SUBSTITUTE($H125, " ", "")</f>
+        <f t="shared" si="5"/>
         <v>http://vocab.fairdatacollective.org/gdmt/hasDuration</v>
       </c>
       <c r="M125" s="506" t="s">
@@ -8349,13 +8352,13 @@
       </c>
     </row>
     <row r="126" spans="1:14" s="14" customFormat="1" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A126" s="708" t="s">
+      <c r="A126" s="565" t="s">
         <v>237</v>
       </c>
-      <c r="B126" s="708"/>
-      <c r="C126" s="708"/>
+      <c r="B126" s="565"/>
+      <c r="C126" s="565"/>
       <c r="D126" s="512" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="E126" s="513" t="s">
         <v>34</v>
@@ -8375,17 +8378,17 @@
     </row>
     <row r="127" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A127" s="423"/>
-      <c r="B127" s="696" t="s">
-        <v>508</v>
-      </c>
-      <c r="C127" s="696"/>
-      <c r="D127" s="690" t="s">
-        <v>511</v>
-      </c>
-      <c r="E127" s="693">
+      <c r="B127" s="549" t="s">
+        <v>507</v>
+      </c>
+      <c r="C127" s="549"/>
+      <c r="D127" s="543" t="s">
+        <v>510</v>
+      </c>
+      <c r="E127" s="546">
         <v>1</v>
       </c>
-      <c r="F127" s="690" t="str">
+      <c r="F127" s="543" t="str">
         <f>Namespace &amp; "has" &amp; ($B127) &amp; "Info"</f>
         <v>http://vocab.fairdatacollective.org/gdmt/hasAwardInfo</v>
       </c>
@@ -8405,7 +8408,7 @@
         <v>36</v>
       </c>
       <c r="L127" s="527" t="str">
-        <f>Namespace &amp; "has" &amp; SUBSTITUTE($H127, " ", "")</f>
+        <f t="shared" ref="L127:L133" si="6">Namespace &amp; "has" &amp; SUBSTITUTE($H127, " ", "")</f>
         <v>http://vocab.fairdatacollective.org/gdmt/hasAwardTitle</v>
       </c>
       <c r="M127" s="524" t="s">
@@ -8417,11 +8420,11 @@
     </row>
     <row r="128" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A128" s="423"/>
-      <c r="B128" s="697"/>
-      <c r="C128" s="697"/>
-      <c r="D128" s="691"/>
-      <c r="E128" s="694"/>
-      <c r="F128" s="691"/>
+      <c r="B128" s="550"/>
+      <c r="C128" s="550"/>
+      <c r="D128" s="544"/>
+      <c r="E128" s="547"/>
+      <c r="F128" s="544"/>
       <c r="G128" s="511" t="s">
         <v>240</v>
       </c>
@@ -8438,7 +8441,7 @@
         <v>68</v>
       </c>
       <c r="L128" s="510" t="str">
-        <f>Namespace &amp; "has" &amp; SUBSTITUTE($H128, " ", "")</f>
+        <f t="shared" si="6"/>
         <v>http://vocab.fairdatacollective.org/gdmt/hasAwardPageIRI</v>
       </c>
       <c r="M128" s="507" t="s">
@@ -8450,11 +8453,11 @@
     </row>
     <row r="129" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A129" s="423"/>
-      <c r="B129" s="709"/>
-      <c r="C129" s="709"/>
-      <c r="D129" s="692"/>
-      <c r="E129" s="695"/>
-      <c r="F129" s="692"/>
+      <c r="B129" s="566"/>
+      <c r="C129" s="566"/>
+      <c r="D129" s="545"/>
+      <c r="E129" s="548"/>
+      <c r="F129" s="545"/>
       <c r="G129" s="528" t="s">
         <v>242</v>
       </c>
@@ -8471,7 +8474,7 @@
         <v>36</v>
       </c>
       <c r="L129" s="531" t="str">
-        <f>Namespace &amp; "has" &amp; SUBSTITUTE($H129, " ", "")</f>
+        <f t="shared" si="6"/>
         <v>http://vocab.fairdatacollective.org/gdmt/hasAwardLocalIdentifier</v>
       </c>
       <c r="M129" s="532" t="s">
@@ -8483,17 +8486,17 @@
     </row>
     <row r="130" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A130" s="423"/>
-      <c r="B130" s="696" t="s">
+      <c r="B130" s="549" t="s">
+        <v>508</v>
+      </c>
+      <c r="C130" s="549"/>
+      <c r="D130" s="552" t="s">
         <v>509</v>
       </c>
-      <c r="C130" s="696"/>
-      <c r="D130" s="551" t="s">
-        <v>510</v>
-      </c>
-      <c r="E130" s="548" t="s">
+      <c r="E130" s="555" t="s">
         <v>54</v>
       </c>
-      <c r="F130" s="690" t="str">
+      <c r="F130" s="543" t="str">
         <f>Namespace &amp; "has" &amp; ($B130)  &amp; "Info"</f>
         <v>http://vocab.fairdatacollective.org/gdmt/hasFunderInfo</v>
       </c>
@@ -8513,7 +8516,7 @@
         <v>36</v>
       </c>
       <c r="L130" s="527" t="str">
-        <f>Namespace &amp; "has" &amp; SUBSTITUTE($H130, " ", "")</f>
+        <f t="shared" si="6"/>
         <v>http://vocab.fairdatacollective.org/gdmt/hasFunderName</v>
       </c>
       <c r="M130" s="524" t="s">
@@ -8525,11 +8528,11 @@
     </row>
     <row r="131" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A131" s="423"/>
-      <c r="B131" s="697"/>
-      <c r="C131" s="697"/>
-      <c r="D131" s="552"/>
-      <c r="E131" s="549"/>
-      <c r="F131" s="691"/>
+      <c r="B131" s="550"/>
+      <c r="C131" s="550"/>
+      <c r="D131" s="553"/>
+      <c r="E131" s="556"/>
+      <c r="F131" s="544"/>
       <c r="G131" s="507" t="s">
         <v>246</v>
       </c>
@@ -8546,7 +8549,7 @@
         <v>68</v>
       </c>
       <c r="L131" s="510" t="str">
-        <f>Namespace &amp; "has" &amp; SUBSTITUTE($H131, " ", "")</f>
+        <f t="shared" si="6"/>
         <v>http://vocab.fairdatacollective.org/gdmt/hasFunderIdentifier</v>
       </c>
       <c r="M131" s="507" t="s">
@@ -8558,11 +8561,11 @@
     </row>
     <row r="132" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A132" s="423"/>
-      <c r="B132" s="697"/>
-      <c r="C132" s="697"/>
-      <c r="D132" s="552"/>
-      <c r="E132" s="549"/>
-      <c r="F132" s="691"/>
+      <c r="B132" s="550"/>
+      <c r="C132" s="550"/>
+      <c r="D132" s="553"/>
+      <c r="E132" s="556"/>
+      <c r="F132" s="544"/>
       <c r="G132" s="511" t="s">
         <v>248</v>
       </c>
@@ -8579,7 +8582,7 @@
         <v>68</v>
       </c>
       <c r="L132" s="510" t="str">
-        <f>Namespace &amp; "has" &amp; SUBSTITUTE($H132, " ", "")</f>
+        <f t="shared" si="6"/>
         <v>http://vocab.fairdatacollective.org/gdmt/hasFunderIdentifierScheme</v>
       </c>
       <c r="M132" s="507" t="s">
@@ -8591,11 +8594,11 @@
     </row>
     <row r="133" spans="1:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A133" s="424"/>
-      <c r="B133" s="698"/>
-      <c r="C133" s="698"/>
-      <c r="D133" s="699"/>
-      <c r="E133" s="700"/>
-      <c r="F133" s="701"/>
+      <c r="B133" s="551"/>
+      <c r="C133" s="551"/>
+      <c r="D133" s="554"/>
+      <c r="E133" s="557"/>
+      <c r="F133" s="558"/>
       <c r="G133" s="519" t="s">
         <v>250</v>
       </c>
@@ -8612,7 +8615,7 @@
         <v>68</v>
       </c>
       <c r="L133" s="522" t="str">
-        <f>Namespace &amp; "has" &amp; SUBSTITUTE($H133, " ", "")</f>
+        <f t="shared" si="6"/>
         <v>http://vocab.fairdatacollective.org/gdmt/hasFunderIdentifierSchemeIRI</v>
       </c>
       <c r="M133" s="523" t="s">
@@ -8636,7 +8639,7 @@
     </row>
     <row r="137" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D137" s="533" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="H137" s="3"/>
       <c r="J137" s="9"/>
@@ -8675,20 +8678,20 @@
     </row>
     <row r="143" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D143" s="3" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="H143" s="3"/>
       <c r="J143" s="9"/>
     </row>
     <row r="144" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D144" s="3" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="J144" s="6"/>
     </row>
     <row r="145" spans="4:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D145" s="5" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="J145" s="6"/>
     </row>
@@ -8700,7 +8703,7 @@
     </row>
     <row r="147" spans="4:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D147" s="5" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="G147" s="7"/>
       <c r="H147" s="7"/>
@@ -8720,13 +8723,13 @@
     </row>
     <row r="150" spans="4:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D150" s="5" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="J150" s="6"/>
     </row>
     <row r="151" spans="4:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D151" s="16" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="J151" s="6"/>
     </row>
@@ -12265,45 +12268,75 @@
   </sheetData>
   <autoFilter ref="H1:N143" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <mergeCells count="134">
-    <mergeCell ref="D127:D129"/>
-    <mergeCell ref="E127:E129"/>
-    <mergeCell ref="F127:F129"/>
-    <mergeCell ref="B130:C133"/>
-    <mergeCell ref="D130:D133"/>
-    <mergeCell ref="E130:E133"/>
-    <mergeCell ref="F130:F133"/>
-    <mergeCell ref="A114:C121"/>
-    <mergeCell ref="A122:C125"/>
-    <mergeCell ref="A126:C126"/>
-    <mergeCell ref="B127:C129"/>
-    <mergeCell ref="E114:E121"/>
-    <mergeCell ref="F114:F121"/>
-    <mergeCell ref="D122:D125"/>
-    <mergeCell ref="D114:D121"/>
-    <mergeCell ref="E122:E125"/>
-    <mergeCell ref="F122:F125"/>
-    <mergeCell ref="E107:E110"/>
-    <mergeCell ref="F107:F110"/>
-    <mergeCell ref="B111:C112"/>
-    <mergeCell ref="D111:D112"/>
-    <mergeCell ref="E111:E112"/>
-    <mergeCell ref="F111:F112"/>
-    <mergeCell ref="A91:C91"/>
-    <mergeCell ref="B92:C95"/>
-    <mergeCell ref="A104:C104"/>
-    <mergeCell ref="B105:C106"/>
-    <mergeCell ref="D105:D106"/>
-    <mergeCell ref="B96:B99"/>
-    <mergeCell ref="B100:B103"/>
-    <mergeCell ref="E105:E106"/>
-    <mergeCell ref="F105:F106"/>
-    <mergeCell ref="C96:C99"/>
-    <mergeCell ref="C100:C103"/>
-    <mergeCell ref="D92:D95"/>
-    <mergeCell ref="E92:E95"/>
-    <mergeCell ref="D96:D99"/>
-    <mergeCell ref="E96:E99"/>
-    <mergeCell ref="D100:D103"/>
+    <mergeCell ref="D5:D7"/>
+    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="D19:D22"/>
+    <mergeCell ref="F61:F63"/>
+    <mergeCell ref="E61:E63"/>
+    <mergeCell ref="D61:D63"/>
+    <mergeCell ref="F53:F55"/>
+    <mergeCell ref="E53:E55"/>
+    <mergeCell ref="D53:D55"/>
+    <mergeCell ref="F96:F99"/>
+    <mergeCell ref="F100:F103"/>
+    <mergeCell ref="D8:D12"/>
+    <mergeCell ref="E8:E12"/>
+    <mergeCell ref="F8:F12"/>
+    <mergeCell ref="F31:F34"/>
+    <mergeCell ref="E31:E34"/>
+    <mergeCell ref="F39:F41"/>
+    <mergeCell ref="F19:F22"/>
+    <mergeCell ref="E19:E22"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="E84:E87"/>
+    <mergeCell ref="F84:F87"/>
+    <mergeCell ref="A3:C4"/>
+    <mergeCell ref="A5:C7"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="D45:D48"/>
+    <mergeCell ref="E45:E48"/>
+    <mergeCell ref="F45:F48"/>
+    <mergeCell ref="D42:D44"/>
+    <mergeCell ref="E42:E44"/>
+    <mergeCell ref="F42:F44"/>
+    <mergeCell ref="D39:D41"/>
+    <mergeCell ref="E39:E41"/>
+    <mergeCell ref="D31:D34"/>
+    <mergeCell ref="D28:D30"/>
+    <mergeCell ref="E28:E30"/>
+    <mergeCell ref="F28:F30"/>
+    <mergeCell ref="D25:D27"/>
+    <mergeCell ref="E25:E27"/>
+    <mergeCell ref="F25:F27"/>
+    <mergeCell ref="E5:E7"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="F5:F7"/>
+    <mergeCell ref="B81:B83"/>
+    <mergeCell ref="C81:C83"/>
+    <mergeCell ref="D81:D83"/>
+    <mergeCell ref="E81:E83"/>
+    <mergeCell ref="F81:F83"/>
+    <mergeCell ref="B53:C55"/>
+    <mergeCell ref="B78:B80"/>
+    <mergeCell ref="C78:C80"/>
+    <mergeCell ref="D78:D80"/>
+    <mergeCell ref="E78:E80"/>
+    <mergeCell ref="F78:F80"/>
+    <mergeCell ref="B68:C68"/>
+    <mergeCell ref="B77:C77"/>
+    <mergeCell ref="B73:C75"/>
+    <mergeCell ref="D65:D66"/>
+    <mergeCell ref="E65:E66"/>
+    <mergeCell ref="F65:F66"/>
+    <mergeCell ref="F73:F75"/>
+    <mergeCell ref="E73:E75"/>
+    <mergeCell ref="D73:D75"/>
+    <mergeCell ref="A59:C59"/>
+    <mergeCell ref="B61:C63"/>
     <mergeCell ref="A8:C12"/>
     <mergeCell ref="A18:C18"/>
     <mergeCell ref="B19:C22"/>
@@ -12328,77 +12361,47 @@
     <mergeCell ref="B45:C48"/>
     <mergeCell ref="A52:C52"/>
     <mergeCell ref="D67:D72"/>
-    <mergeCell ref="B81:B83"/>
-    <mergeCell ref="C81:C83"/>
-    <mergeCell ref="D81:D83"/>
-    <mergeCell ref="E81:E83"/>
-    <mergeCell ref="F81:F83"/>
-    <mergeCell ref="B53:C55"/>
-    <mergeCell ref="B78:B80"/>
-    <mergeCell ref="C78:C80"/>
-    <mergeCell ref="D78:D80"/>
-    <mergeCell ref="E78:E80"/>
-    <mergeCell ref="F78:F80"/>
-    <mergeCell ref="B68:C68"/>
-    <mergeCell ref="B77:C77"/>
-    <mergeCell ref="B73:C75"/>
-    <mergeCell ref="D65:D66"/>
-    <mergeCell ref="E65:E66"/>
-    <mergeCell ref="F65:F66"/>
-    <mergeCell ref="F73:F75"/>
-    <mergeCell ref="E73:E75"/>
-    <mergeCell ref="D73:D75"/>
-    <mergeCell ref="A59:C59"/>
-    <mergeCell ref="B61:C63"/>
-    <mergeCell ref="A3:C4"/>
-    <mergeCell ref="A5:C7"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="D45:D48"/>
-    <mergeCell ref="E45:E48"/>
-    <mergeCell ref="F45:F48"/>
-    <mergeCell ref="D42:D44"/>
-    <mergeCell ref="E42:E44"/>
-    <mergeCell ref="F42:F44"/>
-    <mergeCell ref="D39:D41"/>
-    <mergeCell ref="E39:E41"/>
-    <mergeCell ref="D31:D34"/>
-    <mergeCell ref="D28:D30"/>
-    <mergeCell ref="E28:E30"/>
-    <mergeCell ref="F28:F30"/>
-    <mergeCell ref="D25:D27"/>
-    <mergeCell ref="E25:E27"/>
-    <mergeCell ref="F25:F27"/>
-    <mergeCell ref="E5:E7"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="F3:F4"/>
-    <mergeCell ref="F5:F7"/>
+    <mergeCell ref="E107:E110"/>
+    <mergeCell ref="F107:F110"/>
+    <mergeCell ref="B111:C112"/>
+    <mergeCell ref="D111:D112"/>
+    <mergeCell ref="E111:E112"/>
+    <mergeCell ref="F111:F112"/>
+    <mergeCell ref="A91:C91"/>
+    <mergeCell ref="B92:C95"/>
+    <mergeCell ref="A104:C104"/>
+    <mergeCell ref="B105:C106"/>
+    <mergeCell ref="D105:D106"/>
+    <mergeCell ref="B96:B99"/>
+    <mergeCell ref="B100:B103"/>
+    <mergeCell ref="E105:E106"/>
+    <mergeCell ref="F105:F106"/>
+    <mergeCell ref="C96:C99"/>
+    <mergeCell ref="C100:C103"/>
+    <mergeCell ref="D92:D95"/>
+    <mergeCell ref="E92:E95"/>
+    <mergeCell ref="D96:D99"/>
+    <mergeCell ref="E96:E99"/>
+    <mergeCell ref="D100:D103"/>
     <mergeCell ref="E100:E103"/>
     <mergeCell ref="F92:F95"/>
-    <mergeCell ref="F96:F99"/>
-    <mergeCell ref="F100:F103"/>
-    <mergeCell ref="D8:D12"/>
-    <mergeCell ref="E8:E12"/>
-    <mergeCell ref="F8:F12"/>
-    <mergeCell ref="F31:F34"/>
-    <mergeCell ref="E31:E34"/>
-    <mergeCell ref="F39:F41"/>
-    <mergeCell ref="F19:F22"/>
-    <mergeCell ref="E19:E22"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="E84:E87"/>
-    <mergeCell ref="F84:F87"/>
-    <mergeCell ref="D5:D7"/>
-    <mergeCell ref="F14:F15"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="D19:D22"/>
-    <mergeCell ref="F61:F63"/>
-    <mergeCell ref="E61:E63"/>
-    <mergeCell ref="D61:D63"/>
-    <mergeCell ref="F53:F55"/>
-    <mergeCell ref="E53:E55"/>
-    <mergeCell ref="D53:D55"/>
+    <mergeCell ref="D127:D129"/>
+    <mergeCell ref="E127:E129"/>
+    <mergeCell ref="F127:F129"/>
+    <mergeCell ref="B130:C133"/>
+    <mergeCell ref="D130:D133"/>
+    <mergeCell ref="E130:E133"/>
+    <mergeCell ref="F130:F133"/>
+    <mergeCell ref="A114:C121"/>
+    <mergeCell ref="A122:C125"/>
+    <mergeCell ref="A126:C126"/>
+    <mergeCell ref="B127:C129"/>
+    <mergeCell ref="E114:E121"/>
+    <mergeCell ref="F114:F121"/>
+    <mergeCell ref="D122:D125"/>
+    <mergeCell ref="D114:D121"/>
+    <mergeCell ref="E122:E125"/>
+    <mergeCell ref="F122:F125"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="L4" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
@@ -12430,10 +12433,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A1" s="727" t="s">
+      <c r="A1" s="742" t="s">
         <v>107</v>
       </c>
-      <c r="B1" s="727"/>
+      <c r="B1" s="742"/>
       <c r="C1" s="20" t="s">
         <v>460</v>
       </c>
@@ -12454,17 +12457,17 @@
       <c r="M1" s="28"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A2" s="728"/>
-      <c r="B2" s="729" t="s">
+      <c r="A2" s="737"/>
+      <c r="B2" s="738" t="s">
         <v>461</v>
       </c>
-      <c r="C2" s="730" t="s">
+      <c r="C2" s="743" t="s">
         <v>453</v>
       </c>
-      <c r="D2" s="731" t="s">
+      <c r="D2" s="739" t="s">
         <v>54</v>
       </c>
-      <c r="E2" s="726" t="str">
+      <c r="E2" s="740" t="str">
         <f>Namespace &amp; LOWER($B2)</f>
         <v>http://vocab.fairdatacollective.org/gdmt/contributorname</v>
       </c>
@@ -12494,11 +12497,11 @@
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A3" s="728"/>
-      <c r="B3" s="729"/>
-      <c r="C3" s="730"/>
-      <c r="D3" s="731"/>
-      <c r="E3" s="726"/>
+      <c r="A3" s="737"/>
+      <c r="B3" s="738"/>
+      <c r="C3" s="743"/>
+      <c r="D3" s="739"/>
+      <c r="E3" s="740"/>
       <c r="F3" s="34" t="s">
         <v>111</v>
       </c>
@@ -12525,11 +12528,11 @@
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A4" s="728"/>
-      <c r="B4" s="729"/>
-      <c r="C4" s="730"/>
-      <c r="D4" s="731"/>
-      <c r="E4" s="726"/>
+      <c r="A4" s="737"/>
+      <c r="B4" s="738"/>
+      <c r="C4" s="743"/>
+      <c r="D4" s="739"/>
+      <c r="E4" s="740"/>
       <c r="F4" s="34" t="s">
         <v>113</v>
       </c>
@@ -12556,17 +12559,17 @@
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5" s="728"/>
-      <c r="B5" s="729" t="s">
+      <c r="A5" s="737"/>
+      <c r="B5" s="738" t="s">
         <v>464</v>
       </c>
-      <c r="C5" s="729" t="s">
+      <c r="C5" s="738" t="s">
         <v>454</v>
       </c>
-      <c r="D5" s="731" t="s">
+      <c r="D5" s="739" t="s">
         <v>54</v>
       </c>
-      <c r="E5" s="726" t="str">
+      <c r="E5" s="740" t="str">
         <f>Namespace &amp; LOWER($B5)</f>
         <v>http://vocab.fairdatacollective.org/gdmt/contributoridentifier</v>
       </c>
@@ -12597,11 +12600,11 @@
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A6" s="728"/>
-      <c r="B6" s="729"/>
-      <c r="C6" s="729"/>
-      <c r="D6" s="731"/>
-      <c r="E6" s="726"/>
+      <c r="A6" s="737"/>
+      <c r="B6" s="738"/>
+      <c r="C6" s="738"/>
+      <c r="D6" s="739"/>
+      <c r="E6" s="740"/>
       <c r="F6" s="34" t="s">
         <v>121</v>
       </c>
@@ -12629,11 +12632,11 @@
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A7" s="728"/>
-      <c r="B7" s="729"/>
-      <c r="C7" s="729"/>
-      <c r="D7" s="731"/>
-      <c r="E7" s="726"/>
+      <c r="A7" s="737"/>
+      <c r="B7" s="738"/>
+      <c r="C7" s="738"/>
+      <c r="D7" s="739"/>
+      <c r="E7" s="740"/>
       <c r="F7" s="34" t="s">
         <v>122</v>
       </c>
@@ -12661,17 +12664,17 @@
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A8" s="728"/>
-      <c r="B8" s="729" t="s">
+      <c r="A8" s="737"/>
+      <c r="B8" s="738" t="s">
         <v>465</v>
       </c>
-      <c r="C8" s="729" t="s">
+      <c r="C8" s="738" t="s">
         <v>456</v>
       </c>
-      <c r="D8" s="731" t="s">
+      <c r="D8" s="739" t="s">
         <v>54</v>
       </c>
-      <c r="E8" s="732" t="str">
+      <c r="E8" s="741" t="str">
         <f>Namespace &amp; LOWER($B8)</f>
         <v>http://vocab.fairdatacollective.org/gdmt/contributoraffiliation</v>
       </c>
@@ -12702,11 +12705,11 @@
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A9" s="728"/>
-      <c r="B9" s="729"/>
-      <c r="C9" s="729"/>
-      <c r="D9" s="731"/>
-      <c r="E9" s="732"/>
+      <c r="A9" s="737"/>
+      <c r="B9" s="738"/>
+      <c r="C9" s="738"/>
+      <c r="D9" s="739"/>
+      <c r="E9" s="741"/>
       <c r="F9" s="34" t="s">
         <v>123</v>
       </c>
@@ -12734,11 +12737,11 @@
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A10" s="728"/>
-      <c r="B10" s="729"/>
-      <c r="C10" s="729"/>
-      <c r="D10" s="731"/>
-      <c r="E10" s="732"/>
+      <c r="A10" s="737"/>
+      <c r="B10" s="738"/>
+      <c r="C10" s="738"/>
+      <c r="D10" s="739"/>
+      <c r="E10" s="741"/>
       <c r="F10" s="34" t="s">
         <v>458</v>
       </c>
@@ -12766,11 +12769,11 @@
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A11" s="728"/>
-      <c r="B11" s="729"/>
-      <c r="C11" s="729"/>
-      <c r="D11" s="731"/>
-      <c r="E11" s="732"/>
+      <c r="A11" s="737"/>
+      <c r="B11" s="738"/>
+      <c r="C11" s="738"/>
+      <c r="D11" s="739"/>
+      <c r="E11" s="741"/>
       <c r="F11" s="34" t="s">
         <v>125</v>
       </c>
@@ -12894,22 +12897,22 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="A5:A7"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="C5:C7"/>
-    <mergeCell ref="D5:D7"/>
-    <mergeCell ref="E5:E7"/>
-    <mergeCell ref="A8:A11"/>
-    <mergeCell ref="B8:B11"/>
-    <mergeCell ref="C8:C11"/>
-    <mergeCell ref="D8:D11"/>
-    <mergeCell ref="E8:E11"/>
     <mergeCell ref="E2:E4"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="B2:B4"/>
     <mergeCell ref="C2:C4"/>
     <mergeCell ref="D2:D4"/>
+    <mergeCell ref="A8:A11"/>
+    <mergeCell ref="B8:B11"/>
+    <mergeCell ref="C8:C11"/>
+    <mergeCell ref="D8:D11"/>
+    <mergeCell ref="E8:E11"/>
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="C5:C7"/>
+    <mergeCell ref="D5:D7"/>
+    <mergeCell ref="E5:E7"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="L13" r:id="rId1" xr:uid="{9ABA6EE5-7A54-DF40-9E10-C757BCBA07FF}"/>

</xml_diff>

<commit_message>
some small updates to the template description
</commit_message>
<xml_diff>
--- a/template-description.xlsx
+++ b/template-description.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Secondary_Drive/work/repos/FAIR-data/generic-dataset-metadata-template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B96259B1-314F-6140-9370-C69555C090DF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3303354-C006-E94C-A1B9-CD4EDB9A6C91}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="34400" yWindow="460" windowWidth="34400" windowHeight="28340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3166,32 +3166,53 @@
     <xf numFmtId="0" fontId="11" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="41" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="41" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="41" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="41" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="41" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="41" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="28" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="28" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="28" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -3199,94 +3220,175 @@
     <xf numFmtId="0" fontId="7" fillId="28" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="41" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="41" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="28" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="37" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="37" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="34" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="34" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="35" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="35" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="35" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3297,6 +3399,178 @@
     <xf numFmtId="0" fontId="7" fillId="35" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="37" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="37" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="34" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="34" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="24" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="35" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="35" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="30" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="35" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="35" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="30" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="38" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -3305,12 +3579,6 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="38" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="35" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="35" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="35" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -3361,384 +3629,122 @@
     <xf numFmtId="0" fontId="11" fillId="16" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="24" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="30" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="35" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="35" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="35" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="35" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="30" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="34" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="34" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="26" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="26" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="31" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="31" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="31" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="37" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="37" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="37" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="37" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="16" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="41" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="41" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="41" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="41" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="41" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="41" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="41" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="41" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="34" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="34" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="26" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="26" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3747,19 +3753,13 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3994,10 +3994,10 @@
   <dimension ref="A1:P1034"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="K81" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D51" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G130" sqref="G130:L133"/>
+      <selection pane="bottomRight" activeCell="K78" sqref="K78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4019,11 +4019,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="668" t="s">
+      <c r="A1" s="615" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="668"/>
-      <c r="C1" s="668"/>
+      <c r="B1" s="615"/>
+      <c r="C1" s="615"/>
       <c r="D1" s="44" t="s">
         <v>1</v>
       </c>
@@ -4061,11 +4061,11 @@
       <c r="P1" s="1"/>
     </row>
     <row r="2" spans="1:16" ht="69" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="667" t="s">
+      <c r="A2" s="614" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="667"/>
-      <c r="C2" s="667"/>
+      <c r="B2" s="614"/>
+      <c r="C2" s="614"/>
       <c r="D2" s="121" t="s">
         <v>10</v>
       </c>
@@ -4097,18 +4097,18 @@
       <c r="P2" s="2"/>
     </row>
     <row r="3" spans="1:16" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="662" t="s">
+      <c r="A3" s="609" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="662"/>
-      <c r="C3" s="662"/>
-      <c r="D3" s="684" t="s">
+      <c r="B3" s="609"/>
+      <c r="C3" s="609"/>
+      <c r="D3" s="634" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="686">
+      <c r="E3" s="636">
         <v>1</v>
       </c>
-      <c r="F3" s="687" t="str">
+      <c r="F3" s="637" t="str">
         <f>Namespace &amp; "has" &amp; $A3 &amp; "Info"</f>
         <v>http://vocab.fairdatacollective.org/gdmt/hasResourceTypeInfo</v>
       </c>
@@ -4139,12 +4139,12 @@
       </c>
     </row>
     <row r="4" spans="1:16" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="663"/>
-      <c r="B4" s="663"/>
-      <c r="C4" s="663"/>
-      <c r="D4" s="685"/>
-      <c r="E4" s="581"/>
-      <c r="F4" s="688"/>
+      <c r="A4" s="610"/>
+      <c r="B4" s="610"/>
+      <c r="C4" s="610"/>
+      <c r="D4" s="635"/>
+      <c r="E4" s="582"/>
+      <c r="F4" s="638"/>
       <c r="G4" s="185" t="s">
         <v>22</v>
       </c>
@@ -4172,18 +4172,18 @@
       </c>
     </row>
     <row r="5" spans="1:16" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="664" t="s">
+      <c r="A5" s="611" t="s">
         <v>259</v>
       </c>
-      <c r="B5" s="664"/>
-      <c r="C5" s="664"/>
-      <c r="D5" s="720" t="s">
+      <c r="B5" s="611"/>
+      <c r="C5" s="611"/>
+      <c r="D5" s="543" t="s">
         <v>25</v>
       </c>
-      <c r="E5" s="681">
+      <c r="E5" s="631">
         <v>1</v>
       </c>
-      <c r="F5" s="689" t="str">
+      <c r="F5" s="639" t="str">
         <f>Namespace &amp; "has" &amp; ($A5) &amp; "Info"</f>
         <v>http://vocab.fairdatacollective.org/gdmt/hasDatasetIdentifierInfo</v>
       </c>
@@ -4213,12 +4213,12 @@
       </c>
     </row>
     <row r="6" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="665"/>
-      <c r="B6" s="665"/>
-      <c r="C6" s="665"/>
-      <c r="D6" s="721"/>
-      <c r="E6" s="682"/>
-      <c r="F6" s="690"/>
+      <c r="A6" s="612"/>
+      <c r="B6" s="612"/>
+      <c r="C6" s="612"/>
+      <c r="D6" s="544"/>
+      <c r="E6" s="632"/>
+      <c r="F6" s="640"/>
       <c r="G6" s="53" t="s">
         <v>29</v>
       </c>
@@ -4245,12 +4245,12 @@
       </c>
     </row>
     <row r="7" spans="1:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="666"/>
-      <c r="B7" s="666"/>
-      <c r="C7" s="666"/>
-      <c r="D7" s="722"/>
-      <c r="E7" s="683"/>
-      <c r="F7" s="691"/>
+      <c r="A7" s="613"/>
+      <c r="B7" s="613"/>
+      <c r="C7" s="613"/>
+      <c r="D7" s="545"/>
+      <c r="E7" s="633"/>
+      <c r="F7" s="641"/>
       <c r="G7" s="198" t="s">
         <v>32</v>
       </c>
@@ -4278,18 +4278,18 @@
       </c>
     </row>
     <row r="8" spans="1:16" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="610" t="s">
+      <c r="A8" s="659" t="s">
         <v>33</v>
       </c>
-      <c r="B8" s="610"/>
-      <c r="C8" s="610"/>
-      <c r="D8" s="699" t="s">
+      <c r="B8" s="659"/>
+      <c r="C8" s="659"/>
+      <c r="D8" s="577" t="s">
         <v>276</v>
       </c>
-      <c r="E8" s="702" t="s">
+      <c r="E8" s="580" t="s">
         <v>34</v>
       </c>
-      <c r="F8" s="703" t="str">
+      <c r="F8" s="583" t="str">
         <f>Namespace &amp; "has" &amp; ($A8) &amp; "Info"</f>
         <v>http://vocab.fairdatacollective.org/gdmt/hasRelatedResourcesInfo</v>
       </c>
@@ -4319,12 +4319,12 @@
       </c>
     </row>
     <row r="9" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="611"/>
-      <c r="B9" s="611"/>
-      <c r="C9" s="611"/>
-      <c r="D9" s="700"/>
-      <c r="E9" s="580"/>
-      <c r="F9" s="704"/>
+      <c r="A9" s="660"/>
+      <c r="B9" s="660"/>
+      <c r="C9" s="660"/>
+      <c r="D9" s="578"/>
+      <c r="E9" s="581"/>
+      <c r="F9" s="584"/>
       <c r="G9" s="59" t="s">
         <v>38</v>
       </c>
@@ -4352,12 +4352,12 @@
       </c>
     </row>
     <row r="10" spans="1:16" s="10" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="611"/>
-      <c r="B10" s="611"/>
-      <c r="C10" s="611"/>
-      <c r="D10" s="700"/>
-      <c r="E10" s="580"/>
-      <c r="F10" s="704"/>
+      <c r="A10" s="660"/>
+      <c r="B10" s="660"/>
+      <c r="C10" s="660"/>
+      <c r="D10" s="578"/>
+      <c r="E10" s="581"/>
+      <c r="F10" s="584"/>
       <c r="G10" s="59" t="s">
         <v>272</v>
       </c>
@@ -4386,12 +4386,12 @@
       </c>
     </row>
     <row r="11" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="611"/>
-      <c r="B11" s="611"/>
-      <c r="C11" s="611"/>
-      <c r="D11" s="700"/>
-      <c r="E11" s="580"/>
-      <c r="F11" s="704"/>
+      <c r="A11" s="660"/>
+      <c r="B11" s="660"/>
+      <c r="C11" s="660"/>
+      <c r="D11" s="578"/>
+      <c r="E11" s="581"/>
+      <c r="F11" s="584"/>
       <c r="G11" s="64" t="s">
         <v>41</v>
       </c>
@@ -4419,12 +4419,12 @@
       </c>
     </row>
     <row r="12" spans="1:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="612"/>
-      <c r="B12" s="612"/>
-      <c r="C12" s="612"/>
-      <c r="D12" s="701"/>
-      <c r="E12" s="581"/>
-      <c r="F12" s="705"/>
+      <c r="A12" s="661"/>
+      <c r="B12" s="661"/>
+      <c r="C12" s="661"/>
+      <c r="D12" s="579"/>
+      <c r="E12" s="582"/>
+      <c r="F12" s="585"/>
       <c r="G12" s="211" t="s">
         <v>42</v>
       </c>
@@ -4452,11 +4452,11 @@
       </c>
     </row>
     <row r="13" spans="1:16" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="617" t="s">
+      <c r="A13" s="663" t="s">
         <v>44</v>
       </c>
-      <c r="B13" s="617"/>
-      <c r="C13" s="617"/>
+      <c r="B13" s="663"/>
+      <c r="C13" s="663"/>
       <c r="D13" s="238" t="s">
         <v>45</v>
       </c>
@@ -4493,18 +4493,18 @@
       </c>
     </row>
     <row r="14" spans="1:16" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="618" t="s">
+      <c r="A14" s="664" t="s">
         <v>48</v>
       </c>
-      <c r="B14" s="618"/>
-      <c r="C14" s="618"/>
-      <c r="D14" s="725" t="s">
+      <c r="B14" s="664"/>
+      <c r="C14" s="664"/>
+      <c r="D14" s="548" t="s">
         <v>49</v>
       </c>
-      <c r="E14" s="715" t="s">
+      <c r="E14" s="601" t="s">
         <v>46</v>
       </c>
-      <c r="F14" s="723" t="str">
+      <c r="F14" s="546" t="str">
         <f>Namespace &amp; "has" &amp; ($A14) &amp; "Info"</f>
         <v>http://vocab.fairdatacollective.org/gdmt/hasLanguageInfo</v>
       </c>
@@ -4534,12 +4534,12 @@
       </c>
     </row>
     <row r="15" spans="1:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="619"/>
-      <c r="B15" s="619"/>
-      <c r="C15" s="619"/>
-      <c r="D15" s="726"/>
-      <c r="E15" s="716"/>
-      <c r="F15" s="724"/>
+      <c r="A15" s="665"/>
+      <c r="B15" s="665"/>
+      <c r="C15" s="665"/>
+      <c r="D15" s="549"/>
+      <c r="E15" s="602"/>
+      <c r="F15" s="547"/>
       <c r="G15" s="224" t="s">
         <v>51</v>
       </c>
@@ -4569,11 +4569,11 @@
       <c r="P15" s="11"/>
     </row>
     <row r="16" spans="1:16" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="620" t="s">
+      <c r="A16" s="666" t="s">
         <v>52</v>
       </c>
-      <c r="B16" s="620"/>
-      <c r="C16" s="620"/>
+      <c r="B16" s="666"/>
+      <c r="C16" s="666"/>
       <c r="D16" s="239" t="s">
         <v>53</v>
       </c>
@@ -4610,11 +4610,11 @@
       </c>
     </row>
     <row r="17" spans="1:16" s="11" customFormat="1" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="621" t="s">
+      <c r="A17" s="667" t="s">
         <v>57</v>
       </c>
-      <c r="B17" s="621"/>
-      <c r="C17" s="621"/>
+      <c r="B17" s="667"/>
+      <c r="C17" s="667"/>
       <c r="D17" s="78" t="s">
         <v>58</v>
       </c>
@@ -4653,11 +4653,11 @@
       <c r="P17"/>
     </row>
     <row r="18" spans="1:16" s="11" customFormat="1" ht="17" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="613" t="s">
+      <c r="A18" s="662" t="s">
         <v>62</v>
       </c>
-      <c r="B18" s="613"/>
-      <c r="C18" s="613"/>
+      <c r="B18" s="662"/>
+      <c r="C18" s="662"/>
       <c r="D18" s="240" t="s">
         <v>63</v>
       </c>
@@ -4681,17 +4681,17 @@
     </row>
     <row r="19" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="310"/>
-      <c r="B19" s="614" t="s">
+      <c r="B19" s="550" t="s">
         <v>498</v>
       </c>
-      <c r="C19" s="614"/>
-      <c r="D19" s="614" t="s">
+      <c r="C19" s="550"/>
+      <c r="D19" s="550" t="s">
         <v>466</v>
       </c>
-      <c r="E19" s="712" t="s">
+      <c r="E19" s="598" t="s">
         <v>34</v>
       </c>
-      <c r="F19" s="709" t="str">
+      <c r="F19" s="595" t="str">
         <f>Namespace&amp;($B19) &amp; "Info"</f>
         <v>http://vocab.fairdatacollective.org/gdmt/ControlledTermsInfo</v>
       </c>
@@ -4722,11 +4722,11 @@
     </row>
     <row r="20" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="310"/>
-      <c r="B20" s="615"/>
-      <c r="C20" s="615"/>
-      <c r="D20" s="615"/>
-      <c r="E20" s="713"/>
-      <c r="F20" s="710"/>
+      <c r="B20" s="551"/>
+      <c r="C20" s="551"/>
+      <c r="D20" s="551"/>
+      <c r="E20" s="599"/>
+      <c r="F20" s="596"/>
       <c r="G20" s="79" t="s">
         <v>467</v>
       </c>
@@ -4755,11 +4755,11 @@
     </row>
     <row r="21" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="310"/>
-      <c r="B21" s="615"/>
-      <c r="C21" s="615"/>
-      <c r="D21" s="615"/>
-      <c r="E21" s="713"/>
-      <c r="F21" s="710"/>
+      <c r="B21" s="551"/>
+      <c r="C21" s="551"/>
+      <c r="D21" s="551"/>
+      <c r="E21" s="599"/>
+      <c r="F21" s="596"/>
       <c r="G21" s="83" t="s">
         <v>70</v>
       </c>
@@ -4788,11 +4788,11 @@
     </row>
     <row r="22" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="310"/>
-      <c r="B22" s="616"/>
-      <c r="C22" s="616"/>
-      <c r="D22" s="616"/>
-      <c r="E22" s="714"/>
-      <c r="F22" s="711"/>
+      <c r="B22" s="552"/>
+      <c r="C22" s="552"/>
+      <c r="D22" s="552"/>
+      <c r="E22" s="600"/>
+      <c r="F22" s="597"/>
       <c r="G22" s="127" t="s">
         <v>71</v>
       </c>
@@ -4851,11 +4851,11 @@
       </c>
     </row>
     <row r="24" spans="1:16" s="14" customFormat="1" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="630" t="s">
+      <c r="A24" s="674" t="s">
         <v>72</v>
       </c>
-      <c r="B24" s="630"/>
-      <c r="C24" s="630"/>
+      <c r="B24" s="674"/>
+      <c r="C24" s="674"/>
       <c r="D24" s="241" t="s">
         <v>73</v>
       </c>
@@ -4877,17 +4877,17 @@
     </row>
     <row r="25" spans="1:16" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="17"/>
-      <c r="B25" s="631" t="s">
+      <c r="B25" s="625" t="s">
         <v>450</v>
       </c>
-      <c r="C25" s="631"/>
-      <c r="D25" s="631" t="s">
+      <c r="C25" s="625"/>
+      <c r="D25" s="625" t="s">
         <v>476</v>
       </c>
-      <c r="E25" s="675" t="s">
+      <c r="E25" s="589" t="s">
         <v>46</v>
       </c>
-      <c r="F25" s="678" t="str">
+      <c r="F25" s="628" t="str">
         <f>Namespace &amp; "has" &amp; ($B25) &amp; "Info"</f>
         <v>http://vocab.fairdatacollective.org/gdmt/hasCreatorNameInfo</v>
       </c>
@@ -4918,11 +4918,11 @@
     </row>
     <row r="26" spans="1:16" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="17"/>
-      <c r="B26" s="632"/>
-      <c r="C26" s="632"/>
-      <c r="D26" s="632"/>
-      <c r="E26" s="676"/>
-      <c r="F26" s="679"/>
+      <c r="B26" s="626"/>
+      <c r="C26" s="626"/>
+      <c r="D26" s="626"/>
+      <c r="E26" s="590"/>
+      <c r="F26" s="629"/>
       <c r="G26" s="87" t="s">
         <v>79</v>
       </c>
@@ -4950,11 +4950,11 @@
     </row>
     <row r="27" spans="1:16" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="17"/>
-      <c r="B27" s="633"/>
-      <c r="C27" s="633"/>
-      <c r="D27" s="633"/>
-      <c r="E27" s="677"/>
-      <c r="F27" s="680"/>
+      <c r="B27" s="627"/>
+      <c r="C27" s="627"/>
+      <c r="D27" s="627"/>
+      <c r="E27" s="591"/>
+      <c r="F27" s="630"/>
       <c r="G27" s="136" t="s">
         <v>82</v>
       </c>
@@ -4982,17 +4982,17 @@
     </row>
     <row r="28" spans="1:16" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="17"/>
-      <c r="B28" s="631" t="s">
+      <c r="B28" s="625" t="s">
         <v>451</v>
       </c>
-      <c r="C28" s="631"/>
-      <c r="D28" s="631" t="s">
+      <c r="C28" s="625"/>
+      <c r="D28" s="625" t="s">
         <v>475</v>
       </c>
-      <c r="E28" s="675" t="s">
+      <c r="E28" s="589" t="s">
         <v>522</v>
       </c>
-      <c r="F28" s="678" t="str">
+      <c r="F28" s="628" t="str">
         <f>Namespace &amp; "has" &amp; ($B28) &amp; "Info"</f>
         <v>http://vocab.fairdatacollective.org/gdmt/hasCreatorIdentifierInfo</v>
       </c>
@@ -5024,11 +5024,11 @@
     </row>
     <row r="29" spans="1:16" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="17"/>
-      <c r="B29" s="632"/>
-      <c r="C29" s="632"/>
-      <c r="D29" s="632"/>
-      <c r="E29" s="676"/>
-      <c r="F29" s="679"/>
+      <c r="B29" s="626"/>
+      <c r="C29" s="626"/>
+      <c r="D29" s="626"/>
+      <c r="E29" s="590"/>
+      <c r="F29" s="629"/>
       <c r="G29" s="87" t="s">
         <v>93</v>
       </c>
@@ -5058,11 +5058,11 @@
     </row>
     <row r="30" spans="1:16" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="17"/>
-      <c r="B30" s="633"/>
-      <c r="C30" s="633"/>
-      <c r="D30" s="633"/>
-      <c r="E30" s="677"/>
-      <c r="F30" s="680"/>
+      <c r="B30" s="627"/>
+      <c r="C30" s="627"/>
+      <c r="D30" s="627"/>
+      <c r="E30" s="591"/>
+      <c r="F30" s="630"/>
       <c r="G30" s="136" t="s">
         <v>95</v>
       </c>
@@ -5092,17 +5092,17 @@
     </row>
     <row r="31" spans="1:16" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="17"/>
-      <c r="B31" s="631" t="s">
+      <c r="B31" s="625" t="s">
         <v>452</v>
       </c>
-      <c r="C31" s="631"/>
-      <c r="D31" s="631" t="s">
+      <c r="C31" s="625"/>
+      <c r="D31" s="625" t="s">
         <v>474</v>
       </c>
-      <c r="E31" s="675" t="s">
+      <c r="E31" s="589" t="s">
         <v>34</v>
       </c>
-      <c r="F31" s="706" t="str">
+      <c r="F31" s="586" t="str">
         <f>Namespace &amp; "has" &amp; ($B31) &amp; "Info"</f>
         <v>http://vocab.fairdatacollective.org/gdmt/hasCreatorAffiliationInfo</v>
       </c>
@@ -5134,11 +5134,11 @@
     </row>
     <row r="32" spans="1:16" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="17"/>
-      <c r="B32" s="632"/>
-      <c r="C32" s="632"/>
-      <c r="D32" s="632"/>
-      <c r="E32" s="676"/>
-      <c r="F32" s="707"/>
+      <c r="B32" s="626"/>
+      <c r="C32" s="626"/>
+      <c r="D32" s="626"/>
+      <c r="E32" s="590"/>
+      <c r="F32" s="587"/>
       <c r="G32" s="87" t="s">
         <v>100</v>
       </c>
@@ -5167,11 +5167,11 @@
     </row>
     <row r="33" spans="1:16" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="17"/>
-      <c r="B33" s="632"/>
-      <c r="C33" s="632"/>
-      <c r="D33" s="632"/>
-      <c r="E33" s="676"/>
-      <c r="F33" s="707"/>
+      <c r="B33" s="626"/>
+      <c r="C33" s="626"/>
+      <c r="D33" s="626"/>
+      <c r="E33" s="590"/>
+      <c r="F33" s="587"/>
       <c r="G33" s="87" t="s">
         <v>103</v>
       </c>
@@ -5201,11 +5201,11 @@
     </row>
     <row r="34" spans="1:16" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="17"/>
-      <c r="B34" s="633"/>
-      <c r="C34" s="633"/>
-      <c r="D34" s="633"/>
-      <c r="E34" s="677"/>
-      <c r="F34" s="708"/>
+      <c r="B34" s="627"/>
+      <c r="C34" s="627"/>
+      <c r="D34" s="627"/>
+      <c r="E34" s="591"/>
+      <c r="F34" s="588"/>
       <c r="G34" s="136" t="s">
         <v>105</v>
       </c>
@@ -5334,11 +5334,11 @@
       </c>
     </row>
     <row r="38" spans="1:16" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="634" t="s">
+      <c r="A38" s="675" t="s">
         <v>107</v>
       </c>
-      <c r="B38" s="634"/>
-      <c r="C38" s="634"/>
+      <c r="B38" s="675"/>
+      <c r="C38" s="675"/>
       <c r="D38" s="377" t="s">
         <v>460</v>
       </c>
@@ -5360,17 +5360,17 @@
     </row>
     <row r="39" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="419"/>
-      <c r="B39" s="635" t="s">
+      <c r="B39" s="676" t="s">
         <v>461</v>
       </c>
-      <c r="C39" s="635"/>
-      <c r="D39" s="636" t="s">
+      <c r="C39" s="676"/>
+      <c r="D39" s="616" t="s">
         <v>477</v>
       </c>
-      <c r="E39" s="585" t="s">
+      <c r="E39" s="619" t="s">
         <v>34</v>
       </c>
-      <c r="F39" s="672" t="str">
+      <c r="F39" s="592" t="str">
         <f>Namespace &amp; "has" &amp; ($B39) &amp; "Info"</f>
         <v>http://vocab.fairdatacollective.org/gdmt/hasContributorNameInfo</v>
       </c>
@@ -5401,11 +5401,11 @@
     </row>
     <row r="40" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="419"/>
-      <c r="B40" s="635"/>
-      <c r="C40" s="635"/>
-      <c r="D40" s="637"/>
-      <c r="E40" s="586"/>
-      <c r="F40" s="673"/>
+      <c r="B40" s="676"/>
+      <c r="C40" s="676"/>
+      <c r="D40" s="617"/>
+      <c r="E40" s="620"/>
+      <c r="F40" s="593"/>
       <c r="G40" s="389" t="s">
         <v>111</v>
       </c>
@@ -5433,11 +5433,11 @@
     </row>
     <row r="41" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="419"/>
-      <c r="B41" s="635"/>
-      <c r="C41" s="635"/>
-      <c r="D41" s="638"/>
-      <c r="E41" s="587"/>
-      <c r="F41" s="674"/>
+      <c r="B41" s="676"/>
+      <c r="C41" s="676"/>
+      <c r="D41" s="618"/>
+      <c r="E41" s="621"/>
+      <c r="F41" s="594"/>
       <c r="G41" s="394" t="s">
         <v>113</v>
       </c>
@@ -5465,17 +5465,17 @@
     </row>
     <row r="42" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" s="419"/>
-      <c r="B42" s="636" t="s">
+      <c r="B42" s="616" t="s">
         <v>464</v>
       </c>
-      <c r="C42" s="636"/>
-      <c r="D42" s="636" t="s">
+      <c r="C42" s="616"/>
+      <c r="D42" s="616" t="s">
         <v>478</v>
       </c>
-      <c r="E42" s="585" t="s">
+      <c r="E42" s="619" t="s">
         <v>34</v>
       </c>
-      <c r="F42" s="672" t="str">
+      <c r="F42" s="592" t="str">
         <f>Namespace &amp; "has" &amp; ($B42) &amp; "Info"</f>
         <v>http://vocab.fairdatacollective.org/gdmt/hasContributorIdentifierInfo</v>
       </c>
@@ -5507,11 +5507,11 @@
     </row>
     <row r="43" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="419"/>
-      <c r="B43" s="637"/>
-      <c r="C43" s="637"/>
-      <c r="D43" s="637"/>
-      <c r="E43" s="586"/>
-      <c r="F43" s="673"/>
+      <c r="B43" s="617"/>
+      <c r="C43" s="617"/>
+      <c r="D43" s="617"/>
+      <c r="E43" s="620"/>
+      <c r="F43" s="593"/>
       <c r="G43" s="389" t="s">
         <v>121</v>
       </c>
@@ -5541,11 +5541,11 @@
     </row>
     <row r="44" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="419"/>
-      <c r="B44" s="638"/>
-      <c r="C44" s="638"/>
-      <c r="D44" s="638"/>
-      <c r="E44" s="587"/>
-      <c r="F44" s="674"/>
+      <c r="B44" s="618"/>
+      <c r="C44" s="618"/>
+      <c r="D44" s="618"/>
+      <c r="E44" s="621"/>
+      <c r="F44" s="594"/>
       <c r="G44" s="394" t="s">
         <v>122</v>
       </c>
@@ -5575,17 +5575,17 @@
     </row>
     <row r="45" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="419"/>
-      <c r="B45" s="636" t="s">
+      <c r="B45" s="616" t="s">
         <v>465</v>
       </c>
-      <c r="C45" s="636"/>
-      <c r="D45" s="636" t="s">
+      <c r="C45" s="616"/>
+      <c r="D45" s="616" t="s">
         <v>479</v>
       </c>
-      <c r="E45" s="585" t="s">
+      <c r="E45" s="619" t="s">
         <v>34</v>
       </c>
-      <c r="F45" s="669" t="str">
+      <c r="F45" s="622" t="str">
         <f>Namespace &amp; "has" &amp; ($B45) &amp; "Info"</f>
         <v>http://vocab.fairdatacollective.org/gdmt/hasContributorAffiliationInfo</v>
       </c>
@@ -5617,11 +5617,11 @@
     </row>
     <row r="46" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="419"/>
-      <c r="B46" s="637"/>
-      <c r="C46" s="637"/>
-      <c r="D46" s="637"/>
-      <c r="E46" s="586"/>
-      <c r="F46" s="670"/>
+      <c r="B46" s="617"/>
+      <c r="C46" s="617"/>
+      <c r="D46" s="617"/>
+      <c r="E46" s="620"/>
+      <c r="F46" s="623"/>
       <c r="G46" s="389" t="s">
         <v>123</v>
       </c>
@@ -5650,11 +5650,11 @@
     </row>
     <row r="47" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="419"/>
-      <c r="B47" s="637"/>
-      <c r="C47" s="637"/>
-      <c r="D47" s="637"/>
-      <c r="E47" s="586"/>
-      <c r="F47" s="670"/>
+      <c r="B47" s="617"/>
+      <c r="C47" s="617"/>
+      <c r="D47" s="617"/>
+      <c r="E47" s="620"/>
+      <c r="F47" s="623"/>
       <c r="G47" s="389" t="s">
         <v>458</v>
       </c>
@@ -5684,11 +5684,11 @@
     </row>
     <row r="48" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="419"/>
-      <c r="B48" s="638"/>
-      <c r="C48" s="638"/>
-      <c r="D48" s="638"/>
-      <c r="E48" s="587"/>
-      <c r="F48" s="671"/>
+      <c r="B48" s="618"/>
+      <c r="C48" s="618"/>
+      <c r="D48" s="618"/>
+      <c r="E48" s="621"/>
+      <c r="F48" s="624"/>
       <c r="G48" s="394" t="s">
         <v>125</v>
       </c>
@@ -5821,11 +5821,11 @@
       </c>
     </row>
     <row r="52" spans="1:16" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="639" t="s">
+      <c r="A52" s="677" t="s">
         <v>126</v>
       </c>
-      <c r="B52" s="639"/>
-      <c r="C52" s="639"/>
+      <c r="B52" s="677"/>
+      <c r="C52" s="677"/>
       <c r="D52" s="243" t="s">
         <v>435</v>
       </c>
@@ -5847,17 +5847,17 @@
     </row>
     <row r="53" spans="1:16" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="421"/>
-      <c r="B53" s="648" t="s">
+      <c r="B53" s="568" t="s">
         <v>472</v>
       </c>
-      <c r="C53" s="648"/>
-      <c r="D53" s="648" t="s">
+      <c r="C53" s="568"/>
+      <c r="D53" s="568" t="s">
         <v>473</v>
       </c>
-      <c r="E53" s="734" t="s">
+      <c r="E53" s="565" t="s">
         <v>54</v>
       </c>
-      <c r="F53" s="731" t="str">
+      <c r="F53" s="562" t="str">
         <f>Namespace &amp; "has" &amp; ($B53) &amp; "Info"</f>
         <v>http://vocab.fairdatacollective.org/gdmt/hasPublisherIdentifierInfo</v>
       </c>
@@ -5889,11 +5889,11 @@
     </row>
     <row r="54" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="421"/>
-      <c r="B54" s="649"/>
-      <c r="C54" s="649"/>
-      <c r="D54" s="649"/>
-      <c r="E54" s="735"/>
-      <c r="F54" s="732"/>
+      <c r="B54" s="569"/>
+      <c r="C54" s="569"/>
+      <c r="D54" s="569"/>
+      <c r="E54" s="566"/>
+      <c r="F54" s="563"/>
       <c r="G54" s="93" t="s">
         <v>136</v>
       </c>
@@ -5923,11 +5923,11 @@
     </row>
     <row r="55" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="421"/>
-      <c r="B55" s="650"/>
-      <c r="C55" s="650"/>
-      <c r="D55" s="650"/>
-      <c r="E55" s="736"/>
-      <c r="F55" s="733"/>
+      <c r="B55" s="570"/>
+      <c r="C55" s="570"/>
+      <c r="D55" s="570"/>
+      <c r="E55" s="567"/>
+      <c r="F55" s="564"/>
       <c r="G55" s="252" t="s">
         <v>137</v>
       </c>
@@ -6055,11 +6055,11 @@
       <c r="P58" s="10"/>
     </row>
     <row r="59" spans="1:16" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="660" t="s">
+      <c r="A59" s="658" t="s">
         <v>138</v>
       </c>
-      <c r="B59" s="660"/>
-      <c r="C59" s="660"/>
+      <c r="B59" s="658"/>
+      <c r="C59" s="658"/>
       <c r="D59" s="291" t="s">
         <v>139</v>
       </c>
@@ -6114,17 +6114,17 @@
     </row>
     <row r="61" spans="1:16" s="10" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A61" s="423"/>
-      <c r="B61" s="552" t="s">
+      <c r="B61" s="559" t="s">
         <v>482</v>
       </c>
-      <c r="C61" s="552"/>
-      <c r="D61" s="552" t="s">
+      <c r="C61" s="559"/>
+      <c r="D61" s="559" t="s">
         <v>483</v>
       </c>
-      <c r="E61" s="555" t="s">
+      <c r="E61" s="556" t="s">
         <v>46</v>
       </c>
-      <c r="F61" s="727" t="str">
+      <c r="F61" s="553" t="str">
         <f>Namespace &amp; "has" &amp; ($B61) &amp; "Info"</f>
         <v>http://vocab.fairdatacollective.org/gdmt/hasLicenseIdentifierInfo</v>
       </c>
@@ -6158,11 +6158,11 @@
     </row>
     <row r="62" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="423"/>
-      <c r="B62" s="553"/>
-      <c r="C62" s="553"/>
-      <c r="D62" s="553"/>
-      <c r="E62" s="556"/>
-      <c r="F62" s="728"/>
+      <c r="B62" s="560"/>
+      <c r="C62" s="560"/>
+      <c r="D62" s="560"/>
+      <c r="E62" s="557"/>
+      <c r="F62" s="554"/>
       <c r="G62" s="98" t="s">
         <v>148</v>
       </c>
@@ -6191,11 +6191,11 @@
     </row>
     <row r="63" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="423"/>
-      <c r="B63" s="661"/>
-      <c r="C63" s="661"/>
-      <c r="D63" s="661"/>
-      <c r="E63" s="730"/>
-      <c r="F63" s="729"/>
+      <c r="B63" s="561"/>
+      <c r="C63" s="561"/>
+      <c r="D63" s="561"/>
+      <c r="E63" s="558"/>
+      <c r="F63" s="555"/>
       <c r="G63" s="285" t="s">
         <v>149</v>
       </c>
@@ -6253,18 +6253,18 @@
       <c r="N64" s="272"/>
     </row>
     <row r="65" spans="1:14" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="627" t="s">
+      <c r="A65" s="671" t="s">
         <v>151</v>
       </c>
-      <c r="B65" s="627"/>
-      <c r="C65" s="627"/>
-      <c r="D65" s="653" t="s">
+      <c r="B65" s="671"/>
+      <c r="C65" s="671"/>
+      <c r="D65" s="651" t="s">
         <v>516</v>
       </c>
-      <c r="E65" s="655" t="s">
+      <c r="E65" s="653" t="s">
         <v>54</v>
       </c>
-      <c r="F65" s="653" t="str">
+      <c r="F65" s="651" t="str">
         <f>Namespace &amp; "has" &amp; ($A65) &amp; "Info"</f>
         <v>http://vocab.fairdatacollective.org/gdmt/hasDateInfo</v>
       </c>
@@ -6293,12 +6293,12 @@
       <c r="N65" s="303"/>
     </row>
     <row r="66" spans="1:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="628"/>
-      <c r="B66" s="628"/>
-      <c r="C66" s="628"/>
-      <c r="D66" s="654"/>
-      <c r="E66" s="656"/>
-      <c r="F66" s="654"/>
+      <c r="A66" s="672"/>
+      <c r="B66" s="672"/>
+      <c r="C66" s="672"/>
+      <c r="D66" s="652"/>
+      <c r="E66" s="654"/>
+      <c r="F66" s="652"/>
       <c r="G66" s="535" t="s">
         <v>484</v>
       </c>
@@ -6327,12 +6327,12 @@
       </c>
     </row>
     <row r="67" spans="1:14" s="14" customFormat="1" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="629" t="s">
+      <c r="A67" s="673" t="s">
         <v>154</v>
       </c>
-      <c r="B67" s="629"/>
-      <c r="C67" s="629"/>
-      <c r="D67" s="640" t="s">
+      <c r="B67" s="673"/>
+      <c r="C67" s="673"/>
+      <c r="D67" s="678" t="s">
         <v>159</v>
       </c>
       <c r="E67" s="360" t="s">
@@ -6353,9 +6353,9 @@
     </row>
     <row r="68" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="367"/>
-      <c r="B68" s="651"/>
-      <c r="C68" s="651"/>
-      <c r="D68" s="641"/>
+      <c r="B68" s="649"/>
+      <c r="C68" s="649"/>
+      <c r="D68" s="679"/>
       <c r="E68" s="311"/>
       <c r="F68" s="312"/>
       <c r="G68" s="313" t="s">
@@ -6389,7 +6389,7 @@
       <c r="A69" s="367"/>
       <c r="B69" s="368"/>
       <c r="C69" s="317"/>
-      <c r="D69" s="641"/>
+      <c r="D69" s="679"/>
       <c r="E69" s="319"/>
       <c r="F69" s="312"/>
       <c r="G69" s="313" t="s">
@@ -6423,7 +6423,7 @@
       <c r="A70" s="367"/>
       <c r="B70" s="368"/>
       <c r="C70" s="317"/>
-      <c r="D70" s="641"/>
+      <c r="D70" s="679"/>
       <c r="E70" s="320"/>
       <c r="F70" s="312"/>
       <c r="G70" s="305" t="s">
@@ -6455,7 +6455,7 @@
       <c r="A71" s="367"/>
       <c r="B71" s="368"/>
       <c r="C71" s="317"/>
-      <c r="D71" s="641"/>
+      <c r="D71" s="679"/>
       <c r="E71" s="320"/>
       <c r="F71" s="312"/>
       <c r="G71" s="305" t="s">
@@ -6488,7 +6488,7 @@
       <c r="A72" s="367"/>
       <c r="B72" s="368"/>
       <c r="C72" s="317"/>
-      <c r="D72" s="641"/>
+      <c r="D72" s="679"/>
       <c r="E72" s="319"/>
       <c r="F72" s="312"/>
       <c r="G72" s="305" t="s">
@@ -6519,17 +6519,17 @@
     </row>
     <row r="73" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="367"/>
-      <c r="B73" s="624" t="s">
+      <c r="B73" s="643" t="s">
         <v>488</v>
       </c>
-      <c r="C73" s="624"/>
-      <c r="D73" s="657" t="s">
+      <c r="C73" s="643"/>
+      <c r="D73" s="655" t="s">
         <v>489</v>
       </c>
-      <c r="E73" s="642">
+      <c r="E73" s="603">
         <v>1</v>
       </c>
-      <c r="F73" s="657" t="s">
+      <c r="F73" s="655" t="s">
         <v>524</v>
       </c>
       <c r="G73" s="321" t="s">
@@ -6560,11 +6560,11 @@
     </row>
     <row r="74" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="367"/>
-      <c r="B74" s="625"/>
-      <c r="C74" s="625"/>
-      <c r="D74" s="658"/>
-      <c r="E74" s="643"/>
-      <c r="F74" s="658"/>
+      <c r="B74" s="644"/>
+      <c r="C74" s="644"/>
+      <c r="D74" s="656"/>
+      <c r="E74" s="604"/>
+      <c r="F74" s="656"/>
       <c r="G74" s="305" t="s">
         <v>164</v>
       </c>
@@ -6593,11 +6593,11 @@
     </row>
     <row r="75" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="367"/>
-      <c r="B75" s="626"/>
-      <c r="C75" s="626"/>
-      <c r="D75" s="659"/>
-      <c r="E75" s="644"/>
-      <c r="F75" s="659"/>
+      <c r="B75" s="645"/>
+      <c r="C75" s="645"/>
+      <c r="D75" s="657"/>
+      <c r="E75" s="605"/>
+      <c r="F75" s="657"/>
       <c r="G75" s="326" t="s">
         <v>447</v>
       </c>
@@ -6657,10 +6657,10 @@
     </row>
     <row r="77" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="367"/>
-      <c r="B77" s="652" t="s">
+      <c r="B77" s="650" t="s">
         <v>490</v>
       </c>
-      <c r="C77" s="652"/>
+      <c r="C77" s="650"/>
       <c r="D77" s="353" t="s">
         <v>523</v>
       </c>
@@ -6682,17 +6682,17 @@
     </row>
     <row r="78" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="367"/>
-      <c r="B78" s="623"/>
-      <c r="C78" s="624" t="s">
+      <c r="B78" s="642"/>
+      <c r="C78" s="643" t="s">
         <v>491</v>
       </c>
-      <c r="D78" s="624" t="s">
+      <c r="D78" s="643" t="s">
         <v>492</v>
       </c>
-      <c r="E78" s="642">
+      <c r="E78" s="603">
         <v>1</v>
       </c>
-      <c r="F78" s="645" t="str">
+      <c r="F78" s="646" t="str">
         <f>Namespace &amp; "has" &amp; ($C78) &amp; "Info"</f>
         <v>http://vocab.fairdatacollective.org/gdmt/hasDistributorNameInfo</v>
       </c>
@@ -6723,11 +6723,11 @@
     </row>
     <row r="79" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="367"/>
-      <c r="B79" s="623"/>
-      <c r="C79" s="625"/>
-      <c r="D79" s="625"/>
-      <c r="E79" s="643"/>
-      <c r="F79" s="646"/>
+      <c r="B79" s="642"/>
+      <c r="C79" s="644"/>
+      <c r="D79" s="644"/>
+      <c r="E79" s="604"/>
+      <c r="F79" s="647"/>
       <c r="G79" s="349" t="s">
         <v>170</v>
       </c>
@@ -6755,11 +6755,11 @@
     </row>
     <row r="80" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="367"/>
-      <c r="B80" s="623"/>
-      <c r="C80" s="626"/>
-      <c r="D80" s="626"/>
-      <c r="E80" s="644"/>
-      <c r="F80" s="647"/>
+      <c r="B80" s="642"/>
+      <c r="C80" s="645"/>
+      <c r="D80" s="645"/>
+      <c r="E80" s="605"/>
+      <c r="F80" s="648"/>
       <c r="G80" s="335" t="s">
         <v>172</v>
       </c>
@@ -6787,17 +6787,17 @@
     </row>
     <row r="81" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="367"/>
-      <c r="B81" s="623"/>
-      <c r="C81" s="624" t="s">
+      <c r="B81" s="642"/>
+      <c r="C81" s="643" t="s">
         <v>494</v>
       </c>
-      <c r="D81" s="624" t="s">
+      <c r="D81" s="643" t="s">
         <v>495</v>
       </c>
-      <c r="E81" s="642">
+      <c r="E81" s="603">
         <v>1</v>
       </c>
-      <c r="F81" s="645" t="str">
+      <c r="F81" s="646" t="str">
         <f>Namespace &amp; "has" &amp; ($C81) &amp; "Info"</f>
         <v>http://vocab.fairdatacollective.org/gdmt/hasDistributorIdentifierInfo</v>
       </c>
@@ -6829,11 +6829,11 @@
     </row>
     <row r="82" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="367"/>
-      <c r="B82" s="623"/>
-      <c r="C82" s="625"/>
-      <c r="D82" s="625"/>
-      <c r="E82" s="643"/>
-      <c r="F82" s="646"/>
+      <c r="B82" s="642"/>
+      <c r="C82" s="644"/>
+      <c r="D82" s="644"/>
+      <c r="E82" s="604"/>
+      <c r="F82" s="647"/>
       <c r="G82" s="349" t="s">
         <v>181</v>
       </c>
@@ -6863,11 +6863,11 @@
     </row>
     <row r="83" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="367"/>
-      <c r="B83" s="623"/>
-      <c r="C83" s="626"/>
-      <c r="D83" s="626"/>
-      <c r="E83" s="644"/>
-      <c r="F83" s="647"/>
+      <c r="B83" s="642"/>
+      <c r="C83" s="645"/>
+      <c r="D83" s="645"/>
+      <c r="E83" s="605"/>
+      <c r="F83" s="648"/>
       <c r="G83" s="335" t="s">
         <v>182</v>
       </c>
@@ -6897,17 +6897,17 @@
     </row>
     <row r="84" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="367"/>
-      <c r="B84" s="623"/>
-      <c r="C84" s="624" t="s">
+      <c r="B84" s="642"/>
+      <c r="C84" s="643" t="s">
         <v>496</v>
       </c>
-      <c r="D84" s="624" t="s">
+      <c r="D84" s="643" t="s">
         <v>497</v>
       </c>
-      <c r="E84" s="642" t="s">
+      <c r="E84" s="603" t="s">
         <v>54</v>
       </c>
-      <c r="F84" s="717" t="str">
+      <c r="F84" s="606" t="str">
         <f>Namespace &amp; "has" &amp; ($C84) &amp; "Info"</f>
         <v>http://vocab.fairdatacollective.org/gdmt/hasDistributorAffiliationInfo</v>
       </c>
@@ -6939,11 +6939,11 @@
     </row>
     <row r="85" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="367"/>
-      <c r="B85" s="623"/>
-      <c r="C85" s="625"/>
-      <c r="D85" s="625"/>
-      <c r="E85" s="643"/>
-      <c r="F85" s="718"/>
+      <c r="B85" s="642"/>
+      <c r="C85" s="644"/>
+      <c r="D85" s="644"/>
+      <c r="E85" s="604"/>
+      <c r="F85" s="607"/>
       <c r="G85" s="349" t="s">
         <v>185</v>
       </c>
@@ -6972,11 +6972,11 @@
     </row>
     <row r="86" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="367"/>
-      <c r="B86" s="623"/>
-      <c r="C86" s="625"/>
-      <c r="D86" s="625"/>
-      <c r="E86" s="643"/>
-      <c r="F86" s="718"/>
+      <c r="B86" s="642"/>
+      <c r="C86" s="644"/>
+      <c r="D86" s="644"/>
+      <c r="E86" s="604"/>
+      <c r="F86" s="607"/>
       <c r="G86" s="349" t="s">
         <v>187</v>
       </c>
@@ -7006,11 +7006,11 @@
     </row>
     <row r="87" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="367"/>
-      <c r="B87" s="623"/>
-      <c r="C87" s="626"/>
-      <c r="D87" s="626"/>
-      <c r="E87" s="644"/>
-      <c r="F87" s="719"/>
+      <c r="B87" s="642"/>
+      <c r="C87" s="645"/>
+      <c r="D87" s="645"/>
+      <c r="E87" s="605"/>
+      <c r="F87" s="608"/>
       <c r="G87" s="335" t="s">
         <v>188</v>
       </c>
@@ -7141,11 +7141,11 @@
       <c r="P90"/>
     </row>
     <row r="91" spans="1:16" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A91" s="595" t="s">
+      <c r="A91" s="685" t="s">
         <v>189</v>
       </c>
-      <c r="B91" s="595"/>
-      <c r="C91" s="595"/>
+      <c r="B91" s="685"/>
+      <c r="C91" s="685"/>
       <c r="D91" s="425" t="s">
         <v>408</v>
       </c>
@@ -7167,17 +7167,17 @@
     </row>
     <row r="92" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="421"/>
-      <c r="B92" s="596" t="s">
+      <c r="B92" s="686" t="s">
         <v>283</v>
       </c>
-      <c r="C92" s="596"/>
-      <c r="D92" s="596" t="s">
+      <c r="C92" s="686"/>
+      <c r="D92" s="686" t="s">
         <v>287</v>
       </c>
-      <c r="E92" s="607" t="s">
+      <c r="E92" s="697" t="s">
         <v>54</v>
       </c>
-      <c r="F92" s="693" t="str">
+      <c r="F92" s="571" t="str">
         <f>Namespace &amp; "has" &amp; ($B92) &amp; "Info"</f>
         <v>http://vocab.fairdatacollective.org/gdmt/hasDataStreamInfo</v>
       </c>
@@ -7209,11 +7209,11 @@
     </row>
     <row r="93" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="421"/>
-      <c r="B93" s="597"/>
-      <c r="C93" s="597"/>
-      <c r="D93" s="597"/>
-      <c r="E93" s="608"/>
-      <c r="F93" s="694"/>
+      <c r="B93" s="687"/>
+      <c r="C93" s="687"/>
+      <c r="D93" s="687"/>
+      <c r="E93" s="698"/>
+      <c r="F93" s="572"/>
       <c r="G93" s="105" t="s">
         <v>285</v>
       </c>
@@ -7242,11 +7242,11 @@
     </row>
     <row r="94" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="421"/>
-      <c r="B94" s="597"/>
-      <c r="C94" s="597"/>
-      <c r="D94" s="597"/>
-      <c r="E94" s="608"/>
-      <c r="F94" s="694"/>
+      <c r="B94" s="687"/>
+      <c r="C94" s="687"/>
+      <c r="D94" s="687"/>
+      <c r="E94" s="698"/>
+      <c r="F94" s="572"/>
       <c r="G94" s="109" t="s">
         <v>191</v>
       </c>
@@ -7275,11 +7275,11 @@
     </row>
     <row r="95" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="421"/>
-      <c r="B95" s="598"/>
-      <c r="C95" s="598"/>
-      <c r="D95" s="598"/>
-      <c r="E95" s="609"/>
-      <c r="F95" s="695"/>
+      <c r="B95" s="688"/>
+      <c r="C95" s="688"/>
+      <c r="D95" s="688"/>
+      <c r="E95" s="699"/>
+      <c r="F95" s="573"/>
       <c r="G95" s="443" t="s">
         <v>286</v>
       </c>
@@ -7308,17 +7308,17 @@
     </row>
     <row r="96" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" s="421"/>
-      <c r="B96" s="602"/>
-      <c r="C96" s="596" t="s">
+      <c r="B96" s="692"/>
+      <c r="C96" s="686" t="s">
         <v>281</v>
       </c>
-      <c r="D96" s="596" t="s">
+      <c r="D96" s="686" t="s">
         <v>366</v>
       </c>
-      <c r="E96" s="607">
+      <c r="E96" s="697">
         <v>1</v>
       </c>
-      <c r="F96" s="693" t="str">
+      <c r="F96" s="571" t="str">
         <f>Namespace &amp; "has" &amp; ($C96) &amp; "Info"</f>
         <v>http://vocab.fairdatacollective.org/gdmt/hasDataSourceInfo</v>
       </c>
@@ -7350,11 +7350,11 @@
     </row>
     <row r="97" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" s="421"/>
-      <c r="B97" s="602"/>
-      <c r="C97" s="597"/>
-      <c r="D97" s="597"/>
-      <c r="E97" s="608"/>
-      <c r="F97" s="694"/>
+      <c r="B97" s="692"/>
+      <c r="C97" s="687"/>
+      <c r="D97" s="687"/>
+      <c r="E97" s="698"/>
+      <c r="F97" s="572"/>
       <c r="G97" s="105" t="s">
         <v>195</v>
       </c>
@@ -7383,11 +7383,11 @@
     </row>
     <row r="98" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="421"/>
-      <c r="B98" s="602"/>
-      <c r="C98" s="597"/>
-      <c r="D98" s="597"/>
-      <c r="E98" s="608"/>
-      <c r="F98" s="694"/>
+      <c r="B98" s="692"/>
+      <c r="C98" s="687"/>
+      <c r="D98" s="687"/>
+      <c r="E98" s="698"/>
+      <c r="F98" s="572"/>
       <c r="G98" s="105" t="s">
         <v>197</v>
       </c>
@@ -7416,11 +7416,11 @@
     </row>
     <row r="99" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="421"/>
-      <c r="B99" s="602"/>
-      <c r="C99" s="598"/>
-      <c r="D99" s="598"/>
-      <c r="E99" s="609"/>
-      <c r="F99" s="695"/>
+      <c r="B99" s="692"/>
+      <c r="C99" s="688"/>
+      <c r="D99" s="688"/>
+      <c r="E99" s="699"/>
+      <c r="F99" s="573"/>
       <c r="G99" s="443" t="s">
         <v>198</v>
       </c>
@@ -7449,17 +7449,17 @@
     </row>
     <row r="100" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="421"/>
-      <c r="B100" s="602"/>
-      <c r="C100" s="596" t="s">
+      <c r="B100" s="692"/>
+      <c r="C100" s="686" t="s">
         <v>282</v>
       </c>
-      <c r="D100" s="596" t="s">
+      <c r="D100" s="686" t="s">
         <v>288</v>
       </c>
-      <c r="E100" s="607" t="s">
+      <c r="E100" s="697" t="s">
         <v>54</v>
       </c>
-      <c r="F100" s="696" t="str">
+      <c r="F100" s="574" t="str">
         <f>Namespace &amp; "has" &amp; ($C100) &amp; "Info"</f>
         <v>http://vocab.fairdatacollective.org/gdmt/hasVariableInfo</v>
       </c>
@@ -7491,11 +7491,11 @@
     </row>
     <row r="101" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" s="421"/>
-      <c r="B101" s="602"/>
-      <c r="C101" s="597"/>
-      <c r="D101" s="597"/>
-      <c r="E101" s="608"/>
-      <c r="F101" s="697"/>
+      <c r="B101" s="692"/>
+      <c r="C101" s="687"/>
+      <c r="D101" s="687"/>
+      <c r="E101" s="698"/>
+      <c r="F101" s="575"/>
       <c r="G101" s="105" t="s">
         <v>290</v>
       </c>
@@ -7524,11 +7524,11 @@
     </row>
     <row r="102" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A102" s="421"/>
-      <c r="B102" s="602"/>
-      <c r="C102" s="597"/>
-      <c r="D102" s="597"/>
-      <c r="E102" s="608"/>
-      <c r="F102" s="697"/>
+      <c r="B102" s="692"/>
+      <c r="C102" s="687"/>
+      <c r="D102" s="687"/>
+      <c r="E102" s="698"/>
+      <c r="F102" s="575"/>
       <c r="G102" s="105" t="s">
         <v>291</v>
       </c>
@@ -7557,11 +7557,11 @@
     </row>
     <row r="103" spans="1:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A103" s="422"/>
-      <c r="B103" s="603"/>
-      <c r="C103" s="606"/>
-      <c r="D103" s="606"/>
-      <c r="E103" s="692"/>
-      <c r="F103" s="698"/>
+      <c r="B103" s="693"/>
+      <c r="C103" s="696"/>
+      <c r="D103" s="696"/>
+      <c r="E103" s="700"/>
+      <c r="F103" s="576"/>
       <c r="G103" s="433" t="s">
         <v>292</v>
       </c>
@@ -7589,11 +7589,11 @@
       </c>
     </row>
     <row r="104" spans="1:14" s="14" customFormat="1" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A104" s="599" t="s">
+      <c r="A104" s="689" t="s">
         <v>201</v>
       </c>
-      <c r="B104" s="599"/>
-      <c r="C104" s="599"/>
+      <c r="B104" s="689"/>
+      <c r="C104" s="689"/>
       <c r="D104" s="473" t="s">
         <v>202</v>
       </c>
@@ -7615,17 +7615,17 @@
     </row>
     <row r="105" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A105" s="419"/>
-      <c r="B105" s="591" t="s">
+      <c r="B105" s="668" t="s">
         <v>501</v>
       </c>
-      <c r="C105" s="591"/>
-      <c r="D105" s="600" t="s">
+      <c r="C105" s="668"/>
+      <c r="D105" s="690" t="s">
         <v>500</v>
       </c>
-      <c r="E105" s="604" t="s">
+      <c r="E105" s="694" t="s">
         <v>46</v>
       </c>
-      <c r="F105" s="588" t="str">
+      <c r="F105" s="680" t="str">
         <f>Namespace &amp; "has" &amp; ($B105) &amp; "Info"</f>
         <v>http://vocab.fairdatacollective.org/gdmt/hasSpatialCoveragePointInfo</v>
       </c>
@@ -7657,11 +7657,11 @@
     </row>
     <row r="106" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A106" s="419"/>
-      <c r="B106" s="592"/>
-      <c r="C106" s="592"/>
-      <c r="D106" s="601"/>
-      <c r="E106" s="605"/>
-      <c r="F106" s="590"/>
+      <c r="B106" s="670"/>
+      <c r="C106" s="670"/>
+      <c r="D106" s="691"/>
+      <c r="E106" s="695"/>
+      <c r="F106" s="682"/>
       <c r="G106" s="453" t="s">
         <v>203</v>
       </c>
@@ -7690,17 +7690,17 @@
     </row>
     <row r="107" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A107" s="419"/>
-      <c r="B107" s="591" t="s">
+      <c r="B107" s="668" t="s">
         <v>502</v>
       </c>
-      <c r="C107" s="591"/>
-      <c r="D107" s="591" t="s">
+      <c r="C107" s="668"/>
+      <c r="D107" s="668" t="s">
         <v>503</v>
       </c>
-      <c r="E107" s="585" t="s">
+      <c r="E107" s="619" t="s">
         <v>46</v>
       </c>
-      <c r="F107" s="588" t="str">
+      <c r="F107" s="680" t="str">
         <f>Namespace &amp; "has" &amp; ($B107) &amp; "Info"</f>
         <v>http://vocab.fairdatacollective.org/gdmt/hasSpatialCoverageBoundingBoxInfo</v>
       </c>
@@ -7732,11 +7732,11 @@
     </row>
     <row r="108" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A108" s="419"/>
-      <c r="B108" s="622"/>
-      <c r="C108" s="622"/>
-      <c r="D108" s="622"/>
-      <c r="E108" s="586"/>
-      <c r="F108" s="589"/>
+      <c r="B108" s="669"/>
+      <c r="C108" s="669"/>
+      <c r="D108" s="669"/>
+      <c r="E108" s="620"/>
+      <c r="F108" s="681"/>
       <c r="G108" s="463" t="s">
         <v>209</v>
       </c>
@@ -7765,11 +7765,11 @@
     </row>
     <row r="109" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A109" s="419"/>
-      <c r="B109" s="622"/>
-      <c r="C109" s="622"/>
-      <c r="D109" s="622"/>
-      <c r="E109" s="586"/>
-      <c r="F109" s="589"/>
+      <c r="B109" s="669"/>
+      <c r="C109" s="669"/>
+      <c r="D109" s="669"/>
+      <c r="E109" s="620"/>
+      <c r="F109" s="681"/>
       <c r="G109" s="463" t="s">
         <v>211</v>
       </c>
@@ -7798,11 +7798,11 @@
     </row>
     <row r="110" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A110" s="419"/>
-      <c r="B110" s="592"/>
-      <c r="C110" s="592"/>
-      <c r="D110" s="592"/>
-      <c r="E110" s="587"/>
-      <c r="F110" s="590"/>
+      <c r="B110" s="670"/>
+      <c r="C110" s="670"/>
+      <c r="D110" s="670"/>
+      <c r="E110" s="621"/>
+      <c r="F110" s="682"/>
       <c r="G110" s="468" t="s">
         <v>213</v>
       </c>
@@ -7831,17 +7831,17 @@
     </row>
     <row r="111" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A111" s="419"/>
-      <c r="B111" s="591" t="s">
+      <c r="B111" s="668" t="s">
         <v>504</v>
       </c>
-      <c r="C111" s="591"/>
-      <c r="D111" s="593" t="s">
+      <c r="C111" s="668"/>
+      <c r="D111" s="683" t="s">
         <v>505</v>
       </c>
-      <c r="E111" s="585" t="s">
+      <c r="E111" s="619" t="s">
         <v>46</v>
       </c>
-      <c r="F111" s="588" t="str">
+      <c r="F111" s="680" t="str">
         <f>Namespace &amp; "has" &amp; ($B111) &amp; "Info"</f>
         <v>http://vocab.fairdatacollective.org/gdmt/hasSpatialCoveragePolygonInfo</v>
       </c>
@@ -7873,11 +7873,11 @@
     </row>
     <row r="112" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A112" s="419"/>
-      <c r="B112" s="592"/>
-      <c r="C112" s="592"/>
-      <c r="D112" s="594"/>
-      <c r="E112" s="587"/>
-      <c r="F112" s="590"/>
+      <c r="B112" s="670"/>
+      <c r="C112" s="670"/>
+      <c r="D112" s="684"/>
+      <c r="E112" s="621"/>
+      <c r="F112" s="682"/>
       <c r="G112" s="453" t="s">
         <v>437</v>
       </c>
@@ -7938,18 +7938,18 @@
       </c>
     </row>
     <row r="114" spans="1:14" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A114" s="559" t="s">
+      <c r="A114" s="713" t="s">
         <v>217</v>
       </c>
-      <c r="B114" s="559"/>
-      <c r="C114" s="559"/>
-      <c r="D114" s="576" t="s">
+      <c r="B114" s="713"/>
+      <c r="C114" s="713"/>
+      <c r="D114" s="730" t="s">
         <v>218</v>
       </c>
-      <c r="E114" s="567" t="s">
+      <c r="E114" s="721" t="s">
         <v>46</v>
       </c>
-      <c r="F114" s="570" t="str">
+      <c r="F114" s="724" t="str">
         <f>Namespace &amp; "has" &amp; ($A114) &amp; "Info"</f>
         <v>http://vocab.fairdatacollective.org/gdmt/hasVerticalCoverageInfo</v>
       </c>
@@ -7980,12 +7980,12 @@
       </c>
     </row>
     <row r="115" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A115" s="560"/>
-      <c r="B115" s="560"/>
-      <c r="C115" s="560"/>
-      <c r="D115" s="577"/>
-      <c r="E115" s="568"/>
-      <c r="F115" s="571"/>
+      <c r="A115" s="714"/>
+      <c r="B115" s="714"/>
+      <c r="C115" s="714"/>
+      <c r="D115" s="731"/>
+      <c r="E115" s="722"/>
+      <c r="F115" s="725"/>
       <c r="G115" s="111" t="s">
         <v>221</v>
       </c>
@@ -8013,12 +8013,12 @@
       </c>
     </row>
     <row r="116" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A116" s="560"/>
-      <c r="B116" s="560"/>
-      <c r="C116" s="560"/>
-      <c r="D116" s="577"/>
-      <c r="E116" s="568"/>
-      <c r="F116" s="571"/>
+      <c r="A116" s="714"/>
+      <c r="B116" s="714"/>
+      <c r="C116" s="714"/>
+      <c r="D116" s="731"/>
+      <c r="E116" s="722"/>
+      <c r="F116" s="725"/>
       <c r="G116" s="111" t="s">
         <v>223</v>
       </c>
@@ -8046,12 +8046,12 @@
       </c>
     </row>
     <row r="117" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A117" s="560"/>
-      <c r="B117" s="560"/>
-      <c r="C117" s="560"/>
-      <c r="D117" s="577"/>
-      <c r="E117" s="568"/>
-      <c r="F117" s="571"/>
+      <c r="A117" s="714"/>
+      <c r="B117" s="714"/>
+      <c r="C117" s="714"/>
+      <c r="D117" s="731"/>
+      <c r="E117" s="722"/>
+      <c r="F117" s="725"/>
       <c r="G117" s="111" t="s">
         <v>224</v>
       </c>
@@ -8079,12 +8079,12 @@
       </c>
     </row>
     <row r="118" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A118" s="560"/>
-      <c r="B118" s="560"/>
-      <c r="C118" s="560"/>
-      <c r="D118" s="577"/>
-      <c r="E118" s="568"/>
-      <c r="F118" s="571"/>
+      <c r="A118" s="714"/>
+      <c r="B118" s="714"/>
+      <c r="C118" s="714"/>
+      <c r="D118" s="731"/>
+      <c r="E118" s="722"/>
+      <c r="F118" s="725"/>
       <c r="G118" s="111" t="s">
         <v>225</v>
       </c>
@@ -8112,12 +8112,12 @@
       </c>
     </row>
     <row r="119" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A119" s="560"/>
-      <c r="B119" s="560"/>
-      <c r="C119" s="560"/>
-      <c r="D119" s="577"/>
-      <c r="E119" s="568"/>
-      <c r="F119" s="571"/>
+      <c r="A119" s="714"/>
+      <c r="B119" s="714"/>
+      <c r="C119" s="714"/>
+      <c r="D119" s="731"/>
+      <c r="E119" s="722"/>
+      <c r="F119" s="725"/>
       <c r="G119" s="111" t="s">
         <v>226</v>
       </c>
@@ -8145,12 +8145,12 @@
       </c>
     </row>
     <row r="120" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A120" s="560"/>
-      <c r="B120" s="560"/>
-      <c r="C120" s="560"/>
-      <c r="D120" s="577"/>
-      <c r="E120" s="568"/>
-      <c r="F120" s="571"/>
+      <c r="A120" s="714"/>
+      <c r="B120" s="714"/>
+      <c r="C120" s="714"/>
+      <c r="D120" s="731"/>
+      <c r="E120" s="722"/>
+      <c r="F120" s="725"/>
       <c r="G120" s="111" t="s">
         <v>396</v>
       </c>
@@ -8178,12 +8178,12 @@
       </c>
     </row>
     <row r="121" spans="1:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A121" s="561"/>
-      <c r="B121" s="561"/>
-      <c r="C121" s="561"/>
-      <c r="D121" s="578"/>
-      <c r="E121" s="569"/>
-      <c r="F121" s="572"/>
+      <c r="A121" s="715"/>
+      <c r="B121" s="715"/>
+      <c r="C121" s="715"/>
+      <c r="D121" s="732"/>
+      <c r="E121" s="723"/>
+      <c r="F121" s="726"/>
       <c r="G121" s="534" t="s">
         <v>406</v>
       </c>
@@ -8211,18 +8211,18 @@
       </c>
     </row>
     <row r="122" spans="1:14" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A122" s="562" t="s">
+      <c r="A122" s="716" t="s">
         <v>227</v>
       </c>
-      <c r="B122" s="562"/>
-      <c r="C122" s="562"/>
-      <c r="D122" s="573" t="s">
+      <c r="B122" s="716"/>
+      <c r="C122" s="716"/>
+      <c r="D122" s="727" t="s">
         <v>228</v>
       </c>
-      <c r="E122" s="579" t="s">
+      <c r="E122" s="733" t="s">
         <v>46</v>
       </c>
-      <c r="F122" s="582" t="str">
+      <c r="F122" s="734" t="str">
         <f>Namespace &amp; "has" &amp; ($A122) &amp; "Info"</f>
         <v>http://vocab.fairdatacollective.org/gdmt/hasTemporalCoverageInfo</v>
       </c>
@@ -8253,12 +8253,12 @@
       </c>
     </row>
     <row r="123" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A123" s="563"/>
-      <c r="B123" s="563"/>
-      <c r="C123" s="563"/>
-      <c r="D123" s="574"/>
-      <c r="E123" s="580"/>
-      <c r="F123" s="583"/>
+      <c r="A123" s="717"/>
+      <c r="B123" s="717"/>
+      <c r="C123" s="717"/>
+      <c r="D123" s="728"/>
+      <c r="E123" s="581"/>
+      <c r="F123" s="735"/>
       <c r="G123" s="116" t="s">
         <v>231</v>
       </c>
@@ -8286,12 +8286,12 @@
       </c>
     </row>
     <row r="124" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A124" s="563"/>
-      <c r="B124" s="563"/>
-      <c r="C124" s="563"/>
-      <c r="D124" s="574"/>
-      <c r="E124" s="580"/>
-      <c r="F124" s="583"/>
+      <c r="A124" s="717"/>
+      <c r="B124" s="717"/>
+      <c r="C124" s="717"/>
+      <c r="D124" s="728"/>
+      <c r="E124" s="581"/>
+      <c r="F124" s="735"/>
       <c r="G124" s="116" t="s">
         <v>233</v>
       </c>
@@ -8319,12 +8319,12 @@
       </c>
     </row>
     <row r="125" spans="1:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A125" s="564"/>
-      <c r="B125" s="564"/>
-      <c r="C125" s="564"/>
-      <c r="D125" s="575"/>
-      <c r="E125" s="581"/>
-      <c r="F125" s="584"/>
+      <c r="A125" s="718"/>
+      <c r="B125" s="718"/>
+      <c r="C125" s="718"/>
+      <c r="D125" s="729"/>
+      <c r="E125" s="582"/>
+      <c r="F125" s="736"/>
       <c r="G125" s="502" t="s">
         <v>235</v>
       </c>
@@ -8352,11 +8352,11 @@
       </c>
     </row>
     <row r="126" spans="1:14" s="14" customFormat="1" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A126" s="565" t="s">
+      <c r="A126" s="719" t="s">
         <v>237</v>
       </c>
-      <c r="B126" s="565"/>
-      <c r="C126" s="565"/>
+      <c r="B126" s="719"/>
+      <c r="C126" s="719"/>
       <c r="D126" s="512" t="s">
         <v>506</v>
       </c>
@@ -8378,17 +8378,17 @@
     </row>
     <row r="127" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A127" s="423"/>
-      <c r="B127" s="549" t="s">
+      <c r="B127" s="707" t="s">
         <v>507</v>
       </c>
-      <c r="C127" s="549"/>
-      <c r="D127" s="543" t="s">
+      <c r="C127" s="707"/>
+      <c r="D127" s="701" t="s">
         <v>510</v>
       </c>
-      <c r="E127" s="546">
+      <c r="E127" s="704">
         <v>1</v>
       </c>
-      <c r="F127" s="543" t="str">
+      <c r="F127" s="701" t="str">
         <f>Namespace &amp; "has" &amp; ($B127) &amp; "Info"</f>
         <v>http://vocab.fairdatacollective.org/gdmt/hasAwardInfo</v>
       </c>
@@ -8420,11 +8420,11 @@
     </row>
     <row r="128" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A128" s="423"/>
-      <c r="B128" s="550"/>
-      <c r="C128" s="550"/>
-      <c r="D128" s="544"/>
-      <c r="E128" s="547"/>
-      <c r="F128" s="544"/>
+      <c r="B128" s="708"/>
+      <c r="C128" s="708"/>
+      <c r="D128" s="702"/>
+      <c r="E128" s="705"/>
+      <c r="F128" s="702"/>
       <c r="G128" s="511" t="s">
         <v>240</v>
       </c>
@@ -8453,11 +8453,11 @@
     </row>
     <row r="129" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A129" s="423"/>
-      <c r="B129" s="566"/>
-      <c r="C129" s="566"/>
-      <c r="D129" s="545"/>
-      <c r="E129" s="548"/>
-      <c r="F129" s="545"/>
+      <c r="B129" s="720"/>
+      <c r="C129" s="720"/>
+      <c r="D129" s="703"/>
+      <c r="E129" s="706"/>
+      <c r="F129" s="703"/>
       <c r="G129" s="528" t="s">
         <v>242</v>
       </c>
@@ -8486,17 +8486,17 @@
     </row>
     <row r="130" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A130" s="423"/>
-      <c r="B130" s="549" t="s">
+      <c r="B130" s="707" t="s">
         <v>508</v>
       </c>
-      <c r="C130" s="549"/>
-      <c r="D130" s="552" t="s">
+      <c r="C130" s="707"/>
+      <c r="D130" s="559" t="s">
         <v>509</v>
       </c>
-      <c r="E130" s="555" t="s">
+      <c r="E130" s="556" t="s">
         <v>54</v>
       </c>
-      <c r="F130" s="543" t="str">
+      <c r="F130" s="701" t="str">
         <f>Namespace &amp; "has" &amp; ($B130)  &amp; "Info"</f>
         <v>http://vocab.fairdatacollective.org/gdmt/hasFunderInfo</v>
       </c>
@@ -8528,11 +8528,11 @@
     </row>
     <row r="131" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A131" s="423"/>
-      <c r="B131" s="550"/>
-      <c r="C131" s="550"/>
-      <c r="D131" s="553"/>
-      <c r="E131" s="556"/>
-      <c r="F131" s="544"/>
+      <c r="B131" s="708"/>
+      <c r="C131" s="708"/>
+      <c r="D131" s="560"/>
+      <c r="E131" s="557"/>
+      <c r="F131" s="702"/>
       <c r="G131" s="507" t="s">
         <v>246</v>
       </c>
@@ -8561,11 +8561,11 @@
     </row>
     <row r="132" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A132" s="423"/>
-      <c r="B132" s="550"/>
-      <c r="C132" s="550"/>
-      <c r="D132" s="553"/>
-      <c r="E132" s="556"/>
-      <c r="F132" s="544"/>
+      <c r="B132" s="708"/>
+      <c r="C132" s="708"/>
+      <c r="D132" s="560"/>
+      <c r="E132" s="557"/>
+      <c r="F132" s="702"/>
       <c r="G132" s="511" t="s">
         <v>248</v>
       </c>
@@ -8594,11 +8594,11 @@
     </row>
     <row r="133" spans="1:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A133" s="424"/>
-      <c r="B133" s="551"/>
-      <c r="C133" s="551"/>
-      <c r="D133" s="554"/>
-      <c r="E133" s="557"/>
-      <c r="F133" s="558"/>
+      <c r="B133" s="709"/>
+      <c r="C133" s="709"/>
+      <c r="D133" s="710"/>
+      <c r="E133" s="711"/>
+      <c r="F133" s="712"/>
       <c r="G133" s="519" t="s">
         <v>250</v>
       </c>
@@ -12268,29 +12268,93 @@
   </sheetData>
   <autoFilter ref="H1:N143" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <mergeCells count="134">
-    <mergeCell ref="D5:D7"/>
-    <mergeCell ref="F14:F15"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="D19:D22"/>
-    <mergeCell ref="F61:F63"/>
-    <mergeCell ref="E61:E63"/>
-    <mergeCell ref="D61:D63"/>
-    <mergeCell ref="F53:F55"/>
-    <mergeCell ref="E53:E55"/>
-    <mergeCell ref="D53:D55"/>
-    <mergeCell ref="F96:F99"/>
-    <mergeCell ref="F100:F103"/>
-    <mergeCell ref="D8:D12"/>
-    <mergeCell ref="E8:E12"/>
-    <mergeCell ref="F8:F12"/>
-    <mergeCell ref="F31:F34"/>
-    <mergeCell ref="E31:E34"/>
-    <mergeCell ref="F39:F41"/>
-    <mergeCell ref="F19:F22"/>
-    <mergeCell ref="E19:E22"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="E84:E87"/>
-    <mergeCell ref="F84:F87"/>
+    <mergeCell ref="D127:D129"/>
+    <mergeCell ref="E127:E129"/>
+    <mergeCell ref="F127:F129"/>
+    <mergeCell ref="B130:C133"/>
+    <mergeCell ref="D130:D133"/>
+    <mergeCell ref="E130:E133"/>
+    <mergeCell ref="F130:F133"/>
+    <mergeCell ref="A114:C121"/>
+    <mergeCell ref="A122:C125"/>
+    <mergeCell ref="A126:C126"/>
+    <mergeCell ref="B127:C129"/>
+    <mergeCell ref="E114:E121"/>
+    <mergeCell ref="F114:F121"/>
+    <mergeCell ref="D122:D125"/>
+    <mergeCell ref="D114:D121"/>
+    <mergeCell ref="E122:E125"/>
+    <mergeCell ref="F122:F125"/>
+    <mergeCell ref="E107:E110"/>
+    <mergeCell ref="F107:F110"/>
+    <mergeCell ref="B111:C112"/>
+    <mergeCell ref="D111:D112"/>
+    <mergeCell ref="E111:E112"/>
+    <mergeCell ref="F111:F112"/>
+    <mergeCell ref="A91:C91"/>
+    <mergeCell ref="B92:C95"/>
+    <mergeCell ref="A104:C104"/>
+    <mergeCell ref="B105:C106"/>
+    <mergeCell ref="D105:D106"/>
+    <mergeCell ref="B96:B99"/>
+    <mergeCell ref="B100:B103"/>
+    <mergeCell ref="E105:E106"/>
+    <mergeCell ref="F105:F106"/>
+    <mergeCell ref="C96:C99"/>
+    <mergeCell ref="C100:C103"/>
+    <mergeCell ref="D92:D95"/>
+    <mergeCell ref="E92:E95"/>
+    <mergeCell ref="D96:D99"/>
+    <mergeCell ref="E96:E99"/>
+    <mergeCell ref="D100:D103"/>
+    <mergeCell ref="E100:E103"/>
+    <mergeCell ref="F92:F95"/>
+    <mergeCell ref="A8:C12"/>
+    <mergeCell ref="A18:C18"/>
+    <mergeCell ref="B19:C22"/>
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="A14:C15"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="A17:C17"/>
+    <mergeCell ref="B107:C110"/>
+    <mergeCell ref="D107:D110"/>
+    <mergeCell ref="B84:B87"/>
+    <mergeCell ref="C84:C87"/>
+    <mergeCell ref="D84:D87"/>
+    <mergeCell ref="A65:C66"/>
+    <mergeCell ref="A67:C67"/>
+    <mergeCell ref="A24:C24"/>
+    <mergeCell ref="B25:C27"/>
+    <mergeCell ref="B28:C30"/>
+    <mergeCell ref="B31:C34"/>
+    <mergeCell ref="A38:C38"/>
+    <mergeCell ref="B39:C41"/>
+    <mergeCell ref="B42:C44"/>
+    <mergeCell ref="B45:C48"/>
+    <mergeCell ref="A52:C52"/>
+    <mergeCell ref="D67:D72"/>
+    <mergeCell ref="B81:B83"/>
+    <mergeCell ref="C81:C83"/>
+    <mergeCell ref="D81:D83"/>
+    <mergeCell ref="E81:E83"/>
+    <mergeCell ref="F81:F83"/>
+    <mergeCell ref="B53:C55"/>
+    <mergeCell ref="B78:B80"/>
+    <mergeCell ref="C78:C80"/>
+    <mergeCell ref="D78:D80"/>
+    <mergeCell ref="E78:E80"/>
+    <mergeCell ref="F78:F80"/>
+    <mergeCell ref="B68:C68"/>
+    <mergeCell ref="B77:C77"/>
+    <mergeCell ref="B73:C75"/>
+    <mergeCell ref="D65:D66"/>
+    <mergeCell ref="E65:E66"/>
+    <mergeCell ref="F65:F66"/>
+    <mergeCell ref="F73:F75"/>
+    <mergeCell ref="E73:E75"/>
+    <mergeCell ref="D73:D75"/>
+    <mergeCell ref="A59:C59"/>
+    <mergeCell ref="B61:C63"/>
     <mergeCell ref="A3:C4"/>
     <mergeCell ref="A5:C7"/>
     <mergeCell ref="A2:C2"/>
@@ -12315,93 +12379,29 @@
     <mergeCell ref="E3:E4"/>
     <mergeCell ref="F3:F4"/>
     <mergeCell ref="F5:F7"/>
-    <mergeCell ref="B81:B83"/>
-    <mergeCell ref="C81:C83"/>
-    <mergeCell ref="D81:D83"/>
-    <mergeCell ref="E81:E83"/>
-    <mergeCell ref="F81:F83"/>
-    <mergeCell ref="B53:C55"/>
-    <mergeCell ref="B78:B80"/>
-    <mergeCell ref="C78:C80"/>
-    <mergeCell ref="D78:D80"/>
-    <mergeCell ref="E78:E80"/>
-    <mergeCell ref="F78:F80"/>
-    <mergeCell ref="B68:C68"/>
-    <mergeCell ref="B77:C77"/>
-    <mergeCell ref="B73:C75"/>
-    <mergeCell ref="D65:D66"/>
-    <mergeCell ref="E65:E66"/>
-    <mergeCell ref="F65:F66"/>
-    <mergeCell ref="F73:F75"/>
-    <mergeCell ref="E73:E75"/>
-    <mergeCell ref="D73:D75"/>
-    <mergeCell ref="A59:C59"/>
-    <mergeCell ref="B61:C63"/>
-    <mergeCell ref="A8:C12"/>
-    <mergeCell ref="A18:C18"/>
-    <mergeCell ref="B19:C22"/>
-    <mergeCell ref="A13:C13"/>
-    <mergeCell ref="A14:C15"/>
-    <mergeCell ref="A16:C16"/>
-    <mergeCell ref="A17:C17"/>
-    <mergeCell ref="B107:C110"/>
-    <mergeCell ref="D107:D110"/>
-    <mergeCell ref="B84:B87"/>
-    <mergeCell ref="C84:C87"/>
-    <mergeCell ref="D84:D87"/>
-    <mergeCell ref="A65:C66"/>
-    <mergeCell ref="A67:C67"/>
-    <mergeCell ref="A24:C24"/>
-    <mergeCell ref="B25:C27"/>
-    <mergeCell ref="B28:C30"/>
-    <mergeCell ref="B31:C34"/>
-    <mergeCell ref="A38:C38"/>
-    <mergeCell ref="B39:C41"/>
-    <mergeCell ref="B42:C44"/>
-    <mergeCell ref="B45:C48"/>
-    <mergeCell ref="A52:C52"/>
-    <mergeCell ref="D67:D72"/>
-    <mergeCell ref="E107:E110"/>
-    <mergeCell ref="F107:F110"/>
-    <mergeCell ref="B111:C112"/>
-    <mergeCell ref="D111:D112"/>
-    <mergeCell ref="E111:E112"/>
-    <mergeCell ref="F111:F112"/>
-    <mergeCell ref="A91:C91"/>
-    <mergeCell ref="B92:C95"/>
-    <mergeCell ref="A104:C104"/>
-    <mergeCell ref="B105:C106"/>
-    <mergeCell ref="D105:D106"/>
-    <mergeCell ref="B96:B99"/>
-    <mergeCell ref="B100:B103"/>
-    <mergeCell ref="E105:E106"/>
-    <mergeCell ref="F105:F106"/>
-    <mergeCell ref="C96:C99"/>
-    <mergeCell ref="C100:C103"/>
-    <mergeCell ref="D92:D95"/>
-    <mergeCell ref="E92:E95"/>
-    <mergeCell ref="D96:D99"/>
-    <mergeCell ref="E96:E99"/>
-    <mergeCell ref="D100:D103"/>
-    <mergeCell ref="E100:E103"/>
-    <mergeCell ref="F92:F95"/>
-    <mergeCell ref="D127:D129"/>
-    <mergeCell ref="E127:E129"/>
-    <mergeCell ref="F127:F129"/>
-    <mergeCell ref="B130:C133"/>
-    <mergeCell ref="D130:D133"/>
-    <mergeCell ref="E130:E133"/>
-    <mergeCell ref="F130:F133"/>
-    <mergeCell ref="A114:C121"/>
-    <mergeCell ref="A122:C125"/>
-    <mergeCell ref="A126:C126"/>
-    <mergeCell ref="B127:C129"/>
-    <mergeCell ref="E114:E121"/>
-    <mergeCell ref="F114:F121"/>
-    <mergeCell ref="D122:D125"/>
-    <mergeCell ref="D114:D121"/>
-    <mergeCell ref="E122:E125"/>
-    <mergeCell ref="F122:F125"/>
+    <mergeCell ref="F96:F99"/>
+    <mergeCell ref="F100:F103"/>
+    <mergeCell ref="D8:D12"/>
+    <mergeCell ref="E8:E12"/>
+    <mergeCell ref="F8:F12"/>
+    <mergeCell ref="F31:F34"/>
+    <mergeCell ref="E31:E34"/>
+    <mergeCell ref="F39:F41"/>
+    <mergeCell ref="F19:F22"/>
+    <mergeCell ref="E19:E22"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="E84:E87"/>
+    <mergeCell ref="F84:F87"/>
+    <mergeCell ref="D5:D7"/>
+    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="D19:D22"/>
+    <mergeCell ref="F61:F63"/>
+    <mergeCell ref="E61:E63"/>
+    <mergeCell ref="D61:D63"/>
+    <mergeCell ref="F53:F55"/>
+    <mergeCell ref="E53:E55"/>
+    <mergeCell ref="D53:D55"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="L4" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
@@ -12433,10 +12433,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A1" s="742" t="s">
+      <c r="A1" s="738" t="s">
         <v>107</v>
       </c>
-      <c r="B1" s="742"/>
+      <c r="B1" s="738"/>
       <c r="C1" s="20" t="s">
         <v>460</v>
       </c>
@@ -12457,17 +12457,17 @@
       <c r="M1" s="28"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A2" s="737"/>
-      <c r="B2" s="738" t="s">
+      <c r="A2" s="739"/>
+      <c r="B2" s="740" t="s">
         <v>461</v>
       </c>
-      <c r="C2" s="743" t="s">
+      <c r="C2" s="741" t="s">
         <v>453</v>
       </c>
-      <c r="D2" s="739" t="s">
+      <c r="D2" s="742" t="s">
         <v>54</v>
       </c>
-      <c r="E2" s="740" t="str">
+      <c r="E2" s="737" t="str">
         <f>Namespace &amp; LOWER($B2)</f>
         <v>http://vocab.fairdatacollective.org/gdmt/contributorname</v>
       </c>
@@ -12497,11 +12497,11 @@
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A3" s="737"/>
-      <c r="B3" s="738"/>
-      <c r="C3" s="743"/>
-      <c r="D3" s="739"/>
-      <c r="E3" s="740"/>
+      <c r="A3" s="739"/>
+      <c r="B3" s="740"/>
+      <c r="C3" s="741"/>
+      <c r="D3" s="742"/>
+      <c r="E3" s="737"/>
       <c r="F3" s="34" t="s">
         <v>111</v>
       </c>
@@ -12528,11 +12528,11 @@
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A4" s="737"/>
-      <c r="B4" s="738"/>
-      <c r="C4" s="743"/>
-      <c r="D4" s="739"/>
-      <c r="E4" s="740"/>
+      <c r="A4" s="739"/>
+      <c r="B4" s="740"/>
+      <c r="C4" s="741"/>
+      <c r="D4" s="742"/>
+      <c r="E4" s="737"/>
       <c r="F4" s="34" t="s">
         <v>113</v>
       </c>
@@ -12559,17 +12559,17 @@
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5" s="737"/>
-      <c r="B5" s="738" t="s">
+      <c r="A5" s="739"/>
+      <c r="B5" s="740" t="s">
         <v>464</v>
       </c>
-      <c r="C5" s="738" t="s">
+      <c r="C5" s="740" t="s">
         <v>454</v>
       </c>
-      <c r="D5" s="739" t="s">
+      <c r="D5" s="742" t="s">
         <v>54</v>
       </c>
-      <c r="E5" s="740" t="str">
+      <c r="E5" s="737" t="str">
         <f>Namespace &amp; LOWER($B5)</f>
         <v>http://vocab.fairdatacollective.org/gdmt/contributoridentifier</v>
       </c>
@@ -12600,11 +12600,11 @@
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A6" s="737"/>
-      <c r="B6" s="738"/>
-      <c r="C6" s="738"/>
-      <c r="D6" s="739"/>
-      <c r="E6" s="740"/>
+      <c r="A6" s="739"/>
+      <c r="B6" s="740"/>
+      <c r="C6" s="740"/>
+      <c r="D6" s="742"/>
+      <c r="E6" s="737"/>
       <c r="F6" s="34" t="s">
         <v>121</v>
       </c>
@@ -12632,11 +12632,11 @@
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A7" s="737"/>
-      <c r="B7" s="738"/>
-      <c r="C7" s="738"/>
-      <c r="D7" s="739"/>
-      <c r="E7" s="740"/>
+      <c r="A7" s="739"/>
+      <c r="B7" s="740"/>
+      <c r="C7" s="740"/>
+      <c r="D7" s="742"/>
+      <c r="E7" s="737"/>
       <c r="F7" s="34" t="s">
         <v>122</v>
       </c>
@@ -12664,17 +12664,17 @@
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A8" s="737"/>
-      <c r="B8" s="738" t="s">
+      <c r="A8" s="739"/>
+      <c r="B8" s="740" t="s">
         <v>465</v>
       </c>
-      <c r="C8" s="738" t="s">
+      <c r="C8" s="740" t="s">
         <v>456</v>
       </c>
-      <c r="D8" s="739" t="s">
+      <c r="D8" s="742" t="s">
         <v>54</v>
       </c>
-      <c r="E8" s="741" t="str">
+      <c r="E8" s="743" t="str">
         <f>Namespace &amp; LOWER($B8)</f>
         <v>http://vocab.fairdatacollective.org/gdmt/contributoraffiliation</v>
       </c>
@@ -12705,11 +12705,11 @@
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A9" s="737"/>
-      <c r="B9" s="738"/>
-      <c r="C9" s="738"/>
-      <c r="D9" s="739"/>
-      <c r="E9" s="741"/>
+      <c r="A9" s="739"/>
+      <c r="B9" s="740"/>
+      <c r="C9" s="740"/>
+      <c r="D9" s="742"/>
+      <c r="E9" s="743"/>
       <c r="F9" s="34" t="s">
         <v>123</v>
       </c>
@@ -12737,11 +12737,11 @@
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A10" s="737"/>
-      <c r="B10" s="738"/>
-      <c r="C10" s="738"/>
-      <c r="D10" s="739"/>
-      <c r="E10" s="741"/>
+      <c r="A10" s="739"/>
+      <c r="B10" s="740"/>
+      <c r="C10" s="740"/>
+      <c r="D10" s="742"/>
+      <c r="E10" s="743"/>
       <c r="F10" s="34" t="s">
         <v>458</v>
       </c>
@@ -12769,11 +12769,11 @@
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A11" s="737"/>
-      <c r="B11" s="738"/>
-      <c r="C11" s="738"/>
-      <c r="D11" s="739"/>
-      <c r="E11" s="741"/>
+      <c r="A11" s="739"/>
+      <c r="B11" s="740"/>
+      <c r="C11" s="740"/>
+      <c r="D11" s="742"/>
+      <c r="E11" s="743"/>
       <c r="F11" s="34" t="s">
         <v>125</v>
       </c>
@@ -12897,22 +12897,22 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="C5:C7"/>
+    <mergeCell ref="D5:D7"/>
+    <mergeCell ref="E5:E7"/>
+    <mergeCell ref="A8:A11"/>
+    <mergeCell ref="B8:B11"/>
+    <mergeCell ref="C8:C11"/>
+    <mergeCell ref="D8:D11"/>
+    <mergeCell ref="E8:E11"/>
     <mergeCell ref="E2:E4"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="B2:B4"/>
     <mergeCell ref="C2:C4"/>
     <mergeCell ref="D2:D4"/>
-    <mergeCell ref="A8:A11"/>
-    <mergeCell ref="B8:B11"/>
-    <mergeCell ref="C8:C11"/>
-    <mergeCell ref="D8:D11"/>
-    <mergeCell ref="E8:E11"/>
-    <mergeCell ref="A5:A7"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="C5:C7"/>
-    <mergeCell ref="D5:D7"/>
-    <mergeCell ref="E5:E7"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="L13" r:id="rId1" xr:uid="{9ABA6EE5-7A54-DF40-9E10-C757BCBA07FF}"/>

</xml_diff>